<commit_message>
JinHyeong 기획안(수정) ppt review_crawling_pos_neg.ipynb : 상품 리뷰 웹 크롤링 - 네이버쇼핑, 마켓커리 , 옥션
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B4A5FB-671D-4A47-A8F5-82754CFE99C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ADF597-602E-40F1-B57C-285CAFCFD34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="131">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,48 +426,133 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ㄴ 데이터셋(상품리뷰)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">모델링 제작에있어 참고할만한 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료가 존재해야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키워드 모델링 - 직접해보고 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt제작(간단히)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누가       : 구매자</t>
+  </si>
+  <si>
+    <t>언제       : 구매할 때</t>
+  </si>
+  <si>
+    <t>어디서    : 특정 웹쇼핑몰</t>
+  </si>
+  <si>
+    <t>무엇을    : 상품 리뷰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어떻게    : 간단한 요약, 구매후기 성향 분석 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">              상품추천 평점 예측 </t>
+  </si>
+  <si>
+    <t>왜          : 구매자들의 편리함</t>
+  </si>
+  <si>
+    <t>ppt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획서 발표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>https://wikidocs.net/94600</t>
-  </si>
-  <si>
-    <t>ㄴ 데이터셋(상품리뷰)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">모델링 제작에있어 참고할만한 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자료가 존재해야한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>키워드 모델링 - 직접해보고 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ppt제작(간단히)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>누가       : 구매자</t>
-  </si>
-  <si>
-    <t>언제       : 구매할 때</t>
-  </si>
-  <si>
-    <t>어디서    : 특정 웹쇼핑몰</t>
-  </si>
-  <si>
-    <t>무엇을    : 상품 리뷰</t>
-  </si>
-  <si>
-    <t xml:space="preserve">어떻게    : 간단한 요약, 구매후기 성향 분석 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">              상품추천 평점 예측 </t>
-  </si>
-  <si>
-    <t>왜          : 구매자들의 편리함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획서 ppt , word 파일 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제점 발견</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단순 주요 키워드 추출시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>긍정적인 키워드만 뽑힌다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>따라서 긍정/부정 분류 모델</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>먼저 설정하고 진행하는 것으로 결정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠팡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마켓컬리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버 쇼핑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옥션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 요약 모델 구성이 어렵다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>참고 자료 탐색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제점 해결방안 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>때에 따라서는 방향성을 바꿀 필요도 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">금일 업무 확인 </t>
+  </si>
+  <si>
+    <t>모델 관련 자료 탐색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 키워드 모델을 통해 키워드 분류시, 자주 사용되는 조사나 체언이 뽑히기 때문에 키워드 추출만으로는 리뷰 요약이 어렵다.</t>
+  </si>
+  <si>
+    <t>2. 긍정 부정 분류에서 애매모호한 긍정/부정 문 분류가 어렵다.</t>
+  </si>
+  <si>
+    <t>3. 리뷰 요약 부분에서 데이터의 클린봇(욕설 제거 등) 모델과 세심한 전처리 기능이 탑재된 모델을 필요로 한다.</t>
   </si>
 </sst>
 </file>
@@ -668,7 +753,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,6 +850,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -903,19 +1000,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
@@ -1036,6 +1120,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1045,7 +1144,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1289,13 +1388,13 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
@@ -1388,52 +1487,73 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="13" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="13" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="13" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1442,33 +1562,33 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1479,12 +1599,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2218,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDE6C63-9121-4583-87EA-DA9F0C78BEC1}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -2230,14 +2344,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="99"/>
@@ -2261,13 +2375,15 @@
       <c r="B5" s="39">
         <v>0.375</v>
       </c>
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="118"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="115" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1">
       <c r="B6" s="39">
@@ -2279,13 +2395,15 @@
       <c r="D6" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="145" t="s">
+      <c r="E6" s="128" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="116" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1">
       <c r="B7" s="39">
@@ -2295,9 +2413,13 @@
       <c r="D7" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="146"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="114" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="116" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="8" spans="2:7" s="105" customFormat="1" ht="50.1" customHeight="1">
       <c r="B8" s="101">
@@ -2322,7 +2444,9 @@
       <c r="E9" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="130" t="s">
+        <v>108</v>
+      </c>
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1">
@@ -2332,7 +2456,7 @@
       <c r="C10" s="123"/>
       <c r="D10" s="126"/>
       <c r="E10" s="126"/>
-      <c r="F10" s="34"/>
+      <c r="F10" s="131"/>
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
@@ -2342,7 +2466,7 @@
       <c r="C11" s="124"/>
       <c r="D11" s="127"/>
       <c r="E11" s="126"/>
-      <c r="F11" s="34"/>
+      <c r="F11" s="131"/>
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
@@ -2354,7 +2478,7 @@
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="127"/>
-      <c r="F12" s="34"/>
+      <c r="F12" s="132"/>
       <c r="G12" s="34" t="s">
         <v>26</v>
       </c>
@@ -2404,14 +2528,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C5:G5"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2436,35 +2561,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="136"/>
-      <c r="C3" s="137" t="s">
+      <c r="B3" s="143"/>
+      <c r="C3" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="136"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -2789,15 +2914,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
@@ -2896,7 +3023,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="141" t="s">
+      <c r="A2" s="148" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="104" t="s">
@@ -2908,9 +3035,12 @@
       <c r="D2" s="104" t="s">
         <v>90</v>
       </c>
+      <c r="E2" s="104" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="141"/>
+      <c r="A3" s="148"/>
       <c r="B3" s="104" t="s">
         <v>44</v>
       </c>
@@ -2918,17 +3048,23 @@
       <c r="D3" s="104" t="s">
         <v>92</v>
       </c>
+      <c r="E3" s="104" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="141"/>
+      <c r="A4" s="148"/>
       <c r="B4" s="106" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="104"/>
+      <c r="E4" s="104" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="141"/>
+      <c r="A5" s="148"/>
       <c r="B5" s="106" t="s">
         <v>46</v>
       </c>
@@ -2936,9 +3072,12 @@
       <c r="D5" s="104" t="s">
         <v>93</v>
       </c>
+      <c r="E5" s="104" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="6" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="141"/>
+      <c r="A6" s="148"/>
       <c r="B6" s="104" t="s">
         <v>47</v>
       </c>
@@ -2948,9 +3087,12 @@
       <c r="D6" s="104" t="s">
         <v>94</v>
       </c>
+      <c r="E6" s="104" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="7" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="142" t="s">
+      <c r="A7" s="149" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="104" t="s">
@@ -2962,21 +3104,25 @@
       <c r="D7" s="104" t="s">
         <v>95</v>
       </c>
+      <c r="E7" s="104" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="142"/>
+      <c r="A8" s="149"/>
       <c r="B8" s="104" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="104" t="s">
-        <v>96</v>
-      </c>
+      <c r="D8" s="106" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="104"/>
     </row>
     <row r="9" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="142"/>
+      <c r="A9" s="149"/>
       <c r="B9" s="104" t="s">
         <v>74</v>
       </c>
@@ -2984,11 +3130,12 @@
         <v>80</v>
       </c>
       <c r="D9" s="104" t="s">
-        <v>97</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E9" s="104"/>
     </row>
     <row r="10" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="142"/>
+      <c r="A10" s="149"/>
       <c r="B10" s="106" t="s">
         <v>75</v>
       </c>
@@ -2996,9 +3143,12 @@
         <v>81</v>
       </c>
       <c r="D10" s="104"/>
+      <c r="E10" s="104" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="142"/>
+      <c r="A11" s="149"/>
       <c r="B11" s="106" t="s">
         <v>76</v>
       </c>
@@ -3006,9 +3156,12 @@
         <v>82</v>
       </c>
       <c r="D11" s="104"/>
+      <c r="E11" s="104" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="143" t="s">
+      <c r="A12" s="150" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="107" t="s">
@@ -3018,63 +3171,81 @@
         <v>83</v>
       </c>
       <c r="D12" s="104"/>
+      <c r="E12" s="104" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="143"/>
+      <c r="A13" s="150"/>
       <c r="C13" s="104"/>
       <c r="D13" s="104"/>
+      <c r="E13" s="104" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="143"/>
+      <c r="A14" s="150"/>
       <c r="C14" s="104"/>
       <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
     </row>
     <row r="15" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="143"/>
+      <c r="A15" s="150"/>
       <c r="C15" s="104"/>
       <c r="D15" s="104"/>
+      <c r="E15" s="104" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="16" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="143"/>
+      <c r="A16" s="150"/>
       <c r="C16" s="104"/>
       <c r="D16" s="104"/>
-    </row>
-    <row r="17" spans="1:4" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="144" t="s">
+      <c r="E16" s="104" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="151" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="104"/>
       <c r="C17" s="104"/>
       <c r="D17" s="104"/>
-    </row>
-    <row r="18" spans="1:4" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="144"/>
+      <c r="E17" s="104"/>
+    </row>
+    <row r="18" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="151"/>
       <c r="B18" s="104"/>
       <c r="C18" s="104"/>
       <c r="D18" s="104"/>
-    </row>
-    <row r="19" spans="1:4" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="144"/>
+      <c r="E18" s="104"/>
+    </row>
+    <row r="19" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="151"/>
       <c r="B19" s="104"/>
       <c r="C19" s="104"/>
       <c r="D19" s="104"/>
-    </row>
-    <row r="20" spans="1:4" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="144"/>
+      <c r="E19" s="104"/>
+    </row>
+    <row r="20" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="151"/>
       <c r="B20" s="104"/>
       <c r="C20" s="104"/>
       <c r="D20" s="104"/>
-    </row>
-    <row r="21" spans="1:4" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="144"/>
+      <c r="E20" s="104"/>
+    </row>
+    <row r="21" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="151"/>
       <c r="B21" s="104"/>
       <c r="C21" s="104"/>
       <c r="D21" s="104"/>
-    </row>
-    <row r="22" spans="1:4" s="104" customFormat="1" ht="30" customHeight="1">
+      <c r="E21" s="104"/>
+    </row>
+    <row r="22" spans="1:5" s="104" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="111"/>
     </row>
-    <row r="23" spans="1:4" s="113" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:5" s="113" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="112" t="s">
         <v>69</v>
       </c>
@@ -3087,8 +3258,11 @@
       <c r="D23" s="112" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" customHeight="1">
+      <c r="E23" s="112" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -3096,10 +3270,13 @@
         <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -3110,18 +3287,24 @@
         <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" customHeight="1">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" customHeight="1">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -3132,23 +3315,32 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" customHeight="1">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" customHeight="1">
+      <c r="E28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" customHeight="1">
+      <c r="E29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>60</v>
       </c>
@@ -3156,12 +3348,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" customHeight="1">
+    <row r="31" spans="1:5" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1">
+    <row r="32" spans="1:5" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -3169,12 +3361,12 @@
         <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1">
       <c r="D33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1">
@@ -3185,7 +3377,7 @@
         <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1">
@@ -3193,7 +3385,7 @@
         <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1">
@@ -3201,7 +3393,7 @@
         <v>67</v>
       </c>
       <c r="D36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1">
@@ -3209,12 +3401,12 @@
         <v>68</v>
       </c>
       <c r="D37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1">
       <c r="D38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1">
@@ -3238,6 +3430,7 @@
     <hyperlink ref="B5" r:id="rId2" xr:uid="{B8CA46B6-F650-431E-8EDF-EE9360459047}"/>
     <hyperlink ref="B10" r:id="rId3" xr:uid="{96BBED21-73BF-4773-9C3E-882315F79376}"/>
     <hyperlink ref="B11" r:id="rId4" xr:uid="{EA841544-9F28-4D4C-A884-28E229F43738}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{B30208CB-E405-4159-805B-CA425C839CB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3259,14 +3452,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -3420,15 +3613,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -3595,15 +3788,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="24"/>
@@ -3770,14 +3963,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="96"/>
@@ -3931,15 +4124,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="97"/>
@@ -4059,10 +4252,10 @@
       <c r="E13" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="128" t="s">
+      <c r="F13" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="129"/>
+      <c r="G13" s="136"/>
       <c r="H13" s="32" t="s">
         <v>31</v>
       </c>
@@ -4106,13 +4299,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="98"/>
@@ -4248,35 +4441,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="143" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="136"/>
-      <c r="C3" s="137" t="s">
+      <c r="B3" s="143"/>
+      <c r="C3" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="136"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4495,42 +4688,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="138" t="s">
+      <c r="C23" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="139"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="139"/>
-      <c r="G23" s="140"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="147"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="130"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="132"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="139"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="130" t="s">
+      <c r="C25" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="131"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="131"/>
-      <c r="G25" s="132"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="139"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="135"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="141"/>
+      <c r="G26" s="142"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -4622,35 +4815,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="136"/>
-      <c r="C3" s="137" t="s">
+      <c r="B3" s="143"/>
+      <c r="C3" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="136"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">

</xml_diff>

<commit_message>
JinHyeong JinHyeong 22년12월26일 1주차 6일차 계획표 + 크롤링 방법
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EEDEB1-F145-4333-ADEC-8104C52C433B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848808D8-C2DB-4069-B8A6-FDFF803A69B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31455" yWindow="1200" windowWidth="18465" windowHeight="13950" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="150">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,10 +125,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17일 + 3일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>토(멘토링)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -552,6 +548,86 @@
   </si>
   <si>
     <t>리뷰 요약 모델 구성이 어렵다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16일 + 3일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 트릴리온 - 데이터셋 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분리수거 챗봇 , 제로웨이스트샵 관련 자료 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제를 변경하였습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트릴리온 - 제로웨이스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분리수거 챗봇 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위치 데이터를 통한 지도시각화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈페이지 구성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤 데이터셋이 필요하고 활용이 가능한지를 구체적으로 확인해보자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만일 진행 힘들경우 강사님 도움 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과물이 확실히 존재했으면 좋겠다. - 목적성 구체화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분업을 하자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너무 어렵게 생각하지 말자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델쪽으로 너무 많이 생각한게 아닐까</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금일 업무 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤 데이터셋을 찾아야하는지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터셋 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주간일지 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 구체화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -753,7 +829,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -859,6 +935,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,7 +1226,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1211,12 +1293,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1550,12 +1626,39 @@
     <xf numFmtId="20" fontId="13" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1599,6 +1702,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="18" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="19" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="19" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2332,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDE6C63-9121-4583-87EA-DA9F0C78BEC1}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -2344,191 +2465,191 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="99"/>
-      <c r="C4" s="99" t="s">
+      <c r="B4" s="97"/>
+      <c r="C4" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="99" t="s">
+      <c r="E4" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="99" t="s">
+      <c r="F4" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="99" t="s">
+      <c r="G4" s="97" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="133" t="s">
+      <c r="C5" s="131" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="113" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B6" s="37">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="126" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="114" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B7" s="37">
+        <v>0.45833333333333398</v>
+      </c>
+      <c r="C7" s="98"/>
+      <c r="D7" s="106" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="127"/>
+      <c r="F7" s="112" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" s="103" customFormat="1" ht="50.1" customHeight="1">
+      <c r="B8" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="69"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+    </row>
+    <row r="9" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B9" s="37">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="C9" s="120" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="123" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="123" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="128" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="133" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B10" s="37">
+        <v>0.58333333333333404</v>
+      </c>
+      <c r="C10" s="121"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="134"/>
+    </row>
+    <row r="11" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B11" s="37">
+        <v>0.625</v>
+      </c>
+      <c r="C11" s="122"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="134"/>
+    </row>
+    <row r="12" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B12" s="37">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="125"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="135"/>
+    </row>
+    <row r="13" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B13" s="37">
+        <v>0.70833333333333404</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="115" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="108" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="128" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="116" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
-        <v>0.45833333333333398</v>
-      </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="108" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="129"/>
-      <c r="F7" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="116" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" s="105" customFormat="1" ht="50.1" customHeight="1">
-      <c r="B8" s="101">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-    </row>
-    <row r="9" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="C9" s="122" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="125" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="125" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="130" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="34"/>
-    </row>
-    <row r="10" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
-        <v>0.58333333333333404</v>
-      </c>
-      <c r="C10" s="123"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="34"/>
-    </row>
-    <row r="11" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
-        <v>0.625</v>
-      </c>
-      <c r="C11" s="124"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="34"/>
-    </row>
-    <row r="12" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="C12" s="37" t="s">
+      <c r="E13" s="118"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="50.1" customHeight="1">
+      <c r="B14" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="18" spans="3:4" ht="26.25">
+      <c r="C18" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
-        <v>0.70833333333333404</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="119" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
-        <v>0.75</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-    </row>
-    <row r="18" spans="3:4" ht="26.25">
-      <c r="C18" s="103" t="s">
+      <c r="D18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="26.25">
+      <c r="C19" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="26.25">
-      <c r="C19" s="103" t="s">
+    </row>
+    <row r="20" spans="3:4" ht="26.25">
+      <c r="C20" s="101" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="26.25">
-      <c r="C20" s="103" t="s">
-        <v>42</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="C9:C11"/>
@@ -2537,6 +2658,7 @@
     <mergeCell ref="E9:E12"/>
     <mergeCell ref="F9:F12"/>
     <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G9:G12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2561,35 +2683,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="143"/>
-      <c r="C3" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
+      <c r="B3" s="150"/>
+      <c r="C3" s="151" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="143"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
+      <c r="B4" s="150"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -2618,19 +2740,19 @@
       <c r="B7" s="9"/>
       <c r="C7" s="12"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="31">
+      <c r="E7" s="29">
         <v>1</v>
       </c>
       <c r="F7" s="6">
         <v>2</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="47">
         <v>3</v>
       </c>
-      <c r="H7" s="80">
+      <c r="H7" s="78">
         <v>4</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="10"/>
@@ -2638,10 +2760,10 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
+        <v>22</v>
+      </c>
+      <c r="G8" s="53"/>
+      <c r="H8" s="54"/>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="10"/>
@@ -2649,8 +2771,8 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="10"/>
@@ -2658,8 +2780,8 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="11"/>
@@ -2667,236 +2789,236 @@
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="47">
+      <c r="B12" s="45">
         <v>5</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="45">
         <v>6</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="60">
         <v>7</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="60">
         <v>8</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="60">
         <v>9</v>
       </c>
-      <c r="G12" s="62">
+      <c r="G12" s="60">
         <v>10</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="61">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="52"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="52"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="52"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="65"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="57"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="67"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="65"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="47">
+      <c r="B17" s="45">
         <v>12</v>
       </c>
-      <c r="C17" s="62">
+      <c r="C17" s="60">
         <v>13</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="60">
         <v>14</v>
       </c>
-      <c r="E17" s="62">
+      <c r="E17" s="60">
         <v>15</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="60">
         <v>16</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="60">
         <v>17</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H17" s="61">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="52"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="65"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="63"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="52"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="65"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="63"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="52"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="65"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="63"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="57"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="67"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="65"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="47">
+      <c r="B22" s="45">
         <v>19</v>
       </c>
-      <c r="C22" s="62">
+      <c r="C22" s="60">
         <v>20</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="60">
         <v>21</v>
       </c>
-      <c r="E22" s="62">
+      <c r="E22" s="60">
         <v>22</v>
       </c>
-      <c r="F22" s="62">
+      <c r="F22" s="60">
         <v>23</v>
       </c>
-      <c r="G22" s="62">
+      <c r="G22" s="60">
         <v>24</v>
       </c>
-      <c r="H22" s="63">
+      <c r="H22" s="61">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="52"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="65"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="63"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="52"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="53"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="51"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="52"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="53"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="57"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="75"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="73"/>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="47">
+      <c r="B27" s="45">
         <v>26</v>
       </c>
-      <c r="C27" s="62">
+      <c r="C27" s="60">
         <v>27</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="60">
         <v>28</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="63"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="61"/>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="76"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="76"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="74"/>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="76"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="76"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="74"/>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="76"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="76"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="74"/>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="78"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="78"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2914,515 +3036,593 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="32.75" customWidth="1"/>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.75" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
-      <c r="B1" s="87">
+      <c r="B1" s="85">
         <v>44914</v>
       </c>
-      <c r="C1" s="87">
+      <c r="C1" s="85">
         <v>44915</v>
       </c>
-      <c r="D1" s="87">
+      <c r="D1" s="85">
         <v>44916</v>
       </c>
-      <c r="E1" s="87">
+      <c r="E1" s="85">
         <v>44917</v>
       </c>
-      <c r="F1" s="87">
+      <c r="F1" s="85">
         <v>44918</v>
       </c>
-      <c r="G1" s="87">
+      <c r="G1" s="85">
         <v>44921</v>
       </c>
-      <c r="H1" s="87">
+      <c r="H1" s="85">
         <v>44922</v>
       </c>
-      <c r="I1" s="87">
+      <c r="I1" s="85">
         <v>44923</v>
       </c>
-      <c r="J1" s="87">
+      <c r="J1" s="85">
         <v>44924</v>
       </c>
-      <c r="K1" s="87">
+      <c r="K1" s="85">
         <v>44925</v>
       </c>
-      <c r="L1" s="87">
+      <c r="L1" s="85">
         <v>44928</v>
       </c>
-      <c r="M1" s="87">
+      <c r="M1" s="85">
         <v>44929</v>
       </c>
-      <c r="N1" s="87">
+      <c r="N1" s="85">
         <v>44930</v>
       </c>
-      <c r="O1" s="87">
+      <c r="O1" s="85">
         <v>44931</v>
       </c>
-      <c r="P1" s="87">
+      <c r="P1" s="85">
         <v>44932</v>
       </c>
-      <c r="Q1" s="87">
+      <c r="Q1" s="85">
         <v>44933</v>
       </c>
-      <c r="R1" s="87">
+      <c r="R1" s="85">
         <v>44936</v>
       </c>
-      <c r="S1" s="87">
+      <c r="S1" s="85">
         <v>44937</v>
       </c>
-      <c r="T1" s="87">
+      <c r="T1" s="85">
         <v>44938</v>
       </c>
-      <c r="U1" s="87">
+      <c r="U1" s="85">
         <v>44939</v>
       </c>
-      <c r="V1" s="87">
+      <c r="V1" s="85">
         <v>44940</v>
       </c>
-      <c r="W1" s="87">
+      <c r="W1" s="85">
         <v>44943</v>
       </c>
-      <c r="X1" s="87">
+      <c r="X1" s="85">
         <v>44944</v>
       </c>
-      <c r="Y1" s="87">
+      <c r="Y1" s="85">
         <v>44945</v>
       </c>
-      <c r="Z1" s="87">
+      <c r="Z1" s="85">
         <v>44946</v>
       </c>
-      <c r="AA1" s="87">
+      <c r="AA1" s="85">
         <v>44951</v>
       </c>
-      <c r="AB1" s="87">
+      <c r="AB1" s="85">
         <v>44952</v>
       </c>
-      <c r="AC1" s="87">
+      <c r="AC1" s="85">
         <v>44953</v>
       </c>
-      <c r="AD1" s="87">
+      <c r="AD1" s="85">
         <v>44954</v>
       </c>
-      <c r="AE1" s="87">
+      <c r="AE1" s="85">
         <v>44957</v>
       </c>
-      <c r="AF1" s="87">
+      <c r="AF1" s="85">
         <v>44958</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="148" t="s">
+    <row r="2" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="155" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="102" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="102" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="102" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="164" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="155"/>
+      <c r="B3" s="102" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="102" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="102" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="164"/>
+    </row>
+    <row r="4" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="155"/>
+      <c r="B4" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="102" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="164"/>
+    </row>
+    <row r="5" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="155"/>
+      <c r="B5" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="102" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="102" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="164"/>
+    </row>
+    <row r="6" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="155"/>
+      <c r="B6" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="102" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="102" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="164"/>
+    </row>
+    <row r="7" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="104" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="104" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="104" t="s">
+      <c r="B7" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="102" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="102"/>
+      <c r="G7" s="164"/>
+    </row>
+    <row r="8" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="156"/>
+      <c r="B8" s="102" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="102" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="164"/>
+    </row>
+    <row r="9" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="156"/>
+      <c r="B9" s="102" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="164"/>
+    </row>
+    <row r="10" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="156"/>
+      <c r="B10" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="102"/>
+      <c r="G10" s="164"/>
+    </row>
+    <row r="11" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="156"/>
+      <c r="B11" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="102"/>
+      <c r="G11" s="164"/>
+    </row>
+    <row r="12" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="157" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="102" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="102"/>
+      <c r="G12" s="164"/>
+    </row>
+    <row r="13" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="157"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="102"/>
+      <c r="G13" s="164"/>
+    </row>
+    <row r="14" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A14" s="157"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="164"/>
+    </row>
+    <row r="15" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="157"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="102"/>
+      <c r="G15" s="164"/>
+    </row>
+    <row r="16" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A16" s="157"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="102"/>
+      <c r="G16" s="164"/>
+    </row>
+    <row r="17" spans="1:7" s="91" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="102"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="164"/>
+    </row>
+    <row r="18" spans="1:7" s="91" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="158"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="164"/>
+    </row>
+    <row r="19" spans="1:7" s="91" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="158"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="164"/>
+    </row>
+    <row r="20" spans="1:7" s="91" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="158"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="164"/>
+    </row>
+    <row r="21" spans="1:7" s="91" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="158"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="164"/>
+    </row>
+    <row r="22" spans="1:7" s="102" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="109"/>
+    </row>
+    <row r="23" spans="1:7" s="111" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="111" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="110" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" customHeight="1">
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" customHeight="1">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" customHeight="1">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="104" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="148"/>
-      <c r="B3" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="104" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="148"/>
-      <c r="B4" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="106" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="104" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="148"/>
-      <c r="B6" s="104" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="104" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="104" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="104" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="149" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="104" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="104" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="104" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="149"/>
-      <c r="B8" s="104" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="104" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="106" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="104"/>
-    </row>
-    <row r="9" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="149"/>
-      <c r="B9" s="104" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="104" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="104" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="104"/>
-    </row>
-    <row r="10" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="149"/>
-      <c r="B10" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="104" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="149"/>
-      <c r="B11" s="106" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="104" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="150" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="107" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="104" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="150"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="150"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-    </row>
-    <row r="15" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="150"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" s="92" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="150"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="104" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="151" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-    </row>
-    <row r="18" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="151"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-    </row>
-    <row r="19" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="151"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-    </row>
-    <row r="20" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="151"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-    </row>
-    <row r="21" spans="1:5" s="93" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="151"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-    </row>
-    <row r="22" spans="1:5" s="104" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="111"/>
-    </row>
-    <row r="23" spans="1:5" s="113" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="113" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="112" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="30" customHeight="1">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
         <v>100</v>
-      </c>
-      <c r="E27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" customHeight="1">
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" customHeight="1">
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" customHeight="1">
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" customHeight="1">
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1">
       <c r="D33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1">
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1">
       <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" customHeight="1">
+      <c r="B37" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" customHeight="1">
-      <c r="B37" s="109" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1">
       <c r="D38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1">
       <c r="A39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="110" t="s">
-        <v>72</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A17:A21"/>
+    <mergeCell ref="G2:G21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3440,8 +3640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251ECE8D-9668-40EA-AFB2-EB0A37392AB0}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -3452,143 +3652,155 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="94"/>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="92" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="159" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B8" s="39">
+      <c r="B8" s="99">
         <v>0.5</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="C9" s="161" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="C12" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="119" t="s">
+      <c r="C13" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="81" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <v>0.75</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="D13:F13"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3613,152 +3825,152 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="95"/>
-      <c r="C4" s="95" t="s">
+      <c r="B4" s="93"/>
+      <c r="C4" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="95" t="s">
-        <v>21</v>
+      <c r="H4" s="93" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="32"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="32"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>0.5</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="32"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="32"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="32"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="32"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="119" t="s">
+      <c r="C13" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="32" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="14" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <v>0.75</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3788,152 +4000,152 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="24"/>
-      <c r="C4" s="69" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="24" t="s">
-        <v>21</v>
+      <c r="H4" s="22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="32"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="32"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>0.5</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="32"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="32"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="32"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="32"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="119" t="s">
+      <c r="C13" s="69"/>
+      <c r="D13" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="118"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="120"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="32" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="14" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <v>0.75</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3963,138 +4175,138 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="96"/>
-      <c r="C4" s="69" t="s">
+      <c r="B4" s="94"/>
+      <c r="C4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="96" t="s">
+      <c r="F4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="94" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>0.5</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="119" t="s">
+      <c r="C13" s="69"/>
+      <c r="D13" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="119"/>
+      <c r="G13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="121"/>
-      <c r="G13" s="84" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <v>0.75</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4124,152 +4336,152 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="97"/>
-      <c r="C4" s="69" t="s">
+      <c r="B4" s="95"/>
+      <c r="C4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="95" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="32"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="32"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>0.5</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="32"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="32"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="32"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="32"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="135" t="s">
+      <c r="C13" s="69"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="136" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="137"/>
+      <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="136"/>
-      <c r="H13" s="32" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="14" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <v>0.75</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4299,120 +4511,120 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B4" s="98"/>
-      <c r="C4" s="69" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="98" t="s">
+      <c r="E4" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="98" t="s">
-        <v>22</v>
+      <c r="F4" s="96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>0.5</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="32"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <v>0.75</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4429,8 +4641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:G26"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -4441,35 +4653,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="143"/>
-      <c r="C3" s="144" t="s">
+      <c r="B3" s="150"/>
+      <c r="C3" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="143"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
+      <c r="B4" s="150"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4495,191 +4707,191 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50">
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48">
         <v>1</v>
       </c>
-      <c r="G7" s="50">
+      <c r="G7" s="48">
         <v>2</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="54"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="47">
+      <c r="B12" s="45">
         <v>4</v>
       </c>
-      <c r="C12" s="62">
+      <c r="C12" s="60">
         <v>5</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="60">
         <v>6</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="60">
         <v>7</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="60">
         <v>8</v>
       </c>
-      <c r="G12" s="62">
+      <c r="G12" s="60">
         <v>9</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="61">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="52"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="52"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="52"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="65"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="57"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="67"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="65"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="47">
+      <c r="B17" s="45">
         <v>11</v>
       </c>
-      <c r="C17" s="62">
+      <c r="C17" s="60">
         <v>12</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="60">
         <v>13</v>
       </c>
-      <c r="E17" s="62">
+      <c r="E17" s="60">
         <v>14</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="60">
         <v>15</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="60">
         <v>16</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H17" s="61">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="52"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="65"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="63"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="52"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="65"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="63"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="52"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="65"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="63"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="57"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="67"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="65"/>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="9">
         <v>18</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="23">
         <v>19</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="23">
         <v>20</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="23">
         <v>21</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="23">
         <v>22</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="23">
         <v>23</v>
       </c>
       <c r="H22" s="15">
@@ -4688,61 +4900,61 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="145" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="146"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="146"/>
-      <c r="G23" s="147"/>
+      <c r="C23" s="152" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="153"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="153"/>
+      <c r="G23" s="154"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="137"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="139"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="146"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="137" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="138"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="139"/>
+      <c r="C25" s="144" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="146"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="141"/>
-      <c r="E26" s="141"/>
-      <c r="F26" s="141"/>
-      <c r="G26" s="142"/>
+      <c r="C26" s="147"/>
+      <c r="D26" s="148"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="148"/>
+      <c r="G26" s="149"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="9">
         <v>25</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="44">
         <v>26</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="23">
         <v>27</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="23">
         <v>28</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="23">
         <v>29</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="23">
         <v>30</v>
       </c>
       <c r="H27" s="15">
@@ -4751,42 +4963,48 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
+      <c r="C28" s="138" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="140"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="140"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="C30" s="138" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="139"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="140"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="143"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="C28:G29"/>
+    <mergeCell ref="C30:G31"/>
     <mergeCell ref="C25:G26"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:H2"/>
@@ -4803,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -4815,35 +5033,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="143"/>
-      <c r="C3" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
+      <c r="B3" s="150"/>
+      <c r="C3" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="143"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
+      <c r="B4" s="150"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4872,145 +5090,145 @@
       <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="23">
         <v>2</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>3</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>4</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>5</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <v>6</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="38">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="9">
         <v>8</v>
       </c>
-      <c r="C12" s="62">
+      <c r="C12" s="60">
         <v>9</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="23">
         <v>10</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="23">
         <v>11</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="23">
         <v>12</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="23">
         <v>13</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="38">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="26"/>
-      <c r="C13" s="64" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="26"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="68" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="66" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="26"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="27"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="9">
         <v>15</v>
       </c>
-      <c r="C17" s="62">
+      <c r="C17" s="60">
         <v>16</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="23">
         <v>17</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="23">
         <v>18</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="23">
         <v>19</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="60">
         <v>20</v>
       </c>
       <c r="H17" s="9">
@@ -5018,42 +5236,44 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="26"/>
-      <c r="C18" s="64" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="26"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="26"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="24"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="27"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="9">
@@ -5065,108 +5285,108 @@
       <c r="D22" s="9">
         <v>24</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="23">
         <v>25</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="23">
         <v>26</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="23">
         <v>27</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="38">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28" t="s">
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="9">
         <v>29</v>
       </c>
-      <c r="C27" s="62">
+      <c r="C27" s="60">
         <v>30</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="39">
         <v>31</v>
       </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="45"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="28"/>
-      <c r="C28" s="88" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="28"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="28"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="29"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JinHyeong SubBranch 엑셀 수정
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB366F4A-C5A9-4D13-96E2-6EDD9FF3237B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8799BD-8DBF-4F0A-BBD8-6415578BBC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="319">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1110,13 +1110,6 @@
   </si>
   <si>
     <t>1am 스파클링 10,000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://smartstore.naver.com/pickydiet/products/5135269051?NaPm=ct%3Dlc9ui8js%7Cci%3D031772152f1ad9ad9fe80302366268281112abd9%7Ctr%3Dslsl%7Csn%3D681472%7Chk%3D77d1d7d09008f5506d7fd51a86ae0889ee1d19eb</t>
-  </si>
-  <si>
-    <t>1am스파클링 네이버 스마트스토어</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2369,6 +2362,36 @@
     <xf numFmtId="0" fontId="12" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2519,6 +2542,33 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2532,63 +2582,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3334,14 +3327,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="96"/>
@@ -3365,12 +3358,12 @@
       <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
+      <c r="D5" s="159"/>
+      <c r="E5" s="159"/>
+      <c r="F5" s="159"/>
       <c r="G5" s="112" t="s">
         <v>108</v>
       </c>
@@ -3385,7 +3378,7 @@
       <c r="D6" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="143" t="s">
+      <c r="E6" s="153" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -3403,7 +3396,7 @@
       <c r="D7" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="144"/>
+      <c r="E7" s="154"/>
       <c r="F7" s="111" t="s">
         <v>107</v>
       </c>
@@ -3425,19 +3418,19 @@
       <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="C9" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="140" t="s">
+      <c r="D9" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="140" t="s">
+      <c r="E9" s="150" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="145" t="s">
+      <c r="F9" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="150" t="s">
+      <c r="G9" s="160" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3445,21 +3438,21 @@
       <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="138"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="146"/>
-      <c r="G10" s="151"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="161"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="139"/>
-      <c r="D11" s="142"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="151"/>
+      <c r="C11" s="149"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="161"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="37">
@@ -3469,9 +3462,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="142"/>
-      <c r="F12" s="147"/>
-      <c r="G12" s="152"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="157"/>
+      <c r="G12" s="162"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="37">
@@ -3480,11 +3473,11 @@
       <c r="C13" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="134" t="s">
+      <c r="D13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="135"/>
-      <c r="F13" s="136"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="146"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -3552,35 +3545,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="177"/>
-      <c r="C3" s="178" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="177"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -3905,9 +3898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M5" sqref="M5"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4016,7 +4009,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="201" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="101" t="s">
@@ -4034,7 +4027,7 @@
       <c r="F2" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="186" t="s">
+      <c r="G2" s="205" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="101"/>
@@ -4043,11 +4036,11 @@
         <v>177</v>
       </c>
       <c r="K2" s="87" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="182"/>
+      <c r="A3" s="201"/>
       <c r="B3" s="101" t="s">
         <v>43</v>
       </c>
@@ -4061,7 +4054,7 @@
       <c r="F3" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="186"/>
+      <c r="G3" s="205"/>
       <c r="H3" s="101"/>
       <c r="I3" s="114" t="s">
         <v>164</v>
@@ -4069,12 +4062,12 @@
       <c r="J3" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="190" t="s">
-        <v>291</v>
+      <c r="K3" s="135" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="182"/>
+      <c r="A4" s="201"/>
       <c r="B4" s="103" t="s">
         <v>44</v>
       </c>
@@ -4086,7 +4079,7 @@
       <c r="F4" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="186"/>
+      <c r="G4" s="205"/>
       <c r="H4" s="101"/>
       <c r="I4" s="101" t="s">
         <v>165</v>
@@ -4095,11 +4088,11 @@
         <v>179</v>
       </c>
       <c r="K4" s="87" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="182"/>
+      <c r="A5" s="201"/>
       <c r="B5" s="103" t="s">
         <v>45</v>
       </c>
@@ -4113,7 +4106,7 @@
       <c r="F5" s="101" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="186"/>
+      <c r="G5" s="205"/>
       <c r="H5" s="101"/>
       <c r="I5" s="101" t="s">
         <v>166</v>
@@ -4123,7 +4116,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="182"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="101" t="s">
         <v>46</v>
       </c>
@@ -4139,7 +4132,7 @@
       <c r="F6" s="101" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="186"/>
+      <c r="G6" s="205"/>
       <c r="H6" s="101"/>
       <c r="I6" s="101" t="s">
         <v>168</v>
@@ -4147,7 +4140,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="183" t="s">
+      <c r="A7" s="202" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="101" t="s">
@@ -4163,7 +4156,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="101"/>
-      <c r="G7" s="186"/>
+      <c r="G7" s="205"/>
       <c r="H7" s="101" t="s">
         <v>150</v>
       </c>
@@ -4178,7 +4171,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="183"/>
+      <c r="A8" s="202"/>
       <c r="B8" s="101" t="s">
         <v>48</v>
       </c>
@@ -4190,7 +4183,7 @@
       </c>
       <c r="E8" s="101"/>
       <c r="F8" s="101"/>
-      <c r="G8" s="186"/>
+      <c r="G8" s="205"/>
       <c r="H8" s="101" t="s">
         <v>151</v>
       </c>
@@ -4205,7 +4198,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="183"/>
+      <c r="A9" s="202"/>
       <c r="B9" s="101" t="s">
         <v>73</v>
       </c>
@@ -4217,17 +4210,17 @@
       </c>
       <c r="E9" s="101"/>
       <c r="F9" s="101"/>
-      <c r="G9" s="186"/>
+      <c r="G9" s="205"/>
       <c r="H9" s="101" t="s">
         <v>152</v>
       </c>
       <c r="I9" s="101"/>
       <c r="K9" s="88" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="183"/>
+      <c r="A10" s="202"/>
       <c r="B10" s="103" t="s">
         <v>74</v>
       </c>
@@ -4239,15 +4232,15 @@
         <v>117</v>
       </c>
       <c r="F10" s="101"/>
-      <c r="G10" s="186"/>
+      <c r="G10" s="205"/>
       <c r="H10" s="101"/>
       <c r="I10" s="101"/>
       <c r="K10" s="88" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="183"/>
+      <c r="A11" s="202"/>
       <c r="B11" s="103" t="s">
         <v>75</v>
       </c>
@@ -4259,12 +4252,12 @@
         <v>118</v>
       </c>
       <c r="F11" s="101"/>
-      <c r="G11" s="186"/>
+      <c r="G11" s="205"/>
       <c r="H11" s="101"/>
       <c r="I11" s="101"/>
     </row>
     <row r="12" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="184" t="s">
+      <c r="A12" s="203" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="104" t="s">
@@ -4278,7 +4271,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="101"/>
-      <c r="G12" s="186"/>
+      <c r="G12" s="205"/>
       <c r="H12" s="101" t="s">
         <v>153</v>
       </c>
@@ -4291,14 +4284,14 @@
       </c>
     </row>
     <row r="13" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="184"/>
+      <c r="A13" s="203"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
       <c r="E13" s="101" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="101"/>
-      <c r="G13" s="186"/>
+      <c r="G13" s="205"/>
       <c r="H13" s="101" t="s">
         <v>154</v>
       </c>
@@ -4308,47 +4301,47 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="184"/>
+      <c r="A14" s="203"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
       <c r="E14" s="101"/>
       <c r="F14" s="101"/>
-      <c r="G14" s="186"/>
+      <c r="G14" s="205"/>
       <c r="H14" s="101" t="s">
         <v>155</v>
       </c>
       <c r="I14" s="101"/>
     </row>
     <row r="15" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="184"/>
+      <c r="A15" s="203"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
       <c r="E15" s="101" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="101"/>
-      <c r="G15" s="186"/>
+      <c r="G15" s="205"/>
       <c r="H15" s="101" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="101"/>
     </row>
     <row r="16" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="184"/>
+      <c r="A16" s="203"/>
       <c r="C16" s="101"/>
       <c r="D16" s="101"/>
       <c r="E16" s="101" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="101"/>
-      <c r="G16" s="186"/>
+      <c r="G16" s="205"/>
       <c r="H16" s="101" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="101"/>
     </row>
     <row r="17" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="185" t="s">
+      <c r="A17" s="204" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="101"/>
@@ -4356,7 +4349,7 @@
       <c r="D17" s="101"/>
       <c r="E17" s="101"/>
       <c r="F17" s="101"/>
-      <c r="G17" s="186"/>
+      <c r="G17" s="205"/>
       <c r="H17" s="101"/>
       <c r="I17" s="101"/>
       <c r="J17" s="90" t="s">
@@ -4367,46 +4360,46 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="185"/>
+      <c r="A18" s="204"/>
       <c r="B18" s="101"/>
       <c r="C18" s="101"/>
       <c r="D18" s="101"/>
       <c r="E18" s="101"/>
       <c r="F18" s="101"/>
-      <c r="G18" s="186"/>
+      <c r="G18" s="205"/>
       <c r="H18" s="101"/>
       <c r="I18" s="101"/>
     </row>
     <row r="19" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="185"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="101"/>
       <c r="C19" s="101"/>
       <c r="D19" s="101"/>
       <c r="E19" s="101"/>
       <c r="F19" s="101"/>
-      <c r="G19" s="186"/>
+      <c r="G19" s="205"/>
       <c r="H19" s="101"/>
       <c r="I19" s="101"/>
     </row>
     <row r="20" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="185"/>
+      <c r="A20" s="204"/>
       <c r="B20" s="101"/>
       <c r="C20" s="101"/>
       <c r="D20" s="101"/>
       <c r="E20" s="101"/>
       <c r="F20" s="101"/>
-      <c r="G20" s="186"/>
+      <c r="G20" s="205"/>
       <c r="H20" s="101"/>
       <c r="I20" s="101"/>
     </row>
     <row r="21" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="185"/>
+      <c r="A21" s="204"/>
       <c r="B21" s="101"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
       <c r="E21" s="101"/>
       <c r="F21" s="101"/>
-      <c r="G21" s="186"/>
+      <c r="G21" s="205"/>
       <c r="H21" s="101"/>
       <c r="I21" s="101"/>
     </row>
@@ -4656,8 +4649,8 @@
       <c r="D36" t="s">
         <v>104</v>
       </c>
-      <c r="J36" s="188" t="s">
-        <v>300</v>
+      <c r="J36" s="133" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1">
@@ -4890,8 +4883,8 @@
       </c>
     </row>
     <row r="120" spans="10:10" ht="30" customHeight="1">
-      <c r="J120" s="188" t="s">
-        <v>297</v>
+      <c r="J120" s="133" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="123" spans="10:10" ht="30" customHeight="1">
@@ -4915,8 +4908,8 @@
       </c>
     </row>
     <row r="130" spans="10:10" ht="30" customHeight="1">
-      <c r="J130" s="188" t="s">
-        <v>299</v>
+      <c r="J130" s="133" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="10:10" ht="30" customHeight="1">
@@ -4985,8 +4978,8 @@
       </c>
     </row>
     <row r="159" spans="10:10" ht="30" customHeight="1">
-      <c r="J159" s="188" t="s">
-        <v>298</v>
+      <c r="J159" s="133" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="162" spans="10:10" ht="30" customHeight="1">
@@ -5077,11 +5070,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4682B6DF-860A-46A3-B003-691AA560AE2A}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="17" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="17" topLeftCell="N20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5126,7 +5119,7 @@
       <c r="D2" s="120">
         <v>44924</v>
       </c>
-      <c r="E2" s="191">
+      <c r="E2" s="136">
         <v>44924</v>
       </c>
       <c r="F2" s="120">
@@ -5183,14 +5176,14 @@
       <c r="D3" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E3" s="192" t="s">
+      <c r="E3" s="137" t="s">
         <v>257</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>258</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>257</v>
@@ -5220,10 +5213,10 @@
         <v>118</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>257</v>
@@ -5240,50 +5233,50 @@
       <c r="D4" s="126" t="s">
         <v>261</v>
       </c>
-      <c r="E4" s="193" t="s">
+      <c r="E4" s="138" t="s">
         <v>262</v>
       </c>
       <c r="F4" s="126" t="s">
         <v>263</v>
       </c>
-      <c r="G4" s="187" t="s">
-        <v>293</v>
-      </c>
-      <c r="H4" s="187" t="s">
-        <v>296</v>
-      </c>
-      <c r="I4" s="187" t="s">
+      <c r="G4" s="132" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="132" t="s">
+        <v>294</v>
+      </c>
+      <c r="I4" s="132" t="s">
         <v>262</v>
       </c>
-      <c r="J4" s="187" t="s">
+      <c r="J4" s="132" t="s">
+        <v>299</v>
+      </c>
+      <c r="K4" s="132" t="s">
+        <v>310</v>
+      </c>
+      <c r="L4" s="132" t="s">
+        <v>311</v>
+      </c>
+      <c r="M4" s="127" t="s">
+        <v>309</v>
+      </c>
+      <c r="N4" s="132" t="s">
+        <v>305</v>
+      </c>
+      <c r="O4" s="132" t="s">
         <v>301</v>
       </c>
-      <c r="K4" s="187" t="s">
+      <c r="P4" s="132" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q4" s="132" t="s">
+        <v>303</v>
+      </c>
+      <c r="R4" s="132" t="s">
         <v>312</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="S4" s="132" t="s">
         <v>313</v>
-      </c>
-      <c r="M4" s="127" t="s">
-        <v>311</v>
-      </c>
-      <c r="N4" s="187" t="s">
-        <v>307</v>
-      </c>
-      <c r="O4" s="187" t="s">
-        <v>303</v>
-      </c>
-      <c r="P4" s="187" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q4" s="187" t="s">
-        <v>305</v>
-      </c>
-      <c r="R4" s="187" t="s">
-        <v>314</v>
-      </c>
-      <c r="S4" s="187" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5294,7 +5287,7 @@
         <f>SUM(C5:AC5)</f>
         <v>19127</v>
       </c>
-      <c r="E5" s="192"/>
+      <c r="E5" s="137"/>
       <c r="J5" s="1">
         <v>10000</v>
       </c>
@@ -5313,7 +5306,7 @@
         <f t="shared" ref="B6:B19" si="0">SUM(C6:AC6)</f>
         <v>18414</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="137"/>
       <c r="P6" s="1">
         <v>2000</v>
       </c>
@@ -5332,7 +5325,7 @@
       <c r="D7" s="1">
         <v>11040</v>
       </c>
-      <c r="E7" s="192"/>
+      <c r="E7" s="137"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="122" t="s">
@@ -5342,7 +5335,7 @@
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="E8" s="192"/>
+      <c r="E8" s="137"/>
       <c r="M8" s="1">
         <v>5500</v>
       </c>
@@ -5358,7 +5351,7 @@
         <f t="shared" si="0"/>
         <v>8626</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="137"/>
       <c r="O9" s="1">
         <v>8626</v>
       </c>
@@ -5371,7 +5364,7 @@
         <f t="shared" si="0"/>
         <v>6827</v>
       </c>
-      <c r="E10" s="192"/>
+      <c r="E10" s="137"/>
       <c r="S10" s="1">
         <v>6827</v>
       </c>
@@ -5384,7 +5377,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="192"/>
+      <c r="E11" s="137"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="122" t="s">
@@ -5394,7 +5387,7 @@
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="E12" s="192"/>
+      <c r="E12" s="137"/>
       <c r="F12" s="1">
         <v>2000</v>
       </c>
@@ -5407,7 +5400,7 @@
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="E13" s="192"/>
+      <c r="E13" s="137"/>
       <c r="H13" s="1">
         <v>10000</v>
       </c>
@@ -5420,7 +5413,7 @@
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="E14" s="192"/>
+      <c r="E14" s="137"/>
       <c r="I14" s="1">
         <v>10000</v>
       </c>
@@ -5433,30 +5426,30 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15" s="192"/>
+      <c r="E15" s="137"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="189" t="s">
-        <v>292</v>
+      <c r="A16" s="134" t="s">
+        <v>290</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>10877</v>
       </c>
-      <c r="E16" s="192"/>
+      <c r="E16" s="137"/>
       <c r="R16" s="1">
         <v>10877</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="192" customFormat="1">
-      <c r="A17" s="196" t="s">
+    <row r="17" spans="1:14" s="137" customFormat="1">
+      <c r="A17" s="141" t="s">
         <v>275</v>
       </c>
-      <c r="B17" s="192">
+      <c r="B17" s="137">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="C17" s="192">
+      <c r="C17" s="137">
         <v>1500</v>
       </c>
     </row>
@@ -5468,7 +5461,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="137"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="122" t="s">
@@ -5478,7 +5471,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="192"/>
+      <c r="E19" s="137"/>
     </row>
     <row r="20" spans="1:14" s="129" customFormat="1" ht="17.25" thickBot="1">
       <c r="A20" s="128" t="s">
@@ -5488,7 +5481,7 @@
         <f>SUM(C20:AC20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="194"/>
+      <c r="E20" s="139"/>
     </row>
     <row r="21" spans="1:14" ht="17.25" thickTop="1"/>
     <row r="23" spans="1:14">
@@ -5496,39 +5489,33 @@
         <v>279</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="B24" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="M24" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="B25" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="M25" s="195" t="s">
-        <v>308</v>
-      </c>
-      <c r="N25" s="195"/>
+      <c r="M25" s="140" t="s">
+        <v>306</v>
+      </c>
+      <c r="N25" s="140"/>
     </row>
     <row r="27" spans="1:14">
       <c r="M27" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="M28" s="195" t="s">
-        <v>309</v>
-      </c>
-      <c r="N28" s="195"/>
+      <c r="M28" s="140" t="s">
+        <v>307</v>
+      </c>
+      <c r="N28" s="140"/>
     </row>
     <row r="43" spans="11:11">
-      <c r="K43" s="195"/>
+      <c r="K43" s="140"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5572,14 +5559,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -5623,19 +5610,19 @@
       <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="163" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="140" t="s">
+      <c r="D6" s="150" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="158" t="s">
+      <c r="E6" s="168" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="115" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="161" t="s">
+      <c r="G6" s="171" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5643,13 +5630,13 @@
       <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="154"/>
-      <c r="D7" s="142"/>
-      <c r="E7" s="159"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="169"/>
       <c r="F7" s="115" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="162"/>
+      <c r="G7" s="172"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="98">
@@ -5665,13 +5652,13 @@
       <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="155" t="s">
+      <c r="C9" s="165" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="140" t="s">
+      <c r="D9" s="150" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="158"/>
+      <c r="E9" s="168"/>
       <c r="F9" s="115" t="s">
         <v>247</v>
       </c>
@@ -5683,9 +5670,9 @@
       <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="156"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="160"/>
+      <c r="C10" s="166"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="170"/>
       <c r="F10" s="115" t="s">
         <v>246</v>
       </c>
@@ -5695,9 +5682,9 @@
       <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="157"/>
-      <c r="D11" s="141"/>
-      <c r="E11" s="160"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="170"/>
       <c r="F11" s="115" t="s">
         <v>248</v>
       </c>
@@ -5710,8 +5697,8 @@
       <c r="C12" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="142"/>
-      <c r="E12" s="159"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="169"/>
       <c r="F12" s="115" t="s">
         <v>249</v>
       </c>
@@ -5724,11 +5711,11 @@
       <c r="C13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="134" t="s">
+      <c r="D13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
       <c r="G13" s="130" t="s">
         <v>30</v>
       </c>
@@ -5778,15 +5765,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -5904,12 +5891,12 @@
       <c r="C13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="134" t="s">
+      <c r="D13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="136"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -5953,15 +5940,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -6080,11 +6067,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="134" t="s">
+      <c r="E13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="135"/>
-      <c r="G13" s="136"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -6128,14 +6115,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -6243,10 +6230,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="134" t="s">
+      <c r="E13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="136"/>
+      <c r="F13" s="146"/>
       <c r="G13" s="81" t="s">
         <v>30</v>
       </c>
@@ -6289,15 +6276,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -6417,10 +6404,10 @@
       <c r="E13" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="163" t="s">
+      <c r="F13" s="173" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="164"/>
+      <c r="G13" s="174"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -6464,13 +6451,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -6606,35 +6593,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="177"/>
-      <c r="C3" s="178" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="177"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -6853,42 +6840,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="179" t="s">
+      <c r="C23" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="180"/>
-      <c r="E23" s="180"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="181"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="190"/>
+      <c r="G23" s="191"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="171"/>
-      <c r="D24" s="172"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="173"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="182"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="182"/>
+      <c r="G24" s="183"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="171" t="s">
+      <c r="C25" s="181" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="172"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="173"/>
+      <c r="D25" s="182"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="174"/>
-      <c r="D26" s="175"/>
-      <c r="E26" s="175"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="176"/>
+      <c r="C26" s="184"/>
+      <c r="D26" s="185"/>
+      <c r="E26" s="185"/>
+      <c r="F26" s="185"/>
+      <c r="G26" s="186"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -6916,42 +6903,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="165" t="s">
+      <c r="C28" s="175" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="167"/>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="177"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="165"/>
-      <c r="D29" s="166"/>
-      <c r="E29" s="166"/>
-      <c r="F29" s="166"/>
-      <c r="G29" s="167"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="176"/>
+      <c r="E29" s="176"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="177"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="165" t="s">
+      <c r="C30" s="175" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="166"/>
-      <c r="E30" s="166"/>
-      <c r="F30" s="166"/>
-      <c r="G30" s="167"/>
+      <c r="D30" s="176"/>
+      <c r="E30" s="176"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="177"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="168"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="170"/>
+      <c r="C31" s="178"/>
+      <c r="D31" s="179"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="180"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -6986,35 +6973,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="177"/>
-      <c r="C3" s="178" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="177"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -7039,7 +7026,7 @@
         <v>6</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -7065,56 +7052,56 @@
         <v>7</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="203" t="s">
-        <v>320</v>
-      </c>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
-      <c r="G8" s="205"/>
+      <c r="C8" s="192" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="194"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="197"/>
-      <c r="D9" s="198"/>
-      <c r="E9" s="198"/>
-      <c r="F9" s="198"/>
-      <c r="G9" s="199"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="196"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="197"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="197"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="198"/>
-      <c r="G10" s="199"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="197"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="200"/>
-      <c r="D11" s="201"/>
-      <c r="E11" s="201"/>
-      <c r="F11" s="201"/>
-      <c r="G11" s="202"/>
+      <c r="C11" s="198"/>
+      <c r="D11" s="199"/>
+      <c r="E11" s="199"/>
+      <c r="F11" s="199"/>
+      <c r="G11" s="200"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
JinHyeong 22년12월30일 # 2주차 10일차 계획표
Happy New Year !
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F5199F-53DE-4B0B-850C-29FEF72EF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8799BD-8DBF-4F0A-BBD8-6415578BBC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="319">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -794,9 +794,6 @@
     <t>* 다나와</t>
   </si>
   <si>
-    <t>https://prod.danawa.com/info/?pcode=10151808&amp;keyword=%EC%BD%94%EC%B9%B4%EC%BD%9C%EB%9D%BC+%EC%A0%9C%EB%A1%9C&amp;cate=1623180</t>
-  </si>
-  <si>
     <t>2 -원에이엠 스파클링</t>
   </si>
   <si>
@@ -884,220 +881,353 @@
     <t>https://search.shopping.naver.com/catalog/26235760523?query=%EC%94%A8%EA%B7%B8%EB%9E%A8%20%ED%83%84%EC%82%B0%EC%88%98&amp;NaPm=ct%3Dlc8gn0go%7Cci%3Ddc9b80a4477775ee6885987895f866049c78161c%7Ctr%3Dslsl%7Csn%3D95694%7Chk%3D8d927827a7e71a1e861cfe4def8b41bcaddd6d7e</t>
   </si>
   <si>
+    <t>10 -  트레비</t>
+  </si>
+  <si>
+    <t>https://smartstore.naver.com/ncutong/products/389678131?NaPm=ct%3Dlc8gqj08%7Cci%3D93d639e5458ac224e0e71ea9c43110fc3f0cb27a%7Ctr%3Dslsl%7Csn%3D291784%7Chk%3D1b01f8aa5b1ad26bf8965023f4f0b38f5df3060a</t>
+  </si>
+  <si>
+    <t>11 - 이마트 노브랜드 스파클링 에이드 라임/오렌지 망고</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/catalog/17719148994?query=%EB%85%B8%EB%B8%8C%EB%9E%9C%EB%93%9C%20%EC%8A%A4%ED%8C%8C%ED%81%B4%EB%A7%81&amp;NaPm=ct%3Dlc8gxkv4%7Cci%3D4ef0c247e08c902285fd9a7807717cba7557e6e7%7Ctr%3Dslsl%7Csn%3D95694%7Chk%3D9343ba10954f1e94907f9aaa761d6aa17e8e6fc9</t>
+  </si>
+  <si>
+    <t>https://prod.danawa.com/info/?pcode=11441436&amp;keyword=%EB%85%B8%EB%B8%8C%EB%9E%9C%EB%93%9C+%EC%8A%A4%ED%8C%8C%ED%81%B4%EB%A7%81&amp;cate=1623180</t>
+  </si>
+  <si>
+    <t>------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>쿠팡 사용</t>
+  </si>
+  <si>
+    <t>12. 천연사이다 제로</t>
+  </si>
+  <si>
+    <t>* 쿠팡(29071)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/1650226?itemId=548271199&amp;vendorItemId=76475901781&amp;sourceType=srp_product_ads&amp;clickEventId=43762c0f-83ba-4aa8-8f15-d14c61d896b0&amp;korePlacement=15&amp;koreSubPlacement=5&amp;q=%EC%B2%9C%EC%97%B0%EC%82%AC%EC%9D%B4%EB%8B%A4+%EC%A0%9C%EB%A1%9C&amp;itemsCount=36&amp;searchId=a0c6bdf22e29490fbfd1089a5ce8bc5f&amp;rank=4&amp;isAddedCart=</t>
+  </si>
+  <si>
+    <t>13. 링티제로</t>
+  </si>
+  <si>
+    <t>* 쿠팡(13660)</t>
+  </si>
+  <si>
+    <t>14. 부르르 제로 콜라</t>
+  </si>
+  <si>
+    <t>* 네이버(5663)</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/catalog/29582401677?query=%EB%B6%80%EB%A5%B4%EB%A5%B4%20%EC%A0%9C%EB%A1%9C%EC%BD%9C%EB%9D%BC&amp;NaPm=ct%3Dlc8g5tmw%7Cci%3D24a075e3cf5d522144c3f0b39bfafa7d5590cb08%7Ctr%3Dslsl%7Csn%3D95694%7Chk%3D4595b974b3832034aedf34e163326d83c35c3dd5</t>
+  </si>
+  <si>
+    <t>* 다나와(206)</t>
+  </si>
+  <si>
+    <t>https://prod.danawa.com/info/?pcode=13542677&amp;keyword=%EB%B6%80%EB%A5%B4%EB%A5%B4+%EC%A0%9C%EB%A1%9C%EC%BD%9C%EB%9D%BC+250&amp;cate=1623180</t>
+  </si>
+  <si>
+    <t>* 쿠팡(20337)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2358334857?itemId=4093099810&amp;vendorItemId=72077082112&amp;sourceType=srp_product_ads&amp;clickEventId=0db25017-d1b9-4d0d-945b-f38abea6ab41&amp;korePlacement=15&amp;koreSubPlacement=5&amp;q=%EB%AF%B8%EB%8B%9B%EB%A9%94%EC%9D%B4%EB%93%9C+%EC%8A%A4%ED%8C%8C%ED%81%B4%EB%A7%81+%EC%A0%9C%EB%A1%9C&amp;itemsCount=36&amp;searchId=7246cd2d46b64d7eaff19f647b1a1c92&amp;rank=4&amp;isAddedCart=</t>
+  </si>
+  <si>
+    <t>15. 815콜라제로</t>
+  </si>
+  <si>
+    <t>* 네이버(903)</t>
+  </si>
+  <si>
+    <t>https://prod.danawa.com/info/?pcode=14184779&amp;keyword=815%EC%BD%9C%EB%9D%BC+%EC%A0%9C%EB%A1%9C&amp;cate=1623180#bookmark_cm_opinion</t>
+  </si>
+  <si>
+    <t>* 쿠팡(19849)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/5109971962?itemId=6971621377&amp;vendorItemId=81220073505&amp;src=1032001&amp;spec=10305201&amp;addtag=400&amp;ctag=5109971962&amp;lptag=I6971621377&amp;itime=20221229101243&amp;pageType=PRODUCT&amp;pageValue=5109971962&amp;wPcid=29944207620476015686925&amp;wRef=cr.shopping.naver.com&amp;wTime=20221229101243&amp;redirect=landing&amp;isAddedCart=</t>
+  </si>
+  <si>
+    <t>크롤링 시작 및 역할 분담</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간 점검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크롤링 문제점 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>naver/danawa 크롤링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간점검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 : 제로칼로리 탄산 음료 리뷰 키워드 분석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크롤링 역할 분담 , 전처리 방식 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 총합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 추가 날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크롤링 쇼핑몰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버브랜드숍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다나와</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버쇼핑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크롤링 url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠팡_천연사이다</t>
+  </si>
+  <si>
+    <t>네이버_브숍_펩시</t>
+  </si>
+  <si>
+    <t>다나와_트레비</t>
+  </si>
+  <si>
+    <t>네이버쇼핑_웰치스</t>
+  </si>
+  <si>
+    <t>코카콜라제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원에이엠스파클링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펩시콜라제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부르르제로사이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나랑드사이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칠성사이다제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스프라이트제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웰치스제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>씨그램</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트레비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이마트노브랜드 스파클링 에이드 라임 / 오렌지 망고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천연사이다 제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>링티제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부르르제로콜라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>815콜라제로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url 하이퍼링크 입력시 하이퍼링크 편집으로 축약시킬 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크롤링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>씨그램 10,000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제로코카콜라 다나와 6000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부르르제로사이다 네이버쇼핑 2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부르르제오사이다 네이버브랜드 4500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1am 스파클링 10,000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천연사이다 데이터 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나랑드사이다 8600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칠성사이다제로 6800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천연사이다 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빅토리아 탄산수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버_브숍_빅토리아</t>
+  </si>
+  <si>
+    <t>네이버_스마트스토어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빅토리아 탄산수 16600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다나와_씨그램</t>
+  </si>
+  <si>
     <t>https://prod.danawa.com/info/?pcode=13363343&amp;keyword=%EC%94%A8%EA%B7%B8%EB%9E%A8&amp;cate=1623180</t>
-  </si>
-  <si>
-    <t>10 -  트레비</t>
-  </si>
-  <si>
-    <t>https://smartstore.naver.com/ncutong/products/389678131?NaPm=ct%3Dlc8gqj08%7Cci%3D93d639e5458ac224e0e71ea9c43110fc3f0cb27a%7Ctr%3Dslsl%7Csn%3D291784%7Chk%3D1b01f8aa5b1ad26bf8965023f4f0b38f5df3060a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.coupang.com/vp/products/5688038203?itemId=9412000674&amp;vendorItemId=75252234933&amp;pickType=COU_PICK&amp;q=%EB%A7%81%ED%8B%B0%EC%A0%9C%EB%A1%9C&amp;itemsCount=36&amp;searchId=0f912193a6434ccebbb3d84401abc1e0&amp;rank=1&amp;isAddedCart= </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>https://prod.danawa.com/info/?pcode=3312370&amp;keyword=%ED%83%84%EC%82%B0%EC%88%98&amp;cate=1623180</t>
-  </si>
-  <si>
-    <t>11 - 이마트 노브랜드 스파클링 에이드 라임/오렌지 망고</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/catalog/17719148994?query=%EB%85%B8%EB%B8%8C%EB%9E%9C%EB%93%9C%20%EC%8A%A4%ED%8C%8C%ED%81%B4%EB%A7%81&amp;NaPm=ct%3Dlc8gxkv4%7Cci%3D4ef0c247e08c902285fd9a7807717cba7557e6e7%7Ctr%3Dslsl%7Csn%3D95694%7Chk%3D9343ba10954f1e94907f9aaa761d6aa17e8e6fc9</t>
-  </si>
-  <si>
-    <t>https://prod.danawa.com/info/?pcode=11441436&amp;keyword=%EB%85%B8%EB%B8%8C%EB%9E%9C%EB%93%9C+%EC%8A%A4%ED%8C%8C%ED%81%B4%EB%A7%81&amp;cate=1623180</t>
-  </si>
-  <si>
-    <t>------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>쿠팡 사용</t>
-  </si>
-  <si>
-    <t>12. 천연사이다 제로</t>
-  </si>
-  <si>
-    <t>* 쿠팡(29071)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/1650226?itemId=548271199&amp;vendorItemId=76475901781&amp;sourceType=srp_product_ads&amp;clickEventId=43762c0f-83ba-4aa8-8f15-d14c61d896b0&amp;korePlacement=15&amp;koreSubPlacement=5&amp;q=%EC%B2%9C%EC%97%B0%EC%82%AC%EC%9D%B4%EB%8B%A4+%EC%A0%9C%EB%A1%9C&amp;itemsCount=36&amp;searchId=a0c6bdf22e29490fbfd1089a5ce8bc5f&amp;rank=4&amp;isAddedCart=</t>
-  </si>
-  <si>
-    <t>13. 링티제로</t>
-  </si>
-  <si>
-    <t>* 쿠팡(13660)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/5688038203?itemId=9412000674&amp;vendorItemId=75252234933&amp;pickType=COU_PICK&amp;q=%EB%A7%81%ED%8B%B0%EC%A0%9C%EB%A1%9C&amp;itemsCount=36&amp;searchId=0f912193a6434ccebbb3d84401abc1e0&amp;rank=1&amp;isAddedCart=</t>
-  </si>
-  <si>
-    <t>14. 부르르 제로 콜라</t>
-  </si>
-  <si>
-    <t>* 네이버(5663)</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/catalog/29582401677?query=%EB%B6%80%EB%A5%B4%EB%A5%B4%20%EC%A0%9C%EB%A1%9C%EC%BD%9C%EB%9D%BC&amp;NaPm=ct%3Dlc8g5tmw%7Cci%3D24a075e3cf5d522144c3f0b39bfafa7d5590cb08%7Ctr%3Dslsl%7Csn%3D95694%7Chk%3D4595b974b3832034aedf34e163326d83c35c3dd5</t>
-  </si>
-  <si>
-    <t>* 다나와(206)</t>
-  </si>
-  <si>
-    <t>https://prod.danawa.com/info/?pcode=13542677&amp;keyword=%EB%B6%80%EB%A5%B4%EB%A5%B4+%EC%A0%9C%EB%A1%9C%EC%BD%9C%EB%9D%BC+250&amp;cate=1623180</t>
-  </si>
-  <si>
-    <t>* 쿠팡(20337)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/2358334857?itemId=4093099810&amp;vendorItemId=72077082112&amp;sourceType=srp_product_ads&amp;clickEventId=0db25017-d1b9-4d0d-945b-f38abea6ab41&amp;korePlacement=15&amp;koreSubPlacement=5&amp;q=%EB%AF%B8%EB%8B%9B%EB%A9%94%EC%9D%B4%EB%93%9C+%EC%8A%A4%ED%8C%8C%ED%81%B4%EB%A7%81+%EC%A0%9C%EB%A1%9C&amp;itemsCount=36&amp;searchId=7246cd2d46b64d7eaff19f647b1a1c92&amp;rank=4&amp;isAddedCart=</t>
-  </si>
-  <si>
-    <t>15. 815콜라제로</t>
-  </si>
-  <si>
-    <t>* 네이버(903)</t>
-  </si>
-  <si>
-    <t>https://prod.danawa.com/info/?pcode=14184779&amp;keyword=815%EC%BD%9C%EB%9D%BC+%EC%A0%9C%EB%A1%9C&amp;cate=1623180#bookmark_cm_opinion</t>
-  </si>
-  <si>
-    <t>* 쿠팡(19849)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/5109971962?itemId=6971621377&amp;vendorItemId=81220073505&amp;src=1032001&amp;spec=10305201&amp;addtag=400&amp;ctag=5109971962&amp;lptag=I6971621377&amp;itime=20221229101243&amp;pageType=PRODUCT&amp;pageValue=5109971962&amp;wPcid=29944207620476015686925&amp;wRef=cr.shopping.naver.com&amp;wTime=20221229101243&amp;redirect=landing&amp;isAddedCart=</t>
-  </si>
-  <si>
-    <t>크롤링 시작 및 역할 분담</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간 점검</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크롤링 문제점 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>naver/danawa 크롤링</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간점검</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주제 : 제로칼로리 탄산 음료 리뷰 키워드 분석</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크롤링 역할 분담 , 전처리 방식 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰 총합</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터 추가 날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크롤링 쇼핑몰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">https://prod.danawa.com/info/?pcode=10151808&amp;keyword=%EC%BD%94%EC%B9%B4%EC%BD%9C%EB%9D%BC+%EC%A0%9C%EB%A1%9C&amp;cate=1623180 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다나와_제로콜라</t>
   </si>
   <si>
     <t>네이버브랜드숍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다나와</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네이버쇼핑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크롤링 url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>쿠팡_천연사이다</t>
-  </si>
-  <si>
-    <t>네이버_브숍_펩시</t>
-  </si>
-  <si>
-    <t>다나와_트레비</t>
-  </si>
-  <si>
-    <t>네이버쇼핑_웰치스</t>
-  </si>
-  <si>
-    <t>코카콜라제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>원에이엠스파클링</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>펩시콜라제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부르르제로사이다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나랑드사이다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>칠성사이다제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스프라이트제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>웰치스제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>씨그램</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>트레비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이마트노브랜드 스파클링 에이드 라임 / 오렌지 망고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>천연사이다 제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>링티제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부르르제로콜라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>815콜라제로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url 하이퍼링크 입력시 하이퍼링크 편집으로 축약시킬 것</t>
+  </si>
+  <si>
+    <t>다나와_나랑드사이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버쇼핑_1am</t>
+  </si>
+  <si>
+    <t>네이버_브숍_1am</t>
+  </si>
+  <si>
+    <t>250ml 30캔 약 4500건</t>
+  </si>
+  <si>
+    <t>네이버쇼핑_부르르사이다</t>
+  </si>
+  <si>
+    <t>네이버_브숍_부르르사이다</t>
+  </si>
+  <si>
+    <t>네이버_브숍_부르르사이다2</t>
+  </si>
+  <si>
+    <t>1.5L 12페트 약 1000건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버_브숍_코카콜라제로</t>
+  </si>
+  <si>
+    <t>네이버_브숍_코카콜라제로2</t>
+  </si>
+  <si>
+    <t>네이버_브숍_탄산수</t>
+  </si>
+  <si>
+    <t>다나와_칠성제로</t>
+  </si>
+  <si>
+    <t>분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 명 크롤링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두 명은 전처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다시 구해야하는 데이터를 확인해야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크롤링 , 전처리 , 데이터 정돈화 , 시각화 , 모델 학습 데이터 준비</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1105,7 +1235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1293,6 +1423,14 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -1827,7 +1965,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2065,9 +2203,6 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2179,6 +2314,84 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2266,6 +2479,12 @@
     <xf numFmtId="0" fontId="12" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2323,6 +2542,33 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2336,48 +2582,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3123,30 +3327,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="97"/>
-      <c r="C4" s="97" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="96" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3154,13 +3358,13 @@
       <c r="B5" s="37">
         <v>0.375</v>
       </c>
-      <c r="C5" s="133" t="s">
+      <c r="C5" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="113" t="s">
+      <c r="D5" s="159"/>
+      <c r="E5" s="159"/>
+      <c r="F5" s="159"/>
+      <c r="G5" s="112" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3171,16 +3375,16 @@
       <c r="C6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="106" t="s">
+      <c r="D6" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="128" t="s">
+      <c r="E6" s="153" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="114" t="s">
+      <c r="G6" s="113" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3188,45 +3392,45 @@
       <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="106" t="s">
+      <c r="C7" s="97"/>
+      <c r="D7" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="129"/>
-      <c r="F7" s="112" t="s">
+      <c r="E7" s="154"/>
+      <c r="F7" s="111" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="114" t="s">
+      <c r="G7" s="113" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="103" customFormat="1" ht="50.1" customHeight="1">
-      <c r="B8" s="99">
+    <row r="8" spans="2:7" s="102" customFormat="1" ht="50.1" customHeight="1">
+      <c r="B8" s="98">
         <v>0.5</v>
       </c>
       <c r="C8" s="69"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
       <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="125" t="s">
+      <c r="D9" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="125" t="s">
+      <c r="E9" s="150" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="130" t="s">
+      <c r="F9" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="135" t="s">
+      <c r="G9" s="160" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3234,21 +3438,21 @@
       <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="123"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="136"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="161"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="124"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="136"/>
+      <c r="C11" s="149"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="161"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="37">
@@ -3258,9 +3462,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="137"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="157"/>
+      <c r="G12" s="162"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="37">
@@ -3269,11 +3473,11 @@
       <c r="C13" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="119" t="s">
+      <c r="D13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="121"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="146"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -3289,7 +3493,7 @@
       <c r="G14" s="30"/>
     </row>
     <row r="18" spans="3:4" ht="26.25">
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="100" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -3297,12 +3501,12 @@
       </c>
     </row>
     <row r="19" spans="3:4" ht="26.25">
-      <c r="C19" s="101" t="s">
+      <c r="C19" s="100" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="26.25">
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="100" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3341,35 +3545,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="160"/>
-      <c r="C3" s="161" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="160"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -3694,9 +3898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -3710,498 +3914,531 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
-      <c r="B1" s="85">
+      <c r="B1" s="84">
         <v>44914</v>
       </c>
-      <c r="C1" s="85">
+      <c r="C1" s="84">
         <v>44915</v>
       </c>
-      <c r="D1" s="85">
+      <c r="D1" s="84">
         <v>44916</v>
       </c>
-      <c r="E1" s="85">
+      <c r="E1" s="84">
         <v>44917</v>
       </c>
-      <c r="F1" s="85">
+      <c r="F1" s="84">
         <v>44918</v>
       </c>
-      <c r="G1" s="85">
+      <c r="G1" s="84">
         <v>44921</v>
       </c>
-      <c r="H1" s="85">
+      <c r="H1" s="84">
         <v>44922</v>
       </c>
-      <c r="I1" s="85">
+      <c r="I1" s="84">
         <v>44923</v>
       </c>
-      <c r="J1" s="85">
+      <c r="J1" s="84">
         <v>44924</v>
       </c>
-      <c r="K1" s="85">
+      <c r="K1" s="84">
         <v>44925</v>
       </c>
-      <c r="L1" s="85">
+      <c r="L1" s="84">
         <v>44928</v>
       </c>
-      <c r="M1" s="85">
+      <c r="M1" s="84">
         <v>44929</v>
       </c>
-      <c r="N1" s="85">
+      <c r="N1" s="84">
         <v>44930</v>
       </c>
-      <c r="O1" s="85">
+      <c r="O1" s="84">
         <v>44931</v>
       </c>
-      <c r="P1" s="85">
+      <c r="P1" s="84">
         <v>44932</v>
       </c>
-      <c r="Q1" s="85">
+      <c r="Q1" s="84">
         <v>44933</v>
       </c>
-      <c r="R1" s="85">
+      <c r="R1" s="84">
         <v>44936</v>
       </c>
-      <c r="S1" s="85">
+      <c r="S1" s="84">
         <v>44937</v>
       </c>
-      <c r="T1" s="85">
+      <c r="T1" s="84">
         <v>44938</v>
       </c>
-      <c r="U1" s="85">
+      <c r="U1" s="84">
         <v>44939</v>
       </c>
-      <c r="V1" s="85">
+      <c r="V1" s="84">
         <v>44940</v>
       </c>
-      <c r="W1" s="85">
+      <c r="W1" s="84">
         <v>44943</v>
       </c>
-      <c r="X1" s="85">
+      <c r="X1" s="84">
         <v>44944</v>
       </c>
-      <c r="Y1" s="85">
+      <c r="Y1" s="84">
         <v>44945</v>
       </c>
-      <c r="Z1" s="85">
+      <c r="Z1" s="84">
         <v>44946</v>
       </c>
-      <c r="AA1" s="85">
+      <c r="AA1" s="84">
         <v>44951</v>
       </c>
-      <c r="AB1" s="85">
+      <c r="AB1" s="84">
         <v>44952</v>
       </c>
-      <c r="AC1" s="85">
+      <c r="AC1" s="84">
         <v>44953</v>
       </c>
-      <c r="AD1" s="85">
+      <c r="AD1" s="84">
         <v>44954</v>
       </c>
-      <c r="AE1" s="85">
+      <c r="AE1" s="84">
         <v>44957</v>
       </c>
-      <c r="AF1" s="85">
+      <c r="AF1" s="84">
         <v>44958</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="165" t="s">
+    <row r="2" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="201" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="101" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="F2" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="169" t="s">
+      <c r="G2" s="205" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="88" t="s">
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="87" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="165"/>
-      <c r="B3" s="102" t="s">
+      <c r="K2" s="87" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="201"/>
+      <c r="B3" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102" t="s">
+      <c r="C3" s="101"/>
+      <c r="D3" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="169"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="115" t="s">
+      <c r="G3" s="205"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="114" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="88" t="s">
+      <c r="J3" s="87" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="165"/>
-      <c r="B4" s="104" t="s">
+      <c r="K3" s="135" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="201"/>
+      <c r="B4" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102" t="s">
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="102" t="s">
+      <c r="F4" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="169"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102" t="s">
+      <c r="G4" s="205"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="J4" s="88" t="s">
+      <c r="J4" s="87" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="165"/>
-      <c r="B5" s="104" t="s">
+      <c r="K4" s="87" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="201"/>
+      <c r="B5" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102" t="s">
+      <c r="C5" s="101"/>
+      <c r="D5" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="102" t="s">
+      <c r="F5" s="101" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="169"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102" t="s">
+      <c r="G5" s="205"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="165"/>
-      <c r="B6" s="102" t="s">
+      <c r="K5" s="87" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="201"/>
+      <c r="B6" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="102" t="s">
+      <c r="D6" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="102" t="s">
+      <c r="F6" s="101" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="169"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102" t="s">
+      <c r="G6" s="205"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101" t="s">
         <v>168</v>
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="166" t="s">
+    <row r="7" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="202" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="102" t="s">
+      <c r="C7" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="101" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="101" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="102"/>
-      <c r="G7" s="169"/>
-      <c r="H7" s="102" t="s">
+      <c r="F7" s="101"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="102" t="s">
+      <c r="I7" s="101" t="s">
         <v>167</v>
       </c>
-      <c r="J7" s="89" t="s">
+      <c r="J7" s="88" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="166"/>
-      <c r="B8" s="102" t="s">
+      <c r="K7" s="88" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="202"/>
+      <c r="B8" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="102" t="s">
+      <c r="C8" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="169"/>
-      <c r="H8" s="102" t="s">
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="102" t="s">
+      <c r="I8" s="101" t="s">
         <v>170</v>
       </c>
-      <c r="J8" s="89" t="s">
+      <c r="J8" s="88" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="166"/>
-      <c r="B9" s="102" t="s">
+      <c r="K8" s="88" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="202"/>
+      <c r="B9" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="102" t="s">
+      <c r="D9" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="169"/>
-      <c r="H9" s="102" t="s">
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="101" t="s">
         <v>152</v>
       </c>
-      <c r="I9" s="102"/>
-    </row>
-    <row r="10" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="166"/>
-      <c r="B10" s="104" t="s">
+      <c r="I9" s="101"/>
+      <c r="K9" s="88" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="202"/>
+      <c r="B10" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102" t="s">
+      <c r="D10" s="101"/>
+      <c r="E10" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-    </row>
-    <row r="11" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="166"/>
-      <c r="B11" s="104" t="s">
+      <c r="F10" s="101"/>
+      <c r="G10" s="205"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="K10" s="88" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="202"/>
+      <c r="B11" s="103" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="102" t="s">
+      <c r="C11" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102" t="s">
+      <c r="D11" s="101"/>
+      <c r="E11" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-    </row>
-    <row r="12" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="167" t="s">
+      <c r="F11" s="101"/>
+      <c r="G11" s="205"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="101"/>
+    </row>
+    <row r="12" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="203" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102" t="s">
+      <c r="D12" s="101"/>
+      <c r="E12" s="101" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="102"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="102" t="s">
+      <c r="F12" s="101"/>
+      <c r="G12" s="205"/>
+      <c r="H12" s="101" t="s">
         <v>153</v>
       </c>
-      <c r="I12" s="102"/>
-      <c r="J12" s="90" t="s">
+      <c r="I12" s="101"/>
+      <c r="J12" s="89" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="167"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102" t="s">
+      <c r="K12" s="89" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="203"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="102"/>
-      <c r="G13" s="169"/>
-      <c r="H13" s="102" t="s">
+      <c r="F13" s="101"/>
+      <c r="G13" s="205"/>
+      <c r="H13" s="101" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="102"/>
-    </row>
-    <row r="14" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="167"/>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="102" t="s">
+      <c r="I13" s="101"/>
+      <c r="K13" s="89" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A14" s="203"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="101" t="s">
         <v>155</v>
       </c>
-      <c r="I14" s="102"/>
-    </row>
-    <row r="15" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="167"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102" t="s">
+      <c r="I14" s="101"/>
+    </row>
+    <row r="15" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="203"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="102" t="s">
+      <c r="F15" s="101"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="101" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="102"/>
-    </row>
-    <row r="16" spans="1:32" s="90" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="167"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102" t="s">
+      <c r="I15" s="101"/>
+    </row>
+    <row r="16" spans="1:32" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A16" s="203"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="102"/>
-      <c r="G16" s="169"/>
-      <c r="H16" s="102" t="s">
+      <c r="F16" s="101"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="I16" s="102"/>
-    </row>
-    <row r="17" spans="1:10" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="168" t="s">
+      <c r="I16" s="101"/>
+    </row>
+    <row r="17" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="204" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="102"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="169"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="102"/>
-      <c r="J17" s="91" t="s">
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="101"/>
+      <c r="J17" s="90" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="168"/>
-      <c r="B18" s="102"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="102"/>
-      <c r="I18" s="102"/>
-    </row>
-    <row r="19" spans="1:10" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="168"/>
-      <c r="B19" s="102"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="169"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-    </row>
-    <row r="20" spans="1:10" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="168"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="102"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="102"/>
-    </row>
-    <row r="21" spans="1:10" s="91" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="168"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="169"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="102"/>
-    </row>
-    <row r="22" spans="1:10" s="102" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="109"/>
-    </row>
-    <row r="23" spans="1:10" s="111" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="110" t="s">
+      <c r="K17" s="90" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="204"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="101"/>
+    </row>
+    <row r="19" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="204"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="101"/>
+    </row>
+    <row r="20" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="204"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="101"/>
+    </row>
+    <row r="21" spans="1:11" s="90" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="204"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101"/>
+    </row>
+    <row r="22" spans="1:11" s="101" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="108"/>
+    </row>
+    <row r="23" spans="1:11" s="110" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="111" t="s">
+      <c r="B23" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="110" t="s">
+      <c r="C23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="110" t="s">
+      <c r="D23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="110" t="s">
+      <c r="E23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="110" t="s">
+      <c r="F23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="110" t="s">
+      <c r="G23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="110" t="s">
+      <c r="H23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="110" t="s">
+      <c r="I23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="110" t="s">
+      <c r="J23" s="109" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1">
+    <row r="24" spans="1:11" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -4227,7 +4464,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1">
+    <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -4256,7 +4493,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" customHeight="1">
+    <row r="26" spans="1:11" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -4276,7 +4513,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1">
+    <row r="27" spans="1:11" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -4302,7 +4539,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1">
+    <row r="28" spans="1:11" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -4319,7 +4556,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" customHeight="1">
+    <row r="29" spans="1:11" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -4339,7 +4576,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30" customHeight="1">
+    <row r="30" spans="1:11" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -4353,7 +4590,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30" customHeight="1">
+    <row r="31" spans="1:11" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -4361,7 +4598,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" customHeight="1">
+    <row r="32" spans="1:11" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -4412,12 +4649,12 @@
       <c r="D36" t="s">
         <v>104</v>
       </c>
-      <c r="J36" t="s">
-        <v>192</v>
+      <c r="J36" s="133" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1">
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="106" t="s">
         <v>67</v>
       </c>
       <c r="D37" t="s">
@@ -4433,36 +4670,36 @@
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="108" t="s">
+      <c r="B39" s="107" t="s">
         <v>71</v>
       </c>
       <c r="J39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1">
       <c r="J42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1">
       <c r="J43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1">
       <c r="J44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1">
       <c r="J45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" customHeight="1">
       <c r="J48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="10:10" ht="30" customHeight="1">
@@ -4472,7 +4709,7 @@
     </row>
     <row r="52" spans="10:10" ht="30" customHeight="1">
       <c r="J52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="10:10" ht="30" customHeight="1">
@@ -4482,12 +4719,12 @@
     </row>
     <row r="54" spans="10:10" ht="30" customHeight="1">
       <c r="J54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="10:10" ht="30" customHeight="1">
       <c r="J57" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="10:10" ht="30" customHeight="1">
@@ -4497,12 +4734,12 @@
     </row>
     <row r="61" spans="10:10" ht="30" customHeight="1">
       <c r="J61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="10:10" ht="30" customHeight="1">
       <c r="J63" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="10:10" ht="30" customHeight="1">
@@ -4512,12 +4749,12 @@
     </row>
     <row r="66" spans="10:10" ht="30" customHeight="1">
       <c r="J66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="10:10" ht="30" customHeight="1">
       <c r="J70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="10:10" ht="30" customHeight="1">
@@ -4527,12 +4764,12 @@
     </row>
     <row r="74" spans="10:10" ht="30" customHeight="1">
       <c r="J74" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="10:10" ht="30" customHeight="1">
       <c r="J77" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="10:10" ht="30" customHeight="1">
@@ -4542,12 +4779,12 @@
     </row>
     <row r="81" spans="10:10" ht="30" customHeight="1">
       <c r="J81" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83" spans="10:10" ht="30" customHeight="1">
       <c r="J83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="10:10" ht="30" customHeight="1">
@@ -4557,22 +4794,22 @@
     </row>
     <row r="86" spans="10:10" ht="30" customHeight="1">
       <c r="J86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" spans="10:10" ht="30" customHeight="1">
       <c r="J88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="10:10" ht="30" customHeight="1">
       <c r="J89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="10:10" ht="30" customHeight="1">
       <c r="J92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="10:10" ht="30" customHeight="1">
@@ -4582,12 +4819,12 @@
     </row>
     <row r="96" spans="10:10" ht="30" customHeight="1">
       <c r="J96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98" spans="10:10" ht="30" customHeight="1">
       <c r="J98" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="100" spans="10:10" ht="30" customHeight="1">
@@ -4597,12 +4834,12 @@
     </row>
     <row r="101" spans="10:10" ht="30" customHeight="1">
       <c r="J101" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="10:10" ht="30" customHeight="1">
       <c r="J104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="10:10" ht="30" customHeight="1">
@@ -4612,7 +4849,7 @@
     </row>
     <row r="108" spans="10:10" ht="30" customHeight="1">
       <c r="J108" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="10:10" ht="30" customHeight="1">
@@ -4622,12 +4859,12 @@
     </row>
     <row r="110" spans="10:10" ht="30" customHeight="1">
       <c r="J110" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="10:10" ht="30" customHeight="1">
       <c r="J113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="10:10" ht="30" customHeight="1">
@@ -4637,7 +4874,7 @@
     </row>
     <row r="117" spans="10:10" ht="30" customHeight="1">
       <c r="J117" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="119" spans="10:10" ht="30" customHeight="1">
@@ -4646,13 +4883,13 @@
       </c>
     </row>
     <row r="120" spans="10:10" ht="30" customHeight="1">
-      <c r="J120" t="s">
-        <v>222</v>
+      <c r="J120" s="133" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="123" spans="10:10" ht="30" customHeight="1">
       <c r="J123" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="126" spans="10:10" ht="30" customHeight="1">
@@ -4662,7 +4899,7 @@
     </row>
     <row r="127" spans="10:10" ht="30" customHeight="1">
       <c r="J127" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" spans="10:10" ht="30" customHeight="1">
@@ -4671,13 +4908,13 @@
       </c>
     </row>
     <row r="130" spans="10:10" ht="30" customHeight="1">
-      <c r="J130" t="s">
-        <v>225</v>
+      <c r="J130" s="133" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="10:10" ht="30" customHeight="1">
       <c r="J133" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="136" spans="10:10" ht="30" customHeight="1">
@@ -4687,7 +4924,7 @@
     </row>
     <row r="137" spans="10:10" ht="30" customHeight="1">
       <c r="J137" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="139" spans="10:10" ht="30" customHeight="1">
@@ -4697,112 +4934,112 @@
     </row>
     <row r="140" spans="10:10" ht="30" customHeight="1">
       <c r="J140" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="144" spans="10:10" ht="30" customHeight="1">
       <c r="J144" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="145" spans="10:10" ht="30" customHeight="1">
       <c r="J145" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="146" spans="10:10" ht="30" customHeight="1">
       <c r="J146" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="148" spans="10:10" ht="30" customHeight="1">
       <c r="J148" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="151" spans="10:10" ht="30" customHeight="1">
       <c r="J151" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="152" spans="10:10" ht="30" customHeight="1">
       <c r="J152" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="155" spans="10:10" ht="30" customHeight="1">
       <c r="J155" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="158" spans="10:10" ht="30" customHeight="1">
       <c r="J158" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="159" spans="10:10" ht="30" customHeight="1">
-      <c r="J159" t="s">
-        <v>236</v>
+      <c r="J159" s="133" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="162" spans="10:10" ht="30" customHeight="1">
       <c r="J162" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="165" spans="10:10" ht="30" customHeight="1">
       <c r="J165" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="166" spans="10:10" ht="30" customHeight="1">
       <c r="J166" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="168" spans="10:10" ht="30" customHeight="1">
       <c r="J168" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="169" spans="10:10" ht="30" customHeight="1">
       <c r="J169" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="171" spans="10:10" ht="30" customHeight="1">
       <c r="J171" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="172" spans="10:10" ht="30" customHeight="1">
       <c r="J172" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="175" spans="10:10" ht="30" customHeight="1">
       <c r="J175" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="177" spans="10:10" ht="30" customHeight="1">
       <c r="J177" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="178" spans="10:10" ht="30" customHeight="1">
       <c r="J178" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="180" spans="10:10" ht="30" customHeight="1">
       <c r="J180" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="181" spans="10:10" ht="30" customHeight="1">
       <c r="J181" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4820,6 +5057,10 @@
     <hyperlink ref="B10" r:id="rId3" xr:uid="{96BBED21-73BF-4773-9C3E-882315F79376}"/>
     <hyperlink ref="B11" r:id="rId4" xr:uid="{EA841544-9F28-4D4C-A884-28E229F43738}"/>
     <hyperlink ref="D8" r:id="rId5" xr:uid="{B30208CB-E405-4159-805B-CA425C839CB6}"/>
+    <hyperlink ref="J120" r:id="rId6" xr:uid="{61B73459-D950-4D18-8F84-16C65170BB02}"/>
+    <hyperlink ref="J159" r:id="rId7" xr:uid="{DC750755-783F-424D-BA99-C081F953A85A}"/>
+    <hyperlink ref="J130" r:id="rId8" xr:uid="{B8B17276-48D6-43D1-B6C7-28B90CF4790D}"/>
+    <hyperlink ref="J36" r:id="rId9" xr:uid="{9518D487-D6F8-41EE-9FCB-13199F12B3A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4827,245 +5068,454 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4682B6DF-860A-46A3-B003-691AA560AE2A}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <pane xSplit="5" ySplit="17" topLeftCell="N20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="49.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="20.125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="171" customFormat="1" ht="18" thickTop="1" thickBot="1">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:19" s="117" customFormat="1" ht="18" thickTop="1" thickBot="1">
+      <c r="A1" s="116" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="117" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="121" customFormat="1">
+      <c r="A2" s="118" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="119"/>
+      <c r="C2" s="120">
+        <v>44924</v>
+      </c>
+      <c r="D2" s="120">
+        <v>44924</v>
+      </c>
+      <c r="E2" s="136">
+        <v>44924</v>
+      </c>
+      <c r="F2" s="120">
+        <v>44924</v>
+      </c>
+      <c r="G2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="H2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="I2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="J2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="K2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="L2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="M2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="N2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="O2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="P2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="Q2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="R2" s="120">
+        <v>44925</v>
+      </c>
+      <c r="S2" s="120">
+        <v>44925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="122" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="119"/>
+      <c r="C3" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="171" t="s">
+      <c r="E3" s="137" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="175" customFormat="1">
-      <c r="A2" s="172" t="s">
+      <c r="F3" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="174">
-        <v>44924</v>
-      </c>
-      <c r="D2" s="174">
-        <v>44924</v>
-      </c>
-      <c r="E2" s="174">
-        <v>44924</v>
-      </c>
-      <c r="F2" s="174">
-        <v>44924</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="176" t="s">
+      <c r="G3" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="127" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A4" s="123" t="s">
         <v>259</v>
       </c>
-      <c r="B3" s="173"/>
-      <c r="C3" s="85" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" s="124"/>
+      <c r="C4" s="125" t="s">
         <v>260</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="126" t="s">
         <v>261</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4" s="138" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="181" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A4" s="177" t="s">
+      <c r="F4" s="126" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="178"/>
-      <c r="C4" s="179" t="s">
+      <c r="G4" s="132" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="132" t="s">
+        <v>294</v>
+      </c>
+      <c r="I4" s="132" t="s">
+        <v>262</v>
+      </c>
+      <c r="J4" s="132" t="s">
+        <v>299</v>
+      </c>
+      <c r="K4" s="132" t="s">
+        <v>310</v>
+      </c>
+      <c r="L4" s="132" t="s">
+        <v>311</v>
+      </c>
+      <c r="M4" s="127" t="s">
+        <v>309</v>
+      </c>
+      <c r="N4" s="132" t="s">
+        <v>305</v>
+      </c>
+      <c r="O4" s="132" t="s">
+        <v>301</v>
+      </c>
+      <c r="P4" s="132" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q4" s="132" t="s">
+        <v>303</v>
+      </c>
+      <c r="R4" s="132" t="s">
+        <v>312</v>
+      </c>
+      <c r="S4" s="132" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="122" t="s">
         <v>264</v>
       </c>
-      <c r="D4" s="180" t="s">
+      <c r="B5" s="1">
+        <f>SUM(C5:AC5)</f>
+        <v>19127</v>
+      </c>
+      <c r="E5" s="137"/>
+      <c r="J5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1650</v>
+      </c>
+      <c r="L5" s="1">
+        <v>7477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="122" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="180" t="s">
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:B19" si="0">SUM(C6:AC6)</f>
+        <v>18414</v>
+      </c>
+      <c r="E6" s="137"/>
+      <c r="P6" s="1">
+        <v>2000</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>16414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="122" t="s">
         <v>266</v>
       </c>
-      <c r="F4" s="180" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="176" t="s">
-        <v>268</v>
-      </c>
-      <c r="B5" s="1">
-        <f>SUM(C5:G5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="176" t="s">
-        <v>269</v>
-      </c>
-      <c r="B6" s="1">
-        <f t="shared" ref="B6:B19" si="0">SUM(C6:G6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="176" t="s">
-        <v>270</v>
-      </c>
       <c r="B7" s="1">
-        <f>SUM(C7:G7)</f>
+        <f t="shared" si="0"/>
         <v>11040</v>
       </c>
       <c r="D7" s="1">
         <v>11040</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="176" t="s">
-        <v>271</v>
+      <c r="E7" s="137"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="122" t="s">
+        <v>267</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="176" t="s">
-        <v>272</v>
+        <v>7500</v>
+      </c>
+      <c r="E8" s="137"/>
+      <c r="M8" s="1">
+        <v>5500</v>
+      </c>
+      <c r="N8" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="122" t="s">
+        <v>268</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="176" t="s">
-        <v>273</v>
+        <v>8626</v>
+      </c>
+      <c r="E9" s="137"/>
+      <c r="O9" s="1">
+        <v>8626</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="122" t="s">
+        <v>269</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="176" t="s">
-        <v>274</v>
+        <v>6827</v>
+      </c>
+      <c r="E10" s="137"/>
+      <c r="S10" s="1">
+        <v>6827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="122" t="s">
+        <v>270</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="176" t="s">
-        <v>275</v>
+      <c r="E11" s="137"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="122" t="s">
+        <v>271</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
+      <c r="E12" s="137"/>
       <c r="F12" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="176" t="s">
-        <v>276</v>
+    <row r="13" spans="1:19">
+      <c r="A13" s="122" t="s">
+        <v>272</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="176" t="s">
-        <v>277</v>
+        <v>10000</v>
+      </c>
+      <c r="E13" s="137"/>
+      <c r="H13" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="122" t="s">
+        <v>273</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>9440</v>
-      </c>
-      <c r="E14" s="1">
-        <v>9440</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="176" t="s">
-        <v>278</v>
+        <v>10000</v>
+      </c>
+      <c r="E14" s="137"/>
+      <c r="I14" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="122" t="s">
+        <v>274</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="176" t="s">
-        <v>279</v>
+      <c r="E15" s="137"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="134" t="s">
+        <v>290</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
+        <v>10877</v>
+      </c>
+      <c r="E16" s="137"/>
+      <c r="R16" s="1">
+        <v>10877</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="137" customFormat="1">
+      <c r="A17" s="141" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="137">
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="137">
         <v>1500</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="176" t="s">
-        <v>280</v>
-      </c>
-      <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="176" t="s">
-        <v>281</v>
+    <row r="18" spans="1:14">
+      <c r="A18" s="122" t="s">
+        <v>276</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" s="183" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A19" s="182" t="s">
-        <v>282</v>
-      </c>
-      <c r="B19" s="183">
+      <c r="E18" s="137"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="122" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="17.25" thickTop="1"/>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>283</v>
-      </c>
+      <c r="E19" s="137"/>
+    </row>
+    <row r="20" spans="1:14" s="129" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A20" s="128" t="s">
+        <v>278</v>
+      </c>
+      <c r="B20" s="129">
+        <f>SUM(C20:AC20)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="139"/>
+    </row>
+    <row r="21" spans="1:14" ht="17.25" thickTop="1"/>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="M24" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="M25" s="140" t="s">
+        <v>306</v>
+      </c>
+      <c r="N25" s="140"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="M27" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="M28" s="140" t="s">
+        <v>307</v>
+      </c>
+      <c r="N28" s="140"/>
+    </row>
+    <row r="43" spans="11:11">
+      <c r="K43" s="140"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5074,6 +5524,20 @@
     <hyperlink ref="D4" r:id="rId2" xr:uid="{F45D08DE-934A-4051-B5B4-06924C862F04}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{D20FFCF6-E7A0-4D2C-AEFE-BBBC8EF4FAE9}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{F9C3E08F-981F-40B5-B547-B8FD130A5FF6}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{8CF79851-D722-4B91-9061-7EB19FFA68F1}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{94753DD5-1F0B-4DA7-9B57-E9FC542A513E}"/>
+    <hyperlink ref="I4" r:id="rId7" xr:uid="{81C84F90-C821-47FD-8D31-6BC00A0F2856}"/>
+    <hyperlink ref="J4" r:id="rId8" xr:uid="{28C2398E-3BCD-48ED-8210-DD73AB390A26}"/>
+    <hyperlink ref="O4" r:id="rId9" location="bookmark_cm_opinion " xr:uid="{0CF6F717-8986-486F-9043-068138D55353}"/>
+    <hyperlink ref="P4" r:id="rId10" xr:uid="{FBF0CDB5-292C-40DA-85E2-DC00CBB7B58B}"/>
+    <hyperlink ref="Q4" r:id="rId11" xr:uid="{9489436D-04F7-4A07-A232-AAA01A6C8756}"/>
+    <hyperlink ref="N4" r:id="rId12" xr:uid="{A49FD952-8E14-47BC-8852-3981EFF2C18D}"/>
+    <hyperlink ref="M25" r:id="rId13" xr:uid="{796749B0-98CE-49B2-908F-32724E3A92EB}"/>
+    <hyperlink ref="M28" r:id="rId14" xr:uid="{E269F61B-D3B5-4DF4-A55B-7FE055C3E7F1}"/>
+    <hyperlink ref="K4" r:id="rId15" xr:uid="{20EA6CCB-64F1-4F3E-8C06-B18A60BD46B3}"/>
+    <hyperlink ref="L4" r:id="rId16" xr:uid="{725F7434-A488-4C6E-AA7B-677BD13EC286}"/>
+    <hyperlink ref="R4" r:id="rId17" xr:uid="{45FAD726-0A82-488B-831D-BE4301053818}"/>
+    <hyperlink ref="S4" r:id="rId18" location="bookmark_cm_opinion " xr:uid="{797041DA-9442-4306-8AB5-E3255FBE5884}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5084,7 +5548,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:F13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -5095,30 +5559,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="92"/>
-      <c r="C4" s="92" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="91" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5138,87 +5602,93 @@
       <c r="F5" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="31"/>
+      <c r="G5" s="35" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1">
       <c r="B6" s="37">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="138" t="s">
+      <c r="C6" s="163" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="150" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="143" t="s">
+      <c r="E6" s="168" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="116" t="s">
-        <v>249</v>
-      </c>
-      <c r="G6" s="31"/>
+      <c r="F6" s="115" t="s">
+        <v>245</v>
+      </c>
+      <c r="G6" s="171" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1">
       <c r="B7" s="37">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="116" t="s">
-        <v>250</v>
-      </c>
-      <c r="G7" s="31"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="115" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" s="172"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B8" s="99">
+      <c r="B8" s="98">
         <v>0.5</v>
       </c>
       <c r="C8" s="68"/>
       <c r="D8" s="71"/>
       <c r="E8" s="71"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="71"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
       <c r="B9" s="37">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="165" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="125" t="s">
+      <c r="D9" s="150" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="116" t="s">
-        <v>251</v>
-      </c>
-      <c r="G9" s="31"/>
+      <c r="E9" s="168"/>
+      <c r="F9" s="115" t="s">
+        <v>247</v>
+      </c>
+      <c r="G9" s="131" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1">
       <c r="B10" s="37">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="141"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="116" t="s">
-        <v>250</v>
-      </c>
-      <c r="G10" s="31"/>
+      <c r="C10" s="166"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="115" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="131"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="37">
         <v>0.625</v>
       </c>
-      <c r="C11" s="142"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="116" t="s">
-        <v>252</v>
-      </c>
-      <c r="G11" s="31"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="170"/>
+      <c r="F11" s="115" t="s">
+        <v>248</v>
+      </c>
+      <c r="G11" s="131"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="37">
@@ -5227,12 +5697,12 @@
       <c r="C12" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="127"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="116" t="s">
-        <v>253</v>
-      </c>
-      <c r="G12" s="31"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="169"/>
+      <c r="F12" s="115" t="s">
+        <v>249</v>
+      </c>
+      <c r="G12" s="131"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="37">
@@ -5241,12 +5711,12 @@
       <c r="C13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="119" t="s">
+      <c r="D13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="79" t="s">
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="130" t="s">
         <v>30</v>
       </c>
     </row>
@@ -5261,7 +5731,7 @@
       <c r="G14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="C6:C7"/>
@@ -5270,6 +5740,7 @@
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5294,34 +5765,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="93"/>
-      <c r="C4" s="93" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="92" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5420,12 +5891,12 @@
       <c r="C13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="119" t="s">
+      <c r="D13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="121"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -5469,15 +5940,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -5582,10 +6053,10 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="68"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
@@ -5596,11 +6067,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="119" t="s">
+      <c r="E13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="120"/>
-      <c r="G13" s="121"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -5610,10 +6081,10 @@
         <v>0.75</v>
       </c>
       <c r="C14" s="70"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
       <c r="H14" s="30"/>
     </row>
   </sheetData>
@@ -5632,7 +6103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2AE8B8-BDB7-4F41-A705-8351485C04E1}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -5644,30 +6115,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="94"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="93" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5759,11 +6230,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="119" t="s">
+      <c r="E13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="121"/>
-      <c r="G13" s="82" t="s">
+      <c r="F13" s="146"/>
+      <c r="G13" s="81" t="s">
         <v>30</v>
       </c>
     </row>
@@ -5805,34 +6276,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="95"/>
+      <c r="B4" s="94"/>
       <c r="C4" s="67" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="95" t="s">
+      <c r="H4" s="94" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5929,14 +6400,14 @@
         <v>0.70833333333333404</v>
       </c>
       <c r="C13" s="69"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="84" t="s">
+      <c r="D13" s="82"/>
+      <c r="E13" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="146" t="s">
+      <c r="F13" s="173" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="147"/>
+      <c r="G13" s="174"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -5980,26 +6451,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B4" s="96"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="96" t="s">
+      <c r="F4" s="95" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6122,35 +6593,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="160"/>
-      <c r="C3" s="161" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="160"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -6369,42 +6840,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="162" t="s">
+      <c r="C23" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="163"/>
-      <c r="E23" s="163"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="164"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="190"/>
+      <c r="G23" s="191"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="156"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="182"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="182"/>
+      <c r="G24" s="183"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="154" t="s">
+      <c r="C25" s="181" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="155"/>
-      <c r="E25" s="155"/>
-      <c r="F25" s="155"/>
-      <c r="G25" s="156"/>
+      <c r="D25" s="182"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="157"/>
-      <c r="D26" s="158"/>
-      <c r="E26" s="158"/>
-      <c r="F26" s="158"/>
-      <c r="G26" s="159"/>
+      <c r="C26" s="184"/>
+      <c r="D26" s="185"/>
+      <c r="E26" s="185"/>
+      <c r="F26" s="185"/>
+      <c r="G26" s="186"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -6432,42 +6903,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="148" t="s">
-        <v>254</v>
-      </c>
-      <c r="D28" s="149"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
-      <c r="G28" s="150"/>
+      <c r="C28" s="175" t="s">
+        <v>250</v>
+      </c>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="177"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="148"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="150"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="176"/>
+      <c r="E29" s="176"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="177"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="148" t="s">
-        <v>255</v>
-      </c>
-      <c r="D30" s="149"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="149"/>
-      <c r="G30" s="150"/>
+      <c r="C30" s="175" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" s="176"/>
+      <c r="E30" s="176"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="177"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="151"/>
-      <c r="D31" s="152"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="153"/>
+      <c r="C31" s="178"/>
+      <c r="D31" s="179"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="180"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -6488,10 +6959,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:M31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H4"/>
+      <selection activeCell="K5" sqref="K5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -6501,38 +6972,38 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="160" t="s">
+    <row r="2" spans="2:13" ht="16.5" customHeight="1">
+      <c r="B2" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-    </row>
-    <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="160"/>
-      <c r="C3" s="161" t="s">
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+    </row>
+    <row r="3" spans="2:13" ht="31.5">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-    </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="160"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
-    </row>
-    <row r="6" spans="2:8" ht="17.25">
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+    </row>
+    <row r="4" spans="2:13" ht="16.5" customHeight="1">
+      <c r="B4" s="187"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+    </row>
+    <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -6554,8 +7025,11 @@
       <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:8">
+      <c r="M6" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" s="9">
         <v>1</v>
       </c>
@@ -6577,46 +7051,63 @@
       <c r="H7" s="38">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:8">
+      <c r="M7" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="C8" s="192" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="194"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="2:8">
+      <c r="M8" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="196"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="197"/>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="197"/>
       <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="J10" s="1">
+        <v>19127</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="C11" s="198"/>
+      <c r="D11" s="199"/>
+      <c r="E11" s="199"/>
+      <c r="F11" s="199"/>
+      <c r="G11" s="200"/>
       <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="J11" s="1">
+        <v>18414</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="9">
         <v>8</v>
       </c>
@@ -6638,8 +7129,11 @@
       <c r="H12" s="38">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="J12" s="1">
+        <v>11040</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="24"/>
       <c r="C13" s="62" t="s">
         <v>17</v>
@@ -6651,8 +7145,11 @@
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="J13" s="1">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="62"/>
       <c r="D14" s="24"/>
@@ -6662,8 +7159,11 @@
       <c r="H14" s="66" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="J14" s="1">
+        <v>8626</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="62"/>
       <c r="D15" s="24"/>
@@ -6671,8 +7171,11 @@
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="J15" s="1">
+        <v>6827</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="64"/>
       <c r="D16" s="25"/>
@@ -6680,8 +7183,11 @@
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="9">
         <v>15</v>
       </c>
@@ -6703,8 +7209,11 @@
       <c r="H17" s="9">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="J17" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
       <c r="B18" s="24"/>
       <c r="C18" s="62" t="s">
         <v>17</v>
@@ -6716,8 +7225,11 @@
         <v>17</v>
       </c>
       <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="J18" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
       <c r="B19" s="24"/>
       <c r="C19" s="62"/>
       <c r="D19" s="24"/>
@@ -6725,8 +7237,11 @@
       <c r="F19" s="24"/>
       <c r="G19" s="62"/>
       <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="J19" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="24"/>
       <c r="C20" s="62"/>
       <c r="D20" s="24"/>
@@ -6734,8 +7249,11 @@
       <c r="F20" s="24"/>
       <c r="G20" s="62"/>
       <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
       <c r="B21" s="25"/>
       <c r="C21" s="64"/>
       <c r="D21" s="25"/>
@@ -6743,8 +7261,11 @@
       <c r="F21" s="25"/>
       <c r="G21" s="64"/>
       <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="J21" s="1">
+        <v>10877</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
       <c r="B22" s="9">
         <v>22</v>
       </c>
@@ -6766,8 +7287,11 @@
       <c r="H22" s="38">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="J22" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -6777,8 +7301,11 @@
       <c r="H23" s="26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -6786,8 +7313,11 @@
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -6795,8 +7325,11 @@
       <c r="F25" s="26"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
-    </row>
-    <row r="26" spans="2:8">
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -6805,7 +7338,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:10">
       <c r="B27" s="9">
         <v>29</v>
       </c>
@@ -6820,9 +7353,9 @@
       <c r="G27" s="42"/>
       <c r="H27" s="43"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:10">
       <c r="B28" s="26"/>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="85" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="40"/>
@@ -6831,27 +7364,27 @@
       <c r="G28" s="26"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:10">
       <c r="B29" s="26"/>
-      <c r="C29" s="86"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="40"/>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:10">
       <c r="B30" s="26"/>
-      <c r="C30" s="86"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="40"/>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:10">
       <c r="B31" s="27"/>
-      <c r="C31" s="87"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="41"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
@@ -6859,11 +7392,12 @@
       <c r="H31" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C8:G11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- 2023-01-02 결산 3주차 1일차
결산 엑셀 업데이트
2주차 보고서 작성
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E27F9-6CF7-4B54-9118-C2994E61173E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A0CB5A-DBB8-4F07-8EDE-7EDAE1BAA86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -25,7 +25,8 @@
     <sheet name="2월" sheetId="21" r:id="rId10"/>
     <sheet name="결산" sheetId="29" r:id="rId11"/>
     <sheet name="크롤링" sheetId="30" r:id="rId12"/>
-    <sheet name="크롤링 (2)" sheetId="33" r:id="rId13"/>
+    <sheet name="크롤링 데이터 모음" sheetId="33" r:id="rId13"/>
+    <sheet name="질문 모음집" sheetId="34" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="421">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1336,6 +1337,234 @@
   </si>
   <si>
     <t>cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잔여 크롤링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 주 계획 짜기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀원 피드백</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리 과정 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 목적성 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 목적 잡기\</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리시 필요 모델 조사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 키워드를 보여주는 것</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어떤 목적으로 정확히 보여줄지 </t>
+  </si>
+  <si>
+    <t>요약리뷰의 단점을 보완한 방법</t>
+  </si>
+  <si>
+    <t>(방대한 리뷰를 한 줄로 줄이려다보니, 데이터의 손실(중요한 리뷰의 손실)이 크다.</t>
+  </si>
+  <si>
+    <t>네트워크 분석</t>
+  </si>
+  <si>
+    <t>중요한 점 : 관계를 생각한다.</t>
+  </si>
+  <si>
+    <t>ex ) sns</t>
+  </si>
+  <si>
+    <t>다수의 리뷰에서 공통적으로 등장하는 키워드를 기점으로 시작한다.</t>
+  </si>
+  <si>
+    <t>* 제로슈가 음료와 탄산수의 상품 리뷰 데이터를 가지고 의미 연결망(keyword_network)을 분석하여 네트워크 시각화 서비스</t>
+  </si>
+  <si>
+    <t>1. 노드 개수 / 각 노드마다의 거리 합</t>
+  </si>
+  <si>
+    <t>연결중심성 : 연결이 얼마나 많이 되었느냐</t>
+  </si>
+  <si>
+    <t>근접 중심성 : 거리값이 1에 가까운 녀석</t>
+  </si>
+  <si>
+    <t>매개 중심성 : 노드가 가장 많이 거치는 녀석</t>
+  </si>
+  <si>
+    <t>위세중심성 : 중요한 노드들과 연결되어있는 노드</t>
+  </si>
+  <si>
+    <t>2. Concor 분석</t>
+  </si>
+  <si>
+    <t>하위 집단 분류</t>
+  </si>
+  <si>
+    <t>3. ngram</t>
+  </si>
+  <si>
+    <t>- 2개씩 : bigram</t>
+  </si>
+  <si>
+    <t>--------------------------</t>
+  </si>
+  <si>
+    <t>1. 다방면에  서비스를 할 수 있다면</t>
+  </si>
+  <si>
+    <t>서비스 기획</t>
+  </si>
+  <si>
+    <t xml:space="preserve">상품 리뷰 키워드 분석 -&gt; 리뷰 요약시 손실 데이터가 많다 </t>
+  </si>
+  <si>
+    <t>-&gt; 유용한 데이터를 사용하여 소비자 뿐만 아니라 판매자에게도 유용한 서비스 제공(네트워크 분석)</t>
+  </si>
+  <si>
+    <t>데이터 내용</t>
+  </si>
+  <si>
+    <t>쇼핑몰 사이트 크롤링</t>
+  </si>
+  <si>
+    <t>Q) 실제로 현업에서도 상업적으로 네트워크 분석이 이용중인 사례가 있나요</t>
+  </si>
+  <si>
+    <t>Q) 쇼핑몰 사이트에서 서비스 사용시 유용할까요</t>
+  </si>
+  <si>
+    <t>Concor 공통된 주제는 input인가 output인가</t>
+  </si>
+  <si>
+    <t>구매자 상품의 보완 등을 할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자 상품의 장점 단점 등을 알 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다이어트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당뇨, 고혈압 이런 쪽으로도 연결이 될 것 같다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델링 생각할 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023 01 02</t>
+  </si>
+  <si>
+    <t>해야할 일</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 잔존 크롤링 해결 </t>
+  </si>
+  <si>
+    <t>현재 탄산수</t>
+  </si>
+  <si>
+    <t>트레비 씨그램 빅토리아</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3개</t>
+  </si>
+  <si>
+    <t>-&gt; 차라리 탄산수 5개 제로슈거 10개 이렇게는 어떤지</t>
+  </si>
+  <si>
+    <t>2. 전처리를 위한 데이터 정리 및 분석하기</t>
+  </si>
+  <si>
+    <t>상품명_개수_사이트명_crawling</t>
+  </si>
+  <si>
+    <t>if 사이트 2개 이상</t>
+  </si>
+  <si>
+    <t>상품명_개수_사이트명_번호_crawling</t>
+  </si>
+  <si>
+    <t>번호 [01 , 02 , 03 ....]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 결측값</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 삭제할 값</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 중복값 등등</t>
+  </si>
+  <si>
+    <t>3. 주간보고서 제출하기</t>
+  </si>
+  <si>
+    <t>개행</t>
+  </si>
+  <si>
+    <t>특수문자</t>
+  </si>
+  <si>
+    <t>임티</t>
+  </si>
+  <si>
+    <t>\W</t>
+  </si>
+  <si>
+    <t>전처리 코드 찾자</t>
+  </si>
+  <si>
+    <t>유사/동일 언어 확인</t>
+  </si>
+  <si>
+    <t>일반 명사들로 분리</t>
+  </si>
+  <si>
+    <t>형용사-&gt;명사처리</t>
+  </si>
+  <si>
+    <t>줄임말</t>
+  </si>
+  <si>
+    <t>은어, 비속어</t>
+  </si>
+  <si>
+    <t xml:space="preserve">오타 </t>
+  </si>
+  <si>
+    <t>1. 서칭 - 자연어 처리 방법 서칭</t>
+  </si>
+  <si>
+    <t>개행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디어 서칭</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2176,7 +2405,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2621,6 +2850,36 @@
     <xf numFmtId="20" fontId="13" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2822,44 +3081,20 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3592,8 +3827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDE6C63-9121-4583-87EA-DA9F0C78BEC1}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -3604,14 +3839,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -3635,12 +3870,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -3655,7 +3890,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="159" t="s">
+      <c r="E6" s="169" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -3673,7 +3908,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="160"/>
+      <c r="E7" s="170"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -3695,19 +3930,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="156" t="s">
+      <c r="D9" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="156" t="s">
+      <c r="E9" s="166" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="161" t="s">
+      <c r="F9" s="171" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="166" t="s">
+      <c r="G9" s="176" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3715,21 +3950,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="154"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="162"/>
-      <c r="G10" s="167"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="177"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="155"/>
-      <c r="D11" s="158"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="162"/>
-      <c r="G11" s="167"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="172"/>
+      <c r="G11" s="177"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -3739,9 +3974,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="163"/>
-      <c r="G12" s="168"/>
+      <c r="E12" s="168"/>
+      <c r="F12" s="173"/>
+      <c r="G12" s="178"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -3750,11 +3985,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="150" t="s">
+      <c r="D13" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="151"/>
-      <c r="F13" s="152"/>
+      <c r="E13" s="161"/>
+      <c r="F13" s="162"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -3810,8 +4045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -3822,35 +4057,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="196"/>
-      <c r="C3" s="197" t="s">
+      <c r="B3" s="206"/>
+      <c r="C3" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="196"/>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
+      <c r="B4" s="206"/>
+      <c r="C4" s="207"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="207"/>
+      <c r="G4" s="207"/>
+      <c r="H4" s="207"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4175,19 +4410,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.375" hidden="1" customWidth="1"/>
     <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="32.75" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="25.625" hidden="1" customWidth="1"/>
     <col min="8" max="9" width="31.5" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="115.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
@@ -4286,7 +4523,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="220" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -4304,7 +4541,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="214" t="s">
+      <c r="G2" s="224" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -4315,9 +4552,12 @@
       <c r="K2" s="86" t="s">
         <v>286</v>
       </c>
+      <c r="L2" s="86" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="210"/>
+      <c r="A3" s="220"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -4331,7 +4571,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="214"/>
+      <c r="G3" s="224"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -4342,9 +4582,12 @@
       <c r="K3" s="133" t="s">
         <v>289</v>
       </c>
+      <c r="L3" s="86" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="210"/>
+      <c r="A4" s="220"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -4356,7 +4599,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="214"/>
+      <c r="G4" s="224"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -4367,9 +4610,12 @@
       <c r="K4" s="86" t="s">
         <v>292</v>
       </c>
+      <c r="L4" s="86" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="210"/>
+      <c r="A5" s="220"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -4383,7 +4629,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="214"/>
+      <c r="G5" s="224"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -4391,9 +4637,12 @@
       <c r="K5" s="86" t="s">
         <v>276</v>
       </c>
+      <c r="L5" s="86" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="210"/>
+      <c r="A6" s="220"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -4409,7 +4658,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="214"/>
+      <c r="G6" s="224"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -4417,7 +4666,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="211" t="s">
+      <c r="A7" s="221" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -4433,7 +4682,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="214"/>
+      <c r="G7" s="224"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -4446,9 +4695,12 @@
       <c r="K7" s="87" t="s">
         <v>281</v>
       </c>
+      <c r="L7" s="87" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="211"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -4460,7 +4712,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="214"/>
+      <c r="G8" s="224"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -4473,9 +4725,12 @@
       <c r="K8" s="87" t="s">
         <v>282</v>
       </c>
+      <c r="L8" s="87" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="211"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -4487,7 +4742,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="214"/>
+      <c r="G9" s="224"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -4495,9 +4750,12 @@
       <c r="K9" s="87" t="s">
         <v>287</v>
       </c>
+      <c r="L9" s="87" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="211"/>
+      <c r="A10" s="221"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -4509,7 +4767,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="214"/>
+      <c r="G10" s="224"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -4517,7 +4775,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="211"/>
+      <c r="A11" s="221"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -4529,12 +4787,12 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="214"/>
+      <c r="G11" s="224"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="212" t="s">
+      <c r="A12" s="222" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -4548,7 +4806,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="214"/>
+      <c r="G12" s="224"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -4561,14 +4819,14 @@
       </c>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="212"/>
+      <c r="A13" s="222"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="214"/>
+      <c r="G13" s="224"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -4578,47 +4836,47 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="212"/>
+      <c r="A14" s="222"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="214"/>
+      <c r="G14" s="224"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
       <c r="I14" s="100"/>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="212"/>
+      <c r="A15" s="222"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="214"/>
+      <c r="G15" s="224"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="100"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="212"/>
+      <c r="A16" s="222"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="214"/>
+      <c r="G16" s="224"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
     </row>
-    <row r="17" spans="1:11" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="213" t="s">
+    <row r="17" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="223" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -4626,7 +4884,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="214"/>
+      <c r="G17" s="224"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -4635,55 +4893,61 @@
       <c r="K17" s="89" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="213"/>
+      <c r="L17" s="89" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="223"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="214"/>
+      <c r="G18" s="224"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
-    </row>
-    <row r="19" spans="1:11" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="213"/>
+      <c r="L18" s="89" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="223"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="214"/>
+      <c r="G19" s="224"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
     </row>
-    <row r="20" spans="1:11" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="213"/>
+    <row r="20" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="223"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="214"/>
+      <c r="G20" s="224"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
     </row>
-    <row r="21" spans="1:11" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="213"/>
+    <row r="21" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="223"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="214"/>
+      <c r="G21" s="224"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
     </row>
-    <row r="22" spans="1:11" s="100" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:12" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
     </row>
-    <row r="23" spans="1:11" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:12" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -4715,7 +4979,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1">
+    <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -4740,8 +5004,11 @@
       <c r="J24" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1">
+      <c r="L24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -4770,7 +5037,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" customHeight="1">
+    <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -4789,8 +5056,11 @@
       <c r="J26" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1">
+      <c r="L26" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -4816,7 +5086,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1">
+    <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -4832,8 +5102,11 @@
       <c r="I28" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1">
+      <c r="L28" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -4852,8 +5125,11 @@
       <c r="I29" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1">
+      <c r="L29" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -4867,15 +5143,18 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1">
+    <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
       <c r="I31" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1">
+      <c r="L31" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -4885,16 +5164,22 @@
       <c r="D32" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" customHeight="1">
+      <c r="L32" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="D33" t="s">
         <v>101</v>
       </c>
       <c r="J33" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="30" customHeight="1">
+      <c r="L33" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -4908,7 +5193,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" customHeight="1">
+    <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="B35" t="s">
         <v>65</v>
       </c>
@@ -4918,8 +5203,11 @@
       <c r="J35" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="30" customHeight="1">
+      <c r="L35" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="B36" t="s">
         <v>66</v>
       </c>
@@ -4930,20 +5218,23 @@
         <v>297</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1">
+    <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="B37" s="105" t="s">
         <v>67</v>
       </c>
       <c r="D37" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1">
+      <c r="L37" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="D38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1">
+    <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
@@ -4953,103 +5244,204 @@
       <c r="J39" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="30" customHeight="1">
+      <c r="L39" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30" customHeight="1">
+      <c r="L41" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="J42" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1">
+      <c r="L42" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="J43" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1">
+      <c r="L43" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="30" customHeight="1">
       <c r="J44" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1">
+      <c r="L44" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="30" customHeight="1">
       <c r="J45" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="30" customHeight="1">
+    <row r="46" spans="1:12" ht="30" customHeight="1">
+      <c r="L46" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30" customHeight="1">
+      <c r="L47" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30" customHeight="1">
       <c r="J48" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="10:10" ht="30" customHeight="1">
+    <row r="49" spans="10:12" ht="30" customHeight="1">
+      <c r="L49" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12" ht="30" customHeight="1">
+      <c r="L50" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12" ht="30" customHeight="1">
       <c r="J51" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="10:10" ht="30" customHeight="1">
+    <row r="52" spans="10:12" ht="30" customHeight="1">
       <c r="J52" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="53" spans="10:10" ht="30" customHeight="1">
+      <c r="L52" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="53" spans="10:12" ht="30" customHeight="1">
       <c r="J53" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="54" spans="10:10" ht="30" customHeight="1">
+    <row r="54" spans="10:12" ht="30" customHeight="1">
       <c r="J54" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="10:10" ht="30" customHeight="1">
+    <row r="55" spans="10:12" ht="30" customHeight="1">
+      <c r="L55" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="57" spans="10:12" ht="30" customHeight="1">
       <c r="J57" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="60" spans="10:10" ht="30" customHeight="1">
+      <c r="L57" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="58" spans="10:12" ht="30" customHeight="1">
+      <c r="L58" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="59" spans="10:12" ht="30" customHeight="1">
+      <c r="L59" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="60" spans="10:12" ht="30" customHeight="1">
       <c r="J60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="61" spans="10:10" ht="30" customHeight="1">
+      <c r="L60" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="61" spans="10:12" ht="30" customHeight="1">
       <c r="J61" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="10:10" ht="30" customHeight="1">
+    <row r="62" spans="10:12" ht="30" customHeight="1">
+      <c r="L62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="10:12" ht="30" customHeight="1">
       <c r="J63" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="65" spans="10:10" ht="30" customHeight="1">
+      <c r="L63" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="64" spans="10:12" ht="30" customHeight="1">
+      <c r="L64" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="65" spans="10:12" ht="30" customHeight="1">
       <c r="J65" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="66" spans="10:10" ht="30" customHeight="1">
+      <c r="L65" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12" ht="30" customHeight="1">
       <c r="J66" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="10:10" ht="30" customHeight="1">
+    <row r="67" spans="10:12" ht="30" customHeight="1">
+      <c r="L67" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12" ht="30" customHeight="1">
+      <c r="L68" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="70" spans="10:12" ht="30" customHeight="1">
       <c r="J70" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="73" spans="10:10" ht="30" customHeight="1">
+      <c r="L70" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="71" spans="10:12" ht="30" customHeight="1">
+      <c r="L71" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="10:12" ht="30" customHeight="1">
       <c r="J73" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="74" spans="10:10" ht="30" customHeight="1">
+      <c r="L73" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="74" spans="10:12" ht="30" customHeight="1">
       <c r="J74" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="77" spans="10:10" ht="30" customHeight="1">
+      <c r="L74" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="77" spans="10:12" ht="30" customHeight="1">
       <c r="J77" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="10:10" ht="30" customHeight="1">
+    <row r="80" spans="10:12" ht="30" customHeight="1">
       <c r="J80" t="s">
         <v>189</v>
       </c>
@@ -5347,11 +5739,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4682B6DF-860A-46A3-B003-691AA560AE2A}">
   <dimension ref="A1:BH44"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="21" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="21" topLeftCell="F51" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="H27" sqref="H27"/>
+      <selection pane="topRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6173,11 +6566,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E416609B-A342-4E94-929E-80BF1FFEBFD0}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="12" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="H27" sqref="H27"/>
+      <selection pane="topRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6193,58 +6587,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="116" customFormat="1" ht="18" thickTop="1" thickBot="1">
-      <c r="A1" s="218" t="s">
+      <c r="A1" s="150" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="151" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="219" t="s">
+      <c r="C1" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="D1" s="219" t="s">
+      <c r="D1" s="151" t="s">
         <v>346</v>
       </c>
-      <c r="E1" s="219" t="s">
+      <c r="E1" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="F1" s="219" t="s">
+      <c r="F1" s="151" t="s">
         <v>346</v>
       </c>
-      <c r="G1" s="219" t="s">
+      <c r="G1" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="H1" s="219" t="s">
+      <c r="H1" s="151" t="s">
         <v>346</v>
       </c>
-      <c r="I1" s="219" t="s">
+      <c r="I1" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="J1" s="220" t="s">
+      <c r="J1" s="152" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="156" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="225"/>
-      <c r="C2" s="226" t="s">
+      <c r="B2" s="157"/>
+      <c r="C2" s="225" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226" t="s">
+      <c r="D2" s="225"/>
+      <c r="E2" s="225" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226" t="s">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226" t="s">
+      <c r="H2" s="225"/>
+      <c r="I2" s="225" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="227"/>
+      <c r="J2" s="226"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -6253,341 +6647,269 @@
       <c r="A3" s="121" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="216">
-        <f>SUM(C3:YP3)</f>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B17" si="0">SUM(C3:YP3)</f>
         <v>20000</v>
       </c>
-      <c r="C3" s="216"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216">
+      <c r="E3" s="1">
         <v>10000</v>
       </c>
-      <c r="F3" s="216"/>
-      <c r="G3" s="216">
+      <c r="G3" s="1">
         <v>10000</v>
       </c>
-      <c r="H3" s="216"/>
-      <c r="I3" s="216"/>
-      <c r="J3" s="217"/>
+      <c r="J3" s="149"/>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="121" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="216">
-        <f>SUM(C4:YP4)</f>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
         <v>11054</v>
       </c>
-      <c r="C4" s="216"/>
-      <c r="D4" s="216"/>
-      <c r="E4" s="216">
+      <c r="E4" s="1">
         <v>5364</v>
       </c>
-      <c r="F4" s="216"/>
-      <c r="G4" s="216">
+      <c r="G4" s="1">
         <v>5690</v>
       </c>
-      <c r="H4" s="216"/>
-      <c r="I4" s="216"/>
-      <c r="J4" s="217"/>
+      <c r="J4" s="149"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="121" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="216">
-        <f>SUM(C5:YP5)</f>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
         <v>12652</v>
       </c>
-      <c r="C5" s="216">
+      <c r="C5" s="1">
         <v>2000</v>
       </c>
-      <c r="D5" s="216"/>
-      <c r="E5" s="216">
+      <c r="E5" s="1">
         <v>10000</v>
       </c>
-      <c r="F5" s="216"/>
-      <c r="G5" s="216">
+      <c r="G5" s="1">
         <v>652</v>
       </c>
-      <c r="H5" s="216"/>
-      <c r="I5" s="216"/>
-      <c r="J5" s="217"/>
+      <c r="J5" s="149"/>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="121" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="216">
-        <f>SUM(C6:YP6)</f>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
         <v>10458</v>
       </c>
-      <c r="C6" s="216">
+      <c r="C6" s="1">
         <v>2000</v>
       </c>
-      <c r="D6" s="216"/>
-      <c r="E6" s="216">
+      <c r="E6" s="1">
         <v>1905</v>
       </c>
-      <c r="F6" s="216"/>
-      <c r="G6" s="216">
+      <c r="G6" s="1">
         <v>5053</v>
       </c>
-      <c r="H6" s="216"/>
-      <c r="I6" s="216">
+      <c r="I6" s="1">
         <v>1500</v>
       </c>
-      <c r="J6" s="217"/>
+      <c r="J6" s="149"/>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="121" t="s">
         <v>267</v>
       </c>
-      <c r="B7" s="216">
-        <f>SUM(C7:YP7)</f>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
         <v>10476</v>
       </c>
-      <c r="C7" s="216"/>
-      <c r="D7" s="216"/>
-      <c r="E7" s="216">
+      <c r="E7" s="1">
         <f xml:space="preserve"> SUM(4585 +2295)</f>
         <v>6880</v>
       </c>
-      <c r="F7" s="216"/>
-      <c r="G7" s="216">
+      <c r="G7" s="1">
         <v>3596</v>
       </c>
-      <c r="H7" s="216"/>
-      <c r="I7" s="216"/>
-      <c r="J7" s="217"/>
+      <c r="J7" s="149"/>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="121" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="216">
-        <f>SUM(C8:YP8)</f>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
         <v>10921</v>
       </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216">
+      <c r="E8" s="1">
         <v>2295</v>
       </c>
-      <c r="F8" s="216"/>
-      <c r="G8" s="216">
+      <c r="G8" s="1">
         <v>8626</v>
       </c>
-      <c r="H8" s="216"/>
-      <c r="I8" s="216"/>
-      <c r="J8" s="217"/>
+      <c r="J8" s="149"/>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="121" t="s">
         <v>266</v>
       </c>
-      <c r="B9" s="216">
-        <f>SUM(C9:YP9)</f>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216">
+      <c r="E9" s="1">
         <v>10000</v>
       </c>
-      <c r="F9" s="216"/>
-      <c r="G9" s="216">
+      <c r="G9" s="1">
         <v>10000</v>
       </c>
-      <c r="H9" s="216"/>
-      <c r="I9" s="216"/>
-      <c r="J9" s="217"/>
+      <c r="J9" s="149"/>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="121" t="s">
         <v>269</v>
       </c>
-      <c r="B10" s="216">
-        <f>SUM(C10:YP10)</f>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
         <v>16827</v>
       </c>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216">
+      <c r="E10" s="1">
         <v>10000</v>
       </c>
-      <c r="F10" s="216"/>
-      <c r="G10" s="216">
+      <c r="G10" s="1">
         <v>6827</v>
       </c>
-      <c r="H10" s="216"/>
-      <c r="I10" s="216"/>
-      <c r="J10" s="217"/>
+      <c r="J10" s="149"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="121" t="s">
         <v>271</v>
       </c>
-      <c r="B11" s="216">
-        <f>SUM(C11:YP11)</f>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
         <v>10522</v>
       </c>
-      <c r="C11" s="216">
+      <c r="C11" s="1">
         <v>2000</v>
       </c>
-      <c r="D11" s="216"/>
-      <c r="E11" s="216">
+      <c r="E11" s="1">
         <v>5996</v>
       </c>
-      <c r="F11" s="216"/>
-      <c r="G11" s="216">
+      <c r="G11" s="1">
         <v>2526</v>
       </c>
-      <c r="H11" s="216"/>
-      <c r="I11" s="216"/>
-      <c r="J11" s="217"/>
+      <c r="J11" s="149"/>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="121" t="s">
         <v>347</v>
       </c>
-      <c r="B12" s="216">
-        <f>SUM(C12:YP12)</f>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
         <v>10925</v>
       </c>
-      <c r="C12" s="216">
+      <c r="C12" s="1">
         <f xml:space="preserve"> SUM(1440+1369)</f>
         <v>2809</v>
       </c>
-      <c r="D12" s="216"/>
-      <c r="E12" s="216"/>
-      <c r="F12" s="216"/>
-      <c r="G12" s="216">
+      <c r="G12" s="1">
         <v>8116</v>
       </c>
-      <c r="H12" s="216"/>
-      <c r="I12" s="216"/>
-      <c r="J12" s="217"/>
+      <c r="J12" s="149"/>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="148" t="s">
         <v>344</v>
       </c>
-      <c r="B13" s="216">
-        <f>SUM(C13:YP13)</f>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
         <v>27888</v>
       </c>
-      <c r="C13" s="216"/>
-      <c r="D13" s="216"/>
-      <c r="E13" s="216">
+      <c r="E13" s="1">
         <v>17888</v>
       </c>
-      <c r="F13" s="216"/>
-      <c r="G13" s="216">
+      <c r="G13" s="1">
         <v>10000</v>
       </c>
-      <c r="H13" s="216"/>
-      <c r="I13" s="216"/>
-      <c r="J13" s="217"/>
+      <c r="J13" s="149"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="215" t="s">
+      <c r="A14" s="148" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="216">
-        <f>SUM(C14:YP14)</f>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
         <v>16567</v>
       </c>
-      <c r="C14" s="216"/>
-      <c r="D14" s="216"/>
-      <c r="E14" s="216">
+      <c r="E14" s="1">
         <v>6567</v>
       </c>
-      <c r="F14" s="216"/>
-      <c r="G14" s="216">
+      <c r="G14" s="1">
         <v>10000</v>
       </c>
-      <c r="H14" s="216"/>
-      <c r="I14" s="216"/>
-      <c r="J14" s="217"/>
+      <c r="J14" s="149"/>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" s="215" t="s">
+      <c r="A15" s="148" t="s">
         <v>290</v>
       </c>
-      <c r="B15" s="216">
-        <f>SUM(C15:YP15)</f>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="C15" s="216"/>
-      <c r="D15" s="216"/>
-      <c r="E15" s="216">
+      <c r="E15" s="1">
         <v>10000</v>
       </c>
-      <c r="F15" s="216"/>
-      <c r="G15" s="216"/>
-      <c r="H15" s="216"/>
-      <c r="I15" s="216"/>
-      <c r="J15" s="217"/>
+      <c r="J15" s="149"/>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" s="215" t="s">
+      <c r="A16" s="148" t="s">
         <v>272</v>
       </c>
-      <c r="B16" s="216">
-        <f>SUM(C16:YP16)</f>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="C16" s="216"/>
-      <c r="D16" s="216"/>
-      <c r="E16" s="216">
+      <c r="E16" s="1">
         <v>10000</v>
       </c>
-      <c r="F16" s="216"/>
-      <c r="G16" s="216">
+      <c r="G16" s="1">
         <v>10000</v>
       </c>
-      <c r="H16" s="216"/>
-      <c r="I16" s="216"/>
-      <c r="J16" s="217"/>
+      <c r="J16" s="149"/>
     </row>
     <row r="17" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A17" s="215" t="s">
+      <c r="A17" s="148" t="s">
         <v>273</v>
       </c>
-      <c r="B17" s="216">
-        <f>SUM(C17:YP17)</f>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="C17" s="216"/>
-      <c r="D17" s="216"/>
-      <c r="E17" s="216">
+      <c r="E17" s="1">
         <v>10000</v>
       </c>
-      <c r="F17" s="216"/>
-      <c r="G17" s="216">
+      <c r="G17" s="1">
         <v>10000</v>
       </c>
-      <c r="H17" s="216"/>
-      <c r="I17" s="216"/>
-      <c r="J17" s="217"/>
+      <c r="J17" s="149"/>
     </row>
     <row r="18" spans="1:10" ht="18" thickTop="1" thickBot="1">
-      <c r="A18" s="221" t="s">
+      <c r="A18" s="153" t="s">
         <v>348</v>
       </c>
-      <c r="B18" s="222">
+      <c r="B18" s="154">
         <f>SUM(B3:B17)</f>
         <v>228290</v>
       </c>
-      <c r="C18" s="222"/>
-      <c r="D18" s="222"/>
-      <c r="E18" s="222"/>
-      <c r="F18" s="222"/>
-      <c r="G18" s="222"/>
-      <c r="H18" s="222"/>
-      <c r="I18" s="222"/>
-      <c r="J18" s="223"/>
+      <c r="C18" s="154"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="155"/>
     </row>
     <row r="19" spans="1:10" ht="17.25" thickTop="1"/>
   </sheetData>
@@ -6602,12 +6924,247 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="229" customFormat="1">
+      <c r="A1" s="229" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>414</v>
+      </c>
+      <c r="C14" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C16" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>416</v>
+      </c>
+      <c r="C18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>417</v>
+      </c>
+      <c r="C20" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="C21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="C23" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="C25" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="C28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="C29" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="C31" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" t="s">
+        <v>385</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251ECE8D-9668-40EA-AFB2-EB0A37392AB0}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -6618,14 +7175,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -6669,19 +7226,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="169" t="s">
+      <c r="C6" s="179" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="156" t="s">
+      <c r="D6" s="166" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="174" t="s">
+      <c r="E6" s="184" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="177" t="s">
+      <c r="G6" s="187" t="s">
         <v>280</v>
       </c>
     </row>
@@ -6689,13 +7246,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="175"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="168"/>
+      <c r="E7" s="185"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="178"/>
+      <c r="G7" s="188"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -6711,13 +7268,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="171" t="s">
+      <c r="C9" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="156" t="s">
+      <c r="D9" s="166" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="174"/>
+      <c r="E9" s="184"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -6729,9 +7286,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="172"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="176"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="186"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -6741,9 +7298,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="173"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="176"/>
+      <c r="C11" s="183"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="186"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -6756,8 +7313,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="158"/>
-      <c r="E12" s="175"/>
+      <c r="D12" s="168"/>
+      <c r="E12" s="185"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -6770,11 +7327,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="150" t="s">
+      <c r="D13" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="151"/>
-      <c r="F13" s="151"/>
+      <c r="E13" s="161"/>
+      <c r="F13" s="161"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -6810,10 +7367,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
-  <dimension ref="B2:H14"/>
+  <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -6824,15 +7381,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -6862,7 +7419,9 @@
       <c r="C5" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>143</v>
+      </c>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
       <c r="G5" s="32"/>
@@ -6872,7 +7431,7 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="179" t="s">
+      <c r="C6" s="189" t="s">
         <v>341</v>
       </c>
       <c r="D6" s="32"/>
@@ -6885,7 +7444,7 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="180"/>
+      <c r="C7" s="190"/>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
@@ -6896,7 +7455,7 @@
       <c r="B8" s="36">
         <v>0.5</v>
       </c>
-      <c r="C8" s="181"/>
+      <c r="C8" s="191"/>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
@@ -6958,12 +7517,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="150" t="s">
+      <c r="D13" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="151"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="152"/>
+      <c r="E13" s="161"/>
+      <c r="F13" s="161"/>
+      <c r="G13" s="162"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -6978,6 +7537,308 @@
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="C16" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="227"/>
+      <c r="D17" s="227"/>
+      <c r="E17" s="227"/>
+      <c r="F17" s="227"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="227" t="s">
+        <v>392</v>
+      </c>
+      <c r="D18" s="227"/>
+      <c r="E18" s="227"/>
+      <c r="F18" s="227"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="227"/>
+      <c r="D19" s="228"/>
+      <c r="E19" s="227"/>
+      <c r="F19" s="227"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="227" t="s">
+        <v>393</v>
+      </c>
+      <c r="D20" s="228"/>
+      <c r="E20" s="227"/>
+      <c r="F20" s="227"/>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="227"/>
+      <c r="D21" s="228"/>
+      <c r="E21" s="227"/>
+      <c r="F21" s="227"/>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="227" t="s">
+        <v>394</v>
+      </c>
+      <c r="D22" s="228"/>
+      <c r="E22" s="227"/>
+      <c r="F22" s="227"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="227" t="s">
+        <v>395</v>
+      </c>
+      <c r="D23" s="228"/>
+      <c r="E23" s="227"/>
+      <c r="F23" s="227"/>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="227" t="s">
+        <v>396</v>
+      </c>
+      <c r="D24" s="228"/>
+      <c r="E24" s="227"/>
+      <c r="F24" s="227"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="227"/>
+      <c r="D25" s="228"/>
+      <c r="E25" s="227"/>
+      <c r="F25" s="227"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="227" t="s">
+        <v>397</v>
+      </c>
+      <c r="D26" s="228"/>
+      <c r="E26" s="227"/>
+      <c r="F26" s="227"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="227"/>
+      <c r="D27" s="228"/>
+      <c r="E27" s="227"/>
+      <c r="F27" s="227"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="227" t="s">
+        <v>398</v>
+      </c>
+      <c r="D28" s="228"/>
+      <c r="E28" s="227"/>
+      <c r="F28" s="227"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="227"/>
+      <c r="D29" s="228"/>
+      <c r="E29" s="227"/>
+      <c r="F29" s="227"/>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="227">
+        <v>-1</v>
+      </c>
+      <c r="D30" s="228"/>
+      <c r="E30" s="227"/>
+      <c r="F30" s="227"/>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="227" t="s">
+        <v>399</v>
+      </c>
+      <c r="D31" s="228"/>
+      <c r="E31" s="227"/>
+      <c r="F31" s="227"/>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="227"/>
+      <c r="D32" s="228"/>
+      <c r="E32" s="227"/>
+      <c r="F32" s="227"/>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="227" t="s">
+        <v>400</v>
+      </c>
+      <c r="D33" s="228"/>
+      <c r="E33" s="227"/>
+      <c r="F33" s="227"/>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="227" t="s">
+        <v>401</v>
+      </c>
+      <c r="D34" s="228"/>
+      <c r="E34" s="227"/>
+      <c r="F34" s="227"/>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" s="227"/>
+      <c r="D35" s="228"/>
+      <c r="E35" s="227"/>
+      <c r="F35" s="227"/>
+    </row>
+    <row r="36" spans="3:6">
+      <c r="C36" s="227" t="s">
+        <v>402</v>
+      </c>
+      <c r="D36" s="228"/>
+      <c r="E36" s="227"/>
+      <c r="F36" s="227"/>
+    </row>
+    <row r="37" spans="3:6">
+      <c r="C37" s="227"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="227"/>
+      <c r="F37" s="227"/>
+    </row>
+    <row r="38" spans="3:6">
+      <c r="C38" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="3:6">
+      <c r="C39" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="C41" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="3:6">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="C43" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="3:6">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="3:6">
+      <c r="C47" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="3:6">
+      <c r="C48" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="C51" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="C55" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="3:4">
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="3:4">
+      <c r="C58" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="3:4">
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="3:4">
+      <c r="C60" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="3:4">
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="3:4">
+      <c r="C62" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="3:4">
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="3:4">
+      <c r="C64" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D64"/>
+    </row>
+    <row r="65" spans="3:4">
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="3:4">
+      <c r="C66" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="3:4">
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="3:4">
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="3:4">
+      <c r="D69"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6996,8 +7857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7008,15 +7869,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -7135,11 +7996,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="150" t="s">
+      <c r="E13" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="151"/>
-      <c r="G13" s="152"/>
+      <c r="F13" s="161"/>
+      <c r="G13" s="162"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -7171,8 +8032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2AE8B8-BDB7-4F41-A705-8351485C04E1}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7183,14 +8044,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -7298,10 +8159,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="150" t="s">
+      <c r="E13" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="152"/>
+      <c r="F13" s="162"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -7332,8 +8193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA729C5-F4A6-4AC1-AD36-A96A4028E1F4}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7344,15 +8205,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -7472,10 +8333,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="182" t="s">
+      <c r="F13" s="192" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="183"/>
+      <c r="G13" s="193"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -7507,8 +8368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7519,13 +8380,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -7649,8 +8510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7661,35 +8522,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="196"/>
-      <c r="C3" s="197" t="s">
+      <c r="B3" s="206"/>
+      <c r="C3" s="207" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="196"/>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
+      <c r="B4" s="206"/>
+      <c r="C4" s="207"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="207"/>
+      <c r="G4" s="207"/>
+      <c r="H4" s="207"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -7908,42 +8769,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="198" t="s">
+      <c r="C23" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="199"/>
-      <c r="E23" s="199"/>
-      <c r="F23" s="199"/>
-      <c r="G23" s="200"/>
+      <c r="D23" s="209"/>
+      <c r="E23" s="209"/>
+      <c r="F23" s="209"/>
+      <c r="G23" s="210"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="190"/>
-      <c r="D24" s="191"/>
-      <c r="E24" s="191"/>
-      <c r="F24" s="191"/>
-      <c r="G24" s="192"/>
+      <c r="C24" s="200"/>
+      <c r="D24" s="201"/>
+      <c r="E24" s="201"/>
+      <c r="F24" s="201"/>
+      <c r="G24" s="202"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="190" t="s">
+      <c r="C25" s="200" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="191"/>
-      <c r="E25" s="191"/>
-      <c r="F25" s="191"/>
-      <c r="G25" s="192"/>
+      <c r="D25" s="201"/>
+      <c r="E25" s="201"/>
+      <c r="F25" s="201"/>
+      <c r="G25" s="202"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="193"/>
-      <c r="D26" s="194"/>
-      <c r="E26" s="194"/>
-      <c r="F26" s="194"/>
-      <c r="G26" s="195"/>
+      <c r="C26" s="203"/>
+      <c r="D26" s="204"/>
+      <c r="E26" s="204"/>
+      <c r="F26" s="204"/>
+      <c r="G26" s="205"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -7971,42 +8832,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="184" t="s">
+      <c r="C28" s="194" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="185"/>
-      <c r="E28" s="185"/>
-      <c r="F28" s="185"/>
-      <c r="G28" s="186"/>
+      <c r="D28" s="195"/>
+      <c r="E28" s="195"/>
+      <c r="F28" s="195"/>
+      <c r="G28" s="196"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="184"/>
-      <c r="D29" s="185"/>
-      <c r="E29" s="185"/>
-      <c r="F29" s="185"/>
-      <c r="G29" s="186"/>
+      <c r="C29" s="194"/>
+      <c r="D29" s="195"/>
+      <c r="E29" s="195"/>
+      <c r="F29" s="195"/>
+      <c r="G29" s="196"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="184" t="s">
+      <c r="C30" s="194" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="185"/>
-      <c r="E30" s="185"/>
-      <c r="F30" s="185"/>
-      <c r="G30" s="186"/>
+      <c r="D30" s="195"/>
+      <c r="E30" s="195"/>
+      <c r="F30" s="195"/>
+      <c r="G30" s="196"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="187"/>
-      <c r="D31" s="188"/>
-      <c r="E31" s="188"/>
-      <c r="F31" s="188"/>
-      <c r="G31" s="189"/>
+      <c r="C31" s="197"/>
+      <c r="D31" s="198"/>
+      <c r="E31" s="198"/>
+      <c r="F31" s="198"/>
+      <c r="G31" s="199"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -8029,8 +8890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L5"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8041,35 +8902,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="196"/>
-      <c r="C3" s="197" t="s">
+      <c r="B3" s="206"/>
+      <c r="C3" s="207" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="196"/>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
+      <c r="B4" s="206"/>
+      <c r="C4" s="207"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="207"/>
+      <c r="G4" s="207"/>
+      <c r="H4" s="207"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -8125,13 +8986,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="201" t="s">
+      <c r="C8" s="211" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -8141,20 +9002,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="204"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
-      <c r="G9" s="206"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="204"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
-      <c r="G10" s="206"/>
+      <c r="C10" s="214"/>
+      <c r="D10" s="215"/>
+      <c r="E10" s="215"/>
+      <c r="F10" s="215"/>
+      <c r="G10" s="216"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -8165,11 +9026,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="207"/>
-      <c r="D11" s="208"/>
-      <c r="E11" s="208"/>
-      <c r="F11" s="208"/>
-      <c r="G11" s="209"/>
+      <c r="C11" s="217"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="219"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
23-01-03 3주 2일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EABFB73-0567-4586-9F92-BFA4B0786A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E207D8-23F0-4219-8400-121C28F07CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="465">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1568,16 +1568,157 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오후 강사님 멘토링</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>질문거리 확인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>전처리 절차 확인
  데이터 하나 기준 잡고 전처리 건들이기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오후 강사님 멘토링</t>
+  </si>
+  <si>
+    <t xml:space="preserve">전처리  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>절차 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. data read</t>
+  </si>
+  <si>
+    <t>2. data.lower()</t>
+  </si>
+  <si>
+    <t>대문자를 소문자로 변경</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. 특수문자 제거 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">re.compile('[^가-힣a-zA-Z0-9%]') </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hangul.sub(' ', text) </t>
+  </si>
+  <si>
+    <t>4. 고유명사(제품명 ex) 원에이엠 1am 등)</t>
+  </si>
+  <si>
+    <t>딕셔너리 작성</t>
+  </si>
+  <si>
+    <t>Customized KoNLPy</t>
+  </si>
+  <si>
+    <t>py-haspell전용 딕셔너리를 찾자</t>
+  </si>
+  <si>
+    <t>5. 맞춤법 검사</t>
+  </si>
+  <si>
+    <t>py-hanspell (네이버 맞춤법 검사기)</t>
+  </si>
+  <si>
+    <t>6. 띄어쓰기</t>
+  </si>
+  <si>
+    <t>from pykospacing import Spacing</t>
+  </si>
+  <si>
+    <t>spacing = Spacing()</t>
+  </si>
+  <si>
+    <t>spacing(data)</t>
+  </si>
+  <si>
+    <t>7. 형태소 분석기</t>
+  </si>
+  <si>
+    <t>1. khaiii</t>
+  </si>
+  <si>
+    <t># 이모티콘 , 외래어 , 자모(ex : ㅋㅋㅋ , ㅎㅎ, :) 등)</t>
+  </si>
+  <si>
+    <t>소스트리 체리픽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리 샘플 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강사님 피드백</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획의도 기획 배경 설명하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연관 분석을 진행하고 있다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용 데이터는 특정 사이트에서 리뷰를 크롤링한 데이터셋이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘토분들은 상업적인 측면에서 바라보기 때문에 시점이 다를 것이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wbs 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aws하면 좋지않을까</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://inpa.tistory.com/entry/BootStrap5-%F0%9F%93%9A-%EB%B6%80%ED%8A%B8%EC%8A%A4%ED%8A%B8%EB%9E%A9-%ED%85%9C%ED%94%8C%EB%A6%BF-%EC%82%AC%EC%9D%B4%ED%8A%B8-%EC%A0%95%EB%A6%AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bootstrapmade.com/</t>
+  </si>
+  <si>
+    <t>bootstrapmade</t>
+  </si>
+  <si>
+    <t>themewagon</t>
+  </si>
+  <si>
+    <t>부트스트랩 사이트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘토링 준비 ppt 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 기획의도 보여주기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 시각화 자료를 보여주자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 선례와 실적용 사례(샘플)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 시장성 고른 이유(타당성 必)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2424,7 +2565,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2914,6 +3055,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="13" fillId="25" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3112,23 +3271,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="25" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3873,14 +4029,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -3904,12 +4060,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="180"/>
-      <c r="E5" s="180"/>
-      <c r="F5" s="180"/>
+      <c r="D5" s="186"/>
+      <c r="E5" s="186"/>
+      <c r="F5" s="186"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -3924,7 +4080,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="174" t="s">
+      <c r="E6" s="180" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -3942,7 +4098,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="175"/>
+      <c r="E7" s="181"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -3964,19 +4120,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="168" t="s">
+      <c r="C9" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="171" t="s">
+      <c r="D9" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="171" t="s">
+      <c r="E9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="176" t="s">
+      <c r="F9" s="182" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="181" t="s">
+      <c r="G9" s="187" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3984,21 +4140,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="169"/>
-      <c r="D10" s="172"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="177"/>
-      <c r="G10" s="182"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="188"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="170"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="177"/>
-      <c r="G11" s="182"/>
+      <c r="C11" s="176"/>
+      <c r="D11" s="179"/>
+      <c r="E11" s="178"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="188"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4008,9 +4164,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="173"/>
-      <c r="F12" s="178"/>
-      <c r="G12" s="183"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="189"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4019,11 +4175,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="165" t="s">
+      <c r="D13" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="166"/>
-      <c r="F13" s="167"/>
+      <c r="E13" s="172"/>
+      <c r="F13" s="173"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4091,35 +4247,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="208" t="s">
+      <c r="B2" s="214" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="209"/>
-      <c r="D2" s="209"/>
-      <c r="E2" s="209"/>
-      <c r="F2" s="209"/>
-      <c r="G2" s="209"/>
-      <c r="H2" s="209"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="208"/>
-      <c r="C3" s="209" t="s">
+      <c r="B3" s="214"/>
+      <c r="C3" s="215" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="209"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="209"/>
-      <c r="G3" s="209"/>
-      <c r="H3" s="209"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
+      <c r="G3" s="215"/>
+      <c r="H3" s="215"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="208"/>
-      <c r="C4" s="209"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="209"/>
+      <c r="B4" s="214"/>
+      <c r="C4" s="215"/>
+      <c r="D4" s="215"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
+      <c r="H4" s="215"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4445,8 +4601,8 @@
   <dimension ref="A1:AF181"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L20" sqref="L20"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4459,6 +4615,7 @@
     <col min="8" max="9" width="31.5" hidden="1" customWidth="1"/>
     <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="115.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.25" style="236" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
@@ -4495,7 +4652,7 @@
       <c r="L1" s="83">
         <v>44928</v>
       </c>
-      <c r="M1" s="83">
+      <c r="M1" s="237">
         <v>44929</v>
       </c>
       <c r="N1" s="83">
@@ -4557,7 +4714,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="222" t="s">
+      <c r="A2" s="228" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -4575,7 +4732,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="226" t="s">
+      <c r="G2" s="232" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -4589,9 +4746,12 @@
       <c r="L2" s="86" t="s">
         <v>352</v>
       </c>
+      <c r="M2" s="236" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="222"/>
+      <c r="A3" s="228"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -4605,7 +4765,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="232"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -4619,9 +4779,12 @@
       <c r="L3" s="86" t="s">
         <v>353</v>
       </c>
+      <c r="M3" s="236" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="222"/>
+      <c r="A4" s="228"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -4633,7 +4796,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="226"/>
+      <c r="G4" s="232"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -4647,9 +4810,12 @@
       <c r="L4" s="86" t="s">
         <v>354</v>
       </c>
+      <c r="M4" s="236" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="222"/>
+      <c r="A5" s="228"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -4663,7 +4829,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="226"/>
+      <c r="G5" s="232"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -4674,9 +4840,12 @@
       <c r="L5" s="86" t="s">
         <v>355</v>
       </c>
+      <c r="M5" s="236" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="222"/>
+      <c r="A6" s="228"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -4692,15 +4861,18 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="226"/>
+      <c r="G6" s="232"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
       </c>
       <c r="J6" s="1"/>
+      <c r="M6" s="236" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="223" t="s">
+      <c r="A7" s="229" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -4716,7 +4888,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="226"/>
+      <c r="G7" s="232"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -4732,9 +4904,12 @@
       <c r="L7" s="87" t="s">
         <v>356</v>
       </c>
+      <c r="M7" s="236" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="223"/>
+      <c r="A8" s="229"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -4746,7 +4921,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="226"/>
+      <c r="G8" s="232"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -4762,9 +4937,12 @@
       <c r="L8" s="87" t="s">
         <v>350</v>
       </c>
+      <c r="M8" s="236" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="223"/>
+      <c r="A9" s="229"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -4776,7 +4954,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="226"/>
+      <c r="G9" s="232"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -4787,9 +4965,12 @@
       <c r="L9" s="87" t="s">
         <v>357</v>
       </c>
+      <c r="M9" s="236" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="223"/>
+      <c r="A10" s="229"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -4801,15 +4982,18 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="226"/>
+      <c r="G10" s="232"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
         <v>288</v>
       </c>
+      <c r="M10" s="236" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="223"/>
+      <c r="A11" s="229"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -4821,12 +5005,15 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="226"/>
+      <c r="G11" s="232"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
+      <c r="M11" s="236" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="224" t="s">
+      <c r="A12" s="230" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -4840,7 +5027,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="226"/>
+      <c r="G12" s="232"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -4851,16 +5038,17 @@
       <c r="K12" s="88" t="s">
         <v>283</v>
       </c>
+      <c r="M12" s="236"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="224"/>
+      <c r="A13" s="230"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="226"/>
+      <c r="G13" s="232"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -4868,49 +5056,57 @@
       <c r="K13" s="88" t="s">
         <v>284</v>
       </c>
+      <c r="M13" s="236" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="224"/>
+      <c r="A14" s="230"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="226"/>
+      <c r="G14" s="232"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
       <c r="I14" s="100"/>
+      <c r="M14" s="236" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="224"/>
+      <c r="A15" s="230"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="226"/>
+      <c r="G15" s="232"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="100"/>
+      <c r="M15" s="236"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="224"/>
+      <c r="A16" s="230"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="226"/>
+      <c r="G16" s="232"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
-    </row>
-    <row r="17" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="225" t="s">
+      <c r="M16" s="236"/>
+    </row>
+    <row r="17" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="231" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -4918,7 +5114,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="226"/>
+      <c r="G17" s="232"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -4930,58 +5126,76 @@
       <c r="L17" s="89" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="225"/>
+      <c r="M17" s="236" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="231"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="226"/>
+      <c r="G18" s="232"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="225"/>
+      <c r="M18" s="236" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="231"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="226"/>
+      <c r="G19" s="232"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
-    </row>
-    <row r="20" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="225"/>
+      <c r="M19" s="236" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="231"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="226"/>
+      <c r="G20" s="232"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
-    </row>
-    <row r="21" spans="1:12" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="225"/>
+      <c r="M20" s="236" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="231"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="226"/>
+      <c r="G21" s="232"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
-    </row>
-    <row r="22" spans="1:12" s="100" customFormat="1" ht="30" customHeight="1">
+      <c r="M21" s="236" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
-    </row>
-    <row r="23" spans="1:12" s="109" customFormat="1" ht="30" customHeight="1">
+      <c r="M22" s="236" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5012,8 +5226,11 @@
       <c r="J23" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
+      <c r="M23" s="236" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5041,8 +5258,11 @@
       <c r="L24" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1">
+      <c r="M24" s="236" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5070,8 +5290,11 @@
       <c r="J25" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1">
+      <c r="M25" s="236" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5094,7 +5317,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30" customHeight="1">
+    <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5119,8 +5342,11 @@
       <c r="J27" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="30" customHeight="1">
+      <c r="M27" s="108" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5140,7 +5366,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1">
+    <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5162,8 +5388,11 @@
       <c r="L29" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1">
+      <c r="M29" s="236" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5176,8 +5405,11 @@
       <c r="J30" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="30" customHeight="1">
+      <c r="M30" s="236" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5187,8 +5419,11 @@
       <c r="L31" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="30" customHeight="1">
+      <c r="M31" s="236" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -5201,8 +5436,11 @@
       <c r="L32" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="30" customHeight="1">
+      <c r="M32" s="236" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="D33" t="s">
         <v>101</v>
       </c>
@@ -5212,8 +5450,11 @@
       <c r="L33" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="30" customHeight="1">
+      <c r="M33" s="236" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -5227,7 +5468,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30" customHeight="1">
+    <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="B35" t="s">
         <v>65</v>
       </c>
@@ -5241,7 +5482,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="30" customHeight="1">
+    <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="B36" t="s">
         <v>66</v>
       </c>
@@ -5252,7 +5493,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" customHeight="1">
+    <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="B37" s="105" t="s">
         <v>67</v>
       </c>
@@ -5263,12 +5504,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30" customHeight="1">
+    <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="D38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" customHeight="1">
+    <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
@@ -5282,12 +5523,12 @@
         <v>367</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" customHeight="1">
+    <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="L41" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="30" customHeight="1">
+    <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="J42" t="s">
         <v>193</v>
       </c>
@@ -5295,7 +5536,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="30" customHeight="1">
+    <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="J43" t="s">
         <v>194</v>
       </c>
@@ -5303,7 +5544,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30" customHeight="1">
+    <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="J44" t="s">
         <v>195</v>
       </c>
@@ -5311,22 +5552,22 @@
         <v>371</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="30" customHeight="1">
+    <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="J45" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="30" customHeight="1">
+    <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="L46" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30" customHeight="1">
+    <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="L47" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="30" customHeight="1">
+    <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="J48" t="s">
         <v>197</v>
       </c>
@@ -5774,11 +6015,11 @@
   <dimension ref="A1:BH44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="21" topLeftCell="E51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="21" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H27" sqref="H27"/>
       <selection pane="topRight" activeCell="H27" sqref="H27"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
-      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6600,12 +6841,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E416609B-A342-4E94-929E-80BF1FFEBFD0}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H27" sqref="H27"/>
       <selection pane="topRight" activeCell="H27" sqref="H27"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6657,22 +6898,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="227" t="s">
+      <c r="C2" s="233" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227" t="s">
+      <c r="D2" s="233"/>
+      <c r="E2" s="233" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227" t="s">
+      <c r="F2" s="233"/>
+      <c r="G2" s="233" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="227"/>
-      <c r="I2" s="227" t="s">
+      <c r="H2" s="233"/>
+      <c r="I2" s="233" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="228"/>
+      <c r="J2" s="234"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -6960,24 +7201,25 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="162" customFormat="1">
+    <row r="1" spans="1:4" s="162" customFormat="1">
       <c r="A1" s="162" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>419</v>
       </c>
@@ -6985,12 +7227,15 @@
         <v>358</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>409</v>
       </c>
@@ -6998,38 +7243,52 @@
         <v>359</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="6" spans="1:4">
+      <c r="D6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>410</v>
       </c>
       <c r="C7" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="C8" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="C10" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="B11" t="s">
         <v>412</v>
       </c>
       <c r="C11" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>413</v>
       </c>
@@ -7037,44 +7296,71 @@
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="13" spans="1:4">
+      <c r="D13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" t="s">
         <v>414</v>
       </c>
       <c r="C14" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D14" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16" t="s">
         <v>415</v>
       </c>
       <c r="C16" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="18" spans="2:3">
+      <c r="D16" s="131" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="D17" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>416</v>
       </c>
       <c r="C18" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
+      <c r="D18" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="D19" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
         <v>417</v>
       </c>
       <c r="C20" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="21" spans="2:3">
+      <c r="D20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
       <c r="C21" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:4">
       <c r="B22" t="s">
         <v>418</v>
       </c>
@@ -7082,32 +7368,32 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:4">
       <c r="C23" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:4">
       <c r="C25" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:4">
       <c r="C26" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:4">
       <c r="C29" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:4">
       <c r="C31" t="s">
         <v>376</v>
       </c>
@@ -7189,6 +7475,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D16" r:id="rId1" xr:uid="{B2ACDFE4-1473-4C0C-A217-4E4CD2C24EFD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7197,7 +7486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251ECE8D-9668-40EA-AFB2-EB0A37392AB0}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -7209,14 +7498,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -7260,19 +7549,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="184" t="s">
+      <c r="C6" s="190" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="171" t="s">
+      <c r="D6" s="177" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="189" t="s">
+      <c r="E6" s="195" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="198" t="s">
         <v>280</v>
       </c>
     </row>
@@ -7280,13 +7569,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="185"/>
-      <c r="D7" s="173"/>
-      <c r="E7" s="190"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="179"/>
+      <c r="E7" s="196"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="193"/>
+      <c r="G7" s="199"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -7302,13 +7591,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="186" t="s">
+      <c r="C9" s="192" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="171" t="s">
+      <c r="D9" s="177" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="189"/>
+      <c r="E9" s="195"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -7320,9 +7609,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="187"/>
-      <c r="D10" s="172"/>
-      <c r="E10" s="191"/>
+      <c r="C10" s="193"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="197"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -7332,9 +7621,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="191"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="197"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -7347,8 +7636,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="173"/>
-      <c r="E12" s="190"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="196"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -7361,11 +7650,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="165" t="s">
+      <c r="D13" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="166"/>
-      <c r="F13" s="166"/>
+      <c r="E13" s="172"/>
+      <c r="F13" s="172"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -7403,8 +7692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7417,15 +7706,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -7452,16 +7741,18 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="238" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="30"/>
+      <c r="E5" s="110" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="239"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
@@ -7470,10 +7761,12 @@
       <c r="C6" s="158" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="234" t="s">
-        <v>423</v>
-      </c>
-      <c r="E6" s="32"/>
+      <c r="D6" s="168" t="s">
+        <v>422</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>446</v>
+      </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32"/>
       <c r="H6" s="30"/>
@@ -7483,10 +7776,12 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="159"/>
-      <c r="D7" s="233" t="s">
-        <v>422</v>
-      </c>
-      <c r="E7" s="32"/>
+      <c r="D7" s="167" t="s">
+        <v>421</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>447</v>
+      </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="30"/>
@@ -7495,12 +7790,12 @@
       <c r="B8" s="36">
         <v>0.5</v>
       </c>
-      <c r="C8" s="229"/>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
-      <c r="G8" s="230"/>
-      <c r="H8" s="231"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="164"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="165"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
       <c r="B9" s="36">
@@ -7509,12 +7804,12 @@
       <c r="C9" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="110" t="s">
-        <v>421</v>
-      </c>
-      <c r="E9" s="232"/>
-      <c r="F9" s="232"/>
-      <c r="G9" s="232"/>
+      <c r="D9" s="235" t="s">
+        <v>424</v>
+      </c>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="82"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
@@ -7524,7 +7819,9 @@
       <c r="C10" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="D10" s="232"/>
+      <c r="D10" s="110" t="s">
+        <v>425</v>
+      </c>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -7537,7 +7834,9 @@
       <c r="C11" s="147" t="s">
         <v>341</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="32" t="s">
+        <v>423</v>
+      </c>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
@@ -7548,7 +7847,9 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="147"/>
-      <c r="D12" s="32"/>
+      <c r="D12" s="32" t="s">
+        <v>426</v>
+      </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
@@ -7561,12 +7862,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="165" t="s">
+      <c r="D13" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="166"/>
-      <c r="F13" s="166"/>
-      <c r="G13" s="167"/>
+      <c r="E13" s="172"/>
+      <c r="F13" s="172"/>
+      <c r="G13" s="173"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -7912,15 +8213,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8039,11 +8340,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="165" t="s">
+      <c r="E13" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="166"/>
-      <c r="G13" s="167"/>
+      <c r="F13" s="172"/>
+      <c r="G13" s="173"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8087,14 +8388,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -8202,10 +8503,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="165" t="s">
+      <c r="E13" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="167"/>
+      <c r="F13" s="173"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -8248,15 +8549,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -8376,10 +8677,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="194" t="s">
+      <c r="F13" s="200" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="195"/>
+      <c r="G13" s="201"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8423,13 +8724,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -8565,35 +8866,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="208" t="s">
+      <c r="B2" s="214" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="209"/>
-      <c r="D2" s="209"/>
-      <c r="E2" s="209"/>
-      <c r="F2" s="209"/>
-      <c r="G2" s="209"/>
-      <c r="H2" s="209"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="208"/>
-      <c r="C3" s="209" t="s">
+      <c r="B3" s="214"/>
+      <c r="C3" s="215" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="209"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="209"/>
-      <c r="G3" s="209"/>
-      <c r="H3" s="209"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
+      <c r="G3" s="215"/>
+      <c r="H3" s="215"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="208"/>
-      <c r="C4" s="209"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="209"/>
+      <c r="B4" s="214"/>
+      <c r="C4" s="215"/>
+      <c r="D4" s="215"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
+      <c r="H4" s="215"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -8812,42 +9113,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="210" t="s">
+      <c r="C23" s="216" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="211"/>
-      <c r="E23" s="211"/>
-      <c r="F23" s="211"/>
-      <c r="G23" s="212"/>
+      <c r="D23" s="217"/>
+      <c r="E23" s="217"/>
+      <c r="F23" s="217"/>
+      <c r="G23" s="218"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="202"/>
-      <c r="D24" s="203"/>
-      <c r="E24" s="203"/>
-      <c r="F24" s="203"/>
-      <c r="G24" s="204"/>
+      <c r="C24" s="208"/>
+      <c r="D24" s="209"/>
+      <c r="E24" s="209"/>
+      <c r="F24" s="209"/>
+      <c r="G24" s="210"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="202" t="s">
+      <c r="C25" s="208" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="203"/>
-      <c r="E25" s="203"/>
-      <c r="F25" s="203"/>
-      <c r="G25" s="204"/>
+      <c r="D25" s="209"/>
+      <c r="E25" s="209"/>
+      <c r="F25" s="209"/>
+      <c r="G25" s="210"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="205"/>
-      <c r="D26" s="206"/>
-      <c r="E26" s="206"/>
-      <c r="F26" s="206"/>
-      <c r="G26" s="207"/>
+      <c r="C26" s="211"/>
+      <c r="D26" s="212"/>
+      <c r="E26" s="212"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="213"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -8875,42 +9176,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="196" t="s">
+      <c r="C28" s="202" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="197"/>
-      <c r="E28" s="197"/>
-      <c r="F28" s="197"/>
-      <c r="G28" s="198"/>
+      <c r="D28" s="203"/>
+      <c r="E28" s="203"/>
+      <c r="F28" s="203"/>
+      <c r="G28" s="204"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="196"/>
-      <c r="D29" s="197"/>
-      <c r="E29" s="197"/>
-      <c r="F29" s="197"/>
-      <c r="G29" s="198"/>
+      <c r="C29" s="202"/>
+      <c r="D29" s="203"/>
+      <c r="E29" s="203"/>
+      <c r="F29" s="203"/>
+      <c r="G29" s="204"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="196" t="s">
+      <c r="C30" s="202" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="197"/>
-      <c r="E30" s="197"/>
-      <c r="F30" s="197"/>
-      <c r="G30" s="198"/>
+      <c r="D30" s="203"/>
+      <c r="E30" s="203"/>
+      <c r="F30" s="203"/>
+      <c r="G30" s="204"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="199"/>
-      <c r="D31" s="200"/>
-      <c r="E31" s="200"/>
-      <c r="F31" s="200"/>
-      <c r="G31" s="201"/>
+      <c r="C31" s="205"/>
+      <c r="D31" s="206"/>
+      <c r="E31" s="206"/>
+      <c r="F31" s="206"/>
+      <c r="G31" s="207"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -8933,7 +9234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -8945,35 +9246,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="208" t="s">
+      <c r="B2" s="214" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="209"/>
-      <c r="D2" s="209"/>
-      <c r="E2" s="209"/>
-      <c r="F2" s="209"/>
-      <c r="G2" s="209"/>
-      <c r="H2" s="209"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="208"/>
-      <c r="C3" s="209" t="s">
+      <c r="B3" s="214"/>
+      <c r="C3" s="215" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="209"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="209"/>
-      <c r="G3" s="209"/>
-      <c r="H3" s="209"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
+      <c r="G3" s="215"/>
+      <c r="H3" s="215"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="208"/>
-      <c r="C4" s="209"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="209"/>
+      <c r="B4" s="214"/>
+      <c r="C4" s="215"/>
+      <c r="D4" s="215"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
+      <c r="H4" s="215"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9029,13 +9330,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="213" t="s">
+      <c r="C8" s="219" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="214"/>
-      <c r="E8" s="214"/>
-      <c r="F8" s="214"/>
-      <c r="G8" s="215"/>
+      <c r="D8" s="220"/>
+      <c r="E8" s="220"/>
+      <c r="F8" s="220"/>
+      <c r="G8" s="221"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9045,20 +9346,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="217"/>
-      <c r="E9" s="217"/>
-      <c r="F9" s="217"/>
-      <c r="G9" s="218"/>
+      <c r="C9" s="222"/>
+      <c r="D9" s="223"/>
+      <c r="E9" s="223"/>
+      <c r="F9" s="223"/>
+      <c r="G9" s="224"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="217"/>
-      <c r="E10" s="217"/>
-      <c r="F10" s="217"/>
-      <c r="G10" s="218"/>
+      <c r="C10" s="222"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -9069,11 +9370,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="219"/>
-      <c r="D11" s="220"/>
-      <c r="E11" s="220"/>
-      <c r="F11" s="220"/>
-      <c r="G11" s="221"/>
+      <c r="C11" s="225"/>
+      <c r="D11" s="226"/>
+      <c r="E11" s="226"/>
+      <c r="F11" s="226"/>
+      <c r="G11" s="227"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
23-01-04 3주 3일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E207D8-23F0-4219-8400-121C28F07CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD387C8A-D441-4D8E-ACB4-5A1B94956B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="598" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -45,8 +45,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="519">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1719,6 +1741,177 @@
   </si>
   <si>
     <t>* 시장성 고른 이유(타당성 必)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 맞춤법 검사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘토링 바탕 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서칭 자료 세부분석</t>
+  </si>
+  <si>
+    <t>맞춤법검사 한스펠 성능 확인</t>
+  </si>
+  <si>
+    <t>1. 1~7 실행 (코딩)
+맞춤법검사 한스펠 성능 확인
+2. 8~ (모델링 관련 서칭)
+서칭 자료 세부분석
+3. 멘토링 바탕 작성 (ppt준비)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 주제 개요 설명</t>
+  </si>
+  <si>
+    <t>2. 서비스 대상 소비자 설명</t>
+  </si>
+  <si>
+    <t>3. 서비스 제공 내용 및 상업적 효과 설명</t>
+  </si>
+  <si>
+    <t>4. 전처리 크롤링 설명 , 자연어처리 모델링 종류만 설명</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. 시각화를 위해 사용한 모델링 기법 설명 </t>
+  </si>
+  <si>
+    <t>6. 해당 모델을 사용한 이유 설명</t>
+  </si>
+  <si>
+    <t>7. 시각화 자료 보여주기</t>
+  </si>
+  <si>
+    <t>8. 홈페이지 구현 방식 계획 설명</t>
+  </si>
+  <si>
+    <t>9. 홈페이지 구현 예시 보여주기</t>
+  </si>
+  <si>
+    <t>advise</t>
+  </si>
+  <si>
+    <t>사용설명서 같이 설명해보자</t>
+  </si>
+  <si>
+    <t>서비스 구축 과정</t>
+  </si>
+  <si>
+    <t>저들에게 설명할 수 있을 것이다.</t>
+  </si>
+  <si>
+    <t>상업적인 측면에서 바라본다면 발전 가능성, 상업적 효과 등도 중요하겠지만</t>
+  </si>
+  <si>
+    <t>결국 중요한건 사람을 설득시키는 타당성과 참신함이겠지.</t>
+  </si>
+  <si>
+    <t>Q) 프로젝트 주제가 무엇인가요?</t>
+  </si>
+  <si>
+    <t>A) 제로칼로리 음료들의 상품 리뷰 키워드를 분석하여 서비스 소비자에게 정보를 제공하는 것입니다.</t>
+  </si>
+  <si>
+    <t>Q) 서비스 소비자는 어떤 사람들이죠?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A) 제로칼로리 음료에 대한 정보가 필요한 사람들 : </t>
+  </si>
+  <si>
+    <t>어떤 종류의 제로칼로리 음료가 있는지 , 해당 음료의 후기는 어떠한지 : 맛 , 가격 , 상품의 질 등</t>
+  </si>
+  <si>
+    <t>후기를 통해 좀 더 세부적으로 분류가 가능하다.</t>
+  </si>
+  <si>
+    <t>1. 일반 소비자</t>
+  </si>
+  <si>
+    <t>2. 제품 판매자</t>
+  </si>
+  <si>
+    <t>3. 다이어트 소비자</t>
+  </si>
+  <si>
+    <t>4. 제로칼로리 판매 기업</t>
+  </si>
+  <si>
+    <t>5. 해당 상품에 추천되는 타 상품 판매자</t>
+  </si>
+  <si>
+    <t>Q) 어떤 정보를 제공하죠?</t>
+  </si>
+  <si>
+    <t>A) 제품의 리뷰에서 언급되어지는 단어들을 모아 영향력있는 리뷰 단어를 모으고 연관성을 파악하여 해당 제로칼로리 상품의 주요 키워드를 연관성의 개수만큼 크기를 키워 한 눈에 보여주고 , 해당 키워드와 연관된 자료들을 추가로 제공하는 서비스입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">여기서 연관된 자료란 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 해당 키워드 클릭시 Concor 분석을 통한 세부 분석 </t>
+  </si>
+  <si>
+    <t>2. 세부 분석 후 세부 분석 키워드에서 대표적인 키워드 관련 홈페이지 리뷰 등 정보 제공</t>
+  </si>
+  <si>
+    <t>‘제로’음료란 설탕이나 액상과당 대신에 ‘알룰로스’, ‘스테비아’, ‘에리스리톨’ 등 인공 대체 감미료를 사용해 단맛은 유지하되 칼로리와 당 섭취를 줄여 부담 없이 즐길 수 있는 음료</t>
+  </si>
+  <si>
+    <t>출처 : https://www.sedaily.com/NewsView/26DTC9MQBC</t>
+  </si>
+  <si>
+    <t>Q) 왜 이 주제를 선정하게 되었나요?</t>
+  </si>
+  <si>
+    <t>A) 탄산음료는 당분, 카페인 함량이 높아 치아부식 등의 우려가있어 건강을 생각하는 사람들이 기피하는 음료였습니다.</t>
+  </si>
+  <si>
+    <t>하지만 탄산음료의 청량감과 각 제품들 특유의 '맛' 때문에 끊기가 힘든 음료이기도 합니다.</t>
+  </si>
+  <si>
+    <t>이러한 점을 이유로, 최근 건강을 크게 해치지 않으면서 남녀노소 쉽게 접할 수 있는 음료인 제로칼로리 음료가 부상하고 있습니다.</t>
+  </si>
+  <si>
+    <t>제로 음료란 설탕이나 액상과당 대신에 ‘알룰로스’, ‘스테비아’, ‘에리스리톨’ 등 인공 대체 감미료를 사용해 단맛은 유지하되 칼로리와 당 섭취를 줄여 부담 없이 즐길 수 있는 음료이며 , 최근 2년 사이 시장 규모가 5배나 성장할 정도로 인기가 많은 음료입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그러나 최근 소비자가 급등한 제로칼로리 음료에 대한 관심은 정말 높아졌지만 아쉽게도 해당 상품별 리뷰나 상품에 대한 정보가 부족하여 제로칼로리 상품을 구매하고 낭패를 보는 일도 적지 않았습니다. 따라서 저희는 제로칼로리 음료에 대한 상품 정보에 집중한다면 좋은 서비스를 제공할 수 있지않을까 라는 기점에서 시작하여 위의 주제를 선정하게 되었고 위 서비스를 홈페이지로 구현하게 된다면 </t>
+  </si>
+  <si>
+    <t>https://www.wiseapp.co.kr/insight/detail/217</t>
+  </si>
+  <si>
+    <t>Q) 이 서비스가 상업적으로 효과가 있을까요?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A) </t>
+  </si>
+  <si>
+    <t>Q) 어떤 모델링 기법을 사용할 것인가요?</t>
+  </si>
+  <si>
+    <t>Q) 그 모델링을 사용한 이유는?</t>
+  </si>
+  <si>
+    <t>Q) 데이터는 어떻게 모으셨죠?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>검색해도 내용을 찾기 힘들다 -&gt;  사례가져오자</t>
+  </si>
+  <si>
+    <t>한스펠 , 카이 사용유무 판단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리 시작합시다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1726,7 +1919,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1930,6 +2123,14 @@
     <font>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -2565,7 +2766,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3073,6 +3274,21 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3166,6 +3382,15 @@
     <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3269,21 +3494,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4029,14 +4239,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -4060,12 +4270,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="185" t="s">
+      <c r="C5" s="190" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="186"/>
-      <c r="E5" s="186"/>
-      <c r="F5" s="186"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -4080,7 +4290,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="180" t="s">
+      <c r="E6" s="185" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4098,7 +4308,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="181"/>
+      <c r="E7" s="186"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -4120,19 +4330,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="174" t="s">
+      <c r="C9" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="177" t="s">
+      <c r="D9" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="177" t="s">
+      <c r="E9" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="182" t="s">
+      <c r="F9" s="187" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="187" t="s">
+      <c r="G9" s="192" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4140,21 +4350,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="175"/>
-      <c r="D10" s="178"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="188"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="188"/>
+      <c r="G10" s="193"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="176"/>
-      <c r="D11" s="179"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="183"/>
-      <c r="G11" s="188"/>
+      <c r="C11" s="181"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="188"/>
+      <c r="G11" s="193"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4164,9 +4374,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="189"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="194"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4175,11 +4385,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="171" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="173"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4247,35 +4457,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="214"/>
-      <c r="C3" s="215" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="215"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="214"/>
-      <c r="C4" s="215"/>
-      <c r="D4" s="215"/>
-      <c r="E4" s="215"/>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
-      <c r="H4" s="215"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4602,7 +4812,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M34" sqref="M34"/>
+      <selection pane="topRight" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4615,7 +4825,7 @@
     <col min="8" max="9" width="31.5" hidden="1" customWidth="1"/>
     <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="115.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.25" style="236" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
@@ -4652,7 +4862,7 @@
       <c r="L1" s="83">
         <v>44928</v>
       </c>
-      <c r="M1" s="237">
+      <c r="M1" s="83">
         <v>44929</v>
       </c>
       <c r="N1" s="83">
@@ -4714,7 +4924,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="236" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -4732,7 +4942,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="232" t="s">
+      <c r="G2" s="240" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -4746,12 +4956,15 @@
       <c r="L2" s="86" t="s">
         <v>352</v>
       </c>
-      <c r="M2" s="236" t="s">
+      <c r="M2" t="s">
         <v>427</v>
       </c>
+      <c r="N2" s="86" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="228"/>
+      <c r="A3" s="236"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -4765,7 +4978,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="232"/>
+      <c r="G3" s="240"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -4779,12 +4992,12 @@
       <c r="L3" s="86" t="s">
         <v>353</v>
       </c>
-      <c r="M3" s="236" t="s">
+      <c r="M3" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="228"/>
+      <c r="A4" s="236"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -4796,7 +5009,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="232"/>
+      <c r="G4" s="240"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -4810,12 +5023,12 @@
       <c r="L4" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="M4" s="236" t="s">
+      <c r="M4" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="228"/>
+      <c r="A5" s="236"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -4829,7 +5042,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="232"/>
+      <c r="G5" s="240"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -4840,12 +5053,12 @@
       <c r="L5" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="M5" s="236" t="s">
+      <c r="M5" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="228"/>
+      <c r="A6" s="236"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -4861,18 +5074,18 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="232"/>
+      <c r="G6" s="240"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="M6" s="236" t="s">
+      <c r="M6" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="229" t="s">
+      <c r="A7" s="237" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -4888,7 +5101,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="232"/>
+      <c r="G7" s="240"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -4904,12 +5117,15 @@
       <c r="L7" s="87" t="s">
         <v>356</v>
       </c>
-      <c r="M7" s="236" t="s">
+      <c r="M7" t="s">
         <v>432</v>
       </c>
+      <c r="N7" s="87" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="229"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -4921,7 +5137,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="232"/>
+      <c r="G8" s="240"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -4937,12 +5153,12 @@
       <c r="L8" s="87" t="s">
         <v>350</v>
       </c>
-      <c r="M8" s="236" t="s">
+      <c r="M8" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="229"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -4954,7 +5170,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="232"/>
+      <c r="G9" s="240"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -4965,12 +5181,12 @@
       <c r="L9" s="87" t="s">
         <v>357</v>
       </c>
-      <c r="M9" s="236" t="s">
+      <c r="M9" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="229"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -4982,18 +5198,18 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="232"/>
+      <c r="G10" s="240"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
         <v>288</v>
       </c>
-      <c r="M10" s="236" t="s">
+      <c r="M10" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="229"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5005,15 +5221,15 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="232"/>
+      <c r="G11" s="240"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
-      <c r="M11" s="236" t="s">
+      <c r="M11" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="230" t="s">
+      <c r="A12" s="238" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5027,7 +5243,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="232"/>
+      <c r="G12" s="240"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5038,17 +5254,17 @@
       <c r="K12" s="88" t="s">
         <v>283</v>
       </c>
-      <c r="M12" s="236"/>
+      <c r="M12"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="230"/>
+      <c r="A13" s="238"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="232"/>
+      <c r="G13" s="240"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5056,57 +5272,57 @@
       <c r="K13" s="88" t="s">
         <v>284</v>
       </c>
-      <c r="M13" s="236" t="s">
+      <c r="M13" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="230"/>
+      <c r="A14" s="238"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="232"/>
+      <c r="G14" s="240"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
       <c r="I14" s="100"/>
-      <c r="M14" s="236" t="s">
+      <c r="M14" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="230"/>
+      <c r="A15" s="238"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="232"/>
+      <c r="G15" s="240"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="100"/>
-      <c r="M15" s="236"/>
+      <c r="M15"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="230"/>
+      <c r="A16" s="238"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="232"/>
+      <c r="G16" s="240"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
-      <c r="M16" s="236"/>
-    </row>
-    <row r="17" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="231" t="s">
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="239" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5114,7 +5330,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="232"/>
+      <c r="G17" s="240"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5126,76 +5342,79 @@
       <c r="L17" s="89" t="s">
         <v>350</v>
       </c>
-      <c r="M17" s="236" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="231"/>
+      <c r="M17" t="s">
+        <v>465</v>
+      </c>
+      <c r="N17" s="89" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="239"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="232"/>
+      <c r="G18" s="240"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
         <v>351</v>
       </c>
-      <c r="M18" s="236" t="s">
+      <c r="M18" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="231"/>
+    <row r="19" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="239"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="232"/>
+      <c r="G19" s="240"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
-      <c r="M19" s="236" t="s">
+      <c r="M19" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="231"/>
+    <row r="20" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="239"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="232"/>
+      <c r="G20" s="240"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
-      <c r="M20" s="236" t="s">
+      <c r="M20" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="231"/>
+    <row r="21" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="239"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="232"/>
+      <c r="G21" s="240"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
-      <c r="M21" s="236" t="s">
+      <c r="M21" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="100" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:14" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
-      <c r="M22" s="236" t="s">
+      <c r="M22" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:14" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5226,11 +5445,14 @@
       <c r="J23" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="M23" s="236" t="s">
+      <c r="M23" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="30" customHeight="1">
+      <c r="N23" s="108" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5258,11 +5480,14 @@
       <c r="L24" t="s">
         <v>358</v>
       </c>
-      <c r="M24" s="236" t="s">
+      <c r="M24" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1">
+      <c r="N24" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5290,11 +5515,11 @@
       <c r="J25" t="s">
         <v>185</v>
       </c>
-      <c r="M25" s="236" t="s">
+      <c r="M25" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1">
+    <row r="26" spans="1:14" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5317,7 +5542,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1">
+    <row r="27" spans="1:14" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5346,7 +5571,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1">
+    <row r="28" spans="1:14" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5366,7 +5591,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+    <row r="29" spans="1:14" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5388,11 +5613,11 @@
       <c r="L29" t="s">
         <v>361</v>
       </c>
-      <c r="M29" s="236" t="s">
+      <c r="M29" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1">
+    <row r="30" spans="1:14" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5405,11 +5630,11 @@
       <c r="J30" t="s">
         <v>188</v>
       </c>
-      <c r="M30" s="236" t="s">
+      <c r="M30" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1">
+    <row r="31" spans="1:14" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5419,11 +5644,11 @@
       <c r="L31" t="s">
         <v>362</v>
       </c>
-      <c r="M31" s="236" t="s">
+      <c r="M31" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1">
+    <row r="32" spans="1:14" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -5436,7 +5661,7 @@
       <c r="L32" t="s">
         <v>363</v>
       </c>
-      <c r="M32" s="236" t="s">
+      <c r="M32" t="s">
         <v>463</v>
       </c>
     </row>
@@ -5450,7 +5675,7 @@
       <c r="L33" t="s">
         <v>364</v>
       </c>
-      <c r="M33" s="236" t="s">
+      <c r="M33" t="s">
         <v>464</v>
       </c>
     </row>
@@ -6015,7 +6240,7 @@
   <dimension ref="A1:BH44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="21" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="21" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H27" sqref="H27"/>
       <selection pane="topRight" activeCell="H27" sqref="H27"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
@@ -6898,22 +7123,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="233" t="s">
+      <c r="C2" s="241" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233" t="s">
+      <c r="D2" s="241"/>
+      <c r="E2" s="241" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233" t="s">
+      <c r="F2" s="241"/>
+      <c r="G2" s="241" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233" t="s">
+      <c r="H2" s="241"/>
+      <c r="I2" s="241" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="234"/>
+      <c r="J2" s="242"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -7201,25 +7426,26 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="224.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="162" customFormat="1">
+    <row r="1" spans="1:5" s="162" customFormat="1">
       <c r="A1" s="162" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>419</v>
       </c>
@@ -7227,28 +7453,37 @@
         <v>358</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>408</v>
       </c>
       <c r="D4" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>409</v>
       </c>
       <c r="C5" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="D6" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="B7" t="s">
         <v>410</v>
       </c>
@@ -7258,26 +7493,38 @@
       <c r="D7" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="C8" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>411</v>
       </c>
       <c r="D9" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="C10" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>412</v>
       </c>
@@ -7287,21 +7534,27 @@
       <c r="D11" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>413</v>
       </c>
       <c r="C12" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="D13" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>414</v>
       </c>
@@ -7312,7 +7565,12 @@
         <v>454</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="15" spans="1:5">
+      <c r="E15" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="B16" t="s">
         <v>415</v>
       </c>
@@ -7322,13 +7580,19 @@
       <c r="D16" s="131" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="17" spans="2:4">
+      <c r="E16" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
       <c r="D17" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="18" spans="2:4">
+      <c r="E17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" t="s">
         <v>416</v>
       </c>
@@ -7339,12 +7603,12 @@
         <v>459</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:5">
       <c r="D19" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
         <v>417</v>
       </c>
@@ -7355,12 +7619,16 @@
         <v>458</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:5">
       <c r="C21" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="E21" t="e" cm="1">
+        <f t="array" ref="E21">- 어떻게 설명할 것인지 순서를 정해두자</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>418</v>
       </c>
@@ -7368,109 +7636,260 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:5">
       <c r="C23" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="25" spans="2:4">
+      <c r="E23" t="e" cm="1">
+        <f t="array" ref="E23">- 아래 내용을 대답할 수 있다면</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="E24" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="C25" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:5">
       <c r="C26" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="28" spans="2:4">
+      <c r="E26" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="E27" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
       <c r="C28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:5">
       <c r="C29" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="31" spans="2:4">
+      <c r="E29" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="E30" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
       <c r="C31" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
+    <row r="32" spans="2:5">
+      <c r="E32" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
+      <c r="E33" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5">
       <c r="C34" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="36" spans="3:3">
+      <c r="E34" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5">
+      <c r="E35" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
       <c r="C36" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="37" spans="3:3">
+    <row r="37" spans="3:5">
       <c r="C37" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="38" spans="3:3">
+      <c r="E37" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5">
       <c r="C38" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="39" spans="3:3">
+      <c r="E38" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5">
       <c r="C39" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="41" spans="3:3">
+      <c r="E39" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5">
+      <c r="E40" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5">
       <c r="C41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="3:3">
+      <c r="E41" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
       <c r="C42" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="3:5">
       <c r="C43" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="44" spans="3:3">
+      <c r="E43" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5">
       <c r="C44" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="46" spans="3:3">
+      <c r="E44" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5">
       <c r="C46" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="47" spans="3:3">
+      <c r="E46" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5">
       <c r="C47" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="49" spans="3:3">
+      <c r="E47" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5">
+      <c r="E48" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5">
       <c r="C49" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="3:5">
       <c r="C50" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="52" spans="3:3">
+      <c r="E50" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5">
       <c r="C52" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="53" spans="3:3">
+      <c r="E52" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5">
       <c r="C53" t="s">
         <v>385</v>
+      </c>
+      <c r="E53" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5">
+      <c r="E54" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5">
+      <c r="E55" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5">
+      <c r="E56" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5">
+      <c r="E57" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5">
+      <c r="E59" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5">
+      <c r="E60" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5">
+      <c r="E62" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5">
+      <c r="E63" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5">
+      <c r="E64" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5">
+      <c r="E65" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5">
+      <c r="E66" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5">
+      <c r="E68" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5">
+      <c r="E72" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -7486,7 +7905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251ECE8D-9668-40EA-AFB2-EB0A37392AB0}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -7498,14 +7917,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -7549,19 +7968,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="190" t="s">
+      <c r="C6" s="195" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="177" t="s">
+      <c r="D6" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="195" t="s">
+      <c r="E6" s="200" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="198" t="s">
+      <c r="G6" s="203" t="s">
         <v>280</v>
       </c>
     </row>
@@ -7569,13 +7988,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="191"/>
-      <c r="D7" s="179"/>
-      <c r="E7" s="196"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="201"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="199"/>
+      <c r="G7" s="204"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -7591,13 +8010,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="192" t="s">
+      <c r="C9" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="177" t="s">
+      <c r="D9" s="182" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="195"/>
+      <c r="E9" s="200"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -7609,9 +8028,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="193"/>
-      <c r="D10" s="178"/>
-      <c r="E10" s="197"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="202"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -7621,9 +8040,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="194"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="197"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="202"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -7636,8 +8055,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="179"/>
-      <c r="E12" s="196"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="201"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -7650,11 +8069,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="171" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="172"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -7692,8 +8111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7706,15 +8125,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -7741,7 +8160,7 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="238" t="s">
+      <c r="C5" s="170" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="110" t="s">
@@ -7750,9 +8169,11 @@
       <c r="E5" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="110"/>
+      <c r="F5" s="110" t="s">
+        <v>143</v>
+      </c>
       <c r="G5" s="110"/>
-      <c r="H5" s="239"/>
+      <c r="H5" s="171"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
@@ -7764,10 +8185,12 @@
       <c r="D6" s="168" t="s">
         <v>422</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="172" t="s">
         <v>446</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="32" t="s">
+        <v>518</v>
+      </c>
       <c r="G6" s="32"/>
       <c r="H6" s="30"/>
     </row>
@@ -7779,7 +8202,7 @@
       <c r="D7" s="167" t="s">
         <v>421</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="173" t="s">
         <v>447</v>
       </c>
       <c r="F7" s="32"/>
@@ -7804,10 +8227,12 @@
       <c r="C9" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="235" t="s">
+      <c r="D9" s="169" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="166"/>
+      <c r="E9" s="205" t="s">
+        <v>469</v>
+      </c>
       <c r="F9" s="166"/>
       <c r="G9" s="166"/>
       <c r="H9" s="82"/>
@@ -7822,7 +8247,7 @@
       <c r="D10" s="110" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="206"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="30"/>
@@ -7837,7 +8262,7 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="206"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="30"/>
@@ -7850,7 +8275,7 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="207"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="30"/>
@@ -7862,12 +8287,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="171" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="172"/>
-      <c r="G13" s="173"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8186,9 +8611,10 @@
       <c r="D69"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D13:G13"/>
+    <mergeCell ref="E9:E12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8213,15 +8639,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8340,11 +8766,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="171" t="s">
+      <c r="E13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="172"/>
-      <c r="G13" s="173"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8388,14 +8814,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -8503,10 +8929,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="171" t="s">
+      <c r="E13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="173"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -8549,15 +8975,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -8677,10 +9103,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="200" t="s">
+      <c r="F13" s="208" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="201"/>
+      <c r="G13" s="209"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8724,13 +9150,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -8854,7 +9280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -8866,35 +9292,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="222" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="214"/>
-      <c r="C3" s="215" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="215"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="214"/>
-      <c r="C4" s="215"/>
-      <c r="D4" s="215"/>
-      <c r="E4" s="215"/>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
-      <c r="H4" s="215"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9113,42 +9539,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="216" t="s">
+      <c r="C23" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="217"/>
-      <c r="E23" s="217"/>
-      <c r="F23" s="217"/>
-      <c r="G23" s="218"/>
+      <c r="D23" s="225"/>
+      <c r="E23" s="225"/>
+      <c r="F23" s="225"/>
+      <c r="G23" s="226"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="208"/>
-      <c r="D24" s="209"/>
-      <c r="E24" s="209"/>
-      <c r="F24" s="209"/>
-      <c r="G24" s="210"/>
+      <c r="C24" s="216"/>
+      <c r="D24" s="217"/>
+      <c r="E24" s="217"/>
+      <c r="F24" s="217"/>
+      <c r="G24" s="218"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="208" t="s">
+      <c r="C25" s="216" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="209"/>
-      <c r="E25" s="209"/>
-      <c r="F25" s="209"/>
-      <c r="G25" s="210"/>
+      <c r="D25" s="217"/>
+      <c r="E25" s="217"/>
+      <c r="F25" s="217"/>
+      <c r="G25" s="218"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="211"/>
-      <c r="D26" s="212"/>
-      <c r="E26" s="212"/>
-      <c r="F26" s="212"/>
-      <c r="G26" s="213"/>
+      <c r="C26" s="219"/>
+      <c r="D26" s="220"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="221"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9176,42 +9602,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="202" t="s">
+      <c r="C28" s="210" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="203"/>
-      <c r="E28" s="203"/>
-      <c r="F28" s="203"/>
-      <c r="G28" s="204"/>
+      <c r="D28" s="211"/>
+      <c r="E28" s="211"/>
+      <c r="F28" s="211"/>
+      <c r="G28" s="212"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="203"/>
-      <c r="E29" s="203"/>
-      <c r="F29" s="203"/>
-      <c r="G29" s="204"/>
+      <c r="C29" s="210"/>
+      <c r="D29" s="211"/>
+      <c r="E29" s="211"/>
+      <c r="F29" s="211"/>
+      <c r="G29" s="212"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="202" t="s">
+      <c r="C30" s="210" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="203"/>
-      <c r="E30" s="203"/>
-      <c r="F30" s="203"/>
-      <c r="G30" s="204"/>
+      <c r="D30" s="211"/>
+      <c r="E30" s="211"/>
+      <c r="F30" s="211"/>
+      <c r="G30" s="212"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="205"/>
-      <c r="D31" s="206"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="207"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214"/>
+      <c r="F31" s="214"/>
+      <c r="G31" s="215"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -9234,8 +9660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9246,35 +9672,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="222" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="214"/>
-      <c r="C3" s="215" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="215"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="214"/>
-      <c r="C4" s="215"/>
-      <c r="D4" s="215"/>
-      <c r="E4" s="215"/>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
-      <c r="H4" s="215"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9330,13 +9756,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="219" t="s">
+      <c r="C8" s="227" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="220"/>
-      <c r="E8" s="220"/>
-      <c r="F8" s="220"/>
-      <c r="G8" s="221"/>
+      <c r="D8" s="228"/>
+      <c r="E8" s="228"/>
+      <c r="F8" s="228"/>
+      <c r="G8" s="229"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9346,20 +9772,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="222"/>
-      <c r="D9" s="223"/>
-      <c r="E9" s="223"/>
-      <c r="F9" s="223"/>
-      <c r="G9" s="224"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="231"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="231"/>
+      <c r="G9" s="232"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="222"/>
-      <c r="D10" s="223"/>
-      <c r="E10" s="223"/>
-      <c r="F10" s="223"/>
-      <c r="G10" s="224"/>
+      <c r="C10" s="230"/>
+      <c r="D10" s="231"/>
+      <c r="E10" s="231"/>
+      <c r="F10" s="231"/>
+      <c r="G10" s="232"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -9370,11 +9796,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="225"/>
-      <c r="D11" s="226"/>
-      <c r="E11" s="226"/>
-      <c r="F11" s="226"/>
-      <c r="G11" s="227"/>
+      <c r="C11" s="233"/>
+      <c r="D11" s="234"/>
+      <c r="E11" s="234"/>
+      <c r="F11" s="234"/>
+      <c r="G11" s="235"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
23-01-05 3주 4일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD387C8A-D441-4D8E-ACB4-5A1B94956B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892B3B74-3DD6-4232-9FB4-BE45F8CD107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="598" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="598" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -45,30 +45,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="533">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1911,7 +1889,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전처리 시작합시다.</t>
+    <t>파일합치기 , 형태소사전처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불용어 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벡터화 및 메트릭스 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결산 준비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ppt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리 1만개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두 명이서 각자 1am/제로펩시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스트 네트워크 시각화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과 데이터 합성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개꿀띄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ppt 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의견이 많았으면 좋겠다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제 발생시 말해주기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떻게 설명할 것인지 순서를 정해두자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래 내용을 대답할 수 있다면</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2137,7 +2171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2285,6 +2319,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2766,7 +2812,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3265,9 +3311,6 @@
     <xf numFmtId="0" fontId="13" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3494,6 +3537,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4239,14 +4300,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -4270,12 +4331,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="190" t="s">
+      <c r="C5" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="190"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -4290,7 +4351,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="185" t="s">
+      <c r="E6" s="184" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4308,7 +4369,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="186"/>
+      <c r="E7" s="185"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -4330,19 +4391,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="182" t="s">
+      <c r="E9" s="181" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="187" t="s">
+      <c r="F9" s="186" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="191" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4350,21 +4411,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="188"/>
-      <c r="G10" s="193"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="187"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="181"/>
-      <c r="D11" s="184"/>
-      <c r="E11" s="183"/>
-      <c r="F11" s="188"/>
-      <c r="G11" s="193"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="187"/>
+      <c r="G11" s="192"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4374,9 +4435,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="189"/>
-      <c r="G12" s="194"/>
+      <c r="E12" s="183"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="193"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4385,11 +4446,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="178"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4457,35 +4518,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="221" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223" t="s">
+      <c r="B3" s="221"/>
+      <c r="C3" s="222" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="222"/>
-      <c r="C4" s="223"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="223"/>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="221"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="222"/>
+      <c r="H4" s="222"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4810,9 +4871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
+      <selection pane="topRight" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4924,7 +4985,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="236" t="s">
+      <c r="A2" s="235" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -4942,7 +5003,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="240" t="s">
+      <c r="G2" s="239" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -4962,9 +5023,12 @@
       <c r="N2" s="86" t="s">
         <v>466</v>
       </c>
+      <c r="O2" s="86" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="236"/>
+      <c r="A3" s="235"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -4978,7 +5042,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="240"/>
+      <c r="G3" s="239"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -4997,7 +5061,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="236"/>
+      <c r="A4" s="235"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -5009,7 +5073,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="240"/>
+      <c r="G4" s="239"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -5028,7 +5092,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="236"/>
+      <c r="A5" s="235"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -5042,7 +5106,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="240"/>
+      <c r="G5" s="239"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -5058,7 +5122,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="236"/>
+      <c r="A6" s="235"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -5074,7 +5138,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="240"/>
+      <c r="G6" s="239"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -5085,7 +5149,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="237" t="s">
+      <c r="A7" s="236" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -5101,7 +5165,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="240"/>
+      <c r="G7" s="239"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -5123,9 +5187,12 @@
       <c r="N7" s="87" t="s">
         <v>468</v>
       </c>
+      <c r="O7" s="87" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="237"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -5137,7 +5204,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="240"/>
+      <c r="G8" s="239"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -5158,7 +5225,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="237"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -5170,7 +5237,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="240"/>
+      <c r="G9" s="239"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -5186,7 +5253,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="237"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -5198,7 +5265,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="240"/>
+      <c r="G10" s="239"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -5209,7 +5276,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="237"/>
+      <c r="A11" s="236"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5221,7 +5288,7 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="240"/>
+      <c r="G11" s="239"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
       <c r="M11" t="s">
@@ -5229,7 +5296,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="238" t="s">
+      <c r="A12" s="237" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5243,7 +5310,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="240"/>
+      <c r="G12" s="239"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5257,14 +5324,14 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="238"/>
+      <c r="A13" s="237"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="240"/>
+      <c r="G13" s="239"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5277,12 +5344,12 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="238"/>
+      <c r="A14" s="237"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="240"/>
+      <c r="G14" s="239"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
@@ -5292,14 +5359,14 @@
       </c>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="238"/>
+      <c r="A15" s="237"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="240"/>
+      <c r="G15" s="239"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
@@ -5307,22 +5374,22 @@
       <c r="M15"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="238"/>
+      <c r="A16" s="237"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="240"/>
+      <c r="G16" s="239"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="239" t="s">
+    <row r="17" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="238" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5330,7 +5397,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="240"/>
+      <c r="G17" s="239"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5348,15 +5415,18 @@
       <c r="N17" s="89" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="239"/>
+      <c r="O17" s="89" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="238"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="240"/>
+      <c r="G18" s="239"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
@@ -5366,55 +5436,55 @@
         <v>438</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="239"/>
+    <row r="19" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="238"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="240"/>
+      <c r="G19" s="239"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
       <c r="M19" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="239"/>
+    <row r="20" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="238"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="240"/>
+      <c r="G20" s="239"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
       <c r="M20" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="239"/>
+    <row r="21" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="238"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="240"/>
+      <c r="G21" s="239"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="100" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:15" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
       <c r="M22" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:15" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5451,8 +5521,11 @@
       <c r="N23" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="30" customHeight="1">
+      <c r="O23" s="108" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5486,8 +5559,11 @@
       <c r="N24" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="30" customHeight="1">
+      <c r="O24" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5518,8 +5594,11 @@
       <c r="M25" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="30" customHeight="1">
+      <c r="O25" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5541,8 +5620,11 @@
       <c r="L26" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="30" customHeight="1">
+      <c r="O26" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5571,7 +5653,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="30" customHeight="1">
+    <row r="28" spans="1:15" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5591,7 +5673,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="30" customHeight="1">
+    <row r="29" spans="1:15" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5617,7 +5699,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="30" customHeight="1">
+    <row r="30" spans="1:15" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5634,7 +5716,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="30" customHeight="1">
+    <row r="31" spans="1:15" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5648,7 +5730,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="30" customHeight="1">
+    <row r="32" spans="1:15" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -7067,7 +7149,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H27" sqref="H27"/>
       <selection pane="topRight" activeCell="H27" sqref="H27"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
@@ -7123,22 +7205,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="241" t="s">
+      <c r="C2" s="240" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="241"/>
-      <c r="E2" s="241" t="s">
+      <c r="D2" s="240"/>
+      <c r="E2" s="240" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="241"/>
-      <c r="G2" s="241" t="s">
+      <c r="F2" s="240"/>
+      <c r="G2" s="240" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="241"/>
-      <c r="I2" s="241" t="s">
+      <c r="H2" s="240"/>
+      <c r="I2" s="240" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="242"/>
+      <c r="J2" s="241"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -7428,16 +7510,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="224.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="58.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="162" customFormat="1">
@@ -7623,9 +7705,8 @@
       <c r="C21" t="s">
         <v>369</v>
       </c>
-      <c r="E21" t="e" cm="1">
-        <f t="array" ref="E21">- 어떻게 설명할 것인지 순서를 정해두자</f>
-        <v>#NAME?</v>
+      <c r="E21" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -7640,9 +7721,8 @@
       <c r="C23" t="s">
         <v>371</v>
       </c>
-      <c r="E23" t="e" cm="1">
-        <f t="array" ref="E23">- 아래 내용을 대답할 수 있다면</f>
-        <v>#NAME?</v>
+      <c r="E23" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -7917,14 +7997,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -7968,19 +8048,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="195" t="s">
+      <c r="C6" s="194" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="182" t="s">
+      <c r="D6" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="200" t="s">
+      <c r="E6" s="199" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="203" t="s">
+      <c r="G6" s="202" t="s">
         <v>280</v>
       </c>
     </row>
@@ -7988,13 +8068,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="196"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="201"/>
+      <c r="C7" s="195"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="200"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="204"/>
+      <c r="G7" s="203"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -8010,13 +8090,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="197" t="s">
+      <c r="C9" s="196" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="200"/>
+      <c r="E9" s="199"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -8028,9 +8108,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="198"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="202"/>
+      <c r="C10" s="197"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="201"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -8040,9 +8120,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="183"/>
-      <c r="E11" s="202"/>
+      <c r="C11" s="198"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="201"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -8055,8 +8135,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="201"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="200"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -8069,11 +8149,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -8111,8 +8191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8125,15 +8205,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -8160,7 +8240,7 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="169" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="110" t="s">
@@ -8172,8 +8252,10 @@
       <c r="F5" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="110"/>
-      <c r="H5" s="171"/>
+      <c r="G5" s="110" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="170"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
@@ -8182,16 +8264,15 @@
       <c r="C6" s="158" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="168" t="s">
+      <c r="D6" s="167" t="s">
         <v>422</v>
       </c>
-      <c r="E6" s="172" t="s">
+      <c r="E6" s="171" t="s">
         <v>446</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>518</v>
-      </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="245" t="s">
+        <v>522</v>
+      </c>
       <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
@@ -8199,14 +8280,16 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="159"/>
-      <c r="D7" s="167" t="s">
+      <c r="D7" s="166" t="s">
         <v>421</v>
       </c>
-      <c r="E7" s="173" t="s">
+      <c r="E7" s="172" t="s">
         <v>447</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="F7" s="244" t="s">
+        <v>518</v>
+      </c>
+      <c r="G7" s="246"/>
       <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
@@ -8227,14 +8310,18 @@
       <c r="C9" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="168" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="205" t="s">
+      <c r="E9" s="204" t="s">
         <v>469</v>
       </c>
-      <c r="F9" s="166"/>
-      <c r="G9" s="166"/>
+      <c r="F9" s="171" t="s">
+        <v>519</v>
+      </c>
+      <c r="G9" s="247" t="s">
+        <v>523</v>
+      </c>
       <c r="H9" s="82"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
@@ -8247,9 +8334,13 @@
       <c r="D10" s="110" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="206"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="242" t="s">
+        <v>520</v>
+      </c>
+      <c r="G10" s="247" t="s">
+        <v>524</v>
+      </c>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
@@ -8262,8 +8353,8 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="206"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="205"/>
+      <c r="F11" s="243"/>
       <c r="G11" s="32"/>
       <c r="H11" s="30"/>
     </row>
@@ -8275,8 +8366,10 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="207"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="206"/>
+      <c r="F12" s="171" t="s">
+        <v>521</v>
+      </c>
       <c r="G12" s="32"/>
       <c r="H12" s="30"/>
     </row>
@@ -8287,12 +8380,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="177"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8611,10 +8704,12 @@
       <c r="D69"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8639,15 +8734,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8766,11 +8861,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="177"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8814,14 +8909,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -8929,10 +9024,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="178"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -8975,15 +9070,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -9103,10 +9198,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="208" t="s">
+      <c r="F13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="209"/>
+      <c r="G13" s="208"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9150,13 +9245,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -9292,35 +9387,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="221" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223" t="s">
+      <c r="B3" s="221"/>
+      <c r="C3" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="222"/>
-      <c r="C4" s="223"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="223"/>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="221"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="222"/>
+      <c r="H4" s="222"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9539,42 +9634,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="224" t="s">
+      <c r="C23" s="223" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="225"/>
-      <c r="E23" s="225"/>
-      <c r="F23" s="225"/>
-      <c r="G23" s="226"/>
+      <c r="D23" s="224"/>
+      <c r="E23" s="224"/>
+      <c r="F23" s="224"/>
+      <c r="G23" s="225"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="216"/>
-      <c r="D24" s="217"/>
-      <c r="E24" s="217"/>
-      <c r="F24" s="217"/>
-      <c r="G24" s="218"/>
+      <c r="C24" s="215"/>
+      <c r="D24" s="216"/>
+      <c r="E24" s="216"/>
+      <c r="F24" s="216"/>
+      <c r="G24" s="217"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="216" t="s">
+      <c r="C25" s="215" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="217"/>
-      <c r="E25" s="217"/>
-      <c r="F25" s="217"/>
-      <c r="G25" s="218"/>
+      <c r="D25" s="216"/>
+      <c r="E25" s="216"/>
+      <c r="F25" s="216"/>
+      <c r="G25" s="217"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="219"/>
-      <c r="D26" s="220"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="221"/>
+      <c r="C26" s="218"/>
+      <c r="D26" s="219"/>
+      <c r="E26" s="219"/>
+      <c r="F26" s="219"/>
+      <c r="G26" s="220"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9602,42 +9697,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="210" t="s">
+      <c r="C28" s="209" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="211"/>
-      <c r="E28" s="211"/>
-      <c r="F28" s="211"/>
-      <c r="G28" s="212"/>
+      <c r="D28" s="210"/>
+      <c r="E28" s="210"/>
+      <c r="F28" s="210"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="210"/>
-      <c r="D29" s="211"/>
-      <c r="E29" s="211"/>
-      <c r="F29" s="211"/>
-      <c r="G29" s="212"/>
+      <c r="C29" s="209"/>
+      <c r="D29" s="210"/>
+      <c r="E29" s="210"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="210" t="s">
+      <c r="C30" s="209" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="211"/>
-      <c r="E30" s="211"/>
-      <c r="F30" s="211"/>
-      <c r="G30" s="212"/>
+      <c r="D30" s="210"/>
+      <c r="E30" s="210"/>
+      <c r="F30" s="210"/>
+      <c r="G30" s="211"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="213"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="214"/>
-      <c r="F31" s="214"/>
-      <c r="G31" s="215"/>
+      <c r="C31" s="212"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="213"/>
+      <c r="F31" s="213"/>
+      <c r="G31" s="214"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -9660,8 +9755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9672,35 +9767,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="221" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223" t="s">
+      <c r="B3" s="221"/>
+      <c r="C3" s="222" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="222"/>
-      <c r="C4" s="223"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="223"/>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="221"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="222"/>
+      <c r="H4" s="222"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9756,13 +9851,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="227" t="s">
+      <c r="C8" s="226" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="228"/>
-      <c r="E8" s="228"/>
-      <c r="F8" s="228"/>
-      <c r="G8" s="229"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="227"/>
+      <c r="G8" s="228"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9772,20 +9867,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="230"/>
-      <c r="D9" s="231"/>
-      <c r="E9" s="231"/>
-      <c r="F9" s="231"/>
-      <c r="G9" s="232"/>
+      <c r="C9" s="229"/>
+      <c r="D9" s="230"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="230"/>
+      <c r="G9" s="231"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="230"/>
-      <c r="D10" s="231"/>
-      <c r="E10" s="231"/>
-      <c r="F10" s="231"/>
-      <c r="G10" s="232"/>
+      <c r="C10" s="229"/>
+      <c r="D10" s="230"/>
+      <c r="E10" s="230"/>
+      <c r="F10" s="230"/>
+      <c r="G10" s="231"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -9796,11 +9891,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="234"/>
-      <c r="E11" s="234"/>
-      <c r="F11" s="234"/>
-      <c r="G11" s="235"/>
+      <c r="C11" s="232"/>
+      <c r="D11" s="233"/>
+      <c r="E11" s="233"/>
+      <c r="F11" s="233"/>
+      <c r="G11" s="234"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
Revert "23-01-05 3주 4일차 결산 upload"
This reverts commit a751986d8ab492dc3362d382209f72c0d1ead1eb.
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892B3B74-3DD6-4232-9FB4-BE45F8CD107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD387C8A-D441-4D8E-ACB4-5A1B94956B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="598" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="598" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -45,8 +45,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="519">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1889,63 +1911,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>파일합치기 , 형태소사전처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>불용어 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>벡터화 및 메트릭스 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결산 준비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> ppt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전처리 1만개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>두 명이서 각자 1am/제로펩시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>텍스트 네트워크 시각화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결과 데이터 합성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개꿀띄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> ppt 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>의견이 많았으면 좋겠다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문제 발생시 말해주기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어떻게 설명할 것인지 순서를 정해두자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아래 내용을 대답할 수 있다면</t>
+    <t>전처리 시작합시다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2171,7 +2137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2319,18 +2285,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2812,7 +2766,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3311,6 +3265,9 @@
     <xf numFmtId="0" fontId="13" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3537,24 +3494,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4300,14 +4239,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -4331,12 +4270,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="189" t="s">
+      <c r="C5" s="190" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="190"/>
-      <c r="E5" s="190"/>
-      <c r="F5" s="190"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -4351,7 +4290,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="184" t="s">
+      <c r="E6" s="185" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4369,7 +4308,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="185"/>
+      <c r="E7" s="186"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -4391,19 +4330,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="178" t="s">
+      <c r="C9" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="181" t="s">
+      <c r="D9" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="181" t="s">
+      <c r="E9" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="186" t="s">
+      <c r="F9" s="187" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="191" t="s">
+      <c r="G9" s="192" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4411,21 +4350,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="179"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="182"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="192"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="188"/>
+      <c r="G10" s="193"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="183"/>
-      <c r="E11" s="182"/>
-      <c r="F11" s="187"/>
-      <c r="G11" s="192"/>
+      <c r="C11" s="181"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="188"/>
+      <c r="G11" s="193"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4435,9 +4374,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="183"/>
-      <c r="F12" s="188"/>
-      <c r="G12" s="193"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="194"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4446,11 +4385,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="177"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4518,35 +4457,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="221" t="s">
+      <c r="B2" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="221"/>
-      <c r="C3" s="222" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="221"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4871,9 +4810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O35" sqref="O35"/>
+      <selection pane="topRight" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4985,7 +4924,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="235" t="s">
+      <c r="A2" s="236" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -5003,7 +4942,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="239" t="s">
+      <c r="G2" s="240" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -5023,12 +4962,9 @@
       <c r="N2" s="86" t="s">
         <v>466</v>
       </c>
-      <c r="O2" s="86" t="s">
-        <v>527</v>
-      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="235"/>
+      <c r="A3" s="236"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -5042,7 +4978,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="239"/>
+      <c r="G3" s="240"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -5061,7 +4997,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="235"/>
+      <c r="A4" s="236"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -5073,7 +5009,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="239"/>
+      <c r="G4" s="240"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -5092,7 +5028,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="235"/>
+      <c r="A5" s="236"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -5106,7 +5042,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="239"/>
+      <c r="G5" s="240"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -5122,7 +5058,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="235"/>
+      <c r="A6" s="236"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -5138,7 +5074,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="239"/>
+      <c r="G6" s="240"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -5149,7 +5085,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="236" t="s">
+      <c r="A7" s="237" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -5165,7 +5101,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="239"/>
+      <c r="G7" s="240"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -5187,12 +5123,9 @@
       <c r="N7" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="O7" s="87" t="s">
-        <v>525</v>
-      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -5204,7 +5137,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="239"/>
+      <c r="G8" s="240"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -5225,7 +5158,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -5237,7 +5170,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="239"/>
+      <c r="G9" s="240"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -5253,7 +5186,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -5265,7 +5198,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="239"/>
+      <c r="G10" s="240"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -5276,7 +5209,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="236"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5288,7 +5221,7 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="239"/>
+      <c r="G11" s="240"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
       <c r="M11" t="s">
@@ -5296,7 +5229,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="237" t="s">
+      <c r="A12" s="238" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5310,7 +5243,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="239"/>
+      <c r="G12" s="240"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5324,14 +5257,14 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="237"/>
+      <c r="A13" s="238"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="239"/>
+      <c r="G13" s="240"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5344,12 +5277,12 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="237"/>
+      <c r="A14" s="238"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="239"/>
+      <c r="G14" s="240"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
@@ -5359,14 +5292,14 @@
       </c>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="237"/>
+      <c r="A15" s="238"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="239"/>
+      <c r="G15" s="240"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
@@ -5374,22 +5307,22 @@
       <c r="M15"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="237"/>
+      <c r="A16" s="238"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="239"/>
+      <c r="G16" s="240"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="238" t="s">
+    <row r="17" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="239" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5397,7 +5330,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="239"/>
+      <c r="G17" s="240"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5415,18 +5348,15 @@
       <c r="N17" s="89" t="s">
         <v>467</v>
       </c>
-      <c r="O17" s="89" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="238"/>
+    </row>
+    <row r="18" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="239"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="239"/>
+      <c r="G18" s="240"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
@@ -5436,55 +5366,55 @@
         <v>438</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="238"/>
+    <row r="19" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="239"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="239"/>
+      <c r="G19" s="240"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
       <c r="M19" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="238"/>
+    <row r="20" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="239"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="239"/>
+      <c r="G20" s="240"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
       <c r="M20" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="238"/>
+    <row r="21" spans="1:14" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="239"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="239"/>
+      <c r="G21" s="240"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="100" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:14" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
       <c r="M22" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:14" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5521,11 +5451,8 @@
       <c r="N23" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="108" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="30" customHeight="1">
+    </row>
+    <row r="24" spans="1:14" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5559,11 +5486,8 @@
       <c r="N24" t="s">
         <v>517</v>
       </c>
-      <c r="O24" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="30" customHeight="1">
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5594,11 +5518,8 @@
       <c r="M25" t="s">
         <v>445</v>
       </c>
-      <c r="O25" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="30" customHeight="1">
+    </row>
+    <row r="26" spans="1:14" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5620,11 +5541,8 @@
       <c r="L26" t="s">
         <v>359</v>
       </c>
-      <c r="O26" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="30" customHeight="1">
+    </row>
+    <row r="27" spans="1:14" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5653,7 +5571,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30" customHeight="1">
+    <row r="28" spans="1:14" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5673,7 +5591,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30" customHeight="1">
+    <row r="29" spans="1:14" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5699,7 +5617,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="30" customHeight="1">
+    <row r="30" spans="1:14" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5716,7 +5634,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" customHeight="1">
+    <row r="31" spans="1:14" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5730,7 +5648,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1">
+    <row r="32" spans="1:14" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -7149,7 +7067,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H27" sqref="H27"/>
       <selection pane="topRight" activeCell="H27" sqref="H27"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
@@ -7205,22 +7123,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="240" t="s">
+      <c r="C2" s="241" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="240"/>
-      <c r="E2" s="240" t="s">
+      <c r="D2" s="241"/>
+      <c r="E2" s="241" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="240"/>
-      <c r="G2" s="240" t="s">
+      <c r="F2" s="241"/>
+      <c r="G2" s="241" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="240"/>
-      <c r="I2" s="240" t="s">
+      <c r="H2" s="241"/>
+      <c r="I2" s="241" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="241"/>
+      <c r="J2" s="242"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -7510,16 +7428,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="58.625" customWidth="1"/>
+    <col min="4" max="4" width="224.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="162" customFormat="1">
@@ -7705,8 +7623,9 @@
       <c r="C21" t="s">
         <v>369</v>
       </c>
-      <c r="E21" t="s">
-        <v>531</v>
+      <c r="E21" t="e" cm="1">
+        <f t="array" ref="E21">- 어떻게 설명할 것인지 순서를 정해두자</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -7721,8 +7640,9 @@
       <c r="C23" t="s">
         <v>371</v>
       </c>
-      <c r="E23" t="s">
-        <v>532</v>
+      <c r="E23" t="e" cm="1">
+        <f t="array" ref="E23">- 아래 내용을 대답할 수 있다면</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -7997,14 +7917,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -8048,19 +7968,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="194" t="s">
+      <c r="C6" s="195" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="181" t="s">
+      <c r="D6" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="199" t="s">
+      <c r="E6" s="200" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="202" t="s">
+      <c r="G6" s="203" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8068,13 +7988,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="200"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="201"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="203"/>
+      <c r="G7" s="204"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -8090,13 +8010,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="196" t="s">
+      <c r="C9" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="181" t="s">
+      <c r="D9" s="182" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="199"/>
+      <c r="E9" s="200"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -8108,9 +8028,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="197"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="201"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="202"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -8120,9 +8040,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="198"/>
-      <c r="D11" s="182"/>
-      <c r="E11" s="201"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="202"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -8135,8 +8055,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="183"/>
-      <c r="E12" s="200"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="201"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -8149,11 +8069,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -8191,8 +8111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8205,15 +8125,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -8240,7 +8160,7 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="169" t="s">
+      <c r="C5" s="170" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="110" t="s">
@@ -8252,10 +8172,8 @@
       <c r="F5" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="110" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" s="170"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="171"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
@@ -8264,15 +8182,16 @@
       <c r="C6" s="158" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="167" t="s">
+      <c r="D6" s="168" t="s">
         <v>422</v>
       </c>
-      <c r="E6" s="171" t="s">
+      <c r="E6" s="172" t="s">
         <v>446</v>
       </c>
-      <c r="G6" s="245" t="s">
-        <v>522</v>
-      </c>
+      <c r="F6" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="G6" s="32"/>
       <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
@@ -8280,16 +8199,14 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="159"/>
-      <c r="D7" s="166" t="s">
+      <c r="D7" s="167" t="s">
         <v>421</v>
       </c>
-      <c r="E7" s="172" t="s">
+      <c r="E7" s="173" t="s">
         <v>447</v>
       </c>
-      <c r="F7" s="244" t="s">
-        <v>518</v>
-      </c>
-      <c r="G7" s="246"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
       <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
@@ -8310,18 +8227,14 @@
       <c r="C9" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="169" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="204" t="s">
+      <c r="E9" s="205" t="s">
         <v>469</v>
       </c>
-      <c r="F9" s="171" t="s">
-        <v>519</v>
-      </c>
-      <c r="G9" s="247" t="s">
-        <v>523</v>
-      </c>
+      <c r="F9" s="166"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="82"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
@@ -8334,13 +8247,9 @@
       <c r="D10" s="110" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="205"/>
-      <c r="F10" s="242" t="s">
-        <v>520</v>
-      </c>
-      <c r="G10" s="247" t="s">
-        <v>524</v>
-      </c>
+      <c r="E10" s="206"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
@@ -8353,8 +8262,8 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="205"/>
-      <c r="F11" s="243"/>
+      <c r="E11" s="206"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="30"/>
     </row>
@@ -8366,10 +8275,8 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="206"/>
-      <c r="F12" s="171" t="s">
-        <v>521</v>
-      </c>
+      <c r="E12" s="207"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="30"/>
     </row>
@@ -8380,12 +8287,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8704,12 +8611,10 @@
       <c r="D69"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8734,15 +8639,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8861,11 +8766,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="175" t="s">
+      <c r="E13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8909,14 +8814,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -9024,10 +8929,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="175" t="s">
+      <c r="E13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="177"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -9070,15 +8975,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -9198,10 +9103,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="207" t="s">
+      <c r="F13" s="208" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="208"/>
+      <c r="G13" s="209"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9245,13 +9150,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -9387,35 +9292,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="221" t="s">
+      <c r="B2" s="222" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="221"/>
-      <c r="C3" s="222" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="221"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9634,42 +9539,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="223" t="s">
+      <c r="C23" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="224"/>
-      <c r="E23" s="224"/>
-      <c r="F23" s="224"/>
-      <c r="G23" s="225"/>
+      <c r="D23" s="225"/>
+      <c r="E23" s="225"/>
+      <c r="F23" s="225"/>
+      <c r="G23" s="226"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="215"/>
-      <c r="D24" s="216"/>
-      <c r="E24" s="216"/>
-      <c r="F24" s="216"/>
-      <c r="G24" s="217"/>
+      <c r="C24" s="216"/>
+      <c r="D24" s="217"/>
+      <c r="E24" s="217"/>
+      <c r="F24" s="217"/>
+      <c r="G24" s="218"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="215" t="s">
+      <c r="C25" s="216" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="216"/>
-      <c r="E25" s="216"/>
-      <c r="F25" s="216"/>
-      <c r="G25" s="217"/>
+      <c r="D25" s="217"/>
+      <c r="E25" s="217"/>
+      <c r="F25" s="217"/>
+      <c r="G25" s="218"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="218"/>
-      <c r="D26" s="219"/>
-      <c r="E26" s="219"/>
-      <c r="F26" s="219"/>
-      <c r="G26" s="220"/>
+      <c r="C26" s="219"/>
+      <c r="D26" s="220"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="221"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9697,42 +9602,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="209" t="s">
+      <c r="C28" s="210" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="210"/>
-      <c r="E28" s="210"/>
-      <c r="F28" s="210"/>
-      <c r="G28" s="211"/>
+      <c r="D28" s="211"/>
+      <c r="E28" s="211"/>
+      <c r="F28" s="211"/>
+      <c r="G28" s="212"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="209"/>
-      <c r="D29" s="210"/>
-      <c r="E29" s="210"/>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="C29" s="210"/>
+      <c r="D29" s="211"/>
+      <c r="E29" s="211"/>
+      <c r="F29" s="211"/>
+      <c r="G29" s="212"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="209" t="s">
+      <c r="C30" s="210" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="210"/>
-      <c r="E30" s="210"/>
-      <c r="F30" s="210"/>
-      <c r="G30" s="211"/>
+      <c r="D30" s="211"/>
+      <c r="E30" s="211"/>
+      <c r="F30" s="211"/>
+      <c r="G30" s="212"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="212"/>
-      <c r="D31" s="213"/>
-      <c r="E31" s="213"/>
-      <c r="F31" s="213"/>
-      <c r="G31" s="214"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214"/>
+      <c r="F31" s="214"/>
+      <c r="G31" s="215"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -9755,8 +9660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9767,35 +9672,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="221" t="s">
+      <c r="B2" s="222" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="221"/>
-      <c r="C3" s="222" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="221"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9851,13 +9756,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="226" t="s">
+      <c r="C8" s="227" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="227"/>
-      <c r="E8" s="227"/>
-      <c r="F8" s="227"/>
-      <c r="G8" s="228"/>
+      <c r="D8" s="228"/>
+      <c r="E8" s="228"/>
+      <c r="F8" s="228"/>
+      <c r="G8" s="229"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9867,20 +9772,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="229"/>
-      <c r="D9" s="230"/>
-      <c r="E9" s="230"/>
-      <c r="F9" s="230"/>
-      <c r="G9" s="231"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="231"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="231"/>
+      <c r="G9" s="232"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="229"/>
-      <c r="D10" s="230"/>
-      <c r="E10" s="230"/>
-      <c r="F10" s="230"/>
-      <c r="G10" s="231"/>
+      <c r="C10" s="230"/>
+      <c r="D10" s="231"/>
+      <c r="E10" s="231"/>
+      <c r="F10" s="231"/>
+      <c r="G10" s="232"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -9891,11 +9796,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="232"/>
-      <c r="D11" s="233"/>
-      <c r="E11" s="233"/>
-      <c r="F11" s="233"/>
-      <c r="G11" s="234"/>
+      <c r="C11" s="233"/>
+      <c r="D11" s="234"/>
+      <c r="E11" s="234"/>
+      <c r="F11" s="234"/>
+      <c r="G11" s="235"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
23-01-06 3주 5일차 결산 upload
Mineamine data 수정
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9822424-A6FB-4A56-AA12-CBCDF6732D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F703ADED-B221-48EF-94FB-29DAD9C4F0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="530">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1936,6 +1936,26 @@
   </si>
   <si>
     <t>ppt 초안 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펩시제로 빅토리아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ucient</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펩시제로 사전 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빅토리아 사전 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘토링 잘하자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2790,7 +2810,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3289,9 +3309,6 @@
     <xf numFmtId="0" fontId="13" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3415,6 +3432,12 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3518,6 +3541,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4263,14 +4289,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -4294,12 +4320,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="190" t="s">
+      <c r="C5" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="190"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -4314,7 +4340,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="185" t="s">
+      <c r="E6" s="184" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4332,7 +4358,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="186"/>
+      <c r="E7" s="185"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -4354,19 +4380,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="182" t="s">
+      <c r="E9" s="181" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="187" t="s">
+      <c r="F9" s="186" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="191" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4374,21 +4400,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="188"/>
-      <c r="G10" s="193"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="187"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="181"/>
-      <c r="D11" s="184"/>
-      <c r="E11" s="183"/>
-      <c r="F11" s="188"/>
-      <c r="G11" s="193"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="187"/>
+      <c r="G11" s="192"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4398,9 +4424,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="189"/>
-      <c r="G12" s="194"/>
+      <c r="E12" s="183"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="193"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4409,11 +4435,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="178"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4481,35 +4507,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="223" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="224"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223" t="s">
+      <c r="B3" s="223"/>
+      <c r="C3" s="224" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
+      <c r="D3" s="224"/>
+      <c r="E3" s="224"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="224"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="222"/>
-      <c r="C4" s="223"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="223"/>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="223"/>
+      <c r="C4" s="224"/>
+      <c r="D4" s="224"/>
+      <c r="E4" s="224"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="224"/>
+      <c r="H4" s="224"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4834,9 +4860,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O18" sqref="O18"/>
+      <selection pane="topRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4948,7 +4974,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="236" t="s">
+      <c r="A2" s="237" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -4966,7 +4992,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="240" t="s">
+      <c r="G2" s="241" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -4989,9 +5015,12 @@
       <c r="O2" s="86" t="s">
         <v>518</v>
       </c>
+      <c r="P2" s="86" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="236"/>
+      <c r="A3" s="237"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -5005,7 +5034,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="240"/>
+      <c r="G3" s="241"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -5024,7 +5053,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="236"/>
+      <c r="A4" s="237"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -5036,7 +5065,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="240"/>
+      <c r="G4" s="241"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -5055,7 +5084,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="236"/>
+      <c r="A5" s="237"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -5069,7 +5098,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="240"/>
+      <c r="G5" s="241"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -5085,7 +5114,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="236"/>
+      <c r="A6" s="237"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -5101,7 +5130,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="240"/>
+      <c r="G6" s="241"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -5112,7 +5141,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="237" t="s">
+      <c r="A7" s="238" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -5128,7 +5157,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="240"/>
+      <c r="G7" s="241"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -5153,9 +5182,12 @@
       <c r="O7" s="87" t="s">
         <v>519</v>
       </c>
+      <c r="P7" s="87" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="237"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -5167,7 +5199,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="240"/>
+      <c r="G8" s="241"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -5188,7 +5220,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="237"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -5200,7 +5232,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="240"/>
+      <c r="G9" s="241"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -5216,7 +5248,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="237"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -5228,7 +5260,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="240"/>
+      <c r="G10" s="241"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -5239,7 +5271,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="237"/>
+      <c r="A11" s="238"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5251,7 +5283,7 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="240"/>
+      <c r="G11" s="241"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
       <c r="M11" t="s">
@@ -5259,7 +5291,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="238" t="s">
+      <c r="A12" s="239" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5273,7 +5305,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="240"/>
+      <c r="G12" s="241"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5287,14 +5319,14 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="238"/>
+      <c r="A13" s="239"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="240"/>
+      <c r="G13" s="241"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5307,12 +5339,12 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="238"/>
+      <c r="A14" s="239"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="240"/>
+      <c r="G14" s="241"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
@@ -5322,14 +5354,14 @@
       </c>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="238"/>
+      <c r="A15" s="239"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="240"/>
+      <c r="G15" s="241"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
@@ -5337,22 +5369,22 @@
       <c r="M15"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="238"/>
+      <c r="A16" s="239"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="240"/>
+      <c r="G16" s="241"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="239" t="s">
+    <row r="17" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="240" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5360,7 +5392,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="240"/>
+      <c r="G17" s="241"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5381,15 +5413,18 @@
       <c r="O17" s="89" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="239"/>
+      <c r="P17" s="89" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="240"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="240"/>
+      <c r="G18" s="241"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
@@ -5399,55 +5434,55 @@
         <v>438</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="239"/>
+    <row r="19" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="240"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="240"/>
+      <c r="G19" s="241"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
       <c r="M19" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="239"/>
+    <row r="20" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="240"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="240"/>
+      <c r="G20" s="241"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
       <c r="M20" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="239"/>
+    <row r="21" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="240"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="240"/>
+      <c r="G21" s="241"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="100" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:16" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
       <c r="M22" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:16" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5484,8 +5519,14 @@
       <c r="N23" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="30" customHeight="1">
+      <c r="O23" s="108" t="s">
+        <v>68</v>
+      </c>
+      <c r="P23" s="108" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5519,8 +5560,11 @@
       <c r="N24" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="30" customHeight="1">
+      <c r="P24" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5552,7 +5596,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" customHeight="1">
+    <row r="26" spans="1:16" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5575,7 +5619,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="30" customHeight="1">
+    <row r="27" spans="1:16" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5604,7 +5648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30" customHeight="1">
+    <row r="28" spans="1:16" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5624,7 +5668,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30" customHeight="1">
+    <row r="29" spans="1:16" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5650,7 +5694,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="30" customHeight="1">
+    <row r="30" spans="1:16" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5667,7 +5711,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" customHeight="1">
+    <row r="31" spans="1:16" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5681,7 +5725,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1">
+    <row r="32" spans="1:16" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -7156,22 +7200,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="241" t="s">
+      <c r="C2" s="242" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="241"/>
-      <c r="E2" s="241" t="s">
+      <c r="D2" s="242"/>
+      <c r="E2" s="242" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="241"/>
-      <c r="G2" s="241" t="s">
+      <c r="F2" s="242"/>
+      <c r="G2" s="242" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="241"/>
-      <c r="I2" s="241" t="s">
+      <c r="H2" s="242"/>
+      <c r="I2" s="242" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="242"/>
+      <c r="J2" s="243"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -7461,7 +7505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -7950,14 +7994,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -8001,19 +8045,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="195" t="s">
+      <c r="C6" s="194" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="182" t="s">
+      <c r="D6" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="200" t="s">
+      <c r="E6" s="199" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="203" t="s">
+      <c r="G6" s="202" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8021,13 +8065,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="196"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="201"/>
+      <c r="C7" s="195"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="200"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="204"/>
+      <c r="G7" s="203"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -8043,13 +8087,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="197" t="s">
+      <c r="C9" s="196" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="200"/>
+      <c r="E9" s="199"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -8061,9 +8105,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="198"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="202"/>
+      <c r="C10" s="197"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="201"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -8073,9 +8117,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="183"/>
-      <c r="E11" s="202"/>
+      <c r="C11" s="198"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="201"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -8088,8 +8132,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="201"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="200"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -8102,11 +8146,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -8144,8 +8188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8158,15 +8202,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -8193,7 +8237,7 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="169" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="110" t="s">
@@ -8208,7 +8252,7 @@
       <c r="G5" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="171"/>
+      <c r="H5" s="170"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
@@ -8217,16 +8261,16 @@
       <c r="C6" s="158" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="168" t="s">
+      <c r="D6" s="167" t="s">
         <v>422</v>
       </c>
-      <c r="E6" s="172" t="s">
+      <c r="E6" s="171" t="s">
         <v>446</v>
       </c>
       <c r="F6" s="112" t="s">
         <v>523</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="207" t="s">
         <v>521</v>
       </c>
       <c r="H6" s="30"/>
@@ -8236,16 +8280,16 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="159"/>
-      <c r="D7" s="167" t="s">
+      <c r="D7" s="166" t="s">
         <v>421</v>
       </c>
-      <c r="E7" s="173" t="s">
+      <c r="E7" s="172" t="s">
         <v>447</v>
       </c>
       <c r="F7" s="112" t="s">
         <v>520</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="208"/>
       <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
@@ -8266,16 +8310,16 @@
       <c r="C9" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="168" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="205" t="s">
+      <c r="E9" s="204" t="s">
         <v>469</v>
       </c>
       <c r="F9" s="112" t="s">
         <v>524</v>
       </c>
-      <c r="G9" s="166" t="s">
+      <c r="G9" s="244" t="s">
         <v>522</v>
       </c>
       <c r="H9" s="82"/>
@@ -8290,9 +8334,11 @@
       <c r="D10" s="110" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="206"/>
+      <c r="E10" s="205"/>
       <c r="F10" s="112"/>
-      <c r="G10" s="32"/>
+      <c r="G10" s="244" t="s">
+        <v>525</v>
+      </c>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
@@ -8305,9 +8351,11 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="206"/>
+      <c r="E11" s="205"/>
       <c r="F11" s="112"/>
-      <c r="G11" s="32"/>
+      <c r="G11" s="244" t="s">
+        <v>526</v>
+      </c>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
@@ -8318,9 +8366,9 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="207"/>
+      <c r="E12" s="206"/>
       <c r="F12" s="112"/>
-      <c r="G12" s="32"/>
+      <c r="G12" s="244"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
@@ -8330,12 +8378,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="177"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8654,10 +8702,11 @@
       <c r="D69"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8670,7 +8719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -8682,15 +8731,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8809,11 +8858,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="177"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8857,14 +8906,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -8972,10 +9021,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="178"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -9018,15 +9067,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -9146,10 +9195,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="208" t="s">
+      <c r="F13" s="209" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="209"/>
+      <c r="G13" s="210"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9193,13 +9242,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -9335,35 +9384,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="223" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="224"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223" t="s">
+      <c r="B3" s="223"/>
+      <c r="C3" s="224" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
+      <c r="D3" s="224"/>
+      <c r="E3" s="224"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="224"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="222"/>
-      <c r="C4" s="223"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="223"/>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="223"/>
+      <c r="C4" s="224"/>
+      <c r="D4" s="224"/>
+      <c r="E4" s="224"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="224"/>
+      <c r="H4" s="224"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9582,42 +9631,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="224" t="s">
+      <c r="C23" s="225" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="225"/>
-      <c r="E23" s="225"/>
-      <c r="F23" s="225"/>
-      <c r="G23" s="226"/>
+      <c r="D23" s="226"/>
+      <c r="E23" s="226"/>
+      <c r="F23" s="226"/>
+      <c r="G23" s="227"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="216"/>
-      <c r="D24" s="217"/>
-      <c r="E24" s="217"/>
-      <c r="F24" s="217"/>
-      <c r="G24" s="218"/>
+      <c r="C24" s="217"/>
+      <c r="D24" s="218"/>
+      <c r="E24" s="218"/>
+      <c r="F24" s="218"/>
+      <c r="G24" s="219"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="216" t="s">
+      <c r="C25" s="217" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="217"/>
-      <c r="E25" s="217"/>
-      <c r="F25" s="217"/>
-      <c r="G25" s="218"/>
+      <c r="D25" s="218"/>
+      <c r="E25" s="218"/>
+      <c r="F25" s="218"/>
+      <c r="G25" s="219"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="219"/>
-      <c r="D26" s="220"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="221"/>
+      <c r="C26" s="220"/>
+      <c r="D26" s="221"/>
+      <c r="E26" s="221"/>
+      <c r="F26" s="221"/>
+      <c r="G26" s="222"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9645,42 +9694,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="210" t="s">
+      <c r="C28" s="211" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="211"/>
-      <c r="E28" s="211"/>
-      <c r="F28" s="211"/>
-      <c r="G28" s="212"/>
+      <c r="D28" s="212"/>
+      <c r="E28" s="212"/>
+      <c r="F28" s="212"/>
+      <c r="G28" s="213"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="210"/>
-      <c r="D29" s="211"/>
-      <c r="E29" s="211"/>
-      <c r="F29" s="211"/>
-      <c r="G29" s="212"/>
+      <c r="C29" s="211"/>
+      <c r="D29" s="212"/>
+      <c r="E29" s="212"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="213"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="210" t="s">
+      <c r="C30" s="211" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="211"/>
-      <c r="E30" s="211"/>
-      <c r="F30" s="211"/>
-      <c r="G30" s="212"/>
+      <c r="D30" s="212"/>
+      <c r="E30" s="212"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="213"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="213"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="214"/>
-      <c r="F31" s="214"/>
-      <c r="G31" s="215"/>
+      <c r="C31" s="214"/>
+      <c r="D31" s="215"/>
+      <c r="E31" s="215"/>
+      <c r="F31" s="215"/>
+      <c r="G31" s="216"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -9715,35 +9764,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="223" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="224"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223" t="s">
+      <c r="B3" s="223"/>
+      <c r="C3" s="224" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
+      <c r="D3" s="224"/>
+      <c r="E3" s="224"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="224"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="222"/>
-      <c r="C4" s="223"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="223"/>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="223"/>
+      <c r="C4" s="224"/>
+      <c r="D4" s="224"/>
+      <c r="E4" s="224"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="224"/>
+      <c r="H4" s="224"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9799,13 +9848,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="227" t="s">
+      <c r="C8" s="228" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="228"/>
-      <c r="E8" s="228"/>
-      <c r="F8" s="228"/>
-      <c r="G8" s="229"/>
+      <c r="D8" s="229"/>
+      <c r="E8" s="229"/>
+      <c r="F8" s="229"/>
+      <c r="G8" s="230"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9815,20 +9864,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="230"/>
-      <c r="D9" s="231"/>
-      <c r="E9" s="231"/>
-      <c r="F9" s="231"/>
-      <c r="G9" s="232"/>
+      <c r="C9" s="231"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="232"/>
+      <c r="F9" s="232"/>
+      <c r="G9" s="233"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="230"/>
-      <c r="D10" s="231"/>
-      <c r="E10" s="231"/>
-      <c r="F10" s="231"/>
-      <c r="G10" s="232"/>
+      <c r="C10" s="231"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
+      <c r="F10" s="232"/>
+      <c r="G10" s="233"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -9839,11 +9888,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="234"/>
-      <c r="E11" s="234"/>
-      <c r="F11" s="234"/>
-      <c r="G11" s="235"/>
+      <c r="C11" s="234"/>
+      <c r="D11" s="235"/>
+      <c r="E11" s="235"/>
+      <c r="F11" s="235"/>
+      <c r="G11" s="236"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>

</xml_diff>

<commit_message>
23-01-07 3주 6일차  결산
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F703ADED-B221-48EF-94FB-29DAD9C4F0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39E2B44-D58C-4F89-8C0E-D94E3C19E7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="544">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1956,6 +1956,52 @@
   </si>
   <si>
     <t>멘토링 잘하자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘토링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 개요를 조금 구체화하자.</t>
+  </si>
+  <si>
+    <t>왜 제로탄산의 음료에 집중하는가?</t>
+  </si>
+  <si>
+    <t>왜 건강에 관심이 많아졌을까?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">관심 유발 </t>
+  </si>
+  <si>
+    <t>조언</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 아키텍쳐 생성</t>
+  </si>
+  <si>
+    <t>1- 프로그램의 기능이 무엇인지 명확하게 설명할 수 있어야한다.</t>
+  </si>
+  <si>
+    <t>2- 시각화 결과물 구체화 -&gt; 정확히 무슨 정보를 전달하는가 -&gt; 상업적 효과에서 설득</t>
+  </si>
+  <si>
+    <t xml:space="preserve">역할 분담 명시(R&amp;R)세부적 </t>
+  </si>
+  <si>
+    <t>개요 +</t>
+  </si>
+  <si>
+    <t>계획을 좀 더 구체적으로 짜자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 아키텍쳐 구성 (WBS 사용) 2. 전처리 마무리 3. 시각화 테스팅 완료 4. 웹 구현 설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조 멘토링</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2810,7 +2856,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="245">
+  <cellXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3330,6 +3376,9 @@
     <xf numFmtId="0" fontId="26" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3543,7 +3592,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3573,16 +3637,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>175640</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>499491</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3611,8 +3675,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9086850" y="723900"/>
-          <a:ext cx="7772400" cy="5233415"/>
+          <a:off x="4638675" y="0"/>
+          <a:ext cx="10991850" cy="6909816"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4277,7 +4341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDE6C63-9121-4583-87EA-DA9F0C78BEC1}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -4289,14 +4353,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -4320,12 +4384,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="189" t="s">
+      <c r="C5" s="190" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="190"/>
-      <c r="E5" s="190"/>
-      <c r="F5" s="190"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -4340,7 +4404,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="184" t="s">
+      <c r="E6" s="185" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4358,7 +4422,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="185"/>
+      <c r="E7" s="186"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -4380,19 +4444,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="178" t="s">
+      <c r="C9" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="181" t="s">
+      <c r="D9" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="181" t="s">
+      <c r="E9" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="186" t="s">
+      <c r="F9" s="187" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="191" t="s">
+      <c r="G9" s="192" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4400,21 +4464,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="179"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="182"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="192"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="188"/>
+      <c r="G10" s="193"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="183"/>
-      <c r="E11" s="182"/>
-      <c r="F11" s="187"/>
-      <c r="G11" s="192"/>
+      <c r="C11" s="181"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="188"/>
+      <c r="G11" s="193"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4424,9 +4488,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="183"/>
-      <c r="F12" s="188"/>
-      <c r="G12" s="193"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="194"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4435,11 +4499,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="177"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4507,35 +4571,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="224" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="223"/>
-      <c r="C3" s="224" t="s">
+      <c r="B3" s="224"/>
+      <c r="C3" s="225" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="225"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="225"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="223"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
+      <c r="B4" s="224"/>
+      <c r="C4" s="225"/>
+      <c r="D4" s="225"/>
+      <c r="E4" s="225"/>
+      <c r="F4" s="225"/>
+      <c r="G4" s="225"/>
+      <c r="H4" s="225"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4860,9 +4924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -4974,7 +5038,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="238" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -4992,7 +5056,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="241" t="s">
+      <c r="G2" s="242" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -5018,9 +5082,10 @@
       <c r="P2" s="86" t="s">
         <v>518</v>
       </c>
+      <c r="Q2" s="100"/>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="237"/>
+      <c r="A3" s="238"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -5034,7 +5099,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="241"/>
+      <c r="G3" s="242"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -5051,9 +5116,10 @@
       <c r="M3" t="s">
         <v>428</v>
       </c>
+      <c r="Q3" s="100"/>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="237"/>
+      <c r="A4" s="238"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -5065,7 +5131,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="241"/>
+      <c r="G4" s="242"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -5082,9 +5148,12 @@
       <c r="M4" t="s">
         <v>429</v>
       </c>
+      <c r="Q4" s="100" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="237"/>
+      <c r="A5" s="238"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -5098,7 +5167,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="241"/>
+      <c r="G5" s="242"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -5112,9 +5181,10 @@
       <c r="M5" t="s">
         <v>430</v>
       </c>
+      <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="237"/>
+      <c r="A6" s="238"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -5130,7 +5200,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="241"/>
+      <c r="G6" s="242"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -5139,9 +5209,12 @@
       <c r="M6" t="s">
         <v>431</v>
       </c>
+      <c r="Q6" s="100" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="238" t="s">
+      <c r="A7" s="239" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -5157,7 +5230,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="241"/>
+      <c r="G7" s="242"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -5185,9 +5258,10 @@
       <c r="P7" s="87" t="s">
         <v>527</v>
       </c>
+      <c r="Q7" s="100"/>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="238"/>
+      <c r="A8" s="239"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -5199,7 +5273,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="241"/>
+      <c r="G8" s="242"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -5218,9 +5292,12 @@
       <c r="M8" t="s">
         <v>433</v>
       </c>
+      <c r="Q8" s="100" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="238"/>
+      <c r="A9" s="239"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -5232,7 +5309,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="241"/>
+      <c r="G9" s="242"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -5246,9 +5323,12 @@
       <c r="M9" t="s">
         <v>434</v>
       </c>
+      <c r="Q9" s="100" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="238"/>
+      <c r="A10" s="239"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -5260,7 +5340,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="241"/>
+      <c r="G10" s="242"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -5269,9 +5349,12 @@
       <c r="M10" t="s">
         <v>435</v>
       </c>
+      <c r="Q10" s="100" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="238"/>
+      <c r="A11" s="239"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5283,15 +5366,16 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="241"/>
+      <c r="G11" s="242"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
       <c r="M11" t="s">
         <v>436</v>
       </c>
+      <c r="Q11" s="100"/>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="239" t="s">
+      <c r="A12" s="240" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5305,7 +5389,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="241"/>
+      <c r="G12" s="242"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5317,16 +5401,17 @@
         <v>283</v>
       </c>
       <c r="M12"/>
+      <c r="Q12" s="100"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="239"/>
+      <c r="A13" s="240"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="241"/>
+      <c r="G13" s="242"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5337,14 +5422,15 @@
       <c r="M13" t="s">
         <v>437</v>
       </c>
+      <c r="Q13" s="100"/>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="239"/>
+      <c r="A14" s="240"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="241"/>
+      <c r="G14" s="242"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
@@ -5352,39 +5438,42 @@
       <c r="M14" t="s">
         <v>438</v>
       </c>
+      <c r="Q14" s="100"/>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="239"/>
+      <c r="A15" s="240"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="241"/>
+      <c r="G15" s="242"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="100"/>
       <c r="M15"/>
+      <c r="Q15" s="100"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="239"/>
+      <c r="A16" s="240"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="241"/>
+      <c r="G16" s="242"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
       <c r="M16"/>
-    </row>
-    <row r="17" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="240" t="s">
+      <c r="Q16" s="100"/>
+    </row>
+    <row r="17" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="241" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5392,7 +5481,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="241"/>
+      <c r="G17" s="242"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5416,15 +5505,18 @@
       <c r="P17" s="89" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="240"/>
+      <c r="Q17" s="100" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="241"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="241"/>
+      <c r="G18" s="242"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
@@ -5433,56 +5525,67 @@
       <c r="M18" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="240"/>
+      <c r="Q18" s="100" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="241"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="241"/>
+      <c r="G19" s="242"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
       <c r="M19" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="240"/>
+      <c r="Q19" s="100"/>
+    </row>
+    <row r="20" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="241"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="241"/>
+      <c r="G20" s="242"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
       <c r="M20" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="240"/>
+      <c r="Q20" s="100" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="241"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="241"/>
+      <c r="G21" s="242"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" s="100" customFormat="1" ht="30" customHeight="1">
+      <c r="Q21" s="100"/>
+    </row>
+    <row r="22" spans="1:17" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
       <c r="M22" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" s="109" customFormat="1" ht="30" customHeight="1">
+      <c r="Q22" s="100" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5525,8 +5628,11 @@
       <c r="P23" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="30" customHeight="1">
+      <c r="Q23" s="100" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5563,8 +5669,11 @@
       <c r="P24" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="30" customHeight="1">
+      <c r="Q24" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5595,8 +5704,11 @@
       <c r="M25" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="30" customHeight="1">
+      <c r="Q25" s="108" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5618,8 +5730,11 @@
       <c r="L26" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="30" customHeight="1">
+      <c r="Q26" s="100" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5648,7 +5763,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="30" customHeight="1">
+    <row r="28" spans="1:17" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5668,7 +5783,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="30" customHeight="1">
+    <row r="29" spans="1:17" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5694,7 +5809,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="30" customHeight="1">
+    <row r="30" spans="1:17" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5711,7 +5826,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="30" customHeight="1">
+    <row r="31" spans="1:17" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5725,7 +5840,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="30" customHeight="1">
+    <row r="32" spans="1:17" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -7200,22 +7315,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="242" t="s">
+      <c r="C2" s="243" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="242"/>
-      <c r="E2" s="242" t="s">
+      <c r="D2" s="243"/>
+      <c r="E2" s="243" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="242"/>
-      <c r="G2" s="242" t="s">
+      <c r="F2" s="243"/>
+      <c r="G2" s="243" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="242"/>
-      <c r="I2" s="242" t="s">
+      <c r="H2" s="243"/>
+      <c r="I2" s="243" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="243"/>
+      <c r="J2" s="244"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -7505,8 +7620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -7982,7 +8097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251ECE8D-9668-40EA-AFB2-EB0A37392AB0}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -7994,14 +8109,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -8045,19 +8160,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="194" t="s">
+      <c r="C6" s="195" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="181" t="s">
+      <c r="D6" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="199" t="s">
+      <c r="E6" s="200" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="202" t="s">
+      <c r="G6" s="203" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8065,13 +8180,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="200"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="201"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="203"/>
+      <c r="G7" s="204"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -8087,13 +8202,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="196" t="s">
+      <c r="C9" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="181" t="s">
+      <c r="D9" s="182" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="199"/>
+      <c r="E9" s="200"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -8105,9 +8220,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="197"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="201"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="202"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -8117,9 +8232,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="198"/>
-      <c r="D11" s="182"/>
-      <c r="E11" s="201"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="202"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -8132,8 +8247,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="183"/>
-      <c r="E12" s="200"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="201"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -8146,11 +8261,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -8188,8 +8303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8202,15 +8317,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -8270,10 +8385,12 @@
       <c r="F6" s="112" t="s">
         <v>523</v>
       </c>
-      <c r="G6" s="207" t="s">
+      <c r="G6" s="208" t="s">
         <v>521</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="H6" s="30" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
       <c r="B7" s="36">
@@ -8289,8 +8406,10 @@
       <c r="F7" s="112" t="s">
         <v>520</v>
       </c>
-      <c r="G7" s="208"/>
-      <c r="H7" s="30"/>
+      <c r="G7" s="209"/>
+      <c r="H7" s="30" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
       <c r="B8" s="36">
@@ -8313,13 +8432,13 @@
       <c r="D9" s="168" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="204" t="s">
+      <c r="E9" s="205" t="s">
         <v>469</v>
       </c>
       <c r="F9" s="112" t="s">
         <v>524</v>
       </c>
-      <c r="G9" s="244" t="s">
+      <c r="G9" s="173" t="s">
         <v>522</v>
       </c>
       <c r="H9" s="82"/>
@@ -8334,12 +8453,14 @@
       <c r="D10" s="110" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="205"/>
+      <c r="E10" s="206"/>
       <c r="F10" s="112"/>
-      <c r="G10" s="244" t="s">
+      <c r="G10" s="173" t="s">
         <v>525</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="H10" s="30" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
       <c r="B11" s="36">
@@ -8351,9 +8472,9 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="205"/>
+      <c r="E11" s="206"/>
       <c r="F11" s="112"/>
-      <c r="G11" s="244" t="s">
+      <c r="G11" s="173" t="s">
         <v>526</v>
       </c>
       <c r="H11" s="30"/>
@@ -8366,9 +8487,9 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="206"/>
+      <c r="E12" s="207"/>
       <c r="F12" s="112"/>
-      <c r="G12" s="244"/>
+      <c r="G12" s="173"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
@@ -8378,12 +8499,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8731,15 +8852,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8858,11 +8979,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="175" t="s">
+      <c r="E13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8906,14 +9027,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -9021,10 +9142,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="175" t="s">
+      <c r="E13" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="177"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -9067,15 +9188,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -9195,10 +9316,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="209" t="s">
+      <c r="F13" s="210" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="210"/>
+      <c r="G13" s="211"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9242,13 +9363,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -9372,7 +9493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -9384,35 +9505,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="224" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="223"/>
-      <c r="C3" s="224" t="s">
+      <c r="B3" s="224"/>
+      <c r="C3" s="225" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="225"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="225"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="223"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
+      <c r="B4" s="224"/>
+      <c r="C4" s="225"/>
+      <c r="D4" s="225"/>
+      <c r="E4" s="225"/>
+      <c r="F4" s="225"/>
+      <c r="G4" s="225"/>
+      <c r="H4" s="225"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9631,42 +9752,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="225" t="s">
+      <c r="C23" s="226" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="226"/>
-      <c r="E23" s="226"/>
-      <c r="F23" s="226"/>
-      <c r="G23" s="227"/>
+      <c r="D23" s="227"/>
+      <c r="E23" s="227"/>
+      <c r="F23" s="227"/>
+      <c r="G23" s="228"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="217"/>
-      <c r="D24" s="218"/>
-      <c r="E24" s="218"/>
-      <c r="F24" s="218"/>
-      <c r="G24" s="219"/>
+      <c r="C24" s="218"/>
+      <c r="D24" s="219"/>
+      <c r="E24" s="219"/>
+      <c r="F24" s="219"/>
+      <c r="G24" s="220"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="217" t="s">
+      <c r="C25" s="218" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="218"/>
-      <c r="E25" s="218"/>
-      <c r="F25" s="218"/>
-      <c r="G25" s="219"/>
+      <c r="D25" s="219"/>
+      <c r="E25" s="219"/>
+      <c r="F25" s="219"/>
+      <c r="G25" s="220"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="220"/>
-      <c r="D26" s="221"/>
-      <c r="E26" s="221"/>
-      <c r="F26" s="221"/>
-      <c r="G26" s="222"/>
+      <c r="C26" s="221"/>
+      <c r="D26" s="222"/>
+      <c r="E26" s="222"/>
+      <c r="F26" s="222"/>
+      <c r="G26" s="223"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9694,42 +9815,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="211" t="s">
+      <c r="C28" s="212" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="212"/>
-      <c r="E28" s="212"/>
-      <c r="F28" s="212"/>
-      <c r="G28" s="213"/>
+      <c r="D28" s="213"/>
+      <c r="E28" s="213"/>
+      <c r="F28" s="213"/>
+      <c r="G28" s="214"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="211"/>
-      <c r="D29" s="212"/>
-      <c r="E29" s="212"/>
-      <c r="F29" s="212"/>
-      <c r="G29" s="213"/>
+      <c r="C29" s="212"/>
+      <c r="D29" s="213"/>
+      <c r="E29" s="213"/>
+      <c r="F29" s="213"/>
+      <c r="G29" s="214"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="211" t="s">
+      <c r="C30" s="212" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="212"/>
-      <c r="E30" s="212"/>
-      <c r="F30" s="212"/>
-      <c r="G30" s="213"/>
+      <c r="D30" s="213"/>
+      <c r="E30" s="213"/>
+      <c r="F30" s="213"/>
+      <c r="G30" s="214"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="214"/>
-      <c r="D31" s="215"/>
-      <c r="E31" s="215"/>
-      <c r="F31" s="215"/>
-      <c r="G31" s="216"/>
+      <c r="C31" s="215"/>
+      <c r="D31" s="216"/>
+      <c r="E31" s="216"/>
+      <c r="F31" s="216"/>
+      <c r="G31" s="217"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -9752,8 +9873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9764,35 +9885,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="223"/>
-      <c r="C3" s="224" t="s">
+      <c r="B3" s="224"/>
+      <c r="C3" s="225" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="225"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="225"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="223"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
+      <c r="B4" s="224"/>
+      <c r="C4" s="225"/>
+      <c r="D4" s="225"/>
+      <c r="E4" s="225"/>
+      <c r="F4" s="225"/>
+      <c r="G4" s="225"/>
+      <c r="H4" s="225"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9848,13 +9969,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="228" t="s">
+      <c r="C8" s="229" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="229"/>
-      <c r="E8" s="229"/>
-      <c r="F8" s="229"/>
-      <c r="G8" s="230"/>
+      <c r="D8" s="230"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="230"/>
+      <c r="G8" s="231"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9864,20 +9985,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="231"/>
-      <c r="D9" s="232"/>
-      <c r="E9" s="232"/>
-      <c r="F9" s="232"/>
-      <c r="G9" s="233"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="233"/>
+      <c r="E9" s="233"/>
+      <c r="F9" s="233"/>
+      <c r="G9" s="234"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="231"/>
-      <c r="D10" s="232"/>
-      <c r="E10" s="232"/>
-      <c r="F10" s="232"/>
-      <c r="G10" s="233"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="233"/>
+      <c r="E10" s="233"/>
+      <c r="F10" s="233"/>
+      <c r="G10" s="234"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -9888,11 +10009,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="234"/>
-      <c r="D11" s="235"/>
-      <c r="E11" s="235"/>
-      <c r="F11" s="235"/>
-      <c r="G11" s="236"/>
+      <c r="C11" s="235"/>
+      <c r="D11" s="236"/>
+      <c r="E11" s="236"/>
+      <c r="F11" s="236"/>
+      <c r="G11" s="237"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>
@@ -9929,10 +10050,12 @@
       <c r="C13" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="D13" s="246" t="s">
+        <v>542</v>
+      </c>
+      <c r="E13" s="245"/>
+      <c r="F13" s="245"/>
+      <c r="G13" s="247"/>
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
@@ -9943,10 +10066,10 @@
     <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="D14" s="246"/>
+      <c r="E14" s="245"/>
+      <c r="F14" s="245"/>
+      <c r="G14" s="247"/>
       <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
@@ -9957,10 +10080,10 @@
     <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="61"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="D15" s="246"/>
+      <c r="E15" s="245"/>
+      <c r="F15" s="245"/>
+      <c r="G15" s="247"/>
       <c r="H15" s="24"/>
       <c r="J15" s="1">
         <v>6827</v>
@@ -9969,10 +10092,10 @@
     <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="63"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="D16" s="248"/>
+      <c r="E16" s="249"/>
+      <c r="F16" s="249"/>
+      <c r="G16" s="250"/>
       <c r="H16" s="25"/>
       <c r="J16" s="1">
         <v>0</v>
@@ -10183,7 +10306,8 @@
       <c r="H31" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="D13:G16"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>

</xml_diff>

<commit_message>
23-01-10 4주 1일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39E2B44-D58C-4F89-8C0E-D94E3C19E7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8E99CD-A91A-445A-8E6D-F0AFC2C6C1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="551">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2003,6 +2003,32 @@
   <si>
     <t>조 멘토링</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아키텍쳐 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분업 분담 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코카제로, 스프제로, 원에이엠, 부르르제로사이다, 부르르제로콜라</t>
+  </si>
+  <si>
+    <t>라인바사, 미네마인, 빅토리아, 씨그램, 트레비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리 - 사전정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나랑드사이다, 펩시제로, 칠성제로, 웰치스제로, 이마트노브랜드</t>
   </si>
 </sst>
 </file>
@@ -2856,7 +2882,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3544,6 +3570,24 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3592,23 +3636,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4341,8 +4376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDE6C63-9121-4583-87EA-DA9F0C78BEC1}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -4924,9 +4959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5038,7 +5073,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="238" t="s">
+      <c r="A2" s="244" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -5056,7 +5091,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="242" t="s">
+      <c r="G2" s="248" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -5083,9 +5118,12 @@
         <v>518</v>
       </c>
       <c r="Q2" s="100"/>
+      <c r="R2" s="86" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="238"/>
+      <c r="A3" s="244"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -5099,7 +5137,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="242"/>
+      <c r="G3" s="248"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -5117,9 +5155,10 @@
         <v>428</v>
       </c>
       <c r="Q3" s="100"/>
+      <c r="R3" s="253"/>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="238"/>
+      <c r="A4" s="244"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -5131,7 +5170,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="242"/>
+      <c r="G4" s="248"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -5151,9 +5190,12 @@
       <c r="Q4" s="100" t="s">
         <v>530</v>
       </c>
+      <c r="R4" s="86" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="238"/>
+      <c r="A5" s="244"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -5167,7 +5209,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="242"/>
+      <c r="G5" s="248"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -5184,7 +5226,7 @@
       <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="238"/>
+      <c r="A6" s="244"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -5200,7 +5242,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="242"/>
+      <c r="G6" s="248"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -5214,7 +5256,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="239" t="s">
+      <c r="A7" s="245" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -5230,7 +5272,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="242"/>
+      <c r="G7" s="248"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -5259,9 +5301,12 @@
         <v>527</v>
       </c>
       <c r="Q7" s="100"/>
+      <c r="R7" s="87" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="239"/>
+      <c r="A8" s="245"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -5273,7 +5318,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="242"/>
+      <c r="G8" s="248"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -5297,7 +5342,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="239"/>
+      <c r="A9" s="245"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -5309,7 +5354,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="242"/>
+      <c r="G9" s="248"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -5326,9 +5371,12 @@
       <c r="Q9" s="100" t="s">
         <v>537</v>
       </c>
+      <c r="R9" s="87" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="239"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -5340,7 +5388,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="242"/>
+      <c r="G10" s="248"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -5354,7 +5402,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="239"/>
+      <c r="A11" s="245"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5366,7 +5414,7 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="242"/>
+      <c r="G11" s="248"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
       <c r="M11" t="s">
@@ -5375,7 +5423,7 @@
       <c r="Q11" s="100"/>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="240" t="s">
+      <c r="A12" s="246" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5389,7 +5437,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="242"/>
+      <c r="G12" s="248"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5404,14 +5452,14 @@
       <c r="Q12" s="100"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="240"/>
+      <c r="A13" s="246"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="242"/>
+      <c r="G13" s="248"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5425,12 +5473,12 @@
       <c r="Q13" s="100"/>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="240"/>
+      <c r="A14" s="246"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="242"/>
+      <c r="G14" s="248"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
@@ -5441,14 +5489,14 @@
       <c r="Q14" s="100"/>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="240"/>
+      <c r="A15" s="246"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="242"/>
+      <c r="G15" s="248"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
@@ -5457,14 +5505,14 @@
       <c r="Q15" s="100"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="240"/>
+      <c r="A16" s="246"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="242"/>
+      <c r="G16" s="248"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
@@ -5472,8 +5520,8 @@
       <c r="M16"/>
       <c r="Q16" s="100"/>
     </row>
-    <row r="17" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="241" t="s">
+    <row r="17" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="247" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5481,7 +5529,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="242"/>
+      <c r="G17" s="248"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5508,15 +5556,18 @@
       <c r="Q17" s="100" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="241"/>
+      <c r="R17" s="89" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="247"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="242"/>
+      <c r="G18" s="248"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
@@ -5529,29 +5580,32 @@
         <v>539</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="241"/>
+    <row r="19" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="247"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="242"/>
+      <c r="G19" s="248"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
       <c r="M19" t="s">
         <v>439</v>
       </c>
       <c r="Q19" s="100"/>
-    </row>
-    <row r="20" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="241"/>
+      <c r="R19" s="89" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="247"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="242"/>
+      <c r="G20" s="248"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
       <c r="M20" t="s">
@@ -5561,14 +5615,14 @@
         <v>540</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="241"/>
+    <row r="21" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="247"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="242"/>
+      <c r="G21" s="248"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
       <c r="M21" t="s">
@@ -5576,7 +5630,7 @@
       </c>
       <c r="Q21" s="100"/>
     </row>
-    <row r="22" spans="1:17" s="100" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:18" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
       <c r="M22" t="s">
         <v>442</v>
@@ -5585,7 +5639,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:18" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5632,7 +5686,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="30" customHeight="1">
+    <row r="24" spans="1:18" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5673,7 +5727,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="30" customHeight="1">
+    <row r="25" spans="1:18" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5708,7 +5762,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="30" customHeight="1">
+    <row r="26" spans="1:18" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5734,7 +5788,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="30" customHeight="1">
+    <row r="27" spans="1:18" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5763,7 +5817,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="30" customHeight="1">
+    <row r="28" spans="1:18" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5783,7 +5837,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="30" customHeight="1">
+    <row r="29" spans="1:18" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5809,7 +5863,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="30" customHeight="1">
+    <row r="30" spans="1:18" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5826,7 +5880,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="30" customHeight="1">
+    <row r="31" spans="1:18" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5840,7 +5894,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="30" customHeight="1">
+    <row r="32" spans="1:18" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -7263,7 +7317,7 @@
       <selection activeCell="H27" sqref="H27"/>
       <selection pane="topRight" activeCell="H27" sqref="H27"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -7315,22 +7369,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="243" t="s">
+      <c r="C2" s="249" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243" t="s">
+      <c r="D2" s="249"/>
+      <c r="E2" s="249" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243" t="s">
+      <c r="F2" s="249"/>
+      <c r="G2" s="249" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="243"/>
-      <c r="I2" s="243" t="s">
+      <c r="H2" s="249"/>
+      <c r="I2" s="249" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="244"/>
+      <c r="J2" s="250"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -8303,8 +8357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8840,8 +8894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8888,10 +8942,18 @@
         <v>0.375</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="D5" s="110" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="110" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="110" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="110" t="s">
+        <v>143</v>
+      </c>
       <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
@@ -8899,7 +8961,9 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="31"/>
+      <c r="D6" s="32" t="s">
+        <v>544</v>
+      </c>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
@@ -8910,7 +8974,9 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="31"/>
+      <c r="D7" s="32" t="s">
+        <v>545</v>
+      </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
@@ -8921,18 +8987,20 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="30"/>
+      <c r="D8" s="252"/>
+      <c r="E8" s="251"/>
+      <c r="F8" s="251"/>
+      <c r="G8" s="251"/>
+      <c r="H8" s="252"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="31"/>
+      <c r="D9" s="192" t="s">
+        <v>546</v>
+      </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
@@ -8943,7 +9011,7 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="31"/>
+      <c r="D10" s="193"/>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
@@ -8954,7 +9022,7 @@
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="31"/>
+      <c r="D11" s="193"/>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
@@ -8965,7 +9033,7 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="78"/>
+      <c r="D12" s="194"/>
       <c r="E12" s="78"/>
       <c r="F12" s="78"/>
       <c r="G12" s="78"/>
@@ -9000,9 +9068,10 @@
       <c r="H14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E13:G13"/>
+    <mergeCell ref="D9:D12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9969,13 +10038,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="229" t="s">
+      <c r="C8" s="235" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
-      <c r="G8" s="231"/>
+      <c r="D8" s="236"/>
+      <c r="E8" s="236"/>
+      <c r="F8" s="236"/>
+      <c r="G8" s="237"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -9985,20 +10054,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="232"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
-      <c r="G9" s="234"/>
+      <c r="C9" s="238"/>
+      <c r="D9" s="239"/>
+      <c r="E9" s="239"/>
+      <c r="F9" s="239"/>
+      <c r="G9" s="240"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="232"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="233"/>
-      <c r="F10" s="233"/>
-      <c r="G10" s="234"/>
+      <c r="C10" s="238"/>
+      <c r="D10" s="239"/>
+      <c r="E10" s="239"/>
+      <c r="F10" s="239"/>
+      <c r="G10" s="240"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -10009,11 +10078,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="235"/>
-      <c r="D11" s="236"/>
-      <c r="E11" s="236"/>
-      <c r="F11" s="236"/>
-      <c r="G11" s="237"/>
+      <c r="C11" s="241"/>
+      <c r="D11" s="242"/>
+      <c r="E11" s="242"/>
+      <c r="F11" s="242"/>
+      <c r="G11" s="243"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>
@@ -10050,12 +10119,12 @@
       <c r="C13" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="246" t="s">
+      <c r="D13" s="229" t="s">
         <v>542</v>
       </c>
-      <c r="E13" s="245"/>
-      <c r="F13" s="245"/>
-      <c r="G13" s="247"/>
+      <c r="E13" s="230"/>
+      <c r="F13" s="230"/>
+      <c r="G13" s="231"/>
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
@@ -10066,10 +10135,10 @@
     <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
-      <c r="D14" s="246"/>
-      <c r="E14" s="245"/>
-      <c r="F14" s="245"/>
-      <c r="G14" s="247"/>
+      <c r="D14" s="229"/>
+      <c r="E14" s="230"/>
+      <c r="F14" s="230"/>
+      <c r="G14" s="231"/>
       <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
@@ -10080,10 +10149,10 @@
     <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="61"/>
-      <c r="D15" s="246"/>
-      <c r="E15" s="245"/>
-      <c r="F15" s="245"/>
-      <c r="G15" s="247"/>
+      <c r="D15" s="229"/>
+      <c r="E15" s="230"/>
+      <c r="F15" s="230"/>
+      <c r="G15" s="231"/>
       <c r="H15" s="24"/>
       <c r="J15" s="1">
         <v>6827</v>
@@ -10092,10 +10161,10 @@
     <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="63"/>
-      <c r="D16" s="248"/>
-      <c r="E16" s="249"/>
-      <c r="F16" s="249"/>
-      <c r="G16" s="250"/>
+      <c r="D16" s="232"/>
+      <c r="E16" s="233"/>
+      <c r="F16" s="233"/>
+      <c r="G16" s="234"/>
       <c r="H16" s="25"/>
       <c r="J16" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
23-01-10 4주 2일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8E99CD-A91A-445A-8E6D-F0AFC2C6C1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459024A6-8972-4DF4-A1F0-03EBF97BEB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="561">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2029,6 +2029,46 @@
   </si>
   <si>
     <t>나랑드사이다, 펩시제로, 칠성제로, 웰치스제로, 이마트노브랜드</t>
+  </si>
+  <si>
+    <t>사전작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아키텍쳐 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강사님께 조언 받기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 자료 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리 시각화 관련자료 수집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정확히 어떤 그래프를 만들지 결론을 내고싶다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Django에서 구현하는 방법을 알아야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부트스트랩을 찾자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WBS 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이차트 거리 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2882,7 +2922,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3405,6 +3445,15 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3636,14 +3685,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4388,14 +4431,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="95"/>
@@ -4419,12 +4462,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="190" t="s">
+      <c r="C5" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
       <c r="G5" s="111" t="s">
         <v>108</v>
       </c>
@@ -4439,7 +4482,7 @@
       <c r="D6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="185" t="s">
+      <c r="E6" s="188" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4457,7 +4500,7 @@
       <c r="D7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="186"/>
+      <c r="E7" s="189"/>
       <c r="F7" s="110" t="s">
         <v>107</v>
       </c>
@@ -4479,19 +4522,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="185" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="182" t="s">
+      <c r="E9" s="185" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="187" t="s">
+      <c r="F9" s="190" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="195" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4499,21 +4542,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="188"/>
-      <c r="G10" s="193"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="186"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="196"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="181"/>
-      <c r="D11" s="184"/>
-      <c r="E11" s="183"/>
-      <c r="F11" s="188"/>
-      <c r="G11" s="193"/>
+      <c r="C11" s="184"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="186"/>
+      <c r="F11" s="191"/>
+      <c r="G11" s="196"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4523,9 +4566,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="189"/>
-      <c r="G12" s="194"/>
+      <c r="E12" s="187"/>
+      <c r="F12" s="192"/>
+      <c r="G12" s="197"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4534,11 +4577,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="179" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="178"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="181"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4606,35 +4649,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="224"/>
-      <c r="C3" s="225" t="s">
+      <c r="B3" s="227"/>
+      <c r="C3" s="228" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="225"/>
-      <c r="E3" s="225"/>
-      <c r="F3" s="225"/>
-      <c r="G3" s="225"/>
-      <c r="H3" s="225"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="224"/>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
+      <c r="B4" s="227"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
+      <c r="E4" s="228"/>
+      <c r="F4" s="228"/>
+      <c r="G4" s="228"/>
+      <c r="H4" s="228"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -4959,9 +5002,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5073,7 +5116,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="244" t="s">
+      <c r="A2" s="247" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -5091,7 +5134,7 @@
       <c r="F2" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="248" t="s">
+      <c r="G2" s="251" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="100"/>
@@ -5121,9 +5164,12 @@
       <c r="R2" s="86" t="s">
         <v>549</v>
       </c>
+      <c r="S2" s="254" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="244"/>
+      <c r="A3" s="247"/>
       <c r="B3" s="100" t="s">
         <v>43</v>
       </c>
@@ -5137,7 +5183,7 @@
       <c r="F3" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="248"/>
+      <c r="G3" s="251"/>
       <c r="H3" s="100"/>
       <c r="I3" s="113" t="s">
         <v>164</v>
@@ -5155,10 +5201,11 @@
         <v>428</v>
       </c>
       <c r="Q3" s="100"/>
-      <c r="R3" s="253"/>
+      <c r="R3" s="176"/>
+      <c r="S3" s="254"/>
     </row>
     <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="244"/>
+      <c r="A4" s="247"/>
       <c r="B4" s="102" t="s">
         <v>44</v>
       </c>
@@ -5170,7 +5217,7 @@
       <c r="F4" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="248"/>
+      <c r="G4" s="251"/>
       <c r="H4" s="100"/>
       <c r="I4" s="100" t="s">
         <v>165</v>
@@ -5193,9 +5240,10 @@
       <c r="R4" s="86" t="s">
         <v>547</v>
       </c>
+      <c r="S4" s="254"/>
     </row>
     <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="244"/>
+      <c r="A5" s="247"/>
       <c r="B5" s="102" t="s">
         <v>45</v>
       </c>
@@ -5209,7 +5257,7 @@
       <c r="F5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="248"/>
+      <c r="G5" s="251"/>
       <c r="H5" s="100"/>
       <c r="I5" s="100" t="s">
         <v>166</v>
@@ -5224,9 +5272,10 @@
         <v>430</v>
       </c>
       <c r="Q5" s="100"/>
+      <c r="S5" s="254"/>
     </row>
     <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="244"/>
+      <c r="A6" s="247"/>
       <c r="B6" s="100" t="s">
         <v>46</v>
       </c>
@@ -5242,7 +5291,7 @@
       <c r="F6" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="248"/>
+      <c r="G6" s="251"/>
       <c r="H6" s="100"/>
       <c r="I6" s="100" t="s">
         <v>168</v>
@@ -5254,9 +5303,10 @@
       <c r="Q6" s="100" t="s">
         <v>535</v>
       </c>
+      <c r="S6" s="254"/>
     </row>
     <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="245" t="s">
+      <c r="A7" s="248" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="100" t="s">
@@ -5272,7 +5322,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="100"/>
-      <c r="G7" s="248"/>
+      <c r="G7" s="251"/>
       <c r="H7" s="100" t="s">
         <v>150</v>
       </c>
@@ -5304,9 +5354,10 @@
       <c r="R7" s="87" t="s">
         <v>549</v>
       </c>
+      <c r="S7" s="254"/>
     </row>
     <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="245"/>
+      <c r="A8" s="248"/>
       <c r="B8" s="100" t="s">
         <v>48</v>
       </c>
@@ -5318,7 +5369,7 @@
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="248"/>
+      <c r="G8" s="251"/>
       <c r="H8" s="100" t="s">
         <v>151</v>
       </c>
@@ -5340,9 +5391,10 @@
       <c r="Q8" s="100" t="s">
         <v>536</v>
       </c>
+      <c r="S8" s="254"/>
     </row>
     <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="245"/>
+      <c r="A9" s="248"/>
       <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
@@ -5354,7 +5406,7 @@
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
-      <c r="G9" s="248"/>
+      <c r="G9" s="251"/>
       <c r="H9" s="100" t="s">
         <v>152</v>
       </c>
@@ -5374,9 +5426,10 @@
       <c r="R9" s="87" t="s">
         <v>550</v>
       </c>
+      <c r="S9" s="254"/>
     </row>
     <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="245"/>
+      <c r="A10" s="248"/>
       <c r="B10" s="102" t="s">
         <v>74</v>
       </c>
@@ -5388,7 +5441,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="100"/>
-      <c r="G10" s="248"/>
+      <c r="G10" s="251"/>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
       <c r="K10" s="87" t="s">
@@ -5400,9 +5453,10 @@
       <c r="Q10" s="100" t="s">
         <v>538</v>
       </c>
+      <c r="S10" s="254"/>
     </row>
     <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="245"/>
+      <c r="A11" s="248"/>
       <c r="B11" s="102" t="s">
         <v>75</v>
       </c>
@@ -5414,16 +5468,17 @@
         <v>118</v>
       </c>
       <c r="F11" s="100"/>
-      <c r="G11" s="248"/>
+      <c r="G11" s="251"/>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
       <c r="M11" t="s">
         <v>436</v>
       </c>
       <c r="Q11" s="100"/>
+      <c r="S11" s="254"/>
     </row>
     <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="246" t="s">
+      <c r="A12" s="249" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="103" t="s">
@@ -5437,7 +5492,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="100"/>
-      <c r="G12" s="248"/>
+      <c r="G12" s="251"/>
       <c r="H12" s="100" t="s">
         <v>153</v>
       </c>
@@ -5450,16 +5505,17 @@
       </c>
       <c r="M12"/>
       <c r="Q12" s="100"/>
+      <c r="S12" s="254"/>
     </row>
     <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="246"/>
+      <c r="A13" s="249"/>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
       <c r="E13" s="100" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="100"/>
-      <c r="G13" s="248"/>
+      <c r="G13" s="251"/>
       <c r="H13" s="100" t="s">
         <v>154</v>
       </c>
@@ -5471,14 +5527,15 @@
         <v>437</v>
       </c>
       <c r="Q13" s="100"/>
+      <c r="S13" s="254"/>
     </row>
     <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="246"/>
+      <c r="A14" s="249"/>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="248"/>
+      <c r="G14" s="251"/>
       <c r="H14" s="100" t="s">
         <v>155</v>
       </c>
@@ -5487,41 +5544,44 @@
         <v>438</v>
       </c>
       <c r="Q14" s="100"/>
+      <c r="S14" s="254"/>
     </row>
     <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="246"/>
+      <c r="A15" s="249"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="100"/>
-      <c r="G15" s="248"/>
+      <c r="G15" s="251"/>
       <c r="H15" s="100" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="100"/>
       <c r="M15"/>
       <c r="Q15" s="100"/>
+      <c r="S15" s="254"/>
     </row>
     <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="246"/>
+      <c r="A16" s="249"/>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
       <c r="E16" s="100" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="100"/>
-      <c r="G16" s="248"/>
+      <c r="G16" s="251"/>
       <c r="H16" s="100" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="100"/>
       <c r="M16"/>
       <c r="Q16" s="100"/>
-    </row>
-    <row r="17" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="247" t="s">
+      <c r="S16" s="254"/>
+    </row>
+    <row r="17" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="250" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="100"/>
@@ -5529,7 +5589,7 @@
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
       <c r="F17" s="100"/>
-      <c r="G17" s="248"/>
+      <c r="G17" s="251"/>
       <c r="H17" s="100"/>
       <c r="I17" s="100"/>
       <c r="J17" s="89" t="s">
@@ -5559,15 +5619,16 @@
       <c r="R17" s="89" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="247"/>
+      <c r="S17" s="254"/>
+    </row>
+    <row r="18" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="250"/>
       <c r="B18" s="100"/>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
-      <c r="G18" s="248"/>
+      <c r="G18" s="251"/>
       <c r="H18" s="100"/>
       <c r="I18" s="100"/>
       <c r="L18" s="89" t="s">
@@ -5579,15 +5640,16 @@
       <c r="Q18" s="100" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="247"/>
+      <c r="S18" s="254"/>
+    </row>
+    <row r="19" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="250"/>
       <c r="B19" s="100"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="248"/>
+      <c r="G19" s="251"/>
       <c r="H19" s="100"/>
       <c r="I19" s="100"/>
       <c r="M19" t="s">
@@ -5597,15 +5659,16 @@
       <c r="R19" s="89" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="247"/>
+      <c r="S19" s="254"/>
+    </row>
+    <row r="20" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="250"/>
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
       <c r="E20" s="100"/>
       <c r="F20" s="100"/>
-      <c r="G20" s="248"/>
+      <c r="G20" s="251"/>
       <c r="H20" s="100"/>
       <c r="I20" s="100"/>
       <c r="M20" t="s">
@@ -5614,23 +5677,25 @@
       <c r="Q20" s="100" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" s="89" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="247"/>
+      <c r="S20" s="254"/>
+    </row>
+    <row r="21" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="250"/>
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
-      <c r="G21" s="248"/>
+      <c r="G21" s="251"/>
       <c r="H21" s="100"/>
       <c r="I21" s="100"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
       <c r="Q21" s="100"/>
-    </row>
-    <row r="22" spans="1:18" s="100" customFormat="1" ht="30" customHeight="1">
+      <c r="S21" s="254"/>
+    </row>
+    <row r="22" spans="1:19" s="100" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="107"/>
       <c r="M22" t="s">
         <v>442</v>
@@ -5639,7 +5704,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="109" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:19" s="109" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="108" t="s">
         <v>68</v>
       </c>
@@ -5685,8 +5750,11 @@
       <c r="Q23" s="100" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="30" customHeight="1">
+      <c r="S23" s="108" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5726,8 +5794,11 @@
       <c r="Q24" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="30" customHeight="1">
+      <c r="S24" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5761,8 +5832,11 @@
       <c r="Q25" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="30" customHeight="1">
+      <c r="S25" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5787,8 +5861,11 @@
       <c r="Q26" s="100" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="30" customHeight="1">
+      <c r="S26" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5816,8 +5893,11 @@
       <c r="M27" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="30" customHeight="1">
+      <c r="S27" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5836,8 +5916,11 @@
       <c r="L28" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="30" customHeight="1">
+      <c r="S28" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5863,7 +5946,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="30" customHeight="1">
+    <row r="30" spans="1:19" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5880,7 +5963,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="30" customHeight="1">
+    <row r="31" spans="1:19" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5894,7 +5977,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="30" customHeight="1">
+    <row r="32" spans="1:19" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -6458,7 +6541,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="S2:S21"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A16"/>
@@ -7369,22 +7453,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="157"/>
-      <c r="C2" s="249" t="s">
+      <c r="C2" s="252" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249" t="s">
+      <c r="D2" s="252"/>
+      <c r="E2" s="252" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="249"/>
-      <c r="G2" s="249" t="s">
+      <c r="F2" s="252"/>
+      <c r="G2" s="252" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="249"/>
-      <c r="I2" s="249" t="s">
+      <c r="H2" s="252"/>
+      <c r="I2" s="252" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="250"/>
+      <c r="J2" s="253"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -8163,14 +8247,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -8214,19 +8298,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="195" t="s">
+      <c r="C6" s="198" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="182" t="s">
+      <c r="D6" s="185" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="200" t="s">
+      <c r="E6" s="203" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="203" t="s">
+      <c r="G6" s="206" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8234,13 +8318,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="196"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="201"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="187"/>
+      <c r="E7" s="204"/>
       <c r="F7" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="204"/>
+      <c r="G7" s="207"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="97">
@@ -8256,13 +8340,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="197" t="s">
+      <c r="C9" s="200" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="185" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="200"/>
+      <c r="E9" s="203"/>
       <c r="F9" s="114" t="s">
         <v>247</v>
       </c>
@@ -8274,9 +8358,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="198"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="202"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="205"/>
       <c r="F10" s="114" t="s">
         <v>246</v>
       </c>
@@ -8286,9 +8370,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="183"/>
-      <c r="E11" s="202"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="205"/>
       <c r="F11" s="114" t="s">
         <v>248</v>
       </c>
@@ -8301,8 +8385,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="201"/>
+      <c r="D12" s="187"/>
+      <c r="E12" s="204"/>
       <c r="F12" s="114" t="s">
         <v>249</v>
       </c>
@@ -8315,11 +8399,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="179" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
       <c r="G13" s="128" t="s">
         <v>30</v>
       </c>
@@ -8371,15 +8455,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -8439,7 +8523,7 @@
       <c r="F6" s="112" t="s">
         <v>523</v>
       </c>
-      <c r="G6" s="208" t="s">
+      <c r="G6" s="211" t="s">
         <v>521</v>
       </c>
       <c r="H6" s="30" t="s">
@@ -8460,7 +8544,7 @@
       <c r="F7" s="112" t="s">
         <v>520</v>
       </c>
-      <c r="G7" s="209"/>
+      <c r="G7" s="212"/>
       <c r="H7" s="30" t="s">
         <v>530</v>
       </c>
@@ -8486,7 +8570,7 @@
       <c r="D9" s="168" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="205" t="s">
+      <c r="E9" s="208" t="s">
         <v>469</v>
       </c>
       <c r="F9" s="112" t="s">
@@ -8507,7 +8591,7 @@
       <c r="D10" s="110" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="206"/>
+      <c r="E10" s="209"/>
       <c r="F10" s="112"/>
       <c r="G10" s="173" t="s">
         <v>525</v>
@@ -8526,7 +8610,7 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="206"/>
+      <c r="E11" s="209"/>
       <c r="F11" s="112"/>
       <c r="G11" s="173" t="s">
         <v>526</v>
@@ -8541,7 +8625,7 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="207"/>
+      <c r="E12" s="210"/>
       <c r="F12" s="112"/>
       <c r="G12" s="173"/>
       <c r="H12" s="30"/>
@@ -8553,12 +8637,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="176" t="s">
+      <c r="D13" s="179" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="181"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8894,8 +8978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8906,15 +8990,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -8964,7 +9048,9 @@
       <c r="D6" s="32" t="s">
         <v>544</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="32" t="s">
+        <v>551</v>
+      </c>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="30"/>
@@ -8977,7 +9063,9 @@
       <c r="D7" s="32" t="s">
         <v>545</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="32" t="s">
+        <v>552</v>
+      </c>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="30"/>
@@ -8987,21 +9075,23 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="252"/>
-      <c r="E8" s="251"/>
-      <c r="F8" s="251"/>
-      <c r="G8" s="251"/>
-      <c r="H8" s="252"/>
+      <c r="D8" s="175"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="175"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="195" t="s">
         <v>546</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="32" t="s">
+        <v>554</v>
+      </c>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="30"/>
@@ -9011,8 +9101,10 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="31"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="32" t="s">
+        <v>553</v>
+      </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="30"/>
@@ -9022,8 +9114,10 @@
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="31"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="195" t="s">
+        <v>554</v>
+      </c>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
       <c r="H11" s="30"/>
@@ -9033,8 +9127,8 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="78"/>
+      <c r="D12" s="197"/>
+      <c r="E12" s="197"/>
       <c r="F12" s="78"/>
       <c r="G12" s="78"/>
       <c r="H12" s="30"/>
@@ -9047,11 +9141,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="179" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="181"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9068,10 +9162,11 @@
       <c r="H14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9096,14 +9191,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -9211,10 +9306,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="179" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="178"/>
+      <c r="F13" s="181"/>
       <c r="G13" s="80" t="s">
         <v>30</v>
       </c>
@@ -9257,15 +9352,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -9385,10 +9480,10 @@
       <c r="E13" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="210" t="s">
+      <c r="F13" s="213" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="211"/>
+      <c r="G13" s="214"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9432,13 +9527,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="94"/>
@@ -9574,35 +9669,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="227" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="224"/>
-      <c r="C3" s="225" t="s">
+      <c r="B3" s="227"/>
+      <c r="C3" s="228" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="225"/>
-      <c r="E3" s="225"/>
-      <c r="F3" s="225"/>
-      <c r="G3" s="225"/>
-      <c r="H3" s="225"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="224"/>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
+      <c r="B4" s="227"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
+      <c r="E4" s="228"/>
+      <c r="F4" s="228"/>
+      <c r="G4" s="228"/>
+      <c r="H4" s="228"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9821,42 +9916,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="226" t="s">
+      <c r="C23" s="229" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="227"/>
-      <c r="E23" s="227"/>
-      <c r="F23" s="227"/>
-      <c r="G23" s="228"/>
+      <c r="D23" s="230"/>
+      <c r="E23" s="230"/>
+      <c r="F23" s="230"/>
+      <c r="G23" s="231"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="218"/>
-      <c r="D24" s="219"/>
-      <c r="E24" s="219"/>
-      <c r="F24" s="219"/>
-      <c r="G24" s="220"/>
+      <c r="C24" s="221"/>
+      <c r="D24" s="222"/>
+      <c r="E24" s="222"/>
+      <c r="F24" s="222"/>
+      <c r="G24" s="223"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="218" t="s">
+      <c r="C25" s="221" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="219"/>
-      <c r="E25" s="219"/>
-      <c r="F25" s="219"/>
-      <c r="G25" s="220"/>
+      <c r="D25" s="222"/>
+      <c r="E25" s="222"/>
+      <c r="F25" s="222"/>
+      <c r="G25" s="223"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="221"/>
-      <c r="D26" s="222"/>
-      <c r="E26" s="222"/>
-      <c r="F26" s="222"/>
-      <c r="G26" s="223"/>
+      <c r="C26" s="224"/>
+      <c r="D26" s="225"/>
+      <c r="E26" s="225"/>
+      <c r="F26" s="225"/>
+      <c r="G26" s="226"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9884,42 +9979,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="212" t="s">
+      <c r="C28" s="215" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="213"/>
-      <c r="E28" s="213"/>
-      <c r="F28" s="213"/>
-      <c r="G28" s="214"/>
+      <c r="D28" s="216"/>
+      <c r="E28" s="216"/>
+      <c r="F28" s="216"/>
+      <c r="G28" s="217"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="212"/>
-      <c r="D29" s="213"/>
-      <c r="E29" s="213"/>
-      <c r="F29" s="213"/>
-      <c r="G29" s="214"/>
+      <c r="C29" s="215"/>
+      <c r="D29" s="216"/>
+      <c r="E29" s="216"/>
+      <c r="F29" s="216"/>
+      <c r="G29" s="217"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="212" t="s">
+      <c r="C30" s="215" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="213"/>
-      <c r="E30" s="213"/>
-      <c r="F30" s="213"/>
-      <c r="G30" s="214"/>
+      <c r="D30" s="216"/>
+      <c r="E30" s="216"/>
+      <c r="F30" s="216"/>
+      <c r="G30" s="217"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="215"/>
-      <c r="D31" s="216"/>
-      <c r="E31" s="216"/>
-      <c r="F31" s="216"/>
-      <c r="G31" s="217"/>
+      <c r="C31" s="218"/>
+      <c r="D31" s="219"/>
+      <c r="E31" s="219"/>
+      <c r="F31" s="219"/>
+      <c r="G31" s="220"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -9942,8 +10037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9954,35 +10049,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="227" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="224"/>
-      <c r="C3" s="225" t="s">
+      <c r="B3" s="227"/>
+      <c r="C3" s="228" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="225"/>
-      <c r="E3" s="225"/>
-      <c r="F3" s="225"/>
-      <c r="G3" s="225"/>
-      <c r="H3" s="225"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="224"/>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
+      <c r="B4" s="227"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
+      <c r="E4" s="228"/>
+      <c r="F4" s="228"/>
+      <c r="G4" s="228"/>
+      <c r="H4" s="228"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -10038,13 +10133,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="235" t="s">
+      <c r="C8" s="238" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="236"/>
-      <c r="E8" s="236"/>
-      <c r="F8" s="236"/>
-      <c r="G8" s="237"/>
+      <c r="D8" s="239"/>
+      <c r="E8" s="239"/>
+      <c r="F8" s="239"/>
+      <c r="G8" s="240"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -10054,20 +10149,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="238"/>
-      <c r="D9" s="239"/>
-      <c r="E9" s="239"/>
-      <c r="F9" s="239"/>
-      <c r="G9" s="240"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="242"/>
+      <c r="E9" s="242"/>
+      <c r="F9" s="242"/>
+      <c r="G9" s="243"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="238"/>
-      <c r="D10" s="239"/>
-      <c r="E10" s="239"/>
-      <c r="F10" s="239"/>
-      <c r="G10" s="240"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="242"/>
+      <c r="E10" s="242"/>
+      <c r="F10" s="242"/>
+      <c r="G10" s="243"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -10078,11 +10173,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="241"/>
-      <c r="D11" s="242"/>
-      <c r="E11" s="242"/>
-      <c r="F11" s="242"/>
-      <c r="G11" s="243"/>
+      <c r="C11" s="244"/>
+      <c r="D11" s="245"/>
+      <c r="E11" s="245"/>
+      <c r="F11" s="245"/>
+      <c r="G11" s="246"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>
@@ -10119,12 +10214,12 @@
       <c r="C13" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="229" t="s">
+      <c r="D13" s="232" t="s">
         <v>542</v>
       </c>
-      <c r="E13" s="230"/>
-      <c r="F13" s="230"/>
-      <c r="G13" s="231"/>
+      <c r="E13" s="233"/>
+      <c r="F13" s="233"/>
+      <c r="G13" s="234"/>
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
@@ -10135,10 +10230,10 @@
     <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
-      <c r="D14" s="229"/>
-      <c r="E14" s="230"/>
-      <c r="F14" s="230"/>
-      <c r="G14" s="231"/>
+      <c r="D14" s="232"/>
+      <c r="E14" s="233"/>
+      <c r="F14" s="233"/>
+      <c r="G14" s="234"/>
       <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
@@ -10149,10 +10244,10 @@
     <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="61"/>
-      <c r="D15" s="229"/>
-      <c r="E15" s="230"/>
-      <c r="F15" s="230"/>
-      <c r="G15" s="231"/>
+      <c r="D15" s="232"/>
+      <c r="E15" s="233"/>
+      <c r="F15" s="233"/>
+      <c r="G15" s="234"/>
       <c r="H15" s="24"/>
       <c r="J15" s="1">
         <v>6827</v>
@@ -10161,10 +10256,10 @@
     <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="63"/>
-      <c r="D16" s="232"/>
-      <c r="E16" s="233"/>
-      <c r="F16" s="233"/>
-      <c r="G16" s="234"/>
+      <c r="D16" s="235"/>
+      <c r="E16" s="236"/>
+      <c r="F16" s="236"/>
+      <c r="G16" s="237"/>
       <c r="H16" s="25"/>
       <c r="J16" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
23-01-10 4주 3일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459024A6-8972-4DF4-A1F0-03EBF97BEB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B34C98-2C00-471B-B7FA-DA471E46B6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="2055" windowWidth="15165" windowHeight="10155" tabRatio="598" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="575">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2068,6 +2068,62 @@
   </si>
   <si>
     <t>하이차트 거리 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부트스트랩 찾기 시각화 적용 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부트스트랩 적용 시각화 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부트스트랩 - 페이지 완성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘토링 준비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>산출물 구글드라이브 업로드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 자료 (하이차트) 쟝고 연동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 자료 노드 상품별 수정할 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부트스트랩 연동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지 1 구안</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 사진 다운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지 2 구안 준비 완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조금 속도를 내자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wbs 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화면설계서</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2922,7 +2978,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3157,9 +3213,6 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3445,15 +3498,15 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3664,6 +3717,9 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3683,9 +3739,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4431,30 +4484,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="95"/>
-      <c r="C4" s="95" t="s">
+      <c r="B4" s="94"/>
+      <c r="C4" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="94" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4462,13 +4515,13 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="193" t="s">
+      <c r="C5" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="111" t="s">
+      <c r="D5" s="193"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="193"/>
+      <c r="G5" s="110" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4479,16 +4532,16 @@
       <c r="C6" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="188" t="s">
+      <c r="E6" s="187" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="112" t="s">
+      <c r="G6" s="111" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4496,45 +4549,45 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="104" t="s">
+      <c r="C7" s="95"/>
+      <c r="D7" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="189"/>
-      <c r="F7" s="110" t="s">
+      <c r="E7" s="188"/>
+      <c r="F7" s="109" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="112" t="s">
+      <c r="G7" s="111" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="101" customFormat="1" ht="50.1" customHeight="1">
-      <c r="B8" s="97">
+    <row r="8" spans="2:7" s="100" customFormat="1" ht="50.1" customHeight="1">
+      <c r="B8" s="96">
         <v>0.5</v>
       </c>
       <c r="C8" s="68"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="182" t="s">
+      <c r="C9" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="185" t="s">
+      <c r="D9" s="184" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="185" t="s">
+      <c r="E9" s="184" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="190" t="s">
+      <c r="F9" s="189" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="195" t="s">
+      <c r="G9" s="194" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4542,21 +4595,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="183"/>
-      <c r="D10" s="186"/>
-      <c r="E10" s="186"/>
-      <c r="F10" s="191"/>
-      <c r="G10" s="196"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="190"/>
+      <c r="G10" s="195"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="184"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="186"/>
-      <c r="F11" s="191"/>
-      <c r="G11" s="196"/>
+      <c r="C11" s="183"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="185"/>
+      <c r="F11" s="190"/>
+      <c r="G11" s="195"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4566,9 +4619,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="187"/>
-      <c r="F12" s="192"/>
-      <c r="G12" s="197"/>
+      <c r="E12" s="186"/>
+      <c r="F12" s="191"/>
+      <c r="G12" s="196"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4577,11 +4630,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="179" t="s">
+      <c r="D13" s="178" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="180"/>
-      <c r="F13" s="181"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="180"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4597,7 +4650,7 @@
       <c r="G14" s="30"/>
     </row>
     <row r="18" spans="3:4" ht="26.25">
-      <c r="C18" s="99" t="s">
+      <c r="C18" s="98" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -4605,12 +4658,12 @@
       </c>
     </row>
     <row r="19" spans="3:4" ht="26.25">
-      <c r="C19" s="99" t="s">
+      <c r="C19" s="98" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="26.25">
-      <c r="C20" s="99" t="s">
+      <c r="C20" s="98" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4637,7 +4690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -4649,35 +4702,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="227" t="s">
+      <c r="B2" s="226" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="227"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="227"/>
-      <c r="C3" s="228" t="s">
+      <c r="B3" s="226"/>
+      <c r="C3" s="227" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
-      <c r="H3" s="228"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="227"/>
+      <c r="G3" s="227"/>
+      <c r="H3" s="227"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="227"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
-      <c r="E4" s="228"/>
-      <c r="F4" s="228"/>
-      <c r="G4" s="228"/>
-      <c r="H4" s="228"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="227"/>
+      <c r="D4" s="227"/>
+      <c r="E4" s="227"/>
+      <c r="F4" s="227"/>
+      <c r="G4" s="227"/>
+      <c r="H4" s="227"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -5003,8 +5056,8 @@
   <dimension ref="A1:AF181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S29" sqref="S29"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5018,743 +5071,768 @@
     <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="115.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
-      <c r="B1" s="83">
+      <c r="B1" s="82">
         <v>44914</v>
       </c>
-      <c r="C1" s="83">
+      <c r="C1" s="82">
         <v>44915</v>
       </c>
-      <c r="D1" s="83">
+      <c r="D1" s="82">
         <v>44916</v>
       </c>
-      <c r="E1" s="83">
+      <c r="E1" s="82">
         <v>44917</v>
       </c>
-      <c r="F1" s="83">
+      <c r="F1" s="82">
         <v>44918</v>
       </c>
-      <c r="G1" s="83">
+      <c r="G1" s="82">
         <v>44921</v>
       </c>
-      <c r="H1" s="83">
+      <c r="H1" s="82">
         <v>44922</v>
       </c>
-      <c r="I1" s="83">
+      <c r="I1" s="82">
         <v>44923</v>
       </c>
-      <c r="J1" s="83">
+      <c r="J1" s="82">
         <v>44924</v>
       </c>
-      <c r="K1" s="83">
+      <c r="K1" s="82">
         <v>44925</v>
       </c>
-      <c r="L1" s="83">
+      <c r="L1" s="82">
         <v>44928</v>
       </c>
-      <c r="M1" s="83">
+      <c r="M1" s="82">
         <v>44929</v>
       </c>
-      <c r="N1" s="83">
+      <c r="N1" s="82">
         <v>44930</v>
       </c>
-      <c r="O1" s="83">
+      <c r="O1" s="82">
         <v>44931</v>
       </c>
-      <c r="P1" s="83">
+      <c r="P1" s="82">
         <v>44932</v>
       </c>
-      <c r="Q1" s="83">
+      <c r="Q1" s="82">
         <v>44933</v>
       </c>
-      <c r="R1" s="83">
+      <c r="R1" s="82">
         <v>44936</v>
       </c>
-      <c r="S1" s="83">
+      <c r="S1" s="82">
         <v>44937</v>
       </c>
-      <c r="T1" s="83">
+      <c r="T1" s="82">
         <v>44938</v>
       </c>
-      <c r="U1" s="83">
+      <c r="U1" s="82">
         <v>44939</v>
       </c>
-      <c r="V1" s="83">
+      <c r="V1" s="82">
         <v>44940</v>
       </c>
-      <c r="W1" s="83">
+      <c r="W1" s="82">
         <v>44943</v>
       </c>
-      <c r="X1" s="83">
+      <c r="X1" s="82">
         <v>44944</v>
       </c>
-      <c r="Y1" s="83">
+      <c r="Y1" s="82">
         <v>44945</v>
       </c>
-      <c r="Z1" s="83">
+      <c r="Z1" s="82">
         <v>44946</v>
       </c>
-      <c r="AA1" s="83">
+      <c r="AA1" s="82">
         <v>44951</v>
       </c>
-      <c r="AB1" s="83">
+      <c r="AB1" s="82">
         <v>44952</v>
       </c>
-      <c r="AC1" s="83">
+      <c r="AC1" s="82">
         <v>44953</v>
       </c>
-      <c r="AD1" s="83">
+      <c r="AD1" s="82">
         <v>44954</v>
       </c>
-      <c r="AE1" s="83">
+      <c r="AE1" s="82">
         <v>44957</v>
       </c>
-      <c r="AF1" s="83">
+      <c r="AF1" s="82">
         <v>44958</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
+    <row r="2" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="247" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="99" t="s">
         <v>132</v>
       </c>
       <c r="G2" s="251" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="86" t="s">
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="85" t="s">
         <v>177</v>
       </c>
-      <c r="K2" s="86" t="s">
+      <c r="K2" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="L2" s="86" t="s">
+      <c r="L2" s="85" t="s">
         <v>352</v>
       </c>
       <c r="M2" t="s">
         <v>427</v>
       </c>
-      <c r="N2" s="86" t="s">
+      <c r="N2" s="85" t="s">
         <v>466</v>
       </c>
-      <c r="O2" s="86" t="s">
+      <c r="O2" s="85" t="s">
         <v>518</v>
       </c>
-      <c r="P2" s="86" t="s">
+      <c r="P2" s="85" t="s">
         <v>518</v>
       </c>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="86" t="s">
+      <c r="Q2" s="99"/>
+      <c r="R2" s="85" t="s">
         <v>549</v>
       </c>
-      <c r="S2" s="254" t="s">
+      <c r="S2" s="246" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
+      <c r="T2" s="85" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="247"/>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100" t="s">
+      <c r="C3" s="99"/>
+      <c r="D3" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="100" t="s">
+      <c r="F3" s="99" t="s">
         <v>133</v>
       </c>
       <c r="G3" s="251"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="113" t="s">
+      <c r="H3" s="99"/>
+      <c r="I3" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="86" t="s">
+      <c r="J3" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="133" t="s">
+      <c r="K3" s="132" t="s">
         <v>289</v>
       </c>
-      <c r="L3" s="86" t="s">
+      <c r="L3" s="85" t="s">
         <v>353</v>
       </c>
       <c r="M3" t="s">
         <v>428</v>
       </c>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="176"/>
-      <c r="S3" s="254"/>
-    </row>
-    <row r="4" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
+      <c r="Q3" s="99"/>
+      <c r="R3" s="174"/>
+      <c r="S3" s="246"/>
+      <c r="T3" s="85" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="247"/>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100" t="s">
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="100" t="s">
+      <c r="F4" s="99" t="s">
         <v>134</v>
       </c>
       <c r="G4" s="251"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100" t="s">
+      <c r="H4" s="99"/>
+      <c r="I4" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="J4" s="86" t="s">
+      <c r="J4" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="K4" s="86" t="s">
+      <c r="K4" s="85" t="s">
         <v>292</v>
       </c>
-      <c r="L4" s="86" t="s">
+      <c r="L4" s="85" t="s">
         <v>354</v>
       </c>
       <c r="M4" t="s">
         <v>429</v>
       </c>
-      <c r="Q4" s="100" t="s">
+      <c r="Q4" s="99" t="s">
         <v>530</v>
       </c>
-      <c r="R4" s="86" t="s">
+      <c r="R4" s="85" t="s">
         <v>547</v>
       </c>
-      <c r="S4" s="254"/>
-    </row>
-    <row r="5" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
+      <c r="S4" s="246"/>
+    </row>
+    <row r="5" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="247"/>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100" t="s">
+      <c r="C5" s="99"/>
+      <c r="D5" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="100" t="s">
+      <c r="E5" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="100" t="s">
+      <c r="F5" s="99" t="s">
         <v>135</v>
       </c>
       <c r="G5" s="251"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="99"/>
+      <c r="I5" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="K5" s="86" t="s">
+      <c r="K5" s="85" t="s">
         <v>276</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="85" t="s">
         <v>355</v>
       </c>
       <c r="M5" t="s">
         <v>430</v>
       </c>
-      <c r="Q5" s="100"/>
-      <c r="S5" s="254"/>
-    </row>
-    <row r="6" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
+      <c r="Q5" s="99"/>
+      <c r="S5" s="246"/>
+    </row>
+    <row r="6" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="247"/>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="100" t="s">
+      <c r="E6" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="99" t="s">
         <v>136</v>
       </c>
       <c r="G6" s="251"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100" t="s">
+      <c r="H6" s="99"/>
+      <c r="I6" s="99" t="s">
         <v>168</v>
       </c>
       <c r="J6" s="1"/>
       <c r="M6" t="s">
         <v>431</v>
       </c>
-      <c r="Q6" s="100" t="s">
+      <c r="Q6" s="99" t="s">
         <v>535</v>
       </c>
-      <c r="S6" s="254"/>
-    </row>
-    <row r="7" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="S6" s="246"/>
+    </row>
+    <row r="7" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="248" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="100" t="s">
+      <c r="E7" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="100"/>
+      <c r="F7" s="99"/>
       <c r="G7" s="251"/>
-      <c r="H7" s="100" t="s">
+      <c r="H7" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="100" t="s">
+      <c r="I7" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="J7" s="87" t="s">
+      <c r="J7" s="86" t="s">
         <v>180</v>
       </c>
-      <c r="K7" s="87" t="s">
+      <c r="K7" s="86" t="s">
         <v>281</v>
       </c>
-      <c r="L7" s="87" t="s">
+      <c r="L7" s="86" t="s">
         <v>356</v>
       </c>
       <c r="M7" t="s">
         <v>432</v>
       </c>
-      <c r="N7" s="87" t="s">
+      <c r="N7" s="86" t="s">
         <v>468</v>
       </c>
-      <c r="O7" s="87" t="s">
+      <c r="O7" s="86" t="s">
         <v>519</v>
       </c>
-      <c r="P7" s="87" t="s">
+      <c r="P7" s="86" t="s">
         <v>527</v>
       </c>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="87" t="s">
+      <c r="Q7" s="99"/>
+      <c r="R7" s="86" t="s">
         <v>549</v>
       </c>
-      <c r="S7" s="254"/>
-    </row>
-    <row r="8" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="S7" s="246"/>
+      <c r="T7" s="86" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="248"/>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="102" t="s">
+      <c r="D8" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
       <c r="G8" s="251"/>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="99" t="s">
         <v>170</v>
       </c>
-      <c r="J8" s="87" t="s">
+      <c r="J8" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="K8" s="87" t="s">
+      <c r="K8" s="86" t="s">
         <v>282</v>
       </c>
-      <c r="L8" s="87" t="s">
+      <c r="L8" s="86" t="s">
         <v>350</v>
       </c>
       <c r="M8" t="s">
         <v>433</v>
       </c>
-      <c r="Q8" s="100" t="s">
+      <c r="Q8" s="99" t="s">
         <v>536</v>
       </c>
-      <c r="S8" s="254"/>
-    </row>
-    <row r="9" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="S8" s="246"/>
+      <c r="T8" s="86" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="248"/>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
       <c r="G9" s="251"/>
-      <c r="H9" s="100" t="s">
+      <c r="H9" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="I9" s="100"/>
-      <c r="K9" s="87" t="s">
+      <c r="I9" s="99"/>
+      <c r="K9" s="86" t="s">
         <v>287</v>
       </c>
-      <c r="L9" s="87" t="s">
+      <c r="L9" s="86" t="s">
         <v>357</v>
       </c>
       <c r="M9" t="s">
         <v>434</v>
       </c>
-      <c r="Q9" s="100" t="s">
+      <c r="Q9" s="99" t="s">
         <v>537</v>
       </c>
-      <c r="R9" s="87" t="s">
+      <c r="R9" s="86" t="s">
         <v>550</v>
       </c>
-      <c r="S9" s="254"/>
-    </row>
-    <row r="10" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="S9" s="246"/>
+      <c r="T9" s="86" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="248"/>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="100" t="s">
+      <c r="C10" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100" t="s">
+      <c r="D10" s="99"/>
+      <c r="E10" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="100"/>
+      <c r="F10" s="99"/>
       <c r="G10" s="251"/>
-      <c r="H10" s="100"/>
-      <c r="I10" s="100"/>
-      <c r="K10" s="87" t="s">
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="K10" s="86" t="s">
         <v>288</v>
       </c>
       <c r="M10" t="s">
         <v>435</v>
       </c>
-      <c r="Q10" s="100" t="s">
+      <c r="Q10" s="99" t="s">
         <v>538</v>
       </c>
-      <c r="S10" s="254"/>
-    </row>
-    <row r="11" spans="1:32" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="S10" s="246"/>
+    </row>
+    <row r="11" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="248"/>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100" t="s">
+      <c r="D11" s="99"/>
+      <c r="E11" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="100"/>
+      <c r="F11" s="99"/>
       <c r="G11" s="251"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
       <c r="M11" t="s">
         <v>436</v>
       </c>
-      <c r="Q11" s="100"/>
-      <c r="S11" s="254"/>
-    </row>
-    <row r="12" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="Q11" s="99"/>
+      <c r="S11" s="246"/>
+    </row>
+    <row r="12" spans="1:32" s="87" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A12" s="249" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100" t="s">
+      <c r="D12" s="99"/>
+      <c r="E12" s="99" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="100"/>
+      <c r="F12" s="99"/>
       <c r="G12" s="251"/>
-      <c r="H12" s="100" t="s">
+      <c r="H12" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="I12" s="100"/>
-      <c r="J12" s="88" t="s">
+      <c r="I12" s="99"/>
+      <c r="J12" s="87" t="s">
         <v>182</v>
       </c>
-      <c r="K12" s="88" t="s">
+      <c r="K12" s="87" t="s">
         <v>283</v>
       </c>
       <c r="M12"/>
-      <c r="Q12" s="100"/>
-      <c r="S12" s="254"/>
-    </row>
-    <row r="13" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="Q12" s="99"/>
+      <c r="S12" s="246"/>
+    </row>
+    <row r="13" spans="1:32" s="87" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A13" s="249"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100" t="s">
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="100"/>
+      <c r="F13" s="99"/>
       <c r="G13" s="251"/>
-      <c r="H13" s="100" t="s">
+      <c r="H13" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="100"/>
-      <c r="K13" s="88" t="s">
+      <c r="I13" s="99"/>
+      <c r="K13" s="87" t="s">
         <v>284</v>
       </c>
       <c r="M13" t="s">
         <v>437</v>
       </c>
-      <c r="Q13" s="100"/>
-      <c r="S13" s="254"/>
-    </row>
-    <row r="14" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="Q13" s="99"/>
+      <c r="S13" s="246"/>
+    </row>
+    <row r="14" spans="1:32" s="87" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A14" s="249"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
       <c r="G14" s="251"/>
-      <c r="H14" s="100" t="s">
+      <c r="H14" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="I14" s="100"/>
+      <c r="I14" s="99"/>
       <c r="M14" t="s">
         <v>438</v>
       </c>
-      <c r="Q14" s="100"/>
-      <c r="S14" s="254"/>
-    </row>
-    <row r="15" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="Q14" s="99"/>
+      <c r="S14" s="246"/>
+    </row>
+    <row r="15" spans="1:32" s="87" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A15" s="249"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100" t="s">
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="100"/>
+      <c r="F15" s="99"/>
       <c r="G15" s="251"/>
-      <c r="H15" s="100" t="s">
+      <c r="H15" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="100"/>
+      <c r="I15" s="99"/>
       <c r="M15"/>
-      <c r="Q15" s="100"/>
-      <c r="S15" s="254"/>
-    </row>
-    <row r="16" spans="1:32" s="88" customFormat="1" ht="30" hidden="1" customHeight="1">
+      <c r="Q15" s="99"/>
+      <c r="S15" s="246"/>
+    </row>
+    <row r="16" spans="1:32" s="87" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A16" s="249"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100" t="s">
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="100"/>
+      <c r="F16" s="99"/>
       <c r="G16" s="251"/>
-      <c r="H16" s="100" t="s">
+      <c r="H16" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="I16" s="100"/>
+      <c r="I16" s="99"/>
       <c r="M16"/>
-      <c r="Q16" s="100"/>
-      <c r="S16" s="254"/>
-    </row>
-    <row r="17" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="Q16" s="99"/>
+      <c r="S16" s="246"/>
+    </row>
+    <row r="17" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="250" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="251"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="89" t="s">
+      <c r="H17" s="99"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="K17" s="89" t="s">
+      <c r="K17" s="88" t="s">
         <v>285</v>
       </c>
-      <c r="L17" s="89" t="s">
+      <c r="L17" s="88" t="s">
         <v>350</v>
       </c>
       <c r="M17" t="s">
         <v>465</v>
       </c>
-      <c r="N17" s="89" t="s">
+      <c r="N17" s="88" t="s">
         <v>467</v>
       </c>
-      <c r="O17" s="89" t="s">
+      <c r="O17" s="88" t="s">
         <v>520</v>
       </c>
-      <c r="P17" s="89" t="s">
+      <c r="P17" s="88" t="s">
         <v>528</v>
       </c>
-      <c r="Q17" s="100" t="s">
+      <c r="Q17" s="99" t="s">
         <v>531</v>
       </c>
-      <c r="R17" s="89" t="s">
+      <c r="R17" s="88" t="s">
         <v>549</v>
       </c>
-      <c r="S17" s="254"/>
-    </row>
-    <row r="18" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="S17" s="246"/>
+      <c r="T17" s="88" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A18" s="250"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
       <c r="G18" s="251"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="100"/>
-      <c r="L18" s="89" t="s">
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
+      <c r="L18" s="88" t="s">
         <v>351</v>
       </c>
       <c r="M18" t="s">
         <v>438</v>
       </c>
-      <c r="Q18" s="100" t="s">
+      <c r="Q18" s="99" t="s">
         <v>539</v>
       </c>
-      <c r="S18" s="254"/>
-    </row>
-    <row r="19" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="S18" s="246"/>
+      <c r="T18" s="88" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="250"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
       <c r="G19" s="251"/>
-      <c r="H19" s="100"/>
-      <c r="I19" s="100"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
       <c r="M19" t="s">
         <v>439</v>
       </c>
-      <c r="Q19" s="100"/>
-      <c r="R19" s="89" t="s">
+      <c r="Q19" s="99"/>
+      <c r="R19" s="88" t="s">
         <v>548</v>
       </c>
-      <c r="S19" s="254"/>
-    </row>
-    <row r="20" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="S19" s="246"/>
+    </row>
+    <row r="20" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="250"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
       <c r="G20" s="251"/>
-      <c r="H20" s="100"/>
-      <c r="I20" s="100"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
       <c r="M20" t="s">
         <v>440</v>
       </c>
-      <c r="Q20" s="100" t="s">
+      <c r="Q20" s="99" t="s">
         <v>540</v>
       </c>
-      <c r="S20" s="254"/>
-    </row>
-    <row r="21" spans="1:19" s="89" customFormat="1" ht="30" customHeight="1">
+      <c r="S20" s="246"/>
+    </row>
+    <row r="21" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="250"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
       <c r="G21" s="251"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
-      <c r="Q21" s="100"/>
-      <c r="S21" s="254"/>
-    </row>
-    <row r="22" spans="1:19" s="100" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="107"/>
+      <c r="Q21" s="99"/>
+      <c r="S21" s="246"/>
+    </row>
+    <row r="22" spans="1:20" s="99" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="106"/>
       <c r="M22" t="s">
         <v>442</v>
       </c>
-      <c r="Q22" s="100" t="s">
+      <c r="Q22" s="99" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="109" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="108" t="s">
+    <row r="23" spans="1:20" s="108" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="108" t="s">
+      <c r="D23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="108" t="s">
+      <c r="E23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="108" t="s">
+      <c r="F23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="108" t="s">
+      <c r="G23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="108" t="s">
+      <c r="H23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="108" t="s">
+      <c r="I23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="108" t="s">
+      <c r="J23" s="107" t="s">
         <v>68</v>
       </c>
       <c r="M23" t="s">
         <v>443</v>
       </c>
-      <c r="N23" s="108" t="s">
+      <c r="N23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="108" t="s">
+      <c r="O23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="P23" s="108" t="s">
+      <c r="P23" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="Q23" s="100" t="s">
+      <c r="Q23" s="99" t="s">
         <v>533</v>
       </c>
-      <c r="S23" s="108" t="s">
+      <c r="S23" s="107" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" ht="30" customHeight="1">
+      <c r="T23" s="107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5797,8 +5875,11 @@
       <c r="S24" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" ht="30" customHeight="1">
+      <c r="T24" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5829,14 +5910,17 @@
       <c r="M25" t="s">
         <v>445</v>
       </c>
-      <c r="Q25" s="108" t="s">
+      <c r="Q25" s="107" t="s">
         <v>68</v>
       </c>
       <c r="S25" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" ht="30" customHeight="1">
+      <c r="T25" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5858,14 +5942,17 @@
       <c r="L26" t="s">
         <v>359</v>
       </c>
-      <c r="Q26" s="100" t="s">
+      <c r="Q26" s="99" t="s">
         <v>541</v>
       </c>
       <c r="S26" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" ht="30" customHeight="1">
+      <c r="T26" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5890,14 +5977,14 @@
       <c r="J27" t="s">
         <v>187</v>
       </c>
-      <c r="M27" s="108" t="s">
+      <c r="M27" s="107" t="s">
         <v>68</v>
       </c>
       <c r="S27" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="30" customHeight="1">
+    <row r="28" spans="1:20" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -5920,7 +6007,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="30" customHeight="1">
+    <row r="29" spans="1:20" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -5946,7 +6033,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="30" customHeight="1">
+    <row r="30" spans="1:20" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -5963,7 +6050,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="30" customHeight="1">
+    <row r="31" spans="1:20" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -5977,7 +6064,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="30" customHeight="1">
+    <row r="32" spans="1:20" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -6043,12 +6130,12 @@
       <c r="D36" t="s">
         <v>104</v>
       </c>
-      <c r="J36" s="131" t="s">
+      <c r="J36" s="130" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
-      <c r="B37" s="105" t="s">
+      <c r="B37" s="104" t="s">
         <v>67</v>
       </c>
       <c r="D37" t="s">
@@ -6067,7 +6154,7 @@
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="105" t="s">
         <v>71</v>
       </c>
       <c r="J39" t="s">
@@ -6381,7 +6468,7 @@
       </c>
     </row>
     <row r="120" spans="10:10" ht="30" customHeight="1">
-      <c r="J120" s="131" t="s">
+      <c r="J120" s="130" t="s">
         <v>294</v>
       </c>
     </row>
@@ -6406,7 +6493,7 @@
       </c>
     </row>
     <row r="130" spans="10:10" ht="30" customHeight="1">
-      <c r="J130" s="131" t="s">
+      <c r="J130" s="130" t="s">
         <v>296</v>
       </c>
     </row>
@@ -6476,7 +6563,7 @@
       </c>
     </row>
     <row r="159" spans="10:10" ht="30" customHeight="1">
-      <c r="J159" s="131" t="s">
+      <c r="J159" s="130" t="s">
         <v>295</v>
       </c>
     </row>
@@ -6611,154 +6698,154 @@
     <col min="47" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="116" customFormat="1" ht="18" thickTop="1" thickBot="1">
-      <c r="A1" s="115" t="s">
+    <row r="1" spans="1:60" s="115" customFormat="1" ht="18" thickTop="1" thickBot="1">
+      <c r="A1" s="114" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="115" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="120" customFormat="1">
-      <c r="A2" s="117" t="s">
+    <row r="2" spans="1:60" s="119" customFormat="1">
+      <c r="A2" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="119">
+      <c r="B2" s="117"/>
+      <c r="C2" s="118">
         <v>44924</v>
       </c>
-      <c r="D2" s="134">
+      <c r="D2" s="133">
         <v>44924</v>
       </c>
-      <c r="E2" s="134">
+      <c r="E2" s="133">
         <v>44924</v>
       </c>
-      <c r="F2" s="119">
+      <c r="F2" s="118">
         <v>44924</v>
       </c>
-      <c r="G2" s="119">
+      <c r="G2" s="118">
         <v>44925</v>
       </c>
-      <c r="H2" s="119">
+      <c r="H2" s="118">
         <v>44925</v>
       </c>
-      <c r="I2" s="119">
+      <c r="I2" s="118">
         <v>44925</v>
       </c>
-      <c r="J2" s="119">
+      <c r="J2" s="118">
         <v>44925</v>
       </c>
-      <c r="K2" s="119">
+      <c r="K2" s="118">
         <v>44925</v>
       </c>
-      <c r="L2" s="119">
+      <c r="L2" s="118">
         <v>44925</v>
       </c>
-      <c r="M2" s="119">
+      <c r="M2" s="118">
         <v>44925</v>
       </c>
-      <c r="N2" s="119">
+      <c r="N2" s="118">
         <v>44925</v>
       </c>
-      <c r="O2" s="119">
+      <c r="O2" s="118">
         <v>44925</v>
       </c>
-      <c r="P2" s="119">
+      <c r="P2" s="118">
         <v>44925</v>
       </c>
-      <c r="Q2" s="140">
+      <c r="Q2" s="139">
         <v>44925</v>
       </c>
-      <c r="R2" s="119">
+      <c r="R2" s="118">
         <v>44925</v>
       </c>
-      <c r="S2" s="119">
+      <c r="S2" s="118">
         <v>44927</v>
       </c>
-      <c r="T2" s="119">
+      <c r="T2" s="118">
         <v>44927</v>
       </c>
-      <c r="U2" s="119">
+      <c r="U2" s="118">
         <v>44927</v>
       </c>
-      <c r="V2" s="119">
+      <c r="V2" s="118">
         <v>44927</v>
       </c>
-      <c r="W2" s="119">
+      <c r="W2" s="118">
         <v>44927</v>
       </c>
-      <c r="X2" s="119">
+      <c r="X2" s="118">
         <v>44927</v>
       </c>
-      <c r="Y2" s="119">
+      <c r="Y2" s="118">
         <v>44927</v>
       </c>
-      <c r="Z2" s="119">
+      <c r="Z2" s="118">
         <v>44927</v>
       </c>
-      <c r="AA2" s="119">
+      <c r="AA2" s="118">
         <v>44927</v>
       </c>
-      <c r="AB2" s="119">
+      <c r="AB2" s="118">
         <v>44927</v>
       </c>
-      <c r="AC2" s="119">
+      <c r="AC2" s="118">
         <v>44927</v>
       </c>
-      <c r="AD2" s="119">
+      <c r="AD2" s="118">
         <v>44927</v>
       </c>
-      <c r="AE2" s="119">
+      <c r="AE2" s="118">
         <v>44927</v>
       </c>
-      <c r="AF2" s="119">
+      <c r="AF2" s="118">
         <v>44927</v>
       </c>
-      <c r="AG2" s="119">
+      <c r="AG2" s="118">
         <v>44927</v>
       </c>
-      <c r="AH2" s="119">
+      <c r="AH2" s="118">
         <v>44927</v>
       </c>
-      <c r="AI2" s="119">
+      <c r="AI2" s="118">
         <v>44927</v>
       </c>
-      <c r="AJ2" s="119">
+      <c r="AJ2" s="118">
         <v>44927</v>
       </c>
-      <c r="AK2" s="119">
+      <c r="AK2" s="118">
         <v>44927</v>
       </c>
-      <c r="AL2" s="119">
+      <c r="AL2" s="118">
         <v>44927</v>
       </c>
-      <c r="AM2" s="119">
+      <c r="AM2" s="118">
         <v>44927</v>
       </c>
-      <c r="AN2" s="119">
+      <c r="AN2" s="118">
         <v>44927</v>
       </c>
-      <c r="AO2" s="119">
+      <c r="AO2" s="118">
         <v>44927</v>
       </c>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
+      <c r="AP2" s="118"/>
+      <c r="AQ2" s="118"/>
+      <c r="AR2" s="118"/>
+      <c r="AS2" s="118"/>
+      <c r="AT2" s="118"/>
     </row>
     <row r="3" spans="1:60">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="120" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="117"/>
+      <c r="C3" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="135" t="s">
+      <c r="D3" s="134" t="s">
         <v>256</v>
       </c>
-      <c r="E3" s="135" t="s">
+      <c r="E3" s="134" t="s">
         <v>257</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -6794,7 +6881,7 @@
       <c r="P3" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="Q3" s="141" t="s">
+      <c r="Q3" s="140" t="s">
         <v>291</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -6873,139 +6960,139 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:60" s="126" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A4" s="122" t="s">
+    <row r="4" spans="1:60" s="125" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A4" s="121" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="124" t="s">
+      <c r="B4" s="122"/>
+      <c r="C4" s="123" t="s">
         <v>260</v>
       </c>
-      <c r="D4" s="136" t="s">
+      <c r="D4" s="135" t="s">
         <v>261</v>
       </c>
-      <c r="E4" s="136" t="s">
+      <c r="E4" s="135" t="s">
         <v>262</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="124" t="s">
         <v>263</v>
       </c>
-      <c r="G4" s="130" t="s">
+      <c r="G4" s="129" t="s">
         <v>293</v>
       </c>
-      <c r="H4" s="130" t="s">
+      <c r="H4" s="129" t="s">
         <v>262</v>
       </c>
-      <c r="I4" s="130" t="s">
+      <c r="I4" s="129" t="s">
         <v>298</v>
       </c>
-      <c r="J4" s="130" t="s">
+      <c r="J4" s="129" t="s">
         <v>309</v>
       </c>
-      <c r="K4" s="130" t="s">
+      <c r="K4" s="129" t="s">
         <v>310</v>
       </c>
-      <c r="L4" s="126" t="s">
+      <c r="L4" s="125" t="s">
         <v>308</v>
       </c>
-      <c r="M4" s="130" t="s">
+      <c r="M4" s="129" t="s">
         <v>304</v>
       </c>
-      <c r="N4" s="130" t="s">
+      <c r="N4" s="129" t="s">
         <v>300</v>
       </c>
-      <c r="O4" s="130" t="s">
+      <c r="O4" s="129" t="s">
         <v>301</v>
       </c>
-      <c r="P4" s="130" t="s">
+      <c r="P4" s="129" t="s">
         <v>302</v>
       </c>
-      <c r="Q4" s="142" t="s">
+      <c r="Q4" s="141" t="s">
         <v>311</v>
       </c>
-      <c r="R4" s="130" t="s">
+      <c r="R4" s="129" t="s">
         <v>312</v>
       </c>
-      <c r="S4" s="130" t="s">
+      <c r="S4" s="129" t="s">
         <v>318</v>
       </c>
-      <c r="T4" s="138" t="s">
+      <c r="T4" s="137" t="s">
         <v>319</v>
       </c>
-      <c r="U4" s="130" t="s">
+      <c r="U4" s="129" t="s">
         <v>320</v>
       </c>
-      <c r="V4" s="130" t="s">
+      <c r="V4" s="129" t="s">
         <v>321</v>
       </c>
-      <c r="W4" s="130" t="s">
+      <c r="W4" s="129" t="s">
         <v>322</v>
       </c>
-      <c r="X4" s="130" t="s">
+      <c r="X4" s="129" t="s">
         <v>323</v>
       </c>
-      <c r="Y4" s="130" t="s">
+      <c r="Y4" s="129" t="s">
         <v>324</v>
       </c>
-      <c r="Z4" s="130" t="s">
+      <c r="Z4" s="129" t="s">
         <v>340</v>
       </c>
-      <c r="AA4" s="130" t="s">
+      <c r="AA4" s="129" t="s">
         <v>326</v>
       </c>
-      <c r="AB4" s="130" t="s">
+      <c r="AB4" s="129" t="s">
         <v>327</v>
       </c>
-      <c r="AC4" s="130" t="s">
+      <c r="AC4" s="129" t="s">
         <v>328</v>
       </c>
-      <c r="AD4" s="130" t="s">
+      <c r="AD4" s="129" t="s">
         <v>329</v>
       </c>
-      <c r="AE4" s="130" t="s">
+      <c r="AE4" s="129" t="s">
         <v>330</v>
       </c>
-      <c r="AF4" s="130" t="s">
+      <c r="AF4" s="129" t="s">
         <v>333</v>
       </c>
-      <c r="AG4" s="130" t="s">
+      <c r="AG4" s="129" t="s">
         <v>278</v>
       </c>
-      <c r="AH4" s="130" t="s">
+      <c r="AH4" s="129" t="s">
         <v>323</v>
       </c>
-      <c r="AI4" s="130" t="s">
+      <c r="AI4" s="129" t="s">
         <v>322</v>
       </c>
-      <c r="AJ4" s="130" t="s">
+      <c r="AJ4" s="129" t="s">
         <v>335</v>
       </c>
-      <c r="AK4" s="130" t="s">
+      <c r="AK4" s="129" t="s">
         <v>336</v>
       </c>
-      <c r="AL4" s="130" t="s">
+      <c r="AL4" s="129" t="s">
         <v>337</v>
       </c>
-      <c r="AM4" s="130" t="s">
+      <c r="AM4" s="129" t="s">
         <v>338</v>
       </c>
-      <c r="AN4" s="130" t="s">
+      <c r="AN4" s="129" t="s">
         <v>323</v>
       </c>
-      <c r="AO4" s="130" t="s">
+      <c r="AO4" s="129" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:60">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="120" t="s">
         <v>264</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(C5:ZY5)</f>
         <v>29127</v>
       </c>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
       <c r="I5" s="1">
         <v>10000</v>
       </c>
@@ -7015,28 +7102,28 @@
       <c r="K5" s="1">
         <v>7477</v>
       </c>
-      <c r="Q5" s="141"/>
+      <c r="Q5" s="140"/>
       <c r="S5" s="1">
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:60">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="120" t="s">
         <v>265</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B20" si="0">SUM(C6:ZY6)</f>
         <v>29066</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
       <c r="O6" s="1">
         <v>2000</v>
       </c>
       <c r="P6" s="1">
         <v>16414</v>
       </c>
-      <c r="Q6" s="141"/>
+      <c r="Q6" s="140"/>
       <c r="V6" s="1">
         <v>10000</v>
       </c>
@@ -7045,18 +7132,18 @@
       </c>
     </row>
     <row r="7" spans="1:60">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>266</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="D7" s="135" t="s">
+      <c r="D7" s="134" t="s">
         <v>325</v>
       </c>
-      <c r="E7" s="135"/>
-      <c r="Q7" s="141"/>
+      <c r="E7" s="134"/>
+      <c r="Q7" s="140"/>
       <c r="Z7" s="1">
         <v>10000</v>
       </c>
@@ -7065,22 +7152,22 @@
       </c>
     </row>
     <row r="8" spans="1:60">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="120" t="s">
         <v>267</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>11681</v>
       </c>
-      <c r="D8" s="135"/>
-      <c r="E8" s="135"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
       <c r="L8" s="1">
         <v>1500</v>
       </c>
       <c r="M8" s="1">
         <v>2000</v>
       </c>
-      <c r="Q8" s="141"/>
+      <c r="Q8" s="140"/>
       <c r="W8" s="1">
         <v>4585</v>
       </c>
@@ -7089,34 +7176,34 @@
       </c>
     </row>
     <row r="9" spans="1:60">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="120" t="s">
         <v>268</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>10921</v>
       </c>
-      <c r="D9" s="135"/>
-      <c r="E9" s="135"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
       <c r="N9" s="1">
         <v>8626</v>
       </c>
-      <c r="Q9" s="141"/>
+      <c r="Q9" s="140"/>
       <c r="AB9" s="1">
         <v>2295</v>
       </c>
     </row>
     <row r="10" spans="1:60">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="120" t="s">
         <v>269</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>16827</v>
       </c>
-      <c r="D10" s="135"/>
-      <c r="E10" s="135"/>
-      <c r="Q10" s="141"/>
+      <c r="D10" s="134"/>
+      <c r="E10" s="134"/>
+      <c r="Q10" s="140"/>
       <c r="R10" s="1">
         <v>6827</v>
       </c>
@@ -7125,16 +7212,16 @@
       </c>
     </row>
     <row r="11" spans="1:60">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="120" t="s">
         <v>270</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>11054</v>
       </c>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="Q11" s="141"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="Q11" s="140"/>
       <c r="T11" s="1">
         <v>5364</v>
       </c>
@@ -7143,19 +7230,19 @@
       </c>
     </row>
     <row r="12" spans="1:60">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="120" t="s">
         <v>271</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>10522</v>
       </c>
-      <c r="D12" s="135"/>
-      <c r="E12" s="135"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
       <c r="F12" s="1">
         <v>2000</v>
       </c>
-      <c r="Q12" s="141"/>
+      <c r="Q12" s="140"/>
       <c r="Y12" s="1">
         <v>5996</v>
       </c>
@@ -7164,149 +7251,149 @@
       </c>
     </row>
     <row r="13" spans="1:60">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="120" t="s">
         <v>272</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="D13" s="135"/>
-      <c r="E13" s="135"/>
+      <c r="D13" s="134"/>
+      <c r="E13" s="134"/>
       <c r="G13" s="1">
         <v>10000</v>
       </c>
-      <c r="Q13" s="141"/>
+      <c r="Q13" s="140"/>
       <c r="AC13" s="1">
         <v>10000</v>
       </c>
     </row>
     <row r="14" spans="1:60">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="120" t="s">
         <v>273</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
       <c r="H14" s="1">
         <v>10000</v>
       </c>
-      <c r="Q14" s="141"/>
+      <c r="Q14" s="140"/>
       <c r="AD14" s="1">
         <v>10000</v>
       </c>
     </row>
     <row r="15" spans="1:60">
-      <c r="A15" s="121" t="s">
+      <c r="A15" s="120" t="s">
         <v>274</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>8116</v>
       </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="Q15" s="141"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="Q15" s="140"/>
       <c r="AO15" s="1">
         <v>8116</v>
       </c>
     </row>
     <row r="16" spans="1:60">
-      <c r="A16" s="132" t="s">
+      <c r="A16" s="131" t="s">
         <v>290</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
-      <c r="Q16" s="141" t="s">
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="Q16" s="140" t="s">
         <v>331</v>
       </c>
       <c r="AE16" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:40" s="135" customFormat="1">
-      <c r="A17" s="139" t="s">
+    <row r="17" spans="1:40" s="134" customFormat="1">
+      <c r="A17" s="138" t="s">
         <v>275</v>
       </c>
-      <c r="B17" s="135">
+      <c r="B17" s="134">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="C17" s="135">
+      <c r="C17" s="134">
         <v>1500</v>
       </c>
-      <c r="Q17" s="141"/>
+      <c r="Q17" s="140"/>
     </row>
     <row r="18" spans="1:40">
-      <c r="A18" s="145" t="s">
+      <c r="A18" s="144" t="s">
         <v>276</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="D18" s="135"/>
-      <c r="E18" s="135"/>
-      <c r="Q18" s="141"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
+      <c r="Q18" s="140"/>
       <c r="AF18" s="1">
         <v>1500</v>
       </c>
     </row>
     <row r="19" spans="1:40">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="120" t="s">
         <v>332</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>6575</v>
       </c>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="Q19" s="141"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
+      <c r="Q19" s="140"/>
       <c r="U19" s="1">
         <v>6575</v>
       </c>
     </row>
     <row r="20" spans="1:40">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="120" t="s">
         <v>277</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
         <v>8458</v>
       </c>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="Q20" s="141"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
+      <c r="Q20" s="140"/>
       <c r="X20" s="1">
         <v>1905</v>
       </c>
       <c r="AH20" s="1">
         <v>1500</v>
       </c>
-      <c r="AN20" s="144">
+      <c r="AN20" s="143">
         <v>5053</v>
       </c>
     </row>
-    <row r="21" spans="1:40" s="127" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A21" s="146" t="s">
+    <row r="21" spans="1:40" s="126" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A21" s="145" t="s">
         <v>278</v>
       </c>
-      <c r="B21" s="127">
+      <c r="B21" s="126">
         <f>SUM(C21:ZY21)</f>
         <v>1500</v>
       </c>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="Q21" s="143"/>
-      <c r="AG21" s="127">
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="Q21" s="142"/>
+      <c r="AG21" s="126">
         <v>1500</v>
       </c>
     </row>
@@ -7325,10 +7412,10 @@
       </c>
     </row>
     <row r="26" spans="1:40">
-      <c r="L26" s="138" t="s">
+      <c r="L26" s="137" t="s">
         <v>305</v>
       </c>
-      <c r="M26" s="138"/>
+      <c r="M26" s="137"/>
     </row>
     <row r="28" spans="1:40">
       <c r="L28" s="1" t="s">
@@ -7336,13 +7423,13 @@
       </c>
     </row>
     <row r="29" spans="1:40">
-      <c r="L29" s="138" t="s">
+      <c r="L29" s="137" t="s">
         <v>306</v>
       </c>
-      <c r="M29" s="138"/>
+      <c r="M29" s="137"/>
     </row>
     <row r="44" spans="10:10">
-      <c r="J44" s="138"/>
+      <c r="J44" s="137"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7416,43 +7503,43 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="116" customFormat="1" ht="18" thickTop="1" thickBot="1">
-      <c r="A1" s="150" t="s">
+    <row r="1" spans="1:25" s="115" customFormat="1" ht="18" thickTop="1" thickBot="1">
+      <c r="A1" s="149" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="B1" s="150" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="150" t="s">
         <v>349</v>
       </c>
-      <c r="D1" s="151" t="s">
+      <c r="D1" s="150" t="s">
         <v>346</v>
       </c>
-      <c r="E1" s="151" t="s">
+      <c r="E1" s="150" t="s">
         <v>349</v>
       </c>
-      <c r="F1" s="151" t="s">
+      <c r="F1" s="150" t="s">
         <v>346</v>
       </c>
-      <c r="G1" s="151" t="s">
+      <c r="G1" s="150" t="s">
         <v>349</v>
       </c>
-      <c r="H1" s="151" t="s">
+      <c r="H1" s="150" t="s">
         <v>346</v>
       </c>
-      <c r="I1" s="151" t="s">
+      <c r="I1" s="150" t="s">
         <v>349</v>
       </c>
-      <c r="J1" s="152" t="s">
+      <c r="J1" s="151" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="155" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="157"/>
+      <c r="B2" s="156"/>
       <c r="C2" s="252" t="s">
         <v>258</v>
       </c>
@@ -7474,7 +7561,7 @@
       </c>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="120" t="s">
         <v>264</v>
       </c>
       <c r="B3" s="1">
@@ -7487,10 +7574,10 @@
       <c r="G3" s="1">
         <v>10000</v>
       </c>
-      <c r="J3" s="149"/>
+      <c r="J3" s="148"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="120" t="s">
         <v>270</v>
       </c>
       <c r="B4" s="1">
@@ -7503,10 +7590,10 @@
       <c r="G4" s="1">
         <v>5690</v>
       </c>
-      <c r="J4" s="149"/>
+      <c r="J4" s="148"/>
     </row>
     <row r="5" spans="1:25">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="120" t="s">
         <v>265</v>
       </c>
       <c r="B5" s="1">
@@ -7522,10 +7609,10 @@
       <c r="G5" s="1">
         <v>652</v>
       </c>
-      <c r="J5" s="149"/>
+      <c r="J5" s="148"/>
     </row>
     <row r="6" spans="1:25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="120" t="s">
         <v>277</v>
       </c>
       <c r="B6" s="1">
@@ -7544,10 +7631,10 @@
       <c r="I6" s="1">
         <v>1500</v>
       </c>
-      <c r="J6" s="149"/>
+      <c r="J6" s="148"/>
     </row>
     <row r="7" spans="1:25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>267</v>
       </c>
       <c r="B7" s="1">
@@ -7561,10 +7648,10 @@
       <c r="G7" s="1">
         <v>3596</v>
       </c>
-      <c r="J7" s="149"/>
+      <c r="J7" s="148"/>
     </row>
     <row r="8" spans="1:25">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="120" t="s">
         <v>268</v>
       </c>
       <c r="B8" s="1">
@@ -7577,10 +7664,10 @@
       <c r="G8" s="1">
         <v>8626</v>
       </c>
-      <c r="J8" s="149"/>
+      <c r="J8" s="148"/>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="120" t="s">
         <v>266</v>
       </c>
       <c r="B9" s="1">
@@ -7593,10 +7680,10 @@
       <c r="G9" s="1">
         <v>10000</v>
       </c>
-      <c r="J9" s="149"/>
+      <c r="J9" s="148"/>
     </row>
     <row r="10" spans="1:25">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="120" t="s">
         <v>269</v>
       </c>
       <c r="B10" s="1">
@@ -7609,10 +7696,10 @@
       <c r="G10" s="1">
         <v>6827</v>
       </c>
-      <c r="J10" s="149"/>
+      <c r="J10" s="148"/>
     </row>
     <row r="11" spans="1:25">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="120" t="s">
         <v>271</v>
       </c>
       <c r="B11" s="1">
@@ -7628,10 +7715,10 @@
       <c r="G11" s="1">
         <v>2526</v>
       </c>
-      <c r="J11" s="149"/>
+      <c r="J11" s="148"/>
     </row>
     <row r="12" spans="1:25">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="120" t="s">
         <v>347</v>
       </c>
       <c r="B12" s="1">
@@ -7645,10 +7732,10 @@
       <c r="G12" s="1">
         <v>8116</v>
       </c>
-      <c r="J12" s="149"/>
+      <c r="J12" s="148"/>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" s="148" t="s">
+      <c r="A13" s="147" t="s">
         <v>344</v>
       </c>
       <c r="B13" s="1">
@@ -7661,10 +7748,10 @@
       <c r="G13" s="1">
         <v>10000</v>
       </c>
-      <c r="J13" s="149"/>
+      <c r="J13" s="148"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="148" t="s">
+      <c r="A14" s="147" t="s">
         <v>345</v>
       </c>
       <c r="B14" s="1">
@@ -7677,10 +7764,10 @@
       <c r="G14" s="1">
         <v>10000</v>
       </c>
-      <c r="J14" s="149"/>
+      <c r="J14" s="148"/>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" s="148" t="s">
+      <c r="A15" s="147" t="s">
         <v>290</v>
       </c>
       <c r="B15" s="1">
@@ -7690,10 +7777,10 @@
       <c r="E15" s="1">
         <v>10000</v>
       </c>
-      <c r="J15" s="149"/>
+      <c r="J15" s="148"/>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" s="148" t="s">
+      <c r="A16" s="147" t="s">
         <v>272</v>
       </c>
       <c r="B16" s="1">
@@ -7706,10 +7793,10 @@
       <c r="G16" s="1">
         <v>10000</v>
       </c>
-      <c r="J16" s="149"/>
+      <c r="J16" s="148"/>
     </row>
     <row r="17" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A17" s="148" t="s">
+      <c r="A17" s="147" t="s">
         <v>273</v>
       </c>
       <c r="B17" s="1">
@@ -7722,24 +7809,24 @@
       <c r="G17" s="1">
         <v>10000</v>
       </c>
-      <c r="J17" s="149"/>
+      <c r="J17" s="148"/>
     </row>
     <row r="18" spans="1:10" ht="18" thickTop="1" thickBot="1">
-      <c r="A18" s="153" t="s">
+      <c r="A18" s="152" t="s">
         <v>348</v>
       </c>
-      <c r="B18" s="154">
+      <c r="B18" s="153">
         <f>SUM(B3:B17)</f>
         <v>228290</v>
       </c>
-      <c r="C18" s="154"/>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
-      <c r="J18" s="155"/>
+      <c r="C18" s="153"/>
+      <c r="D18" s="153"/>
+      <c r="E18" s="153"/>
+      <c r="F18" s="153"/>
+      <c r="G18" s="153"/>
+      <c r="H18" s="153"/>
+      <c r="I18" s="153"/>
+      <c r="J18" s="154"/>
     </row>
     <row r="19" spans="1:10" ht="17.25" thickTop="1"/>
   </sheetData>
@@ -7770,8 +7857,8 @@
     <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="162" customFormat="1">
-      <c r="A1" s="162" t="s">
+    <row r="1" spans="1:5" s="161" customFormat="1">
+      <c r="A1" s="161" t="s">
         <v>420</v>
       </c>
     </row>
@@ -7907,7 +7994,7 @@
       <c r="C16" t="s">
         <v>366</v>
       </c>
-      <c r="D16" s="131" t="s">
+      <c r="D16" s="130" t="s">
         <v>455</v>
       </c>
       <c r="E16" t="s">
@@ -8247,30 +8334,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="90"/>
-      <c r="C4" s="90" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="89" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8298,19 +8385,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="198" t="s">
+      <c r="C6" s="197" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="185" t="s">
+      <c r="D6" s="184" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="203" t="s">
+      <c r="E6" s="202" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="114" t="s">
+      <c r="F6" s="113" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="206" t="s">
+      <c r="G6" s="205" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8318,39 +8405,39 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="187"/>
-      <c r="E7" s="204"/>
-      <c r="F7" s="114" t="s">
+      <c r="C7" s="198"/>
+      <c r="D7" s="186"/>
+      <c r="E7" s="203"/>
+      <c r="F7" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="207"/>
+      <c r="G7" s="206"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B8" s="97">
+      <c r="B8" s="96">
         <v>0.5</v>
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="70"/>
       <c r="E8" s="70"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="200" t="s">
+      <c r="C9" s="199" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="185" t="s">
+      <c r="D9" s="184" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="203"/>
-      <c r="F9" s="114" t="s">
+      <c r="E9" s="202"/>
+      <c r="F9" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="G9" s="129" t="s">
+      <c r="G9" s="128" t="s">
         <v>247</v>
       </c>
     </row>
@@ -8358,25 +8445,25 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="201"/>
-      <c r="D10" s="186"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="114" t="s">
+      <c r="C10" s="200"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="204"/>
+      <c r="F10" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="G10" s="129"/>
+      <c r="G10" s="128"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="202"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="205"/>
-      <c r="F11" s="114" t="s">
+      <c r="C11" s="201"/>
+      <c r="D11" s="185"/>
+      <c r="E11" s="204"/>
+      <c r="F11" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="G11" s="129"/>
+      <c r="G11" s="128"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -8385,12 +8472,12 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="187"/>
-      <c r="E12" s="204"/>
-      <c r="F12" s="114" t="s">
+      <c r="D12" s="186"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="113" t="s">
         <v>249</v>
       </c>
-      <c r="G12" s="129"/>
+      <c r="G12" s="128"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -8399,12 +8486,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="179" t="s">
+      <c r="D13" s="178" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="180"/>
-      <c r="F13" s="180"/>
-      <c r="G13" s="128" t="s">
+      <c r="E13" s="179"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="127" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8441,7 +8528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA8B3E0-A018-4F44-9288-A66C82835404}">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -8455,34 +8542,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="91"/>
-      <c r="C4" s="91" t="s">
+      <c r="B4" s="90"/>
+      <c r="C4" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="91" t="s">
+      <c r="D4" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>20</v>
       </c>
     </row>
@@ -8490,40 +8577,40 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="169" t="s">
+      <c r="C5" s="168" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="110" t="s">
+      <c r="F5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="110" t="s">
+      <c r="G5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="170"/>
+      <c r="H5" s="169"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="157" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="167" t="s">
+      <c r="D6" s="166" t="s">
         <v>422</v>
       </c>
-      <c r="E6" s="171" t="s">
+      <c r="E6" s="170" t="s">
         <v>446</v>
       </c>
-      <c r="F6" s="112" t="s">
+      <c r="F6" s="111" t="s">
         <v>523</v>
       </c>
-      <c r="G6" s="211" t="s">
+      <c r="G6" s="210" t="s">
         <v>521</v>
       </c>
       <c r="H6" s="30" t="s">
@@ -8534,17 +8621,17 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="159"/>
-      <c r="D7" s="166" t="s">
+      <c r="C7" s="158"/>
+      <c r="D7" s="165" t="s">
         <v>421</v>
       </c>
-      <c r="E7" s="172" t="s">
+      <c r="E7" s="171" t="s">
         <v>447</v>
       </c>
-      <c r="F7" s="112" t="s">
+      <c r="F7" s="111" t="s">
         <v>520</v>
       </c>
-      <c r="G7" s="212"/>
+      <c r="G7" s="211"/>
       <c r="H7" s="30" t="s">
         <v>530</v>
       </c>
@@ -8553,47 +8640,47 @@
       <c r="B8" s="36">
         <v>0.5</v>
       </c>
-      <c r="C8" s="163"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="164"/>
-      <c r="H8" s="165"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="163"/>
+      <c r="H8" s="164"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="147" t="s">
+      <c r="C9" s="146" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="167" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="208" t="s">
+      <c r="E9" s="207" t="s">
         <v>469</v>
       </c>
-      <c r="F9" s="112" t="s">
+      <c r="F9" s="111" t="s">
         <v>524</v>
       </c>
-      <c r="G9" s="173" t="s">
+      <c r="G9" s="172" t="s">
         <v>522</v>
       </c>
-      <c r="H9" s="82"/>
+      <c r="H9" s="81"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="147" t="s">
+      <c r="C10" s="146" t="s">
         <v>342</v>
       </c>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="109" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="209"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="173" t="s">
+      <c r="E10" s="208"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="172" t="s">
         <v>525</v>
       </c>
       <c r="H10" s="30" t="s">
@@ -8604,15 +8691,15 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="147" t="s">
+      <c r="C11" s="146" t="s">
         <v>341</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="209"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="173" t="s">
+      <c r="E11" s="208"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="172" t="s">
         <v>526</v>
       </c>
       <c r="H11" s="30"/>
@@ -8621,13 +8708,13 @@
       <c r="B12" s="36">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C12" s="147"/>
+      <c r="C12" s="146"/>
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="210"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="173"/>
+      <c r="E12" s="209"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="172"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
@@ -8637,12 +8724,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="179" t="s">
+      <c r="D13" s="178" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="180"/>
-      <c r="F13" s="180"/>
-      <c r="G13" s="181"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="180"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -8664,154 +8751,154 @@
       </c>
     </row>
     <row r="17" spans="3:6">
-      <c r="C17" s="160"/>
-      <c r="D17" s="160"/>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="159"/>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="160" t="s">
+      <c r="C18" s="159" t="s">
         <v>392</v>
       </c>
-      <c r="D18" s="160"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="160"/>
-      <c r="D19" s="161"/>
-      <c r="E19" s="160"/>
-      <c r="F19" s="160"/>
+      <c r="C19" s="159"/>
+      <c r="D19" s="160"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="160" t="s">
+      <c r="C20" s="159" t="s">
         <v>393</v>
       </c>
-      <c r="D20" s="161"/>
-      <c r="E20" s="160"/>
-      <c r="F20" s="160"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="160"/>
-      <c r="D21" s="161"/>
-      <c r="E21" s="160"/>
-      <c r="F21" s="160"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="160"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="160" t="s">
+      <c r="C22" s="159" t="s">
         <v>394</v>
       </c>
-      <c r="D22" s="161"/>
-      <c r="E22" s="160"/>
-      <c r="F22" s="160"/>
+      <c r="D22" s="160"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
     </row>
     <row r="23" spans="3:6">
-      <c r="C23" s="160" t="s">
+      <c r="C23" s="159" t="s">
         <v>395</v>
       </c>
-      <c r="D23" s="161"/>
-      <c r="E23" s="160"/>
-      <c r="F23" s="160"/>
+      <c r="D23" s="160"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
     </row>
     <row r="24" spans="3:6">
-      <c r="C24" s="160" t="s">
+      <c r="C24" s="159" t="s">
         <v>396</v>
       </c>
-      <c r="D24" s="161"/>
-      <c r="E24" s="160"/>
-      <c r="F24" s="160"/>
+      <c r="D24" s="160"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
     </row>
     <row r="25" spans="3:6">
-      <c r="C25" s="160"/>
-      <c r="D25" s="161"/>
-      <c r="E25" s="160"/>
-      <c r="F25" s="160"/>
+      <c r="C25" s="159"/>
+      <c r="D25" s="160"/>
+      <c r="E25" s="159"/>
+      <c r="F25" s="159"/>
     </row>
     <row r="26" spans="3:6">
-      <c r="C26" s="160" t="s">
+      <c r="C26" s="159" t="s">
         <v>397</v>
       </c>
-      <c r="D26" s="161"/>
-      <c r="E26" s="160"/>
-      <c r="F26" s="160"/>
+      <c r="D26" s="160"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
     </row>
     <row r="27" spans="3:6">
-      <c r="C27" s="160"/>
-      <c r="D27" s="161"/>
-      <c r="E27" s="160"/>
-      <c r="F27" s="160"/>
+      <c r="C27" s="159"/>
+      <c r="D27" s="160"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="159"/>
     </row>
     <row r="28" spans="3:6">
-      <c r="C28" s="160" t="s">
+      <c r="C28" s="159" t="s">
         <v>398</v>
       </c>
-      <c r="D28" s="161"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
     </row>
     <row r="29" spans="3:6">
-      <c r="C29" s="160"/>
-      <c r="D29" s="161"/>
-      <c r="E29" s="160"/>
-      <c r="F29" s="160"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="160"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
     </row>
     <row r="30" spans="3:6">
-      <c r="C30" s="160">
+      <c r="C30" s="159">
         <v>-1</v>
       </c>
-      <c r="D30" s="161"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
     </row>
     <row r="31" spans="3:6">
-      <c r="C31" s="160" t="s">
+      <c r="C31" s="159" t="s">
         <v>399</v>
       </c>
-      <c r="D31" s="161"/>
-      <c r="E31" s="160"/>
-      <c r="F31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="159"/>
     </row>
     <row r="32" spans="3:6">
-      <c r="C32" s="160"/>
-      <c r="D32" s="161"/>
-      <c r="E32" s="160"/>
-      <c r="F32" s="160"/>
+      <c r="C32" s="159"/>
+      <c r="D32" s="160"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
     </row>
     <row r="33" spans="3:6">
-      <c r="C33" s="160" t="s">
+      <c r="C33" s="159" t="s">
         <v>400</v>
       </c>
-      <c r="D33" s="161"/>
-      <c r="E33" s="160"/>
-      <c r="F33" s="160"/>
+      <c r="D33" s="160"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
     </row>
     <row r="34" spans="3:6">
-      <c r="C34" s="160" t="s">
+      <c r="C34" s="159" t="s">
         <v>401</v>
       </c>
-      <c r="D34" s="161"/>
-      <c r="E34" s="160"/>
-      <c r="F34" s="160"/>
+      <c r="D34" s="160"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="159"/>
     </row>
     <row r="35" spans="3:6">
-      <c r="C35" s="160"/>
-      <c r="D35" s="161"/>
-      <c r="E35" s="160"/>
-      <c r="F35" s="160"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="160"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
     </row>
     <row r="36" spans="3:6">
-      <c r="C36" s="160" t="s">
+      <c r="C36" s="159" t="s">
         <v>402</v>
       </c>
-      <c r="D36" s="161"/>
-      <c r="E36" s="160"/>
-      <c r="F36" s="160"/>
+      <c r="D36" s="160"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
     </row>
     <row r="37" spans="3:6">
-      <c r="C37" s="160"/>
-      <c r="D37" s="161"/>
-      <c r="E37" s="160"/>
-      <c r="F37" s="160"/>
+      <c r="C37" s="159"/>
+      <c r="D37" s="160"/>
+      <c r="E37" s="159"/>
+      <c r="F37" s="159"/>
     </row>
     <row r="38" spans="3:6">
       <c r="C38" s="1">
@@ -8978,8 +9065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -8990,15 +9077,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -9026,16 +9113,16 @@
         <v>0.375</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="110" t="s">
+      <c r="F5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="110" t="s">
+      <c r="G5" s="109" t="s">
         <v>143</v>
       </c>
       <c r="H5" s="30"/>
@@ -9051,8 +9138,12 @@
       <c r="E6" s="32" t="s">
         <v>551</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="F6" s="194" t="s">
+        <v>561</v>
+      </c>
+      <c r="G6" s="194" t="s">
+        <v>563</v>
+      </c>
       <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
@@ -9066,8 +9157,8 @@
       <c r="E7" s="32" t="s">
         <v>552</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="196"/>
       <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
@@ -9075,25 +9166,27 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="175"/>
-      <c r="E8" s="175"/>
-      <c r="F8" s="174"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="175"/>
+      <c r="D8" s="173"/>
+      <c r="E8" s="173"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="173"/>
+      <c r="H8" s="173"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="195" t="s">
+      <c r="D9" s="194" t="s">
         <v>546</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>554</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="F9" s="194" t="s">
+        <v>562</v>
+      </c>
+      <c r="G9" s="32"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
@@ -9101,12 +9194,12 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="196"/>
+      <c r="D10" s="195"/>
       <c r="E10" s="32" t="s">
         <v>553</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
@@ -9114,12 +9207,14 @@
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="196"/>
-      <c r="E11" s="195" t="s">
+      <c r="D11" s="195"/>
+      <c r="E11" s="194" t="s">
         <v>554</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="F11" s="195"/>
+      <c r="G11" s="32" t="s">
+        <v>564</v>
+      </c>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
@@ -9127,10 +9222,12 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="197"/>
-      <c r="E12" s="197"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="196"/>
+      <c r="F12" s="196"/>
+      <c r="G12" s="175" t="s">
+        <v>565</v>
+      </c>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
@@ -9141,11 +9238,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="179" t="s">
+      <c r="E13" s="178" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="180"/>
-      <c r="G13" s="181"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="180"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9155,18 +9252,21 @@
         <v>0.75</v>
       </c>
       <c r="C14" s="69"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
       <c r="H14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9179,7 +9279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2AE8B8-BDB7-4F41-A705-8351485C04E1}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -9191,30 +9291,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
-      <c r="B4" s="92"/>
+      <c r="B4" s="91"/>
       <c r="C4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="91" t="s">
         <v>5</v>
       </c>
     </row>
@@ -9306,11 +9406,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="179" t="s">
+      <c r="E13" s="178" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="181"/>
-      <c r="G13" s="80" t="s">
+      <c r="F13" s="180"/>
+      <c r="G13" s="79" t="s">
         <v>30</v>
       </c>
     </row>
@@ -9352,34 +9452,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B4" s="93"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="66" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="92" t="s">
         <v>6</v>
       </c>
     </row>
@@ -9476,14 +9576,14 @@
         <v>0.70833333333333404</v>
       </c>
       <c r="C13" s="68"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="82" t="s">
+      <c r="D13" s="80"/>
+      <c r="E13" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="213" t="s">
+      <c r="F13" s="212" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="214"/>
+      <c r="G13" s="213"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9527,26 +9627,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B4" s="94"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="93" t="s">
         <v>21</v>
       </c>
     </row>
@@ -9669,35 +9769,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="227" t="s">
+      <c r="B2" s="226" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="227"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="227"/>
-      <c r="C3" s="228" t="s">
+      <c r="B3" s="226"/>
+      <c r="C3" s="227" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
-      <c r="H3" s="228"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="227"/>
+      <c r="G3" s="227"/>
+      <c r="H3" s="227"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="227"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
-      <c r="E4" s="228"/>
-      <c r="F4" s="228"/>
-      <c r="G4" s="228"/>
-      <c r="H4" s="228"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="227"/>
+      <c r="D4" s="227"/>
+      <c r="E4" s="227"/>
+      <c r="F4" s="227"/>
+      <c r="G4" s="227"/>
+      <c r="H4" s="227"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -9916,42 +10016,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="229" t="s">
+      <c r="C23" s="228" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="230"/>
-      <c r="E23" s="230"/>
-      <c r="F23" s="230"/>
-      <c r="G23" s="231"/>
+      <c r="D23" s="229"/>
+      <c r="E23" s="229"/>
+      <c r="F23" s="229"/>
+      <c r="G23" s="230"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="221"/>
-      <c r="D24" s="222"/>
-      <c r="E24" s="222"/>
-      <c r="F24" s="222"/>
-      <c r="G24" s="223"/>
+      <c r="C24" s="220"/>
+      <c r="D24" s="221"/>
+      <c r="E24" s="221"/>
+      <c r="F24" s="221"/>
+      <c r="G24" s="222"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="221" t="s">
+      <c r="C25" s="220" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="222"/>
-      <c r="E25" s="222"/>
-      <c r="F25" s="222"/>
-      <c r="G25" s="223"/>
+      <c r="D25" s="221"/>
+      <c r="E25" s="221"/>
+      <c r="F25" s="221"/>
+      <c r="G25" s="222"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="224"/>
-      <c r="D26" s="225"/>
-      <c r="E26" s="225"/>
-      <c r="F26" s="225"/>
-      <c r="G26" s="226"/>
+      <c r="C26" s="223"/>
+      <c r="D26" s="224"/>
+      <c r="E26" s="224"/>
+      <c r="F26" s="224"/>
+      <c r="G26" s="225"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -9979,42 +10079,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="215" t="s">
+      <c r="C28" s="214" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="216"/>
-      <c r="E28" s="216"/>
-      <c r="F28" s="216"/>
-      <c r="G28" s="217"/>
+      <c r="D28" s="215"/>
+      <c r="E28" s="215"/>
+      <c r="F28" s="215"/>
+      <c r="G28" s="216"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="215"/>
-      <c r="D29" s="216"/>
-      <c r="E29" s="216"/>
-      <c r="F29" s="216"/>
-      <c r="G29" s="217"/>
+      <c r="C29" s="214"/>
+      <c r="D29" s="215"/>
+      <c r="E29" s="215"/>
+      <c r="F29" s="215"/>
+      <c r="G29" s="216"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="215" t="s">
+      <c r="C30" s="214" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="216"/>
-      <c r="E30" s="216"/>
-      <c r="F30" s="216"/>
-      <c r="G30" s="217"/>
+      <c r="D30" s="215"/>
+      <c r="E30" s="215"/>
+      <c r="F30" s="215"/>
+      <c r="G30" s="216"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="218"/>
-      <c r="D31" s="219"/>
-      <c r="E31" s="219"/>
-      <c r="F31" s="219"/>
-      <c r="G31" s="220"/>
+      <c r="C31" s="217"/>
+      <c r="D31" s="218"/>
+      <c r="E31" s="218"/>
+      <c r="F31" s="218"/>
+      <c r="G31" s="219"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -10037,8 +10137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:G11"/>
+    <sheetView showGridLines="0" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -10049,35 +10149,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="227" t="s">
+      <c r="B2" s="226" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="227"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="227"/>
-      <c r="C3" s="228" t="s">
+      <c r="B3" s="226"/>
+      <c r="C3" s="227" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
-      <c r="H3" s="228"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="227"/>
+      <c r="G3" s="227"/>
+      <c r="H3" s="227"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="227"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
-      <c r="E4" s="228"/>
-      <c r="F4" s="228"/>
-      <c r="G4" s="228"/>
-      <c r="H4" s="228"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="227"/>
+      <c r="D4" s="227"/>
+      <c r="E4" s="227"/>
+      <c r="F4" s="227"/>
+      <c r="G4" s="227"/>
+      <c r="H4" s="227"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -10133,13 +10233,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="238" t="s">
+      <c r="C8" s="237" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
-      <c r="G8" s="240"/>
+      <c r="D8" s="238"/>
+      <c r="E8" s="238"/>
+      <c r="F8" s="238"/>
+      <c r="G8" s="239"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -10149,20 +10249,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="241"/>
-      <c r="D9" s="242"/>
-      <c r="E9" s="242"/>
-      <c r="F9" s="242"/>
-      <c r="G9" s="243"/>
+      <c r="C9" s="240"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
+      <c r="G9" s="242"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="241"/>
-      <c r="D10" s="242"/>
-      <c r="E10" s="242"/>
-      <c r="F10" s="242"/>
-      <c r="G10" s="243"/>
+      <c r="C10" s="240"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
+      <c r="G10" s="242"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -10173,11 +10273,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="244"/>
-      <c r="D11" s="245"/>
-      <c r="E11" s="245"/>
-      <c r="F11" s="245"/>
-      <c r="G11" s="246"/>
+      <c r="C11" s="243"/>
+      <c r="D11" s="244"/>
+      <c r="E11" s="244"/>
+      <c r="F11" s="244"/>
+      <c r="G11" s="245"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>
@@ -10214,12 +10314,12 @@
       <c r="C13" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="232" t="s">
+      <c r="D13" s="231" t="s">
         <v>542</v>
       </c>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="234"/>
+      <c r="E13" s="232"/>
+      <c r="F13" s="232"/>
+      <c r="G13" s="233"/>
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
@@ -10230,10 +10330,10 @@
     <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
-      <c r="D14" s="232"/>
-      <c r="E14" s="233"/>
-      <c r="F14" s="233"/>
-      <c r="G14" s="234"/>
+      <c r="D14" s="231"/>
+      <c r="E14" s="232"/>
+      <c r="F14" s="232"/>
+      <c r="G14" s="233"/>
       <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
@@ -10244,10 +10344,10 @@
     <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="61"/>
-      <c r="D15" s="232"/>
-      <c r="E15" s="233"/>
-      <c r="F15" s="233"/>
-      <c r="G15" s="234"/>
+      <c r="D15" s="231"/>
+      <c r="E15" s="232"/>
+      <c r="F15" s="232"/>
+      <c r="G15" s="233"/>
       <c r="H15" s="24"/>
       <c r="J15" s="1">
         <v>6827</v>
@@ -10256,10 +10356,10 @@
     <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="63"/>
-      <c r="D16" s="235"/>
-      <c r="E16" s="236"/>
-      <c r="F16" s="236"/>
-      <c r="G16" s="237"/>
+      <c r="D16" s="234"/>
+      <c r="E16" s="235"/>
+      <c r="F16" s="235"/>
+      <c r="G16" s="236"/>
       <c r="H16" s="25"/>
       <c r="J16" s="1">
         <v>0</v>
@@ -10433,7 +10533,7 @@
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="26"/>
-      <c r="C28" s="84" t="s">
+      <c r="C28" s="83" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="39"/>
@@ -10444,7 +10544,7 @@
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="26"/>
-      <c r="C29" s="84"/>
+      <c r="C29" s="83"/>
       <c r="D29" s="39"/>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
@@ -10453,7 +10553,7 @@
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="26"/>
-      <c r="C30" s="84"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="39"/>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
@@ -10462,7 +10562,7 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="27"/>
-      <c r="C31" s="85"/>
+      <c r="C31" s="84"/>
       <c r="D31" s="40"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>

</xml_diff>

<commit_message>
23-01-13 4주 4일차 결산 upload
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B34C98-2C00-471B-B7FA-DA471E46B6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495AA0CF-42F2-4013-B6F6-4411C52DC1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2055" windowWidth="15165" windowHeight="10155" tabRatio="598" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="598" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="586">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2124,6 +2124,50 @@
   </si>
   <si>
     <t>화면설계서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 하이차트 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>html 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈페이지 페이지 1 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈페이지 페이지 2 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈페이지 1,2 연동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt 준비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15개의 html 제작  (페이지 2 화면 구성 수정 필요)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두 번째 페이지 사진 비율 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15개 상품에 대한 정보가 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 코드 분류 및 깃푸쉬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2978,7 +3022,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3739,6 +3783,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5055,9 +5114,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U25" sqref="U25"/>
+      <selection pane="topRight" activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5224,6 +5283,9 @@
       <c r="T2" s="85" t="s">
         <v>566</v>
       </c>
+      <c r="U2" s="85" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="247"/>
@@ -5263,6 +5325,9 @@
       <c r="T3" s="85" t="s">
         <v>567</v>
       </c>
+      <c r="U3" s="85" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="4" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="247"/>
@@ -5417,6 +5482,9 @@
       <c r="S7" s="246"/>
       <c r="T7" s="86" t="s">
         <v>568</v>
+      </c>
+      <c r="U7" s="86" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
@@ -5458,6 +5526,9 @@
       <c r="T8" s="86" t="s">
         <v>569</v>
       </c>
+      <c r="U8" s="86" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="248"/>
@@ -5495,6 +5566,9 @@
       <c r="S9" s="246"/>
       <c r="T9" s="86" t="s">
         <v>570</v>
+      </c>
+      <c r="U9" s="86" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="86" customFormat="1" ht="30" customHeight="1">
@@ -5649,7 +5723,7 @@
       <c r="Q16" s="99"/>
       <c r="S16" s="246"/>
     </row>
-    <row r="17" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:21" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="250" t="s">
         <v>34</v>
       </c>
@@ -5692,8 +5766,11 @@
       <c r="T17" s="88" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="U17" s="88" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A18" s="250"/>
       <c r="B18" s="99"/>
       <c r="C18" s="99"/>
@@ -5716,8 +5793,11 @@
       <c r="T18" s="88" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
+      <c r="U18" s="88" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="250"/>
       <c r="B19" s="99"/>
       <c r="C19" s="99"/>
@@ -5736,7 +5816,7 @@
       </c>
       <c r="S19" s="246"/>
     </row>
-    <row r="20" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:21" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="250"/>
       <c r="B20" s="99"/>
       <c r="C20" s="99"/>
@@ -5754,7 +5834,7 @@
       </c>
       <c r="S20" s="246"/>
     </row>
-    <row r="21" spans="1:20" s="88" customFormat="1" ht="30" customHeight="1">
+    <row r="21" spans="1:21" s="88" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="250"/>
       <c r="B21" s="99"/>
       <c r="C21" s="99"/>
@@ -5770,7 +5850,7 @@
       <c r="Q21" s="99"/>
       <c r="S21" s="246"/>
     </row>
-    <row r="22" spans="1:20" s="99" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:21" s="99" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="106"/>
       <c r="M22" t="s">
         <v>442</v>
@@ -5779,7 +5859,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="108" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:21" s="108" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="107" t="s">
         <v>68</v>
       </c>
@@ -5831,8 +5911,11 @@
       <c r="T23" s="107" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" ht="30" customHeight="1">
+      <c r="U23" s="107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -5878,8 +5961,11 @@
       <c r="T24" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="30" customHeight="1">
+      <c r="U24" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -5919,8 +6005,11 @@
       <c r="T25" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="30" customHeight="1">
+      <c r="U25" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5951,8 +6040,11 @@
       <c r="T26" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="30" customHeight="1">
+      <c r="U26" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5984,7 +6076,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="30" customHeight="1">
+    <row r="28" spans="1:21" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -6007,7 +6099,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="30" customHeight="1">
+    <row r="29" spans="1:21" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -6033,7 +6125,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="30" customHeight="1">
+    <row r="30" spans="1:21" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -6050,7 +6142,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="30" customHeight="1">
+    <row r="31" spans="1:21" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -6064,7 +6156,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="30" customHeight="1">
+    <row r="32" spans="1:21" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -7845,7 +7937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7F205-591C-4211-BBE2-E0A0EC11B8A9}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -8529,7 +8621,7 @@
   <dimension ref="B2:H69"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9065,8 +9157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:G13"/>
+    <sheetView showGridLines="0" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9125,7 +9217,9 @@
       <c r="G5" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="30"/>
+      <c r="H5" s="30" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
       <c r="B6" s="36">
@@ -9144,7 +9238,9 @@
       <c r="G6" s="194" t="s">
         <v>563</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="H6" s="254" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
       <c r="B7" s="36">
@@ -9159,7 +9255,7 @@
       </c>
       <c r="F7" s="196"/>
       <c r="G7" s="196"/>
-      <c r="H7" s="30"/>
+      <c r="H7" s="255"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
       <c r="B8" s="36">
@@ -9187,7 +9283,9 @@
         <v>562</v>
       </c>
       <c r="G9" s="32"/>
-      <c r="H9" s="30"/>
+      <c r="H9" s="256" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
       <c r="B10" s="36">
@@ -9200,7 +9298,7 @@
       </c>
       <c r="F10" s="195"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="30"/>
+      <c r="H10" s="257"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
       <c r="B11" s="36">
@@ -9215,7 +9313,7 @@
       <c r="G11" s="32" t="s">
         <v>564</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="257"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -9228,7 +9326,7 @@
       <c r="G12" s="175" t="s">
         <v>565</v>
       </c>
-      <c r="H12" s="30"/>
+      <c r="H12" s="258"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -9259,7 +9357,7 @@
       <c r="H14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="D9:D12"/>
@@ -9267,6 +9365,8 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F9:F12"/>
     <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H9:H12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2023-01-25 6주 1일차 결산
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1E999B-1F2E-42A8-92DE-0A522B8FFFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E97434B-C7DF-4787-AD8E-1DD6DB0FFD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="637">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2328,6 +2328,50 @@
   </si>
   <si>
     <t>1. 스택틱 막대그래프 : 리뷰데이터 비율 만큼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax 그래프 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 그래프 재설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax 상품 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주간 보고서 써야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈페이지 배치 확인해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 분류 ajax 끝내기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 결과 자료 끝내기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼품리뷰수 그래프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품(제로음료) 맛 종류 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt 준비 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json파일 만들어야함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3717,6 +3761,12 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="13" fillId="26" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3977,12 +4027,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="26" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4727,14 +4771,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -4758,12 +4802,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="192" t="s">
+      <c r="C5" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
+      <c r="D5" s="195"/>
+      <c r="E5" s="195"/>
+      <c r="F5" s="195"/>
       <c r="G5" s="109" t="s">
         <v>108</v>
       </c>
@@ -4778,7 +4822,7 @@
       <c r="D6" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="187" t="s">
+      <c r="E6" s="189" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4796,7 +4840,7 @@
       <c r="D7" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="188"/>
+      <c r="E7" s="190"/>
       <c r="F7" s="108" t="s">
         <v>107</v>
       </c>
@@ -4818,19 +4862,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="181" t="s">
+      <c r="C9" s="183" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="184" t="s">
+      <c r="D9" s="186" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="184" t="s">
+      <c r="E9" s="186" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="189" t="s">
+      <c r="F9" s="191" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="194" t="s">
+      <c r="G9" s="196" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4838,21 +4882,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="182"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="195"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="187"/>
+      <c r="E10" s="187"/>
+      <c r="F10" s="192"/>
+      <c r="G10" s="197"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="183"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="185"/>
-      <c r="F11" s="190"/>
-      <c r="G11" s="195"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="187"/>
+      <c r="F11" s="192"/>
+      <c r="G11" s="197"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4862,9 +4906,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="186"/>
-      <c r="F12" s="191"/>
-      <c r="G12" s="196"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="198"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4873,11 +4917,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="178" t="s">
+      <c r="D13" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="179"/>
-      <c r="F13" s="180"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="182"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -4945,35 +4989,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="232" t="s">
+      <c r="B2" s="234" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="232"/>
-      <c r="C3" s="233" t="s">
+      <c r="B3" s="234"/>
+      <c r="C3" s="235" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
+      <c r="D3" s="235"/>
+      <c r="E3" s="235"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="235"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="232"/>
-      <c r="C4" s="233"/>
-      <c r="D4" s="233"/>
-      <c r="E4" s="233"/>
-      <c r="F4" s="233"/>
-      <c r="G4" s="233"/>
-      <c r="H4" s="233"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="235"/>
+      <c r="F4" s="235"/>
+      <c r="G4" s="235"/>
+      <c r="H4" s="235"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -5298,9 +5342,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y47" sqref="Y47"/>
+      <selection pane="topRight" activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5316,6 +5360,8 @@
     <col min="13" max="13" width="47.25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="43.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="42" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1">
@@ -5414,7 +5460,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="256" t="s">
+      <c r="A2" s="258" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="98" t="s">
@@ -5432,7 +5478,7 @@
       <c r="F2" s="98" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="260" t="s">
+      <c r="G2" s="262" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="98"/>
@@ -5462,7 +5508,7 @@
       <c r="R2" s="84" t="s">
         <v>549</v>
       </c>
-      <c r="S2" s="255" t="s">
+      <c r="S2" s="257" t="s">
         <v>555</v>
       </c>
       <c r="T2" s="84" t="s">
@@ -5474,15 +5520,15 @@
       <c r="W2" s="84" t="s">
         <v>588</v>
       </c>
-      <c r="X2" s="255" t="s">
+      <c r="X2" s="257" t="s">
         <v>598</v>
       </c>
-      <c r="Y2" s="255" t="s">
+      <c r="Y2" s="257" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="256"/>
+      <c r="A3" s="258"/>
       <c r="B3" s="98" t="s">
         <v>43</v>
       </c>
@@ -5496,7 +5542,7 @@
       <c r="F3" s="98" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="260"/>
+      <c r="G3" s="262"/>
       <c r="H3" s="98"/>
       <c r="I3" s="111" t="s">
         <v>164</v>
@@ -5515,18 +5561,18 @@
       </c>
       <c r="Q3" s="98"/>
       <c r="R3" s="173"/>
-      <c r="S3" s="255"/>
+      <c r="S3" s="257"/>
       <c r="T3" s="84" t="s">
         <v>567</v>
       </c>
       <c r="U3" s="84" t="s">
         <v>576</v>
       </c>
-      <c r="X3" s="255"/>
-      <c r="Y3" s="255"/>
+      <c r="X3" s="257"/>
+      <c r="Y3" s="257"/>
     </row>
     <row r="4" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="256"/>
+      <c r="A4" s="258"/>
       <c r="B4" s="100" t="s">
         <v>44</v>
       </c>
@@ -5538,7 +5584,7 @@
       <c r="F4" s="98" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="260"/>
+      <c r="G4" s="262"/>
       <c r="H4" s="98"/>
       <c r="I4" s="98" t="s">
         <v>165</v>
@@ -5561,15 +5607,18 @@
       <c r="R4" s="84" t="s">
         <v>547</v>
       </c>
-      <c r="S4" s="255"/>
+      <c r="S4" s="257"/>
       <c r="W4" s="84" t="s">
         <v>597</v>
       </c>
-      <c r="X4" s="255"/>
-      <c r="Y4" s="255"/>
+      <c r="X4" s="257"/>
+      <c r="Y4" s="257"/>
+      <c r="AA4" s="84" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="256"/>
+      <c r="A5" s="258"/>
       <c r="B5" s="100" t="s">
         <v>45</v>
       </c>
@@ -5583,7 +5632,7 @@
       <c r="F5" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="260"/>
+      <c r="G5" s="262"/>
       <c r="H5" s="98"/>
       <c r="I5" s="98" t="s">
         <v>166</v>
@@ -5598,12 +5647,12 @@
         <v>430</v>
       </c>
       <c r="Q5" s="98"/>
-      <c r="S5" s="255"/>
-      <c r="X5" s="255"/>
-      <c r="Y5" s="255"/>
+      <c r="S5" s="257"/>
+      <c r="X5" s="257"/>
+      <c r="Y5" s="257"/>
     </row>
     <row r="6" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="256"/>
+      <c r="A6" s="258"/>
       <c r="B6" s="98" t="s">
         <v>46</v>
       </c>
@@ -5619,7 +5668,7 @@
       <c r="F6" s="98" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="260"/>
+      <c r="G6" s="262"/>
       <c r="H6" s="98"/>
       <c r="I6" s="98" t="s">
         <v>168</v>
@@ -5631,12 +5680,12 @@
       <c r="Q6" s="98" t="s">
         <v>535</v>
       </c>
-      <c r="S6" s="255"/>
-      <c r="X6" s="255"/>
-      <c r="Y6" s="255"/>
+      <c r="S6" s="257"/>
+      <c r="X6" s="257"/>
+      <c r="Y6" s="257"/>
     </row>
     <row r="7" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="257" t="s">
+      <c r="A7" s="259" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="98" t="s">
@@ -5652,7 +5701,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="98"/>
-      <c r="G7" s="260"/>
+      <c r="G7" s="262"/>
       <c r="H7" s="98" t="s">
         <v>150</v>
       </c>
@@ -5684,7 +5733,7 @@
       <c r="R7" s="85" t="s">
         <v>549</v>
       </c>
-      <c r="S7" s="255"/>
+      <c r="S7" s="257"/>
       <c r="T7" s="85" t="s">
         <v>568</v>
       </c>
@@ -5694,11 +5743,11 @@
       <c r="W7" s="84" t="s">
         <v>588</v>
       </c>
-      <c r="X7" s="255"/>
-      <c r="Y7" s="255"/>
+      <c r="X7" s="257"/>
+      <c r="Y7" s="257"/>
     </row>
     <row r="8" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="257"/>
+      <c r="A8" s="259"/>
       <c r="B8" s="98" t="s">
         <v>48</v>
       </c>
@@ -5710,7 +5759,7 @@
       </c>
       <c r="E8" s="98"/>
       <c r="F8" s="98"/>
-      <c r="G8" s="260"/>
+      <c r="G8" s="262"/>
       <c r="H8" s="98" t="s">
         <v>151</v>
       </c>
@@ -5732,7 +5781,7 @@
       <c r="Q8" s="98" t="s">
         <v>536</v>
       </c>
-      <c r="S8" s="255"/>
+      <c r="S8" s="257"/>
       <c r="T8" s="85" t="s">
         <v>569</v>
       </c>
@@ -5742,11 +5791,14 @@
       <c r="W8" s="85" t="s">
         <v>586</v>
       </c>
-      <c r="X8" s="255"/>
-      <c r="Y8" s="255"/>
+      <c r="X8" s="257"/>
+      <c r="Y8" s="257"/>
+      <c r="AA8" s="85" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="257"/>
+      <c r="A9" s="259"/>
       <c r="B9" s="98" t="s">
         <v>73</v>
       </c>
@@ -5758,7 +5810,7 @@
       </c>
       <c r="E9" s="98"/>
       <c r="F9" s="98"/>
-      <c r="G9" s="260"/>
+      <c r="G9" s="262"/>
       <c r="H9" s="98" t="s">
         <v>152</v>
       </c>
@@ -5778,18 +5830,18 @@
       <c r="R9" s="85" t="s">
         <v>550</v>
       </c>
-      <c r="S9" s="255"/>
+      <c r="S9" s="257"/>
       <c r="T9" s="85" t="s">
         <v>570</v>
       </c>
       <c r="U9" s="85" t="s">
         <v>580</v>
       </c>
-      <c r="X9" s="255"/>
-      <c r="Y9" s="255"/>
+      <c r="X9" s="257"/>
+      <c r="Y9" s="257"/>
     </row>
     <row r="10" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="257"/>
+      <c r="A10" s="259"/>
       <c r="B10" s="100" t="s">
         <v>74</v>
       </c>
@@ -5801,7 +5853,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="98"/>
-      <c r="G10" s="260"/>
+      <c r="G10" s="262"/>
       <c r="H10" s="98"/>
       <c r="I10" s="98"/>
       <c r="K10" s="85" t="s">
@@ -5813,12 +5865,12 @@
       <c r="Q10" s="98" t="s">
         <v>538</v>
       </c>
-      <c r="S10" s="255"/>
-      <c r="X10" s="255"/>
-      <c r="Y10" s="255"/>
+      <c r="S10" s="257"/>
+      <c r="X10" s="257"/>
+      <c r="Y10" s="257"/>
     </row>
     <row r="11" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="257"/>
+      <c r="A11" s="259"/>
       <c r="B11" s="100" t="s">
         <v>75</v>
       </c>
@@ -5830,19 +5882,19 @@
         <v>118</v>
       </c>
       <c r="F11" s="98"/>
-      <c r="G11" s="260"/>
+      <c r="G11" s="262"/>
       <c r="H11" s="98"/>
       <c r="I11" s="98"/>
       <c r="M11" t="s">
         <v>436</v>
       </c>
       <c r="Q11" s="98"/>
-      <c r="S11" s="255"/>
-      <c r="X11" s="255"/>
-      <c r="Y11" s="255"/>
+      <c r="S11" s="257"/>
+      <c r="X11" s="257"/>
+      <c r="Y11" s="257"/>
     </row>
     <row r="12" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="258" t="s">
+      <c r="A12" s="260" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="101" t="s">
@@ -5856,7 +5908,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="98"/>
-      <c r="G12" s="260"/>
+      <c r="G12" s="262"/>
       <c r="H12" s="98" t="s">
         <v>153</v>
       </c>
@@ -5869,17 +5921,17 @@
       </c>
       <c r="M12"/>
       <c r="Q12" s="98"/>
-      <c r="S12" s="255"/>
+      <c r="S12" s="257"/>
     </row>
     <row r="13" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="258"/>
+      <c r="A13" s="260"/>
       <c r="C13" s="98"/>
       <c r="D13" s="98"/>
       <c r="E13" s="98" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="98"/>
-      <c r="G13" s="260"/>
+      <c r="G13" s="262"/>
       <c r="H13" s="98" t="s">
         <v>154</v>
       </c>
@@ -5891,15 +5943,15 @@
         <v>437</v>
       </c>
       <c r="Q13" s="98"/>
-      <c r="S13" s="255"/>
+      <c r="S13" s="257"/>
     </row>
     <row r="14" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="258"/>
+      <c r="A14" s="260"/>
       <c r="C14" s="98"/>
       <c r="D14" s="98"/>
       <c r="E14" s="98"/>
       <c r="F14" s="98"/>
-      <c r="G14" s="260"/>
+      <c r="G14" s="262"/>
       <c r="H14" s="98" t="s">
         <v>155</v>
       </c>
@@ -5908,44 +5960,44 @@
         <v>438</v>
       </c>
       <c r="Q14" s="98"/>
-      <c r="S14" s="255"/>
+      <c r="S14" s="257"/>
     </row>
     <row r="15" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="258"/>
+      <c r="A15" s="260"/>
       <c r="C15" s="98"/>
       <c r="D15" s="98"/>
       <c r="E15" s="98" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="98"/>
-      <c r="G15" s="260"/>
+      <c r="G15" s="262"/>
       <c r="H15" s="98" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="98"/>
       <c r="M15"/>
       <c r="Q15" s="98"/>
-      <c r="S15" s="255"/>
+      <c r="S15" s="257"/>
     </row>
     <row r="16" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="258"/>
+      <c r="A16" s="260"/>
       <c r="C16" s="98"/>
       <c r="D16" s="98"/>
       <c r="E16" s="98" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="98"/>
-      <c r="G16" s="260"/>
+      <c r="G16" s="262"/>
       <c r="H16" s="98" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="98"/>
       <c r="M16"/>
       <c r="Q16" s="98"/>
-      <c r="S16" s="255"/>
-    </row>
-    <row r="17" spans="1:25" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="259" t="s">
+      <c r="S16" s="257"/>
+    </row>
+    <row r="17" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="261" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="98"/>
@@ -5953,7 +6005,7 @@
       <c r="D17" s="98"/>
       <c r="E17" s="98"/>
       <c r="F17" s="98"/>
-      <c r="G17" s="260"/>
+      <c r="G17" s="262"/>
       <c r="H17" s="98"/>
       <c r="I17" s="98"/>
       <c r="J17" s="87" t="s">
@@ -5983,7 +6035,7 @@
       <c r="R17" s="87" t="s">
         <v>549</v>
       </c>
-      <c r="S17" s="255"/>
+      <c r="S17" s="257"/>
       <c r="T17" s="87" t="s">
         <v>568</v>
       </c>
@@ -5997,14 +6049,14 @@
         <v>606</v>
       </c>
     </row>
-    <row r="18" spans="1:25" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="259"/>
+    <row r="18" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="261"/>
       <c r="B18" s="98"/>
       <c r="C18" s="98"/>
       <c r="D18" s="98"/>
       <c r="E18" s="98"/>
       <c r="F18" s="98"/>
-      <c r="G18" s="260"/>
+      <c r="G18" s="262"/>
       <c r="H18" s="98"/>
       <c r="I18" s="98"/>
       <c r="L18" s="87" t="s">
@@ -6016,7 +6068,7 @@
       <c r="Q18" s="98" t="s">
         <v>539</v>
       </c>
-      <c r="S18" s="255"/>
+      <c r="S18" s="257"/>
       <c r="T18" s="87" t="s">
         <v>571</v>
       </c>
@@ -6027,14 +6079,14 @@
         <v>596</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="259"/>
+    <row r="19" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="261"/>
       <c r="B19" s="98"/>
       <c r="C19" s="98"/>
       <c r="D19" s="98"/>
       <c r="E19" s="98"/>
       <c r="F19" s="98"/>
-      <c r="G19" s="260"/>
+      <c r="G19" s="262"/>
       <c r="H19" s="98"/>
       <c r="I19" s="98"/>
       <c r="M19" t="s">
@@ -6044,16 +6096,19 @@
       <c r="R19" s="87" t="s">
         <v>548</v>
       </c>
-      <c r="S19" s="255"/>
-    </row>
-    <row r="20" spans="1:25" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="259"/>
+      <c r="S19" s="257"/>
+      <c r="AA19" s="87" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="261"/>
       <c r="B20" s="98"/>
       <c r="C20" s="98"/>
       <c r="D20" s="98"/>
       <c r="E20" s="98"/>
       <c r="F20" s="98"/>
-      <c r="G20" s="260"/>
+      <c r="G20" s="262"/>
       <c r="H20" s="98"/>
       <c r="I20" s="98"/>
       <c r="M20" t="s">
@@ -6062,25 +6117,25 @@
       <c r="Q20" s="98" t="s">
         <v>540</v>
       </c>
-      <c r="S20" s="255"/>
-    </row>
-    <row r="21" spans="1:25" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="259"/>
+      <c r="S20" s="257"/>
+    </row>
+    <row r="21" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="261"/>
       <c r="B21" s="98"/>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
       <c r="E21" s="98"/>
       <c r="F21" s="98"/>
-      <c r="G21" s="260"/>
+      <c r="G21" s="262"/>
       <c r="H21" s="98"/>
       <c r="I21" s="98"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
       <c r="Q21" s="98"/>
-      <c r="S21" s="255"/>
-    </row>
-    <row r="22" spans="1:25" s="98" customFormat="1" ht="30" customHeight="1">
+      <c r="S21" s="257"/>
+    </row>
+    <row r="22" spans="1:27" s="98" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="105"/>
       <c r="M22" t="s">
         <v>442</v>
@@ -6089,7 +6144,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="107" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:27" s="107" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="106" t="s">
         <v>68</v>
       </c>
@@ -6153,8 +6208,11 @@
       <c r="Y23" s="106" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="30" customHeight="1">
+      <c r="AA23" s="107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -6213,7 +6271,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="30" customHeight="1">
+    <row r="25" spans="1:27" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -6265,8 +6323,11 @@
       <c r="Y25" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" ht="30" customHeight="1">
+      <c r="AA25" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -6306,8 +6367,11 @@
       <c r="Y26" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" ht="30" customHeight="1">
+      <c r="AA26" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -6344,8 +6408,11 @@
       <c r="X27" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" ht="30" customHeight="1">
+      <c r="AA27" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -6370,8 +6437,11 @@
       <c r="Y28" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" ht="30" customHeight="1">
+      <c r="AA28" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -6399,8 +6469,11 @@
       <c r="Y29" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" ht="30" customHeight="1">
+      <c r="AA29" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -6419,8 +6492,11 @@
       <c r="Y30" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" ht="30" customHeight="1">
+      <c r="AA30" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -6436,8 +6512,11 @@
       <c r="Y31" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" ht="30" customHeight="1">
+      <c r="AA31" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -6455,6 +6534,9 @@
       </c>
       <c r="Y32" s="87" t="s">
         <v>614</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="30" customHeight="1">
@@ -7954,22 +8036,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="155"/>
-      <c r="C2" s="261" t="s">
+      <c r="C2" s="263" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="261"/>
-      <c r="E2" s="261" t="s">
+      <c r="D2" s="263"/>
+      <c r="E2" s="263" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="261"/>
-      <c r="G2" s="261" t="s">
+      <c r="F2" s="263"/>
+      <c r="G2" s="263" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261" t="s">
+      <c r="H2" s="263"/>
+      <c r="I2" s="263" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="262"/>
+      <c r="J2" s="264"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -8748,14 +8830,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="88"/>
@@ -8799,19 +8881,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="197" t="s">
+      <c r="C6" s="199" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="184" t="s">
+      <c r="D6" s="186" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="202" t="s">
+      <c r="E6" s="204" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="205" t="s">
+      <c r="G6" s="207" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8819,13 +8901,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="198"/>
-      <c r="D7" s="186"/>
-      <c r="E7" s="203"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="205"/>
       <c r="F7" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="206"/>
+      <c r="G7" s="208"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="95">
@@ -8841,13 +8923,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="199" t="s">
+      <c r="C9" s="201" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="184" t="s">
+      <c r="D9" s="186" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="202"/>
+      <c r="E9" s="204"/>
       <c r="F9" s="112" t="s">
         <v>247</v>
       </c>
@@ -8859,9 +8941,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="200"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="204"/>
+      <c r="C10" s="202"/>
+      <c r="D10" s="187"/>
+      <c r="E10" s="206"/>
       <c r="F10" s="112" t="s">
         <v>246</v>
       </c>
@@ -8871,9 +8953,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="201"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="204"/>
+      <c r="C11" s="203"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="206"/>
       <c r="F11" s="112" t="s">
         <v>248</v>
       </c>
@@ -8886,8 +8968,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="186"/>
-      <c r="E12" s="203"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="205"/>
       <c r="F12" s="112" t="s">
         <v>249</v>
       </c>
@@ -8900,11 +8982,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="178" t="s">
+      <c r="D13" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="179"/>
-      <c r="F13" s="179"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="181"/>
       <c r="G13" s="126" t="s">
         <v>30</v>
       </c>
@@ -8956,15 +9038,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="89"/>
@@ -9024,7 +9106,7 @@
       <c r="F6" s="110" t="s">
         <v>523</v>
       </c>
-      <c r="G6" s="210" t="s">
+      <c r="G6" s="212" t="s">
         <v>521</v>
       </c>
       <c r="H6" s="30" t="s">
@@ -9045,7 +9127,7 @@
       <c r="F7" s="110" t="s">
         <v>520</v>
       </c>
-      <c r="G7" s="211"/>
+      <c r="G7" s="213"/>
       <c r="H7" s="30" t="s">
         <v>530</v>
       </c>
@@ -9071,7 +9153,7 @@
       <c r="D9" s="166" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="207" t="s">
+      <c r="E9" s="209" t="s">
         <v>469</v>
       </c>
       <c r="F9" s="110" t="s">
@@ -9092,7 +9174,7 @@
       <c r="D10" s="108" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="208"/>
+      <c r="E10" s="210"/>
       <c r="F10" s="110"/>
       <c r="G10" s="171" t="s">
         <v>525</v>
@@ -9111,7 +9193,7 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="208"/>
+      <c r="E11" s="210"/>
       <c r="F11" s="110"/>
       <c r="G11" s="171" t="s">
         <v>526</v>
@@ -9126,7 +9208,7 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="209"/>
+      <c r="E12" s="211"/>
       <c r="F12" s="110"/>
       <c r="G12" s="171"/>
       <c r="H12" s="30"/>
@@ -9138,12 +9220,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="178" t="s">
+      <c r="D13" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="179"/>
-      <c r="F13" s="179"/>
-      <c r="G13" s="180"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="181"/>
+      <c r="G13" s="182"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9491,15 +9573,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -9554,13 +9636,13 @@
       <c r="E6" s="32" t="s">
         <v>551</v>
       </c>
-      <c r="F6" s="194" t="s">
+      <c r="F6" s="196" t="s">
         <v>561</v>
       </c>
-      <c r="G6" s="194" t="s">
+      <c r="G6" s="196" t="s">
         <v>563</v>
       </c>
-      <c r="H6" s="212" t="s">
+      <c r="H6" s="214" t="s">
         <v>530</v>
       </c>
     </row>
@@ -9575,9 +9657,9 @@
       <c r="E7" s="32" t="s">
         <v>552</v>
       </c>
-      <c r="F7" s="196"/>
-      <c r="G7" s="196"/>
-      <c r="H7" s="213"/>
+      <c r="F7" s="198"/>
+      <c r="G7" s="198"/>
+      <c r="H7" s="215"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
       <c r="B8" s="36">
@@ -9595,17 +9677,17 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="194" t="s">
+      <c r="D9" s="196" t="s">
         <v>546</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>554</v>
       </c>
-      <c r="F9" s="194" t="s">
+      <c r="F9" s="196" t="s">
         <v>562</v>
       </c>
       <c r="G9" s="32"/>
-      <c r="H9" s="214" t="s">
+      <c r="H9" s="216" t="s">
         <v>582</v>
       </c>
     </row>
@@ -9614,41 +9696,41 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="195"/>
+      <c r="D10" s="197"/>
       <c r="E10" s="32" t="s">
         <v>553</v>
       </c>
-      <c r="F10" s="195"/>
+      <c r="F10" s="197"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="215"/>
+      <c r="H10" s="217"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="195"/>
-      <c r="E11" s="194" t="s">
+      <c r="D11" s="197"/>
+      <c r="E11" s="196" t="s">
         <v>554</v>
       </c>
-      <c r="F11" s="195"/>
+      <c r="F11" s="197"/>
       <c r="G11" s="32" t="s">
         <v>564</v>
       </c>
-      <c r="H11" s="215"/>
+      <c r="H11" s="217"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
       <c r="B12" s="36">
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="196"/>
-      <c r="E12" s="196"/>
-      <c r="F12" s="196"/>
+      <c r="D12" s="198"/>
+      <c r="E12" s="198"/>
+      <c r="F12" s="198"/>
       <c r="G12" s="174" t="s">
         <v>565</v>
       </c>
-      <c r="H12" s="216"/>
+      <c r="H12" s="218"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -9658,11 +9740,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="178" t="s">
+      <c r="E13" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="179"/>
-      <c r="G13" s="180"/>
+      <c r="F13" s="181"/>
+      <c r="G13" s="182"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9713,14 +9795,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -9745,13 +9827,13 @@
         <v>0.375</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="217" t="s">
+      <c r="D5" s="219" t="s">
         <v>586</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="217" t="s">
+      <c r="F5" s="219" t="s">
         <v>600</v>
       </c>
       <c r="G5" s="70"/>
@@ -9761,11 +9843,11 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="195"/>
-      <c r="E6" s="187" t="s">
+      <c r="D6" s="197"/>
+      <c r="E6" s="189" t="s">
         <v>592</v>
       </c>
-      <c r="F6" s="195"/>
+      <c r="F6" s="197"/>
       <c r="G6" s="70"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1">
@@ -9773,30 +9855,30 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="196"/>
-      <c r="E7" s="188"/>
-      <c r="F7" s="196"/>
+      <c r="D7" s="198"/>
+      <c r="E7" s="190"/>
+      <c r="F7" s="198"/>
       <c r="G7" s="70"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="36">
         <v>0.5</v>
       </c>
-      <c r="C8" s="263"/>
-      <c r="D8" s="264"/>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
-      <c r="G8" s="264"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="177"/>
+      <c r="F8" s="177"/>
+      <c r="G8" s="177"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1">
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="194" t="s">
+      <c r="D9" s="196" t="s">
         <v>587</v>
       </c>
-      <c r="E9" s="194" t="s">
+      <c r="E9" s="196" t="s">
         <v>593</v>
       </c>
       <c r="F9" s="31" t="s">
@@ -9809,8 +9891,8 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="195"/>
-      <c r="E10" s="195"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
       <c r="F10" s="31" t="s">
         <v>595</v>
       </c>
@@ -9821,8 +9903,8 @@
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="195"/>
-      <c r="E11" s="195"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
       <c r="F11" s="31"/>
       <c r="G11" s="70"/>
     </row>
@@ -9831,8 +9913,8 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="196"/>
-      <c r="E12" s="196"/>
+      <c r="D12" s="198"/>
+      <c r="E12" s="198"/>
       <c r="F12" s="31"/>
       <c r="G12" s="70"/>
     </row>
@@ -9844,10 +9926,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="178" t="s">
+      <c r="E13" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="180"/>
+      <c r="F13" s="182"/>
       <c r="G13" s="175" t="s">
         <v>30</v>
       </c>
@@ -9883,8 +9965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA729C5-F4A6-4AC1-AD36-A96A4028E1F4}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -9895,15 +9977,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -10023,10 +10105,10 @@
       <c r="E13" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="218" t="s">
+      <c r="F13" s="220" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="219"/>
+      <c r="G13" s="221"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -10070,13 +10152,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -10212,35 +10294,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="232" t="s">
+      <c r="B2" s="234" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="232"/>
-      <c r="C3" s="233" t="s">
+      <c r="B3" s="234"/>
+      <c r="C3" s="235" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
+      <c r="D3" s="235"/>
+      <c r="E3" s="235"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="235"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="232"/>
-      <c r="C4" s="233"/>
-      <c r="D4" s="233"/>
-      <c r="E4" s="233"/>
-      <c r="F4" s="233"/>
-      <c r="G4" s="233"/>
-      <c r="H4" s="233"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="235"/>
+      <c r="F4" s="235"/>
+      <c r="G4" s="235"/>
+      <c r="H4" s="235"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -10459,42 +10541,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="234" t="s">
+      <c r="C23" s="236" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="235"/>
-      <c r="E23" s="235"/>
-      <c r="F23" s="235"/>
-      <c r="G23" s="236"/>
+      <c r="D23" s="237"/>
+      <c r="E23" s="237"/>
+      <c r="F23" s="237"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="226"/>
-      <c r="D24" s="227"/>
-      <c r="E24" s="227"/>
-      <c r="F24" s="227"/>
-      <c r="G24" s="228"/>
+      <c r="C24" s="228"/>
+      <c r="D24" s="229"/>
+      <c r="E24" s="229"/>
+      <c r="F24" s="229"/>
+      <c r="G24" s="230"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="226" t="s">
+      <c r="C25" s="228" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="227"/>
-      <c r="E25" s="227"/>
-      <c r="F25" s="227"/>
-      <c r="G25" s="228"/>
+      <c r="D25" s="229"/>
+      <c r="E25" s="229"/>
+      <c r="F25" s="229"/>
+      <c r="G25" s="230"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="229"/>
-      <c r="D26" s="230"/>
-      <c r="E26" s="230"/>
-      <c r="F26" s="230"/>
-      <c r="G26" s="231"/>
+      <c r="C26" s="231"/>
+      <c r="D26" s="232"/>
+      <c r="E26" s="232"/>
+      <c r="F26" s="232"/>
+      <c r="G26" s="233"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -10522,42 +10604,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="220" t="s">
+      <c r="C28" s="222" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="221"/>
-      <c r="E28" s="221"/>
-      <c r="F28" s="221"/>
-      <c r="G28" s="222"/>
+      <c r="D28" s="223"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="220"/>
-      <c r="D29" s="221"/>
-      <c r="E29" s="221"/>
-      <c r="F29" s="221"/>
-      <c r="G29" s="222"/>
+      <c r="C29" s="222"/>
+      <c r="D29" s="223"/>
+      <c r="E29" s="223"/>
+      <c r="F29" s="223"/>
+      <c r="G29" s="224"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="220" t="s">
+      <c r="C30" s="222" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="221"/>
-      <c r="E30" s="221"/>
-      <c r="F30" s="221"/>
-      <c r="G30" s="222"/>
+      <c r="D30" s="223"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="223"/>
-      <c r="D31" s="224"/>
-      <c r="E31" s="224"/>
-      <c r="F31" s="224"/>
-      <c r="G31" s="225"/>
+      <c r="C31" s="225"/>
+      <c r="D31" s="226"/>
+      <c r="E31" s="226"/>
+      <c r="F31" s="226"/>
+      <c r="G31" s="227"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -10580,8 +10662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -10592,35 +10674,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="232" t="s">
+      <c r="B2" s="234" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="232"/>
-      <c r="C3" s="233" t="s">
+      <c r="B3" s="234"/>
+      <c r="C3" s="235" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
+      <c r="D3" s="235"/>
+      <c r="E3" s="235"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="235"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="232"/>
-      <c r="C4" s="233"/>
-      <c r="D4" s="233"/>
-      <c r="E4" s="233"/>
-      <c r="F4" s="233"/>
-      <c r="G4" s="233"/>
-      <c r="H4" s="233"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="235"/>
+      <c r="F4" s="235"/>
+      <c r="G4" s="235"/>
+      <c r="H4" s="235"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -10676,13 +10758,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="246" t="s">
+      <c r="C8" s="248" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="247"/>
-      <c r="E8" s="247"/>
-      <c r="F8" s="247"/>
-      <c r="G8" s="248"/>
+      <c r="D8" s="249"/>
+      <c r="E8" s="249"/>
+      <c r="F8" s="249"/>
+      <c r="G8" s="250"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -10692,20 +10774,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="249"/>
-      <c r="D9" s="250"/>
-      <c r="E9" s="250"/>
-      <c r="F9" s="250"/>
-      <c r="G9" s="251"/>
+      <c r="C9" s="251"/>
+      <c r="D9" s="252"/>
+      <c r="E9" s="252"/>
+      <c r="F9" s="252"/>
+      <c r="G9" s="253"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="249"/>
-      <c r="D10" s="250"/>
-      <c r="E10" s="250"/>
-      <c r="F10" s="250"/>
-      <c r="G10" s="251"/>
+      <c r="C10" s="251"/>
+      <c r="D10" s="252"/>
+      <c r="E10" s="252"/>
+      <c r="F10" s="252"/>
+      <c r="G10" s="253"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -10716,11 +10798,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="252"/>
-      <c r="D11" s="253"/>
-      <c r="E11" s="253"/>
-      <c r="F11" s="253"/>
-      <c r="G11" s="254"/>
+      <c r="C11" s="254"/>
+      <c r="D11" s="255"/>
+      <c r="E11" s="255"/>
+      <c r="F11" s="255"/>
+      <c r="G11" s="256"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>
@@ -10757,12 +10839,12 @@
       <c r="C13" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="240" t="s">
+      <c r="D13" s="242" t="s">
         <v>542</v>
       </c>
-      <c r="E13" s="241"/>
-      <c r="F13" s="241"/>
-      <c r="G13" s="242"/>
+      <c r="E13" s="243"/>
+      <c r="F13" s="243"/>
+      <c r="G13" s="244"/>
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
@@ -10773,10 +10855,10 @@
     <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
-      <c r="D14" s="240"/>
-      <c r="E14" s="241"/>
-      <c r="F14" s="241"/>
-      <c r="G14" s="242"/>
+      <c r="D14" s="242"/>
+      <c r="E14" s="243"/>
+      <c r="F14" s="243"/>
+      <c r="G14" s="244"/>
       <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
@@ -10787,10 +10869,10 @@
     <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="61"/>
-      <c r="D15" s="240"/>
-      <c r="E15" s="241"/>
-      <c r="F15" s="241"/>
-      <c r="G15" s="242"/>
+      <c r="D15" s="242"/>
+      <c r="E15" s="243"/>
+      <c r="F15" s="243"/>
+      <c r="G15" s="244"/>
       <c r="H15" s="24"/>
       <c r="J15" s="1">
         <v>6827</v>
@@ -10799,10 +10881,10 @@
     <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="63"/>
-      <c r="D16" s="243"/>
-      <c r="E16" s="244"/>
-      <c r="F16" s="244"/>
-      <c r="G16" s="245"/>
+      <c r="D16" s="245"/>
+      <c r="E16" s="246"/>
+      <c r="F16" s="246"/>
+      <c r="G16" s="247"/>
       <c r="H16" s="25"/>
       <c r="J16" s="1">
         <v>0</v>
@@ -10853,11 +10935,11 @@
     <row r="19" spans="2:10">
       <c r="B19" s="24"/>
       <c r="C19" s="61"/>
-      <c r="D19" s="237" t="s">
+      <c r="D19" s="239" t="s">
         <v>599</v>
       </c>
-      <c r="E19" s="238"/>
-      <c r="F19" s="239"/>
+      <c r="E19" s="240"/>
+      <c r="F19" s="241"/>
       <c r="G19" s="61"/>
       <c r="H19" s="24"/>
       <c r="J19" s="1">

</xml_diff>

<commit_message>
2023-01-26 6주 2일차 결산
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E97434B-C7DF-4787-AD8E-1DD6DB0FFD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16AC4B3-B5EB-4910-9FCB-AEAA83947BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4095" yWindow="2565" windowWidth="15495" windowHeight="10380" tabRatio="598" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="652">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2372,6 +2372,66 @@
   </si>
   <si>
     <t>json파일 만들어야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 시각화 자료 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 서버(팀원들 가능하게)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 버튼 4개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. html 15개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. html ui 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. html 버튼 css </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당일 역할 분담</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화 정리 및 html 디자인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. ppt 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.  ppt 자료조사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팝업창 15개 , 버튼 css , 로고 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web구성 마무리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>템플릿 찾음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">들어갈 내용 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aws</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3232,7 +3292,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="266">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4027,6 +4087,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5342,9 +5405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA32" sqref="AA32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB34" sqref="AB34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5526,6 +5589,9 @@
       <c r="Y2" s="257" t="s">
         <v>605</v>
       </c>
+      <c r="AB2" s="84" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="258"/>
@@ -5570,6 +5636,9 @@
       </c>
       <c r="X3" s="257"/>
       <c r="Y3" s="257"/>
+      <c r="AB3" s="84" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="4" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="258"/>
@@ -5616,6 +5685,9 @@
       <c r="AA4" s="84" t="s">
         <v>626</v>
       </c>
+      <c r="AB4" s="84" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="258"/>
@@ -5650,6 +5722,9 @@
       <c r="S5" s="257"/>
       <c r="X5" s="257"/>
       <c r="Y5" s="257"/>
+      <c r="AB5" s="84" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="6" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="258"/>
@@ -5745,6 +5820,9 @@
       </c>
       <c r="X7" s="257"/>
       <c r="Y7" s="257"/>
+      <c r="AB7" s="85" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="259"/>
@@ -5796,6 +5874,9 @@
       <c r="AA8" s="85" t="s">
         <v>627</v>
       </c>
+      <c r="AB8" s="85" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="259"/>
@@ -5839,6 +5920,9 @@
       </c>
       <c r="X9" s="257"/>
       <c r="Y9" s="257"/>
+      <c r="AB9" s="85" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="10" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="259"/>
@@ -5996,7 +6080,7 @@
       <c r="Q16" s="98"/>
       <c r="S16" s="257"/>
     </row>
-    <row r="17" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="261" t="s">
         <v>34</v>
       </c>
@@ -6048,8 +6132,11 @@
       <c r="Y17" s="87" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="AB17" s="87" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
       <c r="A18" s="261"/>
       <c r="B18" s="98"/>
       <c r="C18" s="98"/>
@@ -6078,8 +6165,11 @@
       <c r="X18" s="87" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="AB18" s="87" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="261"/>
       <c r="B19" s="98"/>
       <c r="C19" s="98"/>
@@ -6101,7 +6191,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="261"/>
       <c r="B20" s="98"/>
       <c r="C20" s="98"/>
@@ -6119,7 +6209,7 @@
       </c>
       <c r="S20" s="257"/>
     </row>
-    <row r="21" spans="1:27" s="87" customFormat="1" ht="30" customHeight="1">
+    <row r="21" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="261"/>
       <c r="B21" s="98"/>
       <c r="C21" s="98"/>
@@ -6135,7 +6225,7 @@
       <c r="Q21" s="98"/>
       <c r="S21" s="257"/>
     </row>
-    <row r="22" spans="1:27" s="98" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:28" s="98" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="105"/>
       <c r="M22" t="s">
         <v>442</v>
@@ -6144,7 +6234,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="107" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:28" s="107" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="106" t="s">
         <v>68</v>
       </c>
@@ -6211,8 +6301,11 @@
       <c r="AA23" s="107" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" ht="30" customHeight="1">
+      <c r="AB23" s="106" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -6271,7 +6364,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="30" customHeight="1">
+    <row r="25" spans="1:28" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -6326,8 +6419,11 @@
       <c r="AA25" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="30" customHeight="1">
+      <c r="AB25" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -6370,8 +6466,11 @@
       <c r="AA26" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" ht="30" customHeight="1">
+      <c r="AB26" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -6411,8 +6510,11 @@
       <c r="AA27" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" ht="30" customHeight="1">
+      <c r="AB27" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -6440,8 +6542,11 @@
       <c r="AA28" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" ht="30" customHeight="1">
+      <c r="AB28" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -6472,8 +6577,11 @@
       <c r="AA29" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" ht="30" customHeight="1">
+      <c r="AB29" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -6495,8 +6603,11 @@
       <c r="AA30" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" ht="30" customHeight="1">
+      <c r="AB30" s="265" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -6515,8 +6626,11 @@
       <c r="AA31" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" ht="30" customHeight="1">
+      <c r="AB31" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -6537,6 +6651,9 @@
       </c>
       <c r="AA32" t="s">
         <v>636</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="30" customHeight="1">
@@ -9561,7 +9678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF13B7-3145-43F9-AE5D-8745D081A690}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H9" sqref="H9:H12"/>
     </sheetView>
   </sheetViews>
@@ -9965,8 +10082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA729C5-F4A6-4AC1-AD36-A96A4028E1F4}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -10015,7 +10132,9 @@
       <c r="C5" s="67"/>
       <c r="D5" s="70"/>
       <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="F5" s="31" t="s">
+        <v>643</v>
+      </c>
       <c r="G5" s="31"/>
       <c r="H5" s="30"/>
     </row>
@@ -10026,7 +10145,9 @@
       <c r="C6" s="67"/>
       <c r="D6" s="70"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="F6" s="186" t="s">
+        <v>644</v>
+      </c>
       <c r="G6" s="31"/>
       <c r="H6" s="30"/>
     </row>
@@ -10037,7 +10158,7 @@
       <c r="C7" s="67"/>
       <c r="D7" s="70"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="F7" s="188"/>
       <c r="G7" s="31"/>
       <c r="H7" s="30"/>
     </row>
@@ -10047,10 +10168,10 @@
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="70"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="30"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
     </row>
     <row r="9" spans="2:8" ht="50.1" customHeight="1">
       <c r="B9" s="36">
@@ -10059,7 +10180,9 @@
       <c r="C9" s="67"/>
       <c r="D9" s="70"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="F9" s="204" t="s">
+        <v>647</v>
+      </c>
       <c r="G9" s="31"/>
       <c r="H9" s="30"/>
     </row>
@@ -10070,7 +10193,7 @@
       <c r="C10" s="67"/>
       <c r="D10" s="70"/>
       <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="F10" s="205"/>
       <c r="G10" s="31"/>
       <c r="H10" s="30"/>
     </row>
@@ -10081,7 +10204,9 @@
       <c r="C11" s="67"/>
       <c r="D11" s="70"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="F11" s="212" t="s">
+        <v>107</v>
+      </c>
       <c r="G11" s="31"/>
       <c r="H11" s="30"/>
     </row>
@@ -10092,7 +10217,7 @@
       <c r="C12" s="67"/>
       <c r="D12" s="70"/>
       <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="F12" s="213"/>
       <c r="G12" s="31"/>
       <c r="H12" s="30"/>
     </row>
@@ -10125,9 +10250,12 @@
       <c r="H14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10662,8 +10790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>

</xml_diff>

<commit_message>
2023-01-27 6주 3일차 결산
</commit_message>
<xml_diff>
--- a/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
+++ b/final_project/프로젝트 필요 양식/멀티캠퍼스_최종프로젝트_1조_계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiGiraffe0\Documents\multicampus_final_First\final_project\프로젝트 필요 양식\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16AC4B3-B5EB-4910-9FCB-AEAA83947BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AC5F42-7C0B-4960-B753-C72127497AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4095" yWindow="2565" windowWidth="15495" windowHeight="10380" tabRatio="598" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1주차" sheetId="28" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="664">
   <si>
     <t>일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2432,6 +2432,53 @@
   </si>
   <si>
     <t>aws</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt 전체 틀 잡고, 준비</t>
+  </si>
+  <si>
+    <t>ppt 전체 틀 잡고, 준비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt 자료조사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개요 3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전처리과정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt 구성 및 자료조사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체적인 ppt 구성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각화, web</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개요 1,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아키텍쳐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설문지 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3292,7 +3339,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="266">
+  <cellXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3827,6 +3874,9 @@
     <xf numFmtId="0" fontId="12" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4088,8 +4138,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4834,14 +4884,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="93"/>
@@ -4865,12 +4915,12 @@
       <c r="B5" s="36">
         <v>0.375</v>
       </c>
-      <c r="C5" s="194" t="s">
+      <c r="C5" s="195" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="195"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="195"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="196"/>
+      <c r="F5" s="196"/>
       <c r="G5" s="109" t="s">
         <v>108</v>
       </c>
@@ -4885,7 +4935,7 @@
       <c r="D6" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="189" t="s">
+      <c r="E6" s="190" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -4903,7 +4953,7 @@
       <c r="D7" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="190"/>
+      <c r="E7" s="191"/>
       <c r="F7" s="108" t="s">
         <v>107</v>
       </c>
@@ -4925,19 +4975,19 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="183" t="s">
+      <c r="C9" s="184" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="186" t="s">
+      <c r="D9" s="187" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="186" t="s">
+      <c r="E9" s="187" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="191" t="s">
+      <c r="F9" s="192" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="196" t="s">
+      <c r="G9" s="197" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4945,21 +4995,21 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="187"/>
-      <c r="F10" s="192"/>
-      <c r="G10" s="197"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="188"/>
+      <c r="E10" s="188"/>
+      <c r="F10" s="193"/>
+      <c r="G10" s="198"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="185"/>
-      <c r="D11" s="188"/>
-      <c r="E11" s="187"/>
-      <c r="F11" s="192"/>
-      <c r="G11" s="197"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="188"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="198"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1">
       <c r="B12" s="36">
@@ -4969,9 +5019,9 @@
         <v>38</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="188"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="198"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="194"/>
+      <c r="G12" s="199"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -4980,11 +5030,11 @@
       <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="180" t="s">
+      <c r="D13" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="181"/>
-      <c r="F13" s="182"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="183"/>
       <c r="G13" s="32" t="s">
         <v>30</v>
       </c>
@@ -5052,35 +5102,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="234" t="s">
+      <c r="B2" s="235" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="235"/>
-      <c r="D2" s="235"/>
-      <c r="E2" s="235"/>
-      <c r="F2" s="235"/>
-      <c r="G2" s="235"/>
-      <c r="H2" s="235"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
     </row>
     <row r="3" spans="2:9" ht="31.5">
-      <c r="B3" s="234"/>
-      <c r="C3" s="235" t="s">
+      <c r="B3" s="235"/>
+      <c r="C3" s="236" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="235"/>
-      <c r="E3" s="235"/>
-      <c r="F3" s="235"/>
-      <c r="G3" s="235"/>
-      <c r="H3" s="235"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="236"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B4" s="234"/>
-      <c r="C4" s="235"/>
-      <c r="D4" s="235"/>
-      <c r="E4" s="235"/>
-      <c r="F4" s="235"/>
-      <c r="G4" s="235"/>
-      <c r="H4" s="235"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="236"/>
+      <c r="E4" s="236"/>
+      <c r="F4" s="236"/>
+      <c r="G4" s="236"/>
+      <c r="H4" s="236"/>
     </row>
     <row r="6" spans="2:9" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -5405,9 +5455,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCA466B-2AE3-4FD0-8E06-02B936C993AC}">
   <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB34" sqref="AB34"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="30" customHeight="1"/>
@@ -5523,7 +5573,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="258" t="s">
+      <c r="A2" s="259" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="98" t="s">
@@ -5541,7 +5591,7 @@
       <c r="F2" s="98" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="262" t="s">
+      <c r="G2" s="263" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="98"/>
@@ -5571,7 +5621,7 @@
       <c r="R2" s="84" t="s">
         <v>549</v>
       </c>
-      <c r="S2" s="257" t="s">
+      <c r="S2" s="258" t="s">
         <v>555</v>
       </c>
       <c r="T2" s="84" t="s">
@@ -5583,18 +5633,21 @@
       <c r="W2" s="84" t="s">
         <v>588</v>
       </c>
-      <c r="X2" s="257" t="s">
+      <c r="X2" s="258" t="s">
         <v>598</v>
       </c>
-      <c r="Y2" s="257" t="s">
+      <c r="Y2" s="258" t="s">
         <v>605</v>
       </c>
       <c r="AB2" s="84" t="s">
         <v>637</v>
       </c>
+      <c r="AC2" s="84" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="3" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="258"/>
+      <c r="A3" s="259"/>
       <c r="B3" s="98" t="s">
         <v>43</v>
       </c>
@@ -5608,7 +5661,7 @@
       <c r="F3" s="98" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="262"/>
+      <c r="G3" s="263"/>
       <c r="H3" s="98"/>
       <c r="I3" s="111" t="s">
         <v>164</v>
@@ -5627,21 +5680,24 @@
       </c>
       <c r="Q3" s="98"/>
       <c r="R3" s="173"/>
-      <c r="S3" s="257"/>
+      <c r="S3" s="258"/>
       <c r="T3" s="84" t="s">
         <v>567</v>
       </c>
       <c r="U3" s="84" t="s">
         <v>576</v>
       </c>
-      <c r="X3" s="257"/>
-      <c r="Y3" s="257"/>
+      <c r="X3" s="258"/>
+      <c r="Y3" s="258"/>
       <c r="AB3" s="84" t="s">
         <v>638</v>
       </c>
+      <c r="AC3" s="84" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="4" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="258"/>
+      <c r="A4" s="259"/>
       <c r="B4" s="100" t="s">
         <v>44</v>
       </c>
@@ -5653,7 +5709,7 @@
       <c r="F4" s="98" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="262"/>
+      <c r="G4" s="263"/>
       <c r="H4" s="98"/>
       <c r="I4" s="98" t="s">
         <v>165</v>
@@ -5676,21 +5732,24 @@
       <c r="R4" s="84" t="s">
         <v>547</v>
       </c>
-      <c r="S4" s="257"/>
+      <c r="S4" s="258"/>
       <c r="W4" s="84" t="s">
         <v>597</v>
       </c>
-      <c r="X4" s="257"/>
-      <c r="Y4" s="257"/>
+      <c r="X4" s="258"/>
+      <c r="Y4" s="258"/>
       <c r="AA4" s="84" t="s">
         <v>626</v>
       </c>
       <c r="AB4" s="84" t="s">
         <v>639</v>
       </c>
+      <c r="AC4" s="84" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="5" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="258"/>
+      <c r="A5" s="259"/>
       <c r="B5" s="100" t="s">
         <v>45</v>
       </c>
@@ -5704,7 +5763,7 @@
       <c r="F5" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="262"/>
+      <c r="G5" s="263"/>
       <c r="H5" s="98"/>
       <c r="I5" s="98" t="s">
         <v>166</v>
@@ -5719,15 +5778,15 @@
         <v>430</v>
       </c>
       <c r="Q5" s="98"/>
-      <c r="S5" s="257"/>
-      <c r="X5" s="257"/>
-      <c r="Y5" s="257"/>
+      <c r="S5" s="258"/>
+      <c r="X5" s="258"/>
+      <c r="Y5" s="258"/>
       <c r="AB5" s="84" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:32" s="84" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="258"/>
+      <c r="A6" s="259"/>
       <c r="B6" s="98" t="s">
         <v>46</v>
       </c>
@@ -5743,7 +5802,7 @@
       <c r="F6" s="98" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="262"/>
+      <c r="G6" s="263"/>
       <c r="H6" s="98"/>
       <c r="I6" s="98" t="s">
         <v>168</v>
@@ -5755,12 +5814,12 @@
       <c r="Q6" s="98" t="s">
         <v>535</v>
       </c>
-      <c r="S6" s="257"/>
-      <c r="X6" s="257"/>
-      <c r="Y6" s="257"/>
+      <c r="S6" s="258"/>
+      <c r="X6" s="258"/>
+      <c r="Y6" s="258"/>
     </row>
     <row r="7" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="259" t="s">
+      <c r="A7" s="260" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="98" t="s">
@@ -5776,7 +5835,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="98"/>
-      <c r="G7" s="262"/>
+      <c r="G7" s="263"/>
       <c r="H7" s="98" t="s">
         <v>150</v>
       </c>
@@ -5808,7 +5867,7 @@
       <c r="R7" s="85" t="s">
         <v>549</v>
       </c>
-      <c r="S7" s="257"/>
+      <c r="S7" s="258"/>
       <c r="T7" s="85" t="s">
         <v>568</v>
       </c>
@@ -5818,14 +5877,17 @@
       <c r="W7" s="84" t="s">
         <v>588</v>
       </c>
-      <c r="X7" s="257"/>
-      <c r="Y7" s="257"/>
+      <c r="X7" s="258"/>
+      <c r="Y7" s="258"/>
       <c r="AB7" s="85" t="s">
         <v>637</v>
       </c>
+      <c r="AC7" s="85" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="8" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="259"/>
+      <c r="A8" s="260"/>
       <c r="B8" s="98" t="s">
         <v>48</v>
       </c>
@@ -5837,7 +5899,7 @@
       </c>
       <c r="E8" s="98"/>
       <c r="F8" s="98"/>
-      <c r="G8" s="262"/>
+      <c r="G8" s="263"/>
       <c r="H8" s="98" t="s">
         <v>151</v>
       </c>
@@ -5859,7 +5921,7 @@
       <c r="Q8" s="98" t="s">
         <v>536</v>
       </c>
-      <c r="S8" s="257"/>
+      <c r="S8" s="258"/>
       <c r="T8" s="85" t="s">
         <v>569</v>
       </c>
@@ -5869,17 +5931,20 @@
       <c r="W8" s="85" t="s">
         <v>586</v>
       </c>
-      <c r="X8" s="257"/>
-      <c r="Y8" s="257"/>
+      <c r="X8" s="258"/>
+      <c r="Y8" s="258"/>
       <c r="AA8" s="85" t="s">
         <v>627</v>
       </c>
       <c r="AB8" s="85" t="s">
         <v>641</v>
       </c>
+      <c r="AC8" s="85" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="9" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="259"/>
+      <c r="A9" s="260"/>
       <c r="B9" s="98" t="s">
         <v>73</v>
       </c>
@@ -5891,7 +5956,7 @@
       </c>
       <c r="E9" s="98"/>
       <c r="F9" s="98"/>
-      <c r="G9" s="262"/>
+      <c r="G9" s="263"/>
       <c r="H9" s="98" t="s">
         <v>152</v>
       </c>
@@ -5911,21 +5976,24 @@
       <c r="R9" s="85" t="s">
         <v>550</v>
       </c>
-      <c r="S9" s="257"/>
+      <c r="S9" s="258"/>
       <c r="T9" s="85" t="s">
         <v>570</v>
       </c>
       <c r="U9" s="85" t="s">
         <v>580</v>
       </c>
-      <c r="X9" s="257"/>
-      <c r="Y9" s="257"/>
+      <c r="X9" s="258"/>
+      <c r="Y9" s="258"/>
       <c r="AB9" s="85" t="s">
         <v>645</v>
       </c>
+      <c r="AC9" s="85" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="10" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="259"/>
+      <c r="A10" s="260"/>
       <c r="B10" s="100" t="s">
         <v>74</v>
       </c>
@@ -5937,7 +6005,7 @@
         <v>117</v>
       </c>
       <c r="F10" s="98"/>
-      <c r="G10" s="262"/>
+      <c r="G10" s="263"/>
       <c r="H10" s="98"/>
       <c r="I10" s="98"/>
       <c r="K10" s="85" t="s">
@@ -5949,12 +6017,12 @@
       <c r="Q10" s="98" t="s">
         <v>538</v>
       </c>
-      <c r="S10" s="257"/>
-      <c r="X10" s="257"/>
-      <c r="Y10" s="257"/>
+      <c r="S10" s="258"/>
+      <c r="X10" s="258"/>
+      <c r="Y10" s="258"/>
     </row>
     <row r="11" spans="1:32" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="259"/>
+      <c r="A11" s="260"/>
       <c r="B11" s="100" t="s">
         <v>75</v>
       </c>
@@ -5966,19 +6034,19 @@
         <v>118</v>
       </c>
       <c r="F11" s="98"/>
-      <c r="G11" s="262"/>
+      <c r="G11" s="263"/>
       <c r="H11" s="98"/>
       <c r="I11" s="98"/>
       <c r="M11" t="s">
         <v>436</v>
       </c>
       <c r="Q11" s="98"/>
-      <c r="S11" s="257"/>
-      <c r="X11" s="257"/>
-      <c r="Y11" s="257"/>
+      <c r="S11" s="258"/>
+      <c r="X11" s="258"/>
+      <c r="Y11" s="258"/>
     </row>
     <row r="12" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A12" s="260" t="s">
+      <c r="A12" s="261" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="101" t="s">
@@ -5992,7 +6060,7 @@
         <v>119</v>
       </c>
       <c r="F12" s="98"/>
-      <c r="G12" s="262"/>
+      <c r="G12" s="263"/>
       <c r="H12" s="98" t="s">
         <v>153</v>
       </c>
@@ -6005,17 +6073,17 @@
       </c>
       <c r="M12"/>
       <c r="Q12" s="98"/>
-      <c r="S12" s="257"/>
+      <c r="S12" s="258"/>
     </row>
     <row r="13" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A13" s="260"/>
+      <c r="A13" s="261"/>
       <c r="C13" s="98"/>
       <c r="D13" s="98"/>
       <c r="E13" s="98" t="s">
         <v>116</v>
       </c>
       <c r="F13" s="98"/>
-      <c r="G13" s="262"/>
+      <c r="G13" s="263"/>
       <c r="H13" s="98" t="s">
         <v>154</v>
       </c>
@@ -6027,15 +6095,15 @@
         <v>437</v>
       </c>
       <c r="Q13" s="98"/>
-      <c r="S13" s="257"/>
+      <c r="S13" s="258"/>
     </row>
     <row r="14" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A14" s="260"/>
+      <c r="A14" s="261"/>
       <c r="C14" s="98"/>
       <c r="D14" s="98"/>
       <c r="E14" s="98"/>
       <c r="F14" s="98"/>
-      <c r="G14" s="262"/>
+      <c r="G14" s="263"/>
       <c r="H14" s="98" t="s">
         <v>155</v>
       </c>
@@ -6044,44 +6112,44 @@
         <v>438</v>
       </c>
       <c r="Q14" s="98"/>
-      <c r="S14" s="257"/>
+      <c r="S14" s="258"/>
     </row>
     <row r="15" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A15" s="260"/>
+      <c r="A15" s="261"/>
       <c r="C15" s="98"/>
       <c r="D15" s="98"/>
       <c r="E15" s="98" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="98"/>
-      <c r="G15" s="262"/>
+      <c r="G15" s="263"/>
       <c r="H15" s="98" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="98"/>
       <c r="M15"/>
       <c r="Q15" s="98"/>
-      <c r="S15" s="257"/>
+      <c r="S15" s="258"/>
     </row>
     <row r="16" spans="1:32" s="86" customFormat="1" ht="30" hidden="1" customHeight="1">
-      <c r="A16" s="260"/>
+      <c r="A16" s="261"/>
       <c r="C16" s="98"/>
       <c r="D16" s="98"/>
       <c r="E16" s="98" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="98"/>
-      <c r="G16" s="262"/>
+      <c r="G16" s="263"/>
       <c r="H16" s="98" t="s">
         <v>157</v>
       </c>
       <c r="I16" s="98"/>
       <c r="M16"/>
       <c r="Q16" s="98"/>
-      <c r="S16" s="257"/>
-    </row>
-    <row r="17" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="261" t="s">
+      <c r="S16" s="258"/>
+    </row>
+    <row r="17" spans="1:29" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="262" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="98"/>
@@ -6089,7 +6157,7 @@
       <c r="D17" s="98"/>
       <c r="E17" s="98"/>
       <c r="F17" s="98"/>
-      <c r="G17" s="262"/>
+      <c r="G17" s="263"/>
       <c r="H17" s="98"/>
       <c r="I17" s="98"/>
       <c r="J17" s="87" t="s">
@@ -6119,7 +6187,7 @@
       <c r="R17" s="87" t="s">
         <v>549</v>
       </c>
-      <c r="S17" s="257"/>
+      <c r="S17" s="258"/>
       <c r="T17" s="87" t="s">
         <v>568</v>
       </c>
@@ -6135,15 +6203,18 @@
       <c r="AB17" s="87" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="261"/>
+      <c r="AC17" s="87" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="262"/>
       <c r="B18" s="98"/>
       <c r="C18" s="98"/>
       <c r="D18" s="98"/>
       <c r="E18" s="98"/>
       <c r="F18" s="98"/>
-      <c r="G18" s="262"/>
+      <c r="G18" s="263"/>
       <c r="H18" s="98"/>
       <c r="I18" s="98"/>
       <c r="L18" s="87" t="s">
@@ -6155,7 +6226,7 @@
       <c r="Q18" s="98" t="s">
         <v>539</v>
       </c>
-      <c r="S18" s="257"/>
+      <c r="S18" s="258"/>
       <c r="T18" s="87" t="s">
         <v>571</v>
       </c>
@@ -6168,15 +6239,18 @@
       <c r="AB18" s="87" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="261"/>
+      <c r="AC18" s="87" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="262"/>
       <c r="B19" s="98"/>
       <c r="C19" s="98"/>
       <c r="D19" s="98"/>
       <c r="E19" s="98"/>
       <c r="F19" s="98"/>
-      <c r="G19" s="262"/>
+      <c r="G19" s="263"/>
       <c r="H19" s="98"/>
       <c r="I19" s="98"/>
       <c r="M19" t="s">
@@ -6186,19 +6260,22 @@
       <c r="R19" s="87" t="s">
         <v>548</v>
       </c>
-      <c r="S19" s="257"/>
+      <c r="S19" s="258"/>
       <c r="AA19" s="87" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="261"/>
+      <c r="AC19" s="87" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="262"/>
       <c r="B20" s="98"/>
       <c r="C20" s="98"/>
       <c r="D20" s="98"/>
       <c r="E20" s="98"/>
       <c r="F20" s="98"/>
-      <c r="G20" s="262"/>
+      <c r="G20" s="263"/>
       <c r="H20" s="98"/>
       <c r="I20" s="98"/>
       <c r="M20" t="s">
@@ -6207,25 +6284,28 @@
       <c r="Q20" s="98" t="s">
         <v>540</v>
       </c>
-      <c r="S20" s="257"/>
-    </row>
-    <row r="21" spans="1:28" s="87" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="261"/>
+      <c r="S20" s="258"/>
+      <c r="AC20" s="87" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" s="87" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="262"/>
       <c r="B21" s="98"/>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
       <c r="E21" s="98"/>
       <c r="F21" s="98"/>
-      <c r="G21" s="262"/>
+      <c r="G21" s="263"/>
       <c r="H21" s="98"/>
       <c r="I21" s="98"/>
       <c r="M21" t="s">
         <v>441</v>
       </c>
       <c r="Q21" s="98"/>
-      <c r="S21" s="257"/>
-    </row>
-    <row r="22" spans="1:28" s="98" customFormat="1" ht="30" customHeight="1">
+      <c r="S21" s="258"/>
+    </row>
+    <row r="22" spans="1:29" s="98" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="105"/>
       <c r="M22" t="s">
         <v>442</v>
@@ -6234,7 +6314,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="23" spans="1:28" s="107" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:29" s="107" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="106" t="s">
         <v>68</v>
       </c>
@@ -6304,8 +6384,11 @@
       <c r="AB23" s="106" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" ht="30" customHeight="1">
+      <c r="AC23" s="106" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -6363,8 +6446,11 @@
       <c r="Y24" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" ht="30" customHeight="1">
+      <c r="AC24" s="87" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="30" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -6423,7 +6509,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="30" customHeight="1">
+    <row r="26" spans="1:29" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -6470,7 +6556,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="30" customHeight="1">
+    <row r="27" spans="1:29" ht="30" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -6514,7 +6600,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="30" customHeight="1">
+    <row r="28" spans="1:29" ht="30" customHeight="1">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -6546,7 +6632,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="30" customHeight="1">
+    <row r="29" spans="1:29" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -6581,7 +6667,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="30" customHeight="1">
+    <row r="30" spans="1:29" ht="30" customHeight="1">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -6603,11 +6689,11 @@
       <c r="AA30" t="s">
         <v>634</v>
       </c>
-      <c r="AB30" s="265" t="s">
+      <c r="AB30" s="178" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="30" customHeight="1">
+    <row r="31" spans="1:29" ht="30" customHeight="1">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -6630,7 +6716,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="30" customHeight="1">
+    <row r="32" spans="1:29" ht="30" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -8153,22 +8239,22 @@
         <v>255</v>
       </c>
       <c r="B2" s="155"/>
-      <c r="C2" s="263" t="s">
+      <c r="C2" s="264" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263" t="s">
+      <c r="D2" s="264"/>
+      <c r="E2" s="264" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263" t="s">
+      <c r="F2" s="264"/>
+      <c r="G2" s="264" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263" t="s">
+      <c r="H2" s="264"/>
+      <c r="I2" s="264" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="264"/>
+      <c r="J2" s="265"/>
       <c r="Y2" s="1" t="s">
         <v>334</v>
       </c>
@@ -8947,14 +9033,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="88"/>
@@ -8998,19 +9084,19 @@
       <c r="B6" s="36">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C6" s="199" t="s">
+      <c r="C6" s="200" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="186" t="s">
+      <c r="D6" s="187" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="204" t="s">
+      <c r="E6" s="205" t="s">
         <v>163</v>
       </c>
       <c r="F6" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="G6" s="207" t="s">
+      <c r="G6" s="208" t="s">
         <v>280</v>
       </c>
     </row>
@@ -9018,13 +9104,13 @@
       <c r="B7" s="36">
         <v>0.45833333333333398</v>
       </c>
-      <c r="C7" s="200"/>
-      <c r="D7" s="188"/>
-      <c r="E7" s="205"/>
+      <c r="C7" s="201"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="206"/>
       <c r="F7" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="208"/>
+      <c r="G7" s="209"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
       <c r="B8" s="95">
@@ -9040,13 +9126,13 @@
       <c r="B9" s="36">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C9" s="201" t="s">
+      <c r="C9" s="202" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="186" t="s">
+      <c r="D9" s="187" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="204"/>
+      <c r="E9" s="205"/>
       <c r="F9" s="112" t="s">
         <v>247</v>
       </c>
@@ -9058,9 +9144,9 @@
       <c r="B10" s="36">
         <v>0.58333333333333404</v>
       </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="206"/>
+      <c r="C10" s="203"/>
+      <c r="D10" s="188"/>
+      <c r="E10" s="207"/>
       <c r="F10" s="112" t="s">
         <v>246</v>
       </c>
@@ -9070,9 +9156,9 @@
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
-      <c r="C11" s="203"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="206"/>
+      <c r="C11" s="204"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="207"/>
       <c r="F11" s="112" t="s">
         <v>248</v>
       </c>
@@ -9085,8 +9171,8 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="188"/>
-      <c r="E12" s="205"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="206"/>
       <c r="F12" s="112" t="s">
         <v>249</v>
       </c>
@@ -9099,11 +9185,11 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="180" t="s">
+      <c r="D13" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="181"/>
-      <c r="F13" s="181"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="182"/>
       <c r="G13" s="126" t="s">
         <v>30</v>
       </c>
@@ -9155,15 +9241,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="89"/>
@@ -9223,7 +9309,7 @@
       <c r="F6" s="110" t="s">
         <v>523</v>
       </c>
-      <c r="G6" s="212" t="s">
+      <c r="G6" s="213" t="s">
         <v>521</v>
       </c>
       <c r="H6" s="30" t="s">
@@ -9244,7 +9330,7 @@
       <c r="F7" s="110" t="s">
         <v>520</v>
       </c>
-      <c r="G7" s="213"/>
+      <c r="G7" s="214"/>
       <c r="H7" s="30" t="s">
         <v>530</v>
       </c>
@@ -9270,7 +9356,7 @@
       <c r="D9" s="166" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="209" t="s">
+      <c r="E9" s="210" t="s">
         <v>469</v>
       </c>
       <c r="F9" s="110" t="s">
@@ -9291,7 +9377,7 @@
       <c r="D10" s="108" t="s">
         <v>425</v>
       </c>
-      <c r="E10" s="210"/>
+      <c r="E10" s="211"/>
       <c r="F10" s="110"/>
       <c r="G10" s="171" t="s">
         <v>525</v>
@@ -9310,7 +9396,7 @@
       <c r="D11" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E11" s="210"/>
+      <c r="E11" s="211"/>
       <c r="F11" s="110"/>
       <c r="G11" s="171" t="s">
         <v>526</v>
@@ -9325,7 +9411,7 @@
       <c r="D12" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="E12" s="211"/>
+      <c r="E12" s="212"/>
       <c r="F12" s="110"/>
       <c r="G12" s="171"/>
       <c r="H12" s="30"/>
@@ -9337,12 +9423,12 @@
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="180" t="s">
+      <c r="D13" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="181"/>
-      <c r="F13" s="181"/>
-      <c r="G13" s="182"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="182"/>
+      <c r="G13" s="183"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9690,15 +9776,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="22"/>
@@ -9753,13 +9839,13 @@
       <c r="E6" s="32" t="s">
         <v>551</v>
       </c>
-      <c r="F6" s="196" t="s">
+      <c r="F6" s="197" t="s">
         <v>561</v>
       </c>
-      <c r="G6" s="196" t="s">
+      <c r="G6" s="197" t="s">
         <v>563</v>
       </c>
-      <c r="H6" s="214" t="s">
+      <c r="H6" s="215" t="s">
         <v>530</v>
       </c>
     </row>
@@ -9774,9 +9860,9 @@
       <c r="E7" s="32" t="s">
         <v>552</v>
       </c>
-      <c r="F7" s="198"/>
-      <c r="G7" s="198"/>
-      <c r="H7" s="215"/>
+      <c r="F7" s="199"/>
+      <c r="G7" s="199"/>
+      <c r="H7" s="216"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
       <c r="B8" s="36">
@@ -9794,17 +9880,17 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="196" t="s">
+      <c r="D9" s="197" t="s">
         <v>546</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>554</v>
       </c>
-      <c r="F9" s="196" t="s">
+      <c r="F9" s="197" t="s">
         <v>562</v>
       </c>
       <c r="G9" s="32"/>
-      <c r="H9" s="216" t="s">
+      <c r="H9" s="217" t="s">
         <v>582</v>
       </c>
     </row>
@@ -9813,41 +9899,41 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="197"/>
+      <c r="D10" s="198"/>
       <c r="E10" s="32" t="s">
         <v>553</v>
       </c>
-      <c r="F10" s="197"/>
+      <c r="F10" s="198"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="217"/>
+      <c r="H10" s="218"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
       <c r="B11" s="36">
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="196" t="s">
+      <c r="D11" s="198"/>
+      <c r="E11" s="197" t="s">
         <v>554</v>
       </c>
-      <c r="F11" s="197"/>
+      <c r="F11" s="198"/>
       <c r="G11" s="32" t="s">
         <v>564</v>
       </c>
-      <c r="H11" s="217"/>
+      <c r="H11" s="218"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
       <c r="B12" s="36">
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="198"/>
-      <c r="E12" s="198"/>
-      <c r="F12" s="198"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="199"/>
+      <c r="F12" s="199"/>
       <c r="G12" s="174" t="s">
         <v>565</v>
       </c>
-      <c r="H12" s="218"/>
+      <c r="H12" s="219"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
       <c r="B13" s="36">
@@ -9857,11 +9943,11 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="180" t="s">
+      <c r="E13" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="181"/>
-      <c r="G13" s="182"/>
+      <c r="F13" s="182"/>
+      <c r="G13" s="183"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -9912,14 +9998,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1">
       <c r="B4" s="90"/>
@@ -9944,13 +10030,13 @@
         <v>0.375</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="219" t="s">
+      <c r="D5" s="220" t="s">
         <v>586</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="219" t="s">
+      <c r="F5" s="220" t="s">
         <v>600</v>
       </c>
       <c r="G5" s="70"/>
@@ -9960,11 +10046,11 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="189" t="s">
+      <c r="D6" s="198"/>
+      <c r="E6" s="190" t="s">
         <v>592</v>
       </c>
-      <c r="F6" s="197"/>
+      <c r="F6" s="198"/>
       <c r="G6" s="70"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1">
@@ -9972,9 +10058,9 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="198"/>
-      <c r="E7" s="190"/>
-      <c r="F7" s="198"/>
+      <c r="D7" s="199"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="199"/>
       <c r="G7" s="70"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1">
@@ -9992,10 +10078,10 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="196" t="s">
+      <c r="D9" s="197" t="s">
         <v>587</v>
       </c>
-      <c r="E9" s="196" t="s">
+      <c r="E9" s="197" t="s">
         <v>593</v>
       </c>
       <c r="F9" s="31" t="s">
@@ -10008,8 +10094,8 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="198"/>
       <c r="F10" s="31" t="s">
         <v>595</v>
       </c>
@@ -10020,8 +10106,8 @@
         <v>0.625</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
+      <c r="D11" s="198"/>
+      <c r="E11" s="198"/>
       <c r="F11" s="31"/>
       <c r="G11" s="70"/>
     </row>
@@ -10030,8 +10116,8 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="198"/>
-      <c r="E12" s="198"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="199"/>
       <c r="F12" s="31"/>
       <c r="G12" s="70"/>
     </row>
@@ -10043,10 +10129,10 @@
       <c r="D13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="180" t="s">
+      <c r="E13" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="182"/>
+      <c r="F13" s="183"/>
       <c r="G13" s="175" t="s">
         <v>30</v>
       </c>
@@ -10082,8 +10168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA729C5-F4A6-4AC1-AD36-A96A4028E1F4}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -10094,15 +10180,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
     </row>
     <row r="4" spans="2:8" ht="50.1" customHeight="1">
       <c r="B4" s="91"/>
@@ -10135,7 +10221,9 @@
       <c r="F5" s="31" t="s">
         <v>643</v>
       </c>
-      <c r="G5" s="31"/>
+      <c r="G5" s="266" t="s">
+        <v>653</v>
+      </c>
       <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="50.1" customHeight="1">
@@ -10145,10 +10233,10 @@
       <c r="C6" s="67"/>
       <c r="D6" s="70"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="186" t="s">
+      <c r="F6" s="187" t="s">
         <v>644</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="188"/>
       <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="50.1" customHeight="1">
@@ -10158,8 +10246,8 @@
       <c r="C7" s="67"/>
       <c r="D7" s="70"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="188"/>
-      <c r="G7" s="31"/>
+      <c r="F7" s="189"/>
+      <c r="G7" s="189"/>
       <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="50.1" customHeight="1">
@@ -10180,10 +10268,12 @@
       <c r="C9" s="67"/>
       <c r="D9" s="70"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="204" t="s">
+      <c r="F9" s="205" t="s">
         <v>647</v>
       </c>
-      <c r="G9" s="31"/>
+      <c r="G9" s="197" t="s">
+        <v>652</v>
+      </c>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:8" ht="50.1" customHeight="1">
@@ -10193,8 +10283,8 @@
       <c r="C10" s="67"/>
       <c r="D10" s="70"/>
       <c r="E10" s="31"/>
-      <c r="F10" s="205"/>
-      <c r="G10" s="31"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="198"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="50.1" customHeight="1">
@@ -10204,10 +10294,10 @@
       <c r="C11" s="67"/>
       <c r="D11" s="70"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="212" t="s">
+      <c r="F11" s="213" t="s">
         <v>107</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="198"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="50.1" customHeight="1">
@@ -10217,8 +10307,8 @@
       <c r="C12" s="67"/>
       <c r="D12" s="70"/>
       <c r="E12" s="31"/>
-      <c r="F12" s="213"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="214"/>
+      <c r="G12" s="199"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="50.1" customHeight="1">
@@ -10230,10 +10320,10 @@
       <c r="E13" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="220" t="s">
+      <c r="F13" s="221" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="221"/>
+      <c r="G13" s="222"/>
       <c r="H13" s="30" t="s">
         <v>30</v>
       </c>
@@ -10250,12 +10340,14 @@
       <c r="H14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="G9:G12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10280,13 +10372,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
       <c r="B4" s="92"/>
@@ -10422,35 +10514,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B2" s="234" t="s">
+      <c r="B2" s="235" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="235"/>
-      <c r="D2" s="235"/>
-      <c r="E2" s="235"/>
-      <c r="F2" s="235"/>
-      <c r="G2" s="235"/>
-      <c r="H2" s="235"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
     </row>
     <row r="3" spans="2:8" ht="31.5">
-      <c r="B3" s="234"/>
-      <c r="C3" s="235" t="s">
+      <c r="B3" s="235"/>
+      <c r="C3" s="236" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="235"/>
-      <c r="E3" s="235"/>
-      <c r="F3" s="235"/>
-      <c r="G3" s="235"/>
-      <c r="H3" s="235"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="236"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B4" s="234"/>
-      <c r="C4" s="235"/>
-      <c r="D4" s="235"/>
-      <c r="E4" s="235"/>
-      <c r="F4" s="235"/>
-      <c r="G4" s="235"/>
-      <c r="H4" s="235"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="236"/>
+      <c r="E4" s="236"/>
+      <c r="F4" s="236"/>
+      <c r="G4" s="236"/>
+      <c r="H4" s="236"/>
     </row>
     <row r="6" spans="2:8" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -10669,42 +10761,42 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="10"/>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="237" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="237"/>
-      <c r="E23" s="237"/>
-      <c r="F23" s="237"/>
-      <c r="G23" s="238"/>
+      <c r="D23" s="238"/>
+      <c r="E23" s="238"/>
+      <c r="F23" s="238"/>
+      <c r="G23" s="239"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="10"/>
-      <c r="C24" s="228"/>
-      <c r="D24" s="229"/>
-      <c r="E24" s="229"/>
-      <c r="F24" s="229"/>
-      <c r="G24" s="230"/>
+      <c r="C24" s="229"/>
+      <c r="D24" s="230"/>
+      <c r="E24" s="230"/>
+      <c r="F24" s="230"/>
+      <c r="G24" s="231"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="10"/>
-      <c r="C25" s="228" t="s">
+      <c r="C25" s="229" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="229"/>
-      <c r="E25" s="229"/>
-      <c r="F25" s="229"/>
-      <c r="G25" s="230"/>
+      <c r="D25" s="230"/>
+      <c r="E25" s="230"/>
+      <c r="F25" s="230"/>
+      <c r="G25" s="231"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="11"/>
-      <c r="C26" s="231"/>
-      <c r="D26" s="232"/>
-      <c r="E26" s="232"/>
-      <c r="F26" s="232"/>
-      <c r="G26" s="233"/>
+      <c r="C26" s="232"/>
+      <c r="D26" s="233"/>
+      <c r="E26" s="233"/>
+      <c r="F26" s="233"/>
+      <c r="G26" s="234"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="2:8">
@@ -10732,42 +10824,42 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="17"/>
-      <c r="C28" s="222" t="s">
+      <c r="C28" s="223" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="223"/>
-      <c r="E28" s="223"/>
-      <c r="F28" s="223"/>
-      <c r="G28" s="224"/>
+      <c r="D28" s="224"/>
+      <c r="E28" s="224"/>
+      <c r="F28" s="224"/>
+      <c r="G28" s="225"/>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="17"/>
-      <c r="C29" s="222"/>
-      <c r="D29" s="223"/>
-      <c r="E29" s="223"/>
-      <c r="F29" s="223"/>
-      <c r="G29" s="224"/>
+      <c r="C29" s="223"/>
+      <c r="D29" s="224"/>
+      <c r="E29" s="224"/>
+      <c r="F29" s="224"/>
+      <c r="G29" s="225"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="17"/>
-      <c r="C30" s="222" t="s">
+      <c r="C30" s="223" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="223"/>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="224"/>
+      <c r="D30" s="224"/>
+      <c r="E30" s="224"/>
+      <c r="F30" s="224"/>
+      <c r="G30" s="225"/>
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18"/>
-      <c r="C31" s="225"/>
-      <c r="D31" s="226"/>
-      <c r="E31" s="226"/>
-      <c r="F31" s="226"/>
-      <c r="G31" s="227"/>
+      <c r="C31" s="226"/>
+      <c r="D31" s="227"/>
+      <c r="E31" s="227"/>
+      <c r="F31" s="227"/>
+      <c r="G31" s="228"/>
       <c r="H31" s="18"/>
     </row>
   </sheetData>
@@ -10802,35 +10894,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B2" s="234" t="s">
+      <c r="B2" s="235" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="235"/>
-      <c r="D2" s="235"/>
-      <c r="E2" s="235"/>
-      <c r="F2" s="235"/>
-      <c r="G2" s="235"/>
-      <c r="H2" s="235"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
     </row>
     <row r="3" spans="2:13" ht="31.5">
-      <c r="B3" s="234"/>
-      <c r="C3" s="235" t="s">
+      <c r="B3" s="235"/>
+      <c r="C3" s="236" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="235"/>
-      <c r="E3" s="235"/>
-      <c r="F3" s="235"/>
-      <c r="G3" s="235"/>
-      <c r="H3" s="235"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="236"/>
     </row>
     <row r="4" spans="2:13" ht="16.5" customHeight="1">
-      <c r="B4" s="234"/>
-      <c r="C4" s="235"/>
-      <c r="D4" s="235"/>
-      <c r="E4" s="235"/>
-      <c r="F4" s="235"/>
-      <c r="G4" s="235"/>
-      <c r="H4" s="235"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="236"/>
+      <c r="E4" s="236"/>
+      <c r="F4" s="236"/>
+      <c r="G4" s="236"/>
+      <c r="H4" s="236"/>
     </row>
     <row r="6" spans="2:13" ht="17.25">
       <c r="B6" s="2" t="s">
@@ -10886,13 +10978,13 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="24"/>
-      <c r="C8" s="248" t="s">
+      <c r="C8" s="249" t="s">
         <v>317</v>
       </c>
-      <c r="D8" s="249"/>
-      <c r="E8" s="249"/>
-      <c r="F8" s="249"/>
-      <c r="G8" s="250"/>
+      <c r="D8" s="250"/>
+      <c r="E8" s="250"/>
+      <c r="F8" s="250"/>
+      <c r="G8" s="251"/>
       <c r="H8" s="24" t="s">
         <v>15</v>
       </c>
@@ -10902,20 +10994,20 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="24"/>
-      <c r="C9" s="251"/>
-      <c r="D9" s="252"/>
-      <c r="E9" s="252"/>
-      <c r="F9" s="252"/>
-      <c r="G9" s="253"/>
+      <c r="C9" s="252"/>
+      <c r="D9" s="253"/>
+      <c r="E9" s="253"/>
+      <c r="F9" s="253"/>
+      <c r="G9" s="254"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="24"/>
-      <c r="C10" s="251"/>
-      <c r="D10" s="252"/>
-      <c r="E10" s="252"/>
-      <c r="F10" s="252"/>
-      <c r="G10" s="253"/>
+      <c r="C10" s="252"/>
+      <c r="D10" s="253"/>
+      <c r="E10" s="253"/>
+      <c r="F10" s="253"/>
+      <c r="G10" s="254"/>
       <c r="H10" s="24"/>
       <c r="J10" s="1">
         <v>19127</v>
@@ -10926,11 +11018,11 @@
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="25"/>
-      <c r="C11" s="254"/>
-      <c r="D11" s="255"/>
-      <c r="E11" s="255"/>
-      <c r="F11" s="255"/>
-      <c r="G11" s="256"/>
+      <c r="C11" s="255"/>
+      <c r="D11" s="256"/>
+      <c r="E11" s="256"/>
+      <c r="F11" s="256"/>
+      <c r="G11" s="257"/>
       <c r="H11" s="25"/>
       <c r="J11" s="1">
         <v>18414</v>
@@ -10967,12 +11059,12 @@
       <c r="C13" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="242" t="s">
+      <c r="D13" s="243" t="s">
         <v>542</v>
       </c>
-      <c r="E13" s="243"/>
-      <c r="F13" s="243"/>
-      <c r="G13" s="244"/>
+      <c r="E13" s="244"/>
+      <c r="F13" s="244"/>
+      <c r="G13" s="245"/>
       <c r="H13" s="24" t="s">
         <v>14</v>
       </c>
@@ -10983,10 +11075,10 @@
     <row r="14" spans="2:13">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
-      <c r="D14" s="242"/>
-      <c r="E14" s="243"/>
-      <c r="F14" s="243"/>
-      <c r="G14" s="244"/>
+      <c r="D14" s="243"/>
+      <c r="E14" s="244"/>
+      <c r="F14" s="244"/>
+      <c r="G14" s="245"/>
       <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
@@ -10997,10 +11089,10 @@
     <row r="15" spans="2:13">
       <c r="B15" s="24"/>
       <c r="C15" s="61"/>
-      <c r="D15" s="242"/>
-      <c r="E15" s="243"/>
-      <c r="F15" s="243"/>
-      <c r="G15" s="244"/>
+      <c r="D15" s="243"/>
+      <c r="E15" s="244"/>
+      <c r="F15" s="244"/>
+      <c r="G15" s="245"/>
       <c r="H15" s="24"/>
       <c r="J15" s="1">
         <v>6827</v>
@@ -11009,10 +11101,10 @@
     <row r="16" spans="2:13">
       <c r="B16" s="25"/>
       <c r="C16" s="63"/>
-      <c r="D16" s="245"/>
-      <c r="E16" s="246"/>
-      <c r="F16" s="246"/>
-      <c r="G16" s="247"/>
+      <c r="D16" s="246"/>
+      <c r="E16" s="247"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="248"/>
       <c r="H16" s="25"/>
       <c r="J16" s="1">
         <v>0</v>
@@ -11063,11 +11155,11 @@
     <row r="19" spans="2:10">
       <c r="B19" s="24"/>
       <c r="C19" s="61"/>
-      <c r="D19" s="239" t="s">
+      <c r="D19" s="240" t="s">
         <v>599</v>
       </c>
-      <c r="E19" s="240"/>
-      <c r="F19" s="241"/>
+      <c r="E19" s="241"/>
+      <c r="F19" s="242"/>
       <c r="G19" s="61"/>
       <c r="H19" s="24"/>
       <c r="J19" s="1">

</xml_diff>